<commit_message>
cps include other NILF
</commit_message>
<xml_diff>
--- a/1-Data-Codes/2-Final_Data/L_1999.xlsx
+++ b/1-Data-Codes/2-Final_Data/L_1999.xlsx
@@ -446,49 +446,49 @@
         </is>
       </c>
       <c r="B2">
-        <v>439.550696856062</v>
+        <v>880.626869372828</v>
       </c>
       <c r="C2">
-        <v>39.7529242166197</v>
+        <v>32.9909579140803</v>
       </c>
       <c r="D2">
-        <v>84.8999997965967</v>
+        <v>70.8827548295604</v>
       </c>
       <c r="E2">
-        <v>94.0368544866281</v>
+        <v>78.45011750803489</v>
       </c>
       <c r="F2">
-        <v>21.7674805433987</v>
+        <v>18.0610184063369</v>
       </c>
       <c r="G2">
-        <v>29.658882741226</v>
+        <v>25.0685985958796</v>
       </c>
       <c r="H2">
-        <v>45.9569381321516</v>
+        <v>38.1171766202186</v>
       </c>
       <c r="I2">
-        <v>23.3280728772823</v>
+        <v>19.3528069798599</v>
       </c>
       <c r="J2">
-        <v>86.4032077397664</v>
+        <v>72.1265509522174</v>
       </c>
       <c r="K2">
-        <v>27.6952963002944</v>
+        <v>23.4458519567515</v>
       </c>
       <c r="L2">
-        <v>43.8114174382046</v>
+        <v>36.3640469687735</v>
       </c>
       <c r="M2">
-        <v>58.0984702616072</v>
+        <v>49.1197621695025</v>
       </c>
       <c r="N2">
-        <v>34.8916988176533</v>
+        <v>29.416542064031</v>
       </c>
       <c r="O2">
-        <v>2066.12271699213</v>
+        <v>1729.41044535951</v>
       </c>
       <c r="P2">
-        <v>54.6143841127811</v>
+        <v>47.1555427693103</v>
       </c>
     </row>
     <row r="3">
@@ -498,49 +498,49 @@
         </is>
       </c>
       <c r="B3">
-        <v>69.65697161690581</v>
+        <v>99.87958678024791</v>
       </c>
       <c r="C3">
-        <v>3.39571106666952</v>
+        <v>3.1310697155839</v>
       </c>
       <c r="D3">
-        <v>0.541737783327743</v>
+        <v>0.481454533742216</v>
       </c>
       <c r="E3">
-        <v>1.71652080238352</v>
+        <v>1.54140807849281</v>
       </c>
       <c r="F3">
-        <v>11.4122033589613</v>
+        <v>10.2812471614954</v>
       </c>
       <c r="G3">
-        <v>1.10287443024848</v>
+        <v>0.989668329299163</v>
       </c>
       <c r="H3">
-        <v>0.181335601128473</v>
+        <v>0.237845091980672</v>
       </c>
       <c r="I3">
-        <v>0.769887366969499</v>
+        <v>0.691656023427396</v>
       </c>
       <c r="J3">
-        <v>0.681741302097272</v>
+        <v>0.608622775176926</v>
       </c>
       <c r="K3">
-        <v>0.734002106925687</v>
+        <v>0.6558604586874081</v>
       </c>
       <c r="L3">
-        <v>0.433275711645637</v>
+        <v>0.38345854974616</v>
       </c>
       <c r="M3">
-        <v>1.47338848059433</v>
+        <v>1.39754100682496</v>
       </c>
       <c r="N3">
-        <v>1.26319133714609</v>
+        <v>1.13378547992054</v>
       </c>
       <c r="O3">
-        <v>300.805821189843</v>
+        <v>273.702657320687</v>
       </c>
       <c r="P3">
-        <v>11.9254641820751</v>
+        <v>10.9782647915221</v>
       </c>
     </row>
     <row r="4">
@@ -550,49 +550,49 @@
         </is>
       </c>
       <c r="B4">
-        <v>546.60678190415</v>
+        <v>910.368958813005</v>
       </c>
       <c r="C4">
-        <v>19.3098849973202</v>
+        <v>16.768934296197</v>
       </c>
       <c r="D4">
-        <v>10.9270770888138</v>
+        <v>9.491005270082811</v>
       </c>
       <c r="E4">
-        <v>15.5077547726791</v>
+        <v>13.4598550333781</v>
       </c>
       <c r="F4">
-        <v>11.3091855355207</v>
+        <v>9.819518341323819</v>
       </c>
       <c r="G4">
-        <v>16.034696086762</v>
+        <v>14.4227631604536</v>
       </c>
       <c r="H4">
-        <v>5.82756436221507</v>
+        <v>5.56493731579996</v>
       </c>
       <c r="I4">
-        <v>10.3603163240503</v>
+        <v>8.98995925864066</v>
       </c>
       <c r="J4">
-        <v>31.6959353331239</v>
+        <v>28.0111262689024</v>
       </c>
       <c r="K4">
-        <v>13.571279095973</v>
+        <v>11.7945400585141</v>
       </c>
       <c r="L4">
-        <v>110.462047543517</v>
+        <v>96.31585328265901</v>
       </c>
       <c r="M4">
-        <v>73.52224782555661</v>
+        <v>63.7780385587697</v>
       </c>
       <c r="N4">
-        <v>43.521448146487</v>
+        <v>38.2667782115534</v>
       </c>
       <c r="O4">
-        <v>2587.16805612819</v>
+        <v>2273.94114297833</v>
       </c>
       <c r="P4">
-        <v>43.1923090713892</v>
+        <v>38.0231732392639</v>
       </c>
     </row>
     <row r="5">
@@ -602,49 +602,49 @@
         </is>
       </c>
       <c r="B5">
-        <v>231.829702239487</v>
+        <v>519.660985662407</v>
       </c>
       <c r="C5">
-        <v>71.2057456456042</v>
+        <v>57.9454516682765</v>
       </c>
       <c r="D5">
-        <v>24.3143263492269</v>
+        <v>19.7978917932569</v>
       </c>
       <c r="E5">
-        <v>38.8955822903471</v>
+        <v>31.6548562224411</v>
       </c>
       <c r="F5">
-        <v>2.95800707361404</v>
+        <v>2.4270840885265</v>
       </c>
       <c r="G5">
-        <v>14.1658525869183</v>
+        <v>11.5423881087472</v>
       </c>
       <c r="H5">
-        <v>16.3156004106482</v>
+        <v>13.2824799246698</v>
       </c>
       <c r="I5">
-        <v>12.1551558521036</v>
+        <v>9.897171797936309</v>
       </c>
       <c r="J5">
-        <v>47.2443090595813</v>
+        <v>38.456006681837</v>
       </c>
       <c r="K5">
-        <v>34.1906421599367</v>
+        <v>28.1456104440175</v>
       </c>
       <c r="L5">
-        <v>33.9288628284224</v>
+        <v>27.9389976906553</v>
       </c>
       <c r="M5">
-        <v>20.3590650458094</v>
+        <v>16.5911908315753</v>
       </c>
       <c r="N5">
-        <v>24.0718722954273</v>
+        <v>19.9125323455726</v>
       </c>
       <c r="O5">
-        <v>1245.17137678331</v>
+        <v>1027.50192034216</v>
       </c>
       <c r="P5">
-        <v>52.6818506391926</v>
+        <v>44.7333825895591</v>
       </c>
     </row>
     <row r="6">
@@ -654,49 +654,49 @@
         </is>
       </c>
       <c r="B6">
-        <v>4036.05100295307</v>
+        <v>5996.69404674058</v>
       </c>
       <c r="C6">
-        <v>214.276351998491</v>
+        <v>192.70692038665</v>
       </c>
       <c r="D6">
-        <v>349.466290377014</v>
+        <v>313.74734107682</v>
       </c>
       <c r="E6">
-        <v>129.880217804304</v>
+        <v>116.296902150511</v>
       </c>
       <c r="F6">
-        <v>65.3789871280527</v>
+        <v>59.4553704754713</v>
       </c>
       <c r="G6">
-        <v>143.463282891283</v>
+        <v>128.407269089246</v>
       </c>
       <c r="H6">
-        <v>89.8389429822402</v>
+        <v>80.02307233803489</v>
       </c>
       <c r="I6">
-        <v>68.5067220474682</v>
+        <v>61.6287385347997</v>
       </c>
       <c r="J6">
-        <v>236.678367200047</v>
+        <v>211.447505772444</v>
       </c>
       <c r="K6">
-        <v>193.276342135957</v>
+        <v>175.205600103884</v>
       </c>
       <c r="L6">
-        <v>632.349724631384</v>
+        <v>565.772430070455</v>
       </c>
       <c r="M6">
-        <v>421.544834760045</v>
+        <v>377.959606451273</v>
       </c>
       <c r="N6">
-        <v>412.812732884522</v>
+        <v>370.188362569557</v>
       </c>
       <c r="O6">
-        <v>16144.4949271346</v>
+        <v>14519.4691901651</v>
       </c>
       <c r="P6">
-        <v>312.639230323526</v>
+        <v>281.655597878665</v>
       </c>
     </row>
     <row r="7">
@@ -706,49 +706,49 @@
         </is>
       </c>
       <c r="B7">
-        <v>332.770676761967</v>
+        <v>595.546369672757</v>
       </c>
       <c r="C7">
-        <v>38.6048109193713</v>
+        <v>34.933619092928</v>
       </c>
       <c r="D7">
-        <v>6.82644438552753</v>
+        <v>6.09708359714507</v>
       </c>
       <c r="E7">
-        <v>16.0054559815791</v>
+        <v>14.2989887756996</v>
       </c>
       <c r="F7">
-        <v>20.4532213193549</v>
+        <v>18.2776185660558</v>
       </c>
       <c r="G7">
-        <v>12.0875714890038</v>
+        <v>10.8031727648949</v>
       </c>
       <c r="H7">
-        <v>12.3226054797119</v>
+        <v>11.0136620590001</v>
       </c>
       <c r="I7">
-        <v>12.2413407528131</v>
+        <v>10.9418232246552</v>
       </c>
       <c r="J7">
-        <v>25.8684623080091</v>
+        <v>23.120520984079</v>
       </c>
       <c r="K7">
-        <v>29.1199720258262</v>
+        <v>26.4542131806825</v>
       </c>
       <c r="L7">
-        <v>78.0661646119613</v>
+        <v>70.63250611858121</v>
       </c>
       <c r="M7">
-        <v>27.6642113087002</v>
+        <v>24.721089358147</v>
       </c>
       <c r="N7">
-        <v>44.8246257764524</v>
+        <v>40.069820607378</v>
       </c>
       <c r="O7">
-        <v>2337.18669675397</v>
+        <v>2109.72088513858</v>
       </c>
       <c r="P7">
-        <v>28.7128305672375</v>
+        <v>26.1237166209137</v>
       </c>
     </row>
     <row r="8">
@@ -758,49 +758,49 @@
         </is>
       </c>
       <c r="B8">
-        <v>274.854204271769</v>
+        <v>480.541030086974</v>
       </c>
       <c r="C8">
-        <v>18.6264708049117</v>
+        <v>17.1396514165494</v>
       </c>
       <c r="D8">
-        <v>10.4160944648717</v>
+        <v>9.316977391856771</v>
       </c>
       <c r="E8">
-        <v>14.9442512189751</v>
+        <v>13.3764806062381</v>
       </c>
       <c r="F8">
-        <v>3.23237031727372</v>
+        <v>2.8933745692754</v>
       </c>
       <c r="G8">
-        <v>38.2958187205528</v>
+        <v>34.288450969646</v>
       </c>
       <c r="H8">
-        <v>16.3774217554725</v>
+        <v>14.6607347854669</v>
       </c>
       <c r="I8">
-        <v>2.26793438422228</v>
+        <v>2.02864669497607</v>
       </c>
       <c r="J8">
-        <v>50.9255523911951</v>
+        <v>46.9909980511296</v>
       </c>
       <c r="K8">
-        <v>52.465601490369</v>
+        <v>46.9748460106991</v>
       </c>
       <c r="L8">
-        <v>50.2782604631957</v>
+        <v>45.0097607812675</v>
       </c>
       <c r="M8">
-        <v>77.4699572645827</v>
+        <v>70.75720444612981</v>
       </c>
       <c r="N8">
-        <v>51.6665717010271</v>
+        <v>46.2549817345791</v>
       </c>
       <c r="O8">
-        <v>1741.7362359451</v>
+        <v>1574.08598332351</v>
       </c>
       <c r="P8">
-        <v>7.27073998313657</v>
+        <v>6.50836525532381</v>
       </c>
     </row>
     <row r="9">
@@ -810,49 +810,49 @@
         </is>
       </c>
       <c r="B9">
-        <v>60.6282374930436</v>
+        <v>120.323835799842</v>
       </c>
       <c r="C9">
-        <v>8.83843926403892</v>
+        <v>7.77883512021922</v>
       </c>
       <c r="D9">
-        <v>1.97337715132316</v>
+        <v>1.71285511502378</v>
       </c>
       <c r="E9">
-        <v>4.83210945298075</v>
+        <v>4.19053516875917</v>
       </c>
       <c r="F9">
-        <v>2.80525716695778</v>
+        <v>2.43298438201349</v>
       </c>
       <c r="G9">
-        <v>28.2870704385185</v>
+        <v>24.6381490739067</v>
       </c>
       <c r="H9">
-        <v>4.27599205658637</v>
+        <v>3.82179671062446</v>
       </c>
       <c r="I9">
-        <v>0.8546372696672711</v>
+        <v>0.742122702190297</v>
       </c>
       <c r="J9">
-        <v>3.72811569900723</v>
+        <v>3.34837820807518</v>
       </c>
       <c r="K9">
-        <v>4.629674593173</v>
+        <v>4.01551225726424</v>
       </c>
       <c r="L9">
-        <v>3.8025153933286</v>
+        <v>3.29912678050639</v>
       </c>
       <c r="M9">
-        <v>10.310252597922</v>
+        <v>9.053620318312159</v>
       </c>
       <c r="N9">
-        <v>5.85046986008488</v>
+        <v>5.07379343271493</v>
       </c>
       <c r="O9">
-        <v>403.374186767496</v>
+        <v>354.289117816761</v>
       </c>
       <c r="P9">
-        <v>6.5703979642099</v>
+        <v>6.04007008582979</v>
       </c>
     </row>
     <row r="10">
@@ -862,49 +862,49 @@
         </is>
       </c>
       <c r="B10">
-        <v>1576.08273957645</v>
+        <v>2922.3197780863</v>
       </c>
       <c r="C10">
-        <v>73.9502583092906</v>
+        <v>63.7647807652841</v>
       </c>
       <c r="D10">
-        <v>56.5361409667909</v>
+        <v>49.4087402680209</v>
       </c>
       <c r="E10">
-        <v>56.1026227594654</v>
+        <v>49.0266326424347</v>
       </c>
       <c r="F10">
-        <v>11.9221908643199</v>
+        <v>10.2120844845851</v>
       </c>
       <c r="G10">
-        <v>54.1539870084222</v>
+        <v>46.3140031821666</v>
       </c>
       <c r="H10">
-        <v>30.6403967730364</v>
+        <v>26.7295613696293</v>
       </c>
       <c r="I10">
-        <v>50.7338530772043</v>
+        <v>43.3536493701569</v>
       </c>
       <c r="J10">
-        <v>62.7878533710905</v>
+        <v>54.240070660702</v>
       </c>
       <c r="K10">
-        <v>68.2572082126463</v>
+        <v>58.9052741638122</v>
       </c>
       <c r="L10">
-        <v>168.38002885741</v>
+        <v>144.4464558569</v>
       </c>
       <c r="M10">
-        <v>121.284195335544</v>
+        <v>104.759874144099</v>
       </c>
       <c r="N10">
-        <v>133.143464746784</v>
+        <v>114.869550370995</v>
       </c>
       <c r="O10">
-        <v>8945.906007069731</v>
+        <v>7734.83247631022</v>
       </c>
       <c r="P10">
-        <v>106.753522546073</v>
+        <v>93.4515373249847</v>
       </c>
     </row>
     <row r="11">
@@ -914,49 +914,49 @@
         </is>
       </c>
       <c r="B11">
-        <v>708.13115433275</v>
+        <v>1325.24094592297</v>
       </c>
       <c r="C11">
-        <v>83.6741122646164</v>
+        <v>73.882054419531</v>
       </c>
       <c r="D11">
-        <v>208.977490788622</v>
+        <v>181.774724156334</v>
       </c>
       <c r="E11">
-        <v>119.195972348976</v>
+        <v>103.970154958801</v>
       </c>
       <c r="F11">
-        <v>10.9824894900382</v>
+        <v>9.51769287565074</v>
       </c>
       <c r="G11">
-        <v>44.7898062882644</v>
+        <v>39.4989903842233</v>
       </c>
       <c r="H11">
-        <v>25.5556769674866</v>
+        <v>22.1371808142329</v>
       </c>
       <c r="I11">
-        <v>22.015754322755</v>
+        <v>19.0776520893582</v>
       </c>
       <c r="J11">
-        <v>65.2493750898434</v>
+        <v>56.5430065568769</v>
       </c>
       <c r="K11">
-        <v>62.7569786164996</v>
+        <v>54.3841164828221</v>
       </c>
       <c r="L11">
-        <v>90.0178906967333</v>
+        <v>78.013596009998</v>
       </c>
       <c r="M11">
-        <v>67.1721962897232</v>
+        <v>58.2163600024796</v>
       </c>
       <c r="N11">
-        <v>73.8952243525826</v>
+        <v>64.7277122831393</v>
       </c>
       <c r="O11">
-        <v>4051.5414457753</v>
+        <v>3550.40769025899</v>
       </c>
       <c r="P11">
-        <v>41.4663479362527</v>
+        <v>38.0300389316832</v>
       </c>
     </row>
     <row r="12">
@@ -966,49 +966,49 @@
         </is>
       </c>
       <c r="B12">
-        <v>127.009025175124</v>
+        <v>196.659707752949</v>
       </c>
       <c r="C12">
-        <v>13.336306195092</v>
+        <v>11.9745800454517</v>
       </c>
       <c r="D12">
-        <v>4.50975125666041</v>
+        <v>4.04648422342273</v>
       </c>
       <c r="E12">
-        <v>0.912496905824525</v>
+        <v>0.816252806555824</v>
       </c>
       <c r="F12">
-        <v>1.40590970992187</v>
+        <v>1.26040316531491</v>
       </c>
       <c r="G12">
-        <v>1.11909329667189</v>
+        <v>1.00202072317796</v>
       </c>
       <c r="H12">
-        <v>0.362454891053192</v>
+        <v>0.324106183104064</v>
       </c>
       <c r="I12">
-        <v>1.89204970974556</v>
+        <v>1.69778358735847</v>
       </c>
       <c r="J12">
-        <v>1.24950610805329</v>
+        <v>1.11854014011125</v>
       </c>
       <c r="K12">
-        <v>0.7585913835760501</v>
+        <v>0.679380169298104</v>
       </c>
       <c r="L12">
-        <v>1.12966573211168</v>
+        <v>1.00890013650881</v>
       </c>
       <c r="M12">
-        <v>5.7774828799816</v>
+        <v>5.18582426524184</v>
       </c>
       <c r="N12">
-        <v>4.24282093776494</v>
+        <v>3.80715123922989</v>
       </c>
       <c r="O12">
-        <v>668.490717898108</v>
+        <v>603.607857297338</v>
       </c>
       <c r="P12">
-        <v>21.4244220964293</v>
+        <v>20.4313030617076</v>
       </c>
     </row>
     <row r="13">
@@ -1018,49 +1018,49 @@
         </is>
       </c>
       <c r="B13">
-        <v>118.089406312842</v>
+        <v>198.121546975493</v>
       </c>
       <c r="C13">
-        <v>30.5723109939428</v>
+        <v>27.3351568897384</v>
       </c>
       <c r="D13">
-        <v>2.38554816513682</v>
+        <v>2.12136120194854</v>
       </c>
       <c r="E13">
-        <v>17.7189526779882</v>
+        <v>15.8958667734533</v>
       </c>
       <c r="F13">
-        <v>5.80512995732899</v>
+        <v>5.16640168467483</v>
       </c>
       <c r="G13">
-        <v>6.20279901246013</v>
+        <v>5.51940527616049</v>
       </c>
       <c r="H13">
-        <v>2.55113254377667</v>
+        <v>2.26927567228706</v>
       </c>
       <c r="I13">
-        <v>2.41468925130346</v>
+        <v>2.14810757581839</v>
       </c>
       <c r="J13">
-        <v>6.67822955528653</v>
+        <v>5.94235979288646</v>
       </c>
       <c r="K13">
-        <v>5.58441360042247</v>
+        <v>4.96982278396638</v>
       </c>
       <c r="L13">
-        <v>31.1371331165029</v>
+        <v>28.0932669217353</v>
       </c>
       <c r="M13">
-        <v>5.25872045174611</v>
+        <v>4.67993563878822</v>
       </c>
       <c r="N13">
-        <v>7.71968367662897</v>
+        <v>6.87021538399899</v>
       </c>
       <c r="O13">
-        <v>594.930081512261</v>
+        <v>533.4171594384191</v>
       </c>
       <c r="P13">
-        <v>54.6834317792086</v>
+        <v>49.1817806350607</v>
       </c>
     </row>
     <row r="14">
@@ -1070,49 +1070,49 @@
         </is>
       </c>
       <c r="B14">
-        <v>1184.38855699652</v>
+        <v>1927.56779707315</v>
       </c>
       <c r="C14">
-        <v>141.299330743881</v>
+        <v>126.784990628812</v>
       </c>
       <c r="D14">
-        <v>22.8090871574875</v>
+        <v>20.3755751182095</v>
       </c>
       <c r="E14">
-        <v>70.6848088917596</v>
+        <v>63.1830810756283</v>
       </c>
       <c r="F14">
-        <v>18.8985447874614</v>
+        <v>17.3357605370785</v>
       </c>
       <c r="G14">
-        <v>128.710424037931</v>
+        <v>115.974981500317</v>
       </c>
       <c r="H14">
-        <v>68.90221590694939</v>
+        <v>62.046876173648</v>
       </c>
       <c r="I14">
-        <v>41.7128371863914</v>
+        <v>37.292601766527</v>
       </c>
       <c r="J14">
-        <v>167.388120645409</v>
+        <v>150.999347704135</v>
       </c>
       <c r="K14">
-        <v>231.146061678002</v>
+        <v>208.468365585892</v>
       </c>
       <c r="L14">
-        <v>200.619709602356</v>
+        <v>179.815018050927</v>
       </c>
       <c r="M14">
-        <v>111.397942203179</v>
+        <v>99.5792257257807</v>
       </c>
       <c r="N14">
-        <v>114.86539657266</v>
+        <v>102.684668399769</v>
       </c>
       <c r="O14">
-        <v>6214.21184077542</v>
+        <v>5609.05174601724</v>
       </c>
       <c r="P14">
-        <v>43.5161279784771</v>
+        <v>39.390970477924</v>
       </c>
     </row>
     <row r="15">
@@ -1122,49 +1122,49 @@
         </is>
       </c>
       <c r="B15">
-        <v>519.046360541961</v>
+        <v>947.433184502429</v>
       </c>
       <c r="C15">
-        <v>38.5252444281453</v>
+        <v>34.4086180631402</v>
       </c>
       <c r="D15">
-        <v>18.1219452306009</v>
+        <v>15.8690461158909</v>
       </c>
       <c r="E15">
-        <v>66.7987632830754</v>
+        <v>58.5162172267104</v>
       </c>
       <c r="F15">
-        <v>16.2594827229902</v>
+        <v>14.2453903641304</v>
       </c>
       <c r="G15">
-        <v>53.2889249165507</v>
+        <v>47.3415112955349</v>
       </c>
       <c r="H15">
-        <v>58.2238356213839</v>
+        <v>51.661034487475</v>
       </c>
       <c r="I15">
-        <v>54.3001509043537</v>
+        <v>47.5687882969829</v>
       </c>
       <c r="J15">
-        <v>227.33668904646</v>
+        <v>200.476069137659</v>
       </c>
       <c r="K15">
-        <v>124.824085196695</v>
+        <v>111.326648381254</v>
       </c>
       <c r="L15">
-        <v>80.30130472557789</v>
+        <v>71.66427387001799</v>
       </c>
       <c r="M15">
-        <v>181.608102230727</v>
+        <v>162.379906831843</v>
       </c>
       <c r="N15">
-        <v>114.218753019483</v>
+        <v>100.720191404153</v>
       </c>
       <c r="O15">
-        <v>2691.01103279885</v>
+        <v>2383.96939774711</v>
       </c>
       <c r="P15">
-        <v>51.3584092268481</v>
+        <v>47.6428069096457</v>
       </c>
     </row>
     <row r="16">
@@ -1174,49 +1174,49 @@
         </is>
       </c>
       <c r="B16">
-        <v>169.967067819565</v>
+        <v>334.014791003096</v>
       </c>
       <c r="C16">
-        <v>71.4678710509581</v>
+        <v>65.3586681723006</v>
       </c>
       <c r="D16">
-        <v>17.7512310938474</v>
+        <v>16.0645463924195</v>
       </c>
       <c r="E16">
-        <v>17.8540908052749</v>
+        <v>16.1575315359967</v>
       </c>
       <c r="F16">
-        <v>5.27377579626386</v>
+        <v>4.77262665244336</v>
       </c>
       <c r="G16">
-        <v>17.4603716109142</v>
+        <v>15.8039386015776</v>
       </c>
       <c r="H16">
-        <v>16.630160027489</v>
+        <v>15.053460585439</v>
       </c>
       <c r="I16">
-        <v>12.1876207302271</v>
+        <v>11.0320240129759</v>
       </c>
       <c r="J16">
-        <v>49.7304425923856</v>
+        <v>45.0169460897291</v>
       </c>
       <c r="K16">
-        <v>60.7302965398834</v>
+        <v>55.6367233620095</v>
       </c>
       <c r="L16">
-        <v>35.7518590162278</v>
+        <v>32.6855241761649</v>
       </c>
       <c r="M16">
-        <v>16.3378346086902</v>
+        <v>14.7788097336027</v>
       </c>
       <c r="N16">
-        <v>32.6576910041027</v>
+        <v>29.558460996696</v>
       </c>
       <c r="O16">
-        <v>1436.84025638715</v>
+        <v>1312.10370414818</v>
       </c>
       <c r="P16">
-        <v>102.613716727444</v>
+        <v>95.2165300168148</v>
       </c>
     </row>
     <row r="17">
@@ -1226,49 +1226,49 @@
         </is>
       </c>
       <c r="B17">
-        <v>201.578260669119</v>
+        <v>354.118436693893</v>
       </c>
       <c r="C17">
-        <v>30.4257967860101</v>
+        <v>27.4930425509592</v>
       </c>
       <c r="D17">
-        <v>8.88915379381797</v>
+        <v>8.027592137719891</v>
       </c>
       <c r="E17">
-        <v>10.7632546282208</v>
+        <v>9.715500851299209</v>
       </c>
       <c r="F17">
-        <v>14.4102294588512</v>
+        <v>13.0143011403895</v>
       </c>
       <c r="G17">
-        <v>13.8046067803039</v>
+        <v>12.4711187378769</v>
       </c>
       <c r="H17">
-        <v>9.58874774158811</v>
+        <v>8.657249488025229</v>
       </c>
       <c r="I17">
-        <v>8.79300215525185</v>
+        <v>7.94405551882832</v>
       </c>
       <c r="J17">
-        <v>22.3404640501746</v>
+        <v>20.4849316858812</v>
       </c>
       <c r="K17">
-        <v>27.8014733865941</v>
+        <v>25.1178273075355</v>
       </c>
       <c r="L17">
-        <v>15.6842786906978</v>
+        <v>14.156652696269</v>
       </c>
       <c r="M17">
-        <v>87.1416751066531</v>
+        <v>79.08275177754589</v>
       </c>
       <c r="N17">
-        <v>18.1110430821918</v>
+        <v>16.3583470321655</v>
       </c>
       <c r="O17">
-        <v>1349.4036165051</v>
+        <v>1226.63042760495</v>
       </c>
       <c r="P17">
-        <v>63.3031201795329</v>
+        <v>58.7664870858442</v>
       </c>
     </row>
     <row r="18">
@@ -1278,49 +1278,49 @@
         </is>
       </c>
       <c r="B18">
-        <v>435.646838059019</v>
+        <v>839.14776350022</v>
       </c>
       <c r="C18">
-        <v>39.3298357835196</v>
+        <v>32.5520903361579</v>
       </c>
       <c r="D18">
-        <v>22.3553191624801</v>
+        <v>18.5103252527292</v>
       </c>
       <c r="E18">
-        <v>35.6180301422424</v>
+        <v>30.351636034262</v>
       </c>
       <c r="F18">
-        <v>47.525305752052</v>
+        <v>40.6263072121668</v>
       </c>
       <c r="G18">
-        <v>39.8632885354194</v>
+        <v>32.9905227833032</v>
       </c>
       <c r="H18">
-        <v>25.4359355764698</v>
+        <v>21.0551609636316</v>
       </c>
       <c r="I18">
-        <v>11.5202302228586</v>
+        <v>9.541441526527009</v>
       </c>
       <c r="J18">
-        <v>38.9250600127937</v>
+        <v>32.246398546898</v>
       </c>
       <c r="K18">
-        <v>46.1214699680331</v>
+        <v>38.1872555986806</v>
       </c>
       <c r="L18">
-        <v>54.5536151352576</v>
+        <v>46.4703593380309</v>
       </c>
       <c r="M18">
-        <v>70.9274658979156</v>
+        <v>58.7227117583695</v>
       </c>
       <c r="N18">
-        <v>26.4607954274973</v>
+        <v>22.3615843147832</v>
       </c>
       <c r="O18">
-        <v>1945.89441494702</v>
+        <v>1623.34265454442</v>
       </c>
       <c r="P18">
-        <v>54.8353297612951</v>
+        <v>48.9067233638985</v>
       </c>
     </row>
     <row r="19">
@@ -1330,49 +1330,49 @@
         </is>
       </c>
       <c r="B19">
-        <v>539.4223487442609</v>
+        <v>914.082123620849</v>
       </c>
       <c r="C19">
-        <v>34.1012732028344</v>
+        <v>29.2245753872958</v>
       </c>
       <c r="D19">
-        <v>20.3005885278443</v>
+        <v>17.1051421055931</v>
       </c>
       <c r="E19">
-        <v>28.5280095994035</v>
+        <v>24.023479670697</v>
       </c>
       <c r="F19">
-        <v>112.307589703786</v>
+        <v>96.0301099301853</v>
       </c>
       <c r="G19">
-        <v>51.0786732575551</v>
+        <v>43.0037095628364</v>
       </c>
       <c r="H19">
-        <v>7.45181776898328</v>
+        <v>6.28146006319015</v>
       </c>
       <c r="I19">
-        <v>9.76712368284066</v>
+        <v>8.228509623541029</v>
       </c>
       <c r="J19">
-        <v>15.5857250408936</v>
+        <v>13.6429414149605</v>
       </c>
       <c r="K19">
-        <v>16.7931005023012</v>
+        <v>14.1589314015608</v>
       </c>
       <c r="L19">
-        <v>9.997713719547111</v>
+        <v>8.955013198010111</v>
       </c>
       <c r="M19">
-        <v>31.6255245498183</v>
+        <v>27.1378029127332</v>
       </c>
       <c r="N19">
-        <v>12.0263277531223</v>
+        <v>10.1461408753343</v>
       </c>
       <c r="O19">
-        <v>2145.99753356136</v>
+        <v>1827.93361602091</v>
       </c>
       <c r="P19">
-        <v>44.3488322747907</v>
+        <v>39.3786296577106</v>
       </c>
     </row>
     <row r="20">
@@ -1382,49 +1382,49 @@
         </is>
       </c>
       <c r="B20">
-        <v>97.8357889749484</v>
+        <v>201.378971010919</v>
       </c>
       <c r="C20">
-        <v>10.626967743248</v>
+        <v>9.365039611076149</v>
       </c>
       <c r="D20">
-        <v>21.0891784986153</v>
+        <v>18.4177024306412</v>
       </c>
       <c r="E20">
-        <v>37.2719957726578</v>
+        <v>32.4280578632098</v>
       </c>
       <c r="F20">
-        <v>0.7947958831681921</v>
+        <v>0.689078879378622</v>
       </c>
       <c r="G20">
-        <v>1.66464688838034</v>
+        <v>1.44366432813385</v>
       </c>
       <c r="H20">
-        <v>4.79530955230874</v>
+        <v>4.31386041274117</v>
       </c>
       <c r="I20">
-        <v>1.01452264581123</v>
+        <v>0.879587283620681</v>
       </c>
       <c r="J20">
-        <v>4.02058923255072</v>
+        <v>3.48698269628341</v>
       </c>
       <c r="K20">
-        <v>5.89677058797119</v>
+        <v>5.27104975375041</v>
       </c>
       <c r="L20">
-        <v>11.0926367592814</v>
+        <v>9.61149560809611</v>
       </c>
       <c r="M20">
-        <v>25.6504321085559</v>
+        <v>22.2088643137272</v>
       </c>
       <c r="N20">
-        <v>5.92089638114851</v>
+        <v>5.29291015138251</v>
       </c>
       <c r="O20">
-        <v>667.67231666675</v>
+        <v>582.918692080631</v>
       </c>
       <c r="P20">
-        <v>24.7992771138158</v>
+        <v>22.4401685282581</v>
       </c>
     </row>
     <row r="21">
@@ -1434,49 +1434,49 @@
         </is>
       </c>
       <c r="B21">
-        <v>480.907060604583</v>
+        <v>839.039684615126</v>
       </c>
       <c r="C21">
-        <v>35.6617413444163</v>
+        <v>32.0951581235593</v>
       </c>
       <c r="D21">
-        <v>12.2457446887887</v>
+        <v>10.7517649835086</v>
       </c>
       <c r="E21">
-        <v>21.2233525152203</v>
+        <v>19.3885786529658</v>
       </c>
       <c r="F21">
-        <v>3.84602112847336</v>
+        <v>3.37496289729722</v>
       </c>
       <c r="G21">
-        <v>25.5213286321971</v>
+        <v>22.4313915003937</v>
       </c>
       <c r="H21">
-        <v>12.3611467585171</v>
+        <v>10.8611507230871</v>
       </c>
       <c r="I21">
-        <v>10.5390633980862</v>
+        <v>9.26195844816591</v>
       </c>
       <c r="J21">
-        <v>24.0563775828897</v>
+        <v>21.1408438026066</v>
       </c>
       <c r="K21">
-        <v>21.3844708354736</v>
+        <v>18.7921080515391</v>
       </c>
       <c r="L21">
-        <v>34.4648870534185</v>
+        <v>30.291323394083</v>
       </c>
       <c r="M21">
-        <v>43.6802496304524</v>
+        <v>38.3927753795673</v>
       </c>
       <c r="N21">
-        <v>21.5213707646989</v>
+        <v>18.9154100606515</v>
       </c>
       <c r="O21">
-        <v>2946.19996745527</v>
+        <v>2622.35987584634</v>
       </c>
       <c r="P21">
-        <v>28.9465597148108</v>
+        <v>25.4623555759288</v>
       </c>
     </row>
     <row r="22">
@@ -1486,49 +1486,49 @@
         </is>
       </c>
       <c r="B22">
-        <v>492.594081325675</v>
+        <v>948.118627037897</v>
       </c>
       <c r="C22">
-        <v>24.924086929453</v>
+        <v>21.939177866103</v>
       </c>
       <c r="D22">
-        <v>41.8819446235472</v>
+        <v>37.2519051181855</v>
       </c>
       <c r="E22">
-        <v>33.8727549510657</v>
+        <v>30.207788158726</v>
       </c>
       <c r="F22">
-        <v>3.88743262099113</v>
+        <v>3.42214774517</v>
       </c>
       <c r="G22">
-        <v>40.6497699444217</v>
+        <v>35.7757424184891</v>
       </c>
       <c r="H22">
-        <v>38.5324168941712</v>
+        <v>33.9109595802639</v>
       </c>
       <c r="I22">
-        <v>10.7847510037518</v>
+        <v>9.889006029960409</v>
       </c>
       <c r="J22">
-        <v>65.4229697055268</v>
+        <v>58.3793766255936</v>
       </c>
       <c r="K22">
-        <v>60.9712370206511</v>
+        <v>53.6604932339116</v>
       </c>
       <c r="L22">
-        <v>150.664935623388</v>
+        <v>133.393081444068</v>
       </c>
       <c r="M22">
-        <v>27.0270896928369</v>
+        <v>23.7895461993814</v>
       </c>
       <c r="N22">
-        <v>114.168100655328</v>
+        <v>100.476721970467</v>
       </c>
       <c r="O22">
-        <v>3430.1040199199</v>
+        <v>3048.2067669042</v>
       </c>
       <c r="P22">
-        <v>24.6153338856538</v>
+        <v>21.6795842878557</v>
       </c>
     </row>
     <row r="23">
@@ -1538,49 +1538,49 @@
         </is>
       </c>
       <c r="B23">
-        <v>905.128123656388</v>
+        <v>1622.72451377556</v>
       </c>
       <c r="C23">
-        <v>60.2445797255618</v>
+        <v>52.569487289442</v>
       </c>
       <c r="D23">
-        <v>19.7064441167877</v>
+        <v>17.1916509474503</v>
       </c>
       <c r="E23">
-        <v>44.8163846471369</v>
+        <v>39.1011918870334</v>
       </c>
       <c r="F23">
-        <v>4.24603548190353</v>
+        <v>4.12544239150013</v>
       </c>
       <c r="G23">
-        <v>78.1437816215099</v>
+        <v>68.1829529701774</v>
       </c>
       <c r="H23">
-        <v>81.5978633243644</v>
+        <v>71.1903106234081</v>
       </c>
       <c r="I23">
-        <v>26.7113001991899</v>
+        <v>23.3059147059899</v>
       </c>
       <c r="J23">
-        <v>188.730223876498</v>
+        <v>167.153667737721</v>
       </c>
       <c r="K23">
-        <v>179.57465553681</v>
+        <v>157.509112593937</v>
       </c>
       <c r="L23">
-        <v>62.9360314812464</v>
+        <v>55.7499113106022</v>
       </c>
       <c r="M23">
-        <v>701.936293827358</v>
+        <v>616.954736008991</v>
       </c>
       <c r="N23">
-        <v>122.013324248371</v>
+        <v>106.870679718288</v>
       </c>
       <c r="O23">
-        <v>4486.91689685019</v>
+        <v>3964.49721238944</v>
       </c>
       <c r="P23">
-        <v>47.9899071967306</v>
+        <v>43.5650617302365</v>
       </c>
     </row>
     <row r="24">
@@ -1590,49 +1590,49 @@
         </is>
       </c>
       <c r="B24">
-        <v>319.794876179674</v>
+        <v>566.460542245841</v>
       </c>
       <c r="C24">
-        <v>49.9454846420063</v>
+        <v>45.7309228151562</v>
       </c>
       <c r="D24">
-        <v>14.9779855422997</v>
+        <v>13.7094547959318</v>
       </c>
       <c r="E24">
-        <v>46.6692168361617</v>
+        <v>42.7285289236648</v>
       </c>
       <c r="F24">
-        <v>17.5338813434414</v>
+        <v>16.0536317488587</v>
       </c>
       <c r="G24">
-        <v>30.289887711489</v>
+        <v>27.7314396215158</v>
       </c>
       <c r="H24">
-        <v>25.4512417303042</v>
+        <v>23.7819399801807</v>
       </c>
       <c r="I24">
-        <v>16.992011823301</v>
+        <v>15.5573406721035</v>
       </c>
       <c r="J24">
-        <v>43.8327137943043</v>
+        <v>40.1267388495266</v>
       </c>
       <c r="K24">
-        <v>107.742976675127</v>
+        <v>98.6633781603317</v>
       </c>
       <c r="L24">
-        <v>74.8692072104558</v>
+        <v>68.5445160233035</v>
       </c>
       <c r="M24">
-        <v>21.987764955433</v>
+        <v>20.108825168259</v>
       </c>
       <c r="N24">
-        <v>97.1402913298796</v>
+        <v>88.94693247575481</v>
       </c>
       <c r="O24">
-        <v>2489.6375148546</v>
+        <v>2296.19188245015</v>
       </c>
       <c r="P24">
-        <v>100.201673579626</v>
+        <v>92.7306544809347</v>
       </c>
     </row>
     <row r="25">
@@ -1642,49 +1642,49 @@
         </is>
       </c>
       <c r="B25">
-        <v>282.986320368274</v>
+        <v>539.385026097631</v>
       </c>
       <c r="C25">
-        <v>55.0752827150305</v>
+        <v>46.518841542389</v>
       </c>
       <c r="D25">
-        <v>22.54459547836</v>
+        <v>19.4577660142224</v>
       </c>
       <c r="E25">
-        <v>47.5622925555812</v>
+        <v>39.9189883291451</v>
       </c>
       <c r="F25">
-        <v>32.958103775388</v>
+        <v>27.4283450604598</v>
       </c>
       <c r="G25">
-        <v>12.0566724024917</v>
+        <v>10.3878071526179</v>
       </c>
       <c r="H25">
-        <v>19.8409559784456</v>
+        <v>16.5092530489047</v>
       </c>
       <c r="I25">
-        <v>6.01539930308926</v>
+        <v>5.35568890154511</v>
       </c>
       <c r="J25">
-        <v>23.4433215582591</v>
+        <v>19.8640422235227</v>
       </c>
       <c r="K25">
-        <v>27.158187353942</v>
+        <v>22.6051898374343</v>
       </c>
       <c r="L25">
-        <v>34.6903744141583</v>
+        <v>29.5678561473986</v>
       </c>
       <c r="M25">
-        <v>41.4543915068314</v>
+        <v>34.5020664362315</v>
       </c>
       <c r="N25">
-        <v>36.7034944885874</v>
+        <v>30.5434465793455</v>
       </c>
       <c r="O25">
-        <v>1248.1722226997</v>
+        <v>1055.01721036501</v>
       </c>
       <c r="P25">
-        <v>52.6923046191807</v>
+        <v>46.2923913502756</v>
       </c>
     </row>
     <row r="26">
@@ -1694,49 +1694,49 @@
         </is>
       </c>
       <c r="B26">
-        <v>430.379413397833</v>
+        <v>808.305760752846</v>
       </c>
       <c r="C26">
-        <v>73.2255539246631</v>
+        <v>65.6489635658512</v>
       </c>
       <c r="D26">
-        <v>18.7984783576418</v>
+        <v>16.6689414873</v>
       </c>
       <c r="E26">
-        <v>43.4619626894183</v>
+        <v>38.5434779604663</v>
       </c>
       <c r="F26">
-        <v>8.32607087807941</v>
+        <v>7.38526672977478</v>
       </c>
       <c r="G26">
-        <v>52.9466671304979</v>
+        <v>46.9619887546387</v>
       </c>
       <c r="H26">
-        <v>23.4566381543458</v>
+        <v>20.8029442195974</v>
       </c>
       <c r="I26">
-        <v>18.5864811084889</v>
+        <v>16.4844045802342</v>
       </c>
       <c r="J26">
-        <v>67.71842419826611</v>
+        <v>60.0636141435348</v>
       </c>
       <c r="K26">
-        <v>66.1747741508479</v>
+        <v>59.4012337450077</v>
       </c>
       <c r="L26">
-        <v>39.3516754547724</v>
+        <v>34.9002288991616</v>
       </c>
       <c r="M26">
-        <v>83.16675573902541</v>
+        <v>75.8773583158338</v>
       </c>
       <c r="N26">
-        <v>46.2036257893663</v>
+        <v>40.977920812906</v>
       </c>
       <c r="O26">
-        <v>2914.93363481855</v>
+        <v>2600.31751223387</v>
       </c>
       <c r="P26">
-        <v>56.1626872595482</v>
+        <v>50.5532270552522</v>
       </c>
     </row>
     <row r="27">
@@ -1746,49 +1746,49 @@
         </is>
       </c>
       <c r="B27">
-        <v>78.0077773430523</v>
+        <v>140.573751363302</v>
       </c>
       <c r="C27">
-        <v>4.49837680444406</v>
+        <v>3.96124892551835</v>
       </c>
       <c r="D27">
-        <v>1.23970433257735</v>
+        <v>1.09112742918001</v>
       </c>
       <c r="E27">
-        <v>13.6811211215299</v>
+        <v>12.0415246270566</v>
       </c>
       <c r="F27">
-        <v>7.6188550376746</v>
+        <v>6.70618606602504</v>
       </c>
       <c r="G27">
-        <v>0.797715708176084</v>
+        <v>0.702513597448498</v>
       </c>
       <c r="H27">
-        <v>0.416171820842229</v>
+        <v>0.366534921712657</v>
       </c>
       <c r="I27">
-        <v>2.60128319708854</v>
+        <v>2.28920924558393</v>
       </c>
       <c r="J27">
-        <v>5.50977665643178</v>
+        <v>4.94638886359155</v>
       </c>
       <c r="K27">
-        <v>2.28214608109716</v>
+        <v>2.01042806832806</v>
       </c>
       <c r="L27">
-        <v>2.81508029739535</v>
+        <v>2.48192501502413</v>
       </c>
       <c r="M27">
-        <v>1.71938942020242</v>
+        <v>1.51664672801614</v>
       </c>
       <c r="N27">
-        <v>7.04018464371605</v>
+        <v>6.19796791347159</v>
       </c>
       <c r="O27">
-        <v>467.048871924523</v>
+        <v>415.685674299533</v>
       </c>
       <c r="P27">
-        <v>47.443440921418</v>
+        <v>42.1487680913994</v>
       </c>
     </row>
     <row r="28">
@@ -1798,49 +1798,49 @@
         </is>
       </c>
       <c r="B28">
-        <v>101.875042676824</v>
+        <v>189.496183339868</v>
       </c>
       <c r="C28">
-        <v>30.2407678543083</v>
+        <v>28.0044262889178</v>
       </c>
       <c r="D28">
-        <v>3.27896792061558</v>
+        <v>2.99106869478376</v>
       </c>
       <c r="E28">
-        <v>6.19739152829163</v>
+        <v>5.65711782095564</v>
       </c>
       <c r="F28">
-        <v>2.86557811450783</v>
+        <v>2.61335902780851</v>
       </c>
       <c r="G28">
-        <v>8.224379344218249</v>
+        <v>7.5107813907564</v>
       </c>
       <c r="H28">
-        <v>9.394126654468961</v>
+        <v>8.581816203238869</v>
       </c>
       <c r="I28">
-        <v>4.6550168306468</v>
+        <v>4.43833831919274</v>
       </c>
       <c r="J28">
-        <v>17.064081921672</v>
+        <v>15.5840992373442</v>
       </c>
       <c r="K28">
-        <v>18.2890687209292</v>
+        <v>16.7069225200633</v>
       </c>
       <c r="L28">
-        <v>14.89969937538</v>
+        <v>13.7912766564364</v>
       </c>
       <c r="M28">
-        <v>7.65193797006868</v>
+        <v>6.98234176006313</v>
       </c>
       <c r="N28">
-        <v>13.3308052229051</v>
+        <v>12.172800429456</v>
       </c>
       <c r="O28">
-        <v>865.694263589965</v>
+        <v>795.746234688734</v>
       </c>
       <c r="P28">
-        <v>92.01219233149649</v>
+        <v>85.39655381116459</v>
       </c>
     </row>
     <row r="29">
@@ -1850,49 +1850,49 @@
         </is>
       </c>
       <c r="B29">
-        <v>191.147606849061</v>
+        <v>322.452310021209</v>
       </c>
       <c r="C29">
-        <v>6.18094376164016</v>
+        <v>5.45250198631043</v>
       </c>
       <c r="D29">
-        <v>4.13356944484771</v>
+        <v>3.64742965904264</v>
       </c>
       <c r="E29">
-        <v>2.64669537096863</v>
+        <v>2.33507973463641</v>
       </c>
       <c r="F29">
-        <v>17.8929082133307</v>
+        <v>15.9938694462648</v>
       </c>
       <c r="G29">
-        <v>3.03472918280656</v>
+        <v>2.6773584003731</v>
       </c>
       <c r="H29">
-        <v>2.89557985299833</v>
+        <v>2.55391189689644</v>
       </c>
       <c r="I29">
-        <v>6.29220390425349</v>
+        <v>5.54833434169032</v>
       </c>
       <c r="J29">
-        <v>5.96316613989324</v>
+        <v>5.26161220750469</v>
       </c>
       <c r="K29">
-        <v>4.40574438690928</v>
+        <v>3.88885634670775</v>
       </c>
       <c r="L29">
-        <v>5.51922629954214</v>
+        <v>4.87254420530103</v>
       </c>
       <c r="M29">
-        <v>2.66690702825569</v>
+        <v>2.35725257758319</v>
       </c>
       <c r="N29">
-        <v>11.9760859456032</v>
+        <v>10.7795449654614</v>
       </c>
       <c r="O29">
-        <v>1120.43268292901</v>
+        <v>997.859455673869</v>
       </c>
       <c r="P29">
-        <v>4.30561737742219</v>
+        <v>3.81360584686136</v>
       </c>
     </row>
     <row r="30">
@@ -1902,49 +1902,49 @@
         </is>
       </c>
       <c r="B30">
-        <v>88.5390526786106</v>
+        <v>163.635815401152</v>
       </c>
       <c r="C30">
-        <v>5.45136077007131</v>
+        <v>5.05843142382786</v>
       </c>
       <c r="D30">
-        <v>8.743373024842629</v>
+        <v>7.85311698486403</v>
       </c>
       <c r="E30">
-        <v>9.80565813515347</v>
+        <v>8.808196704673479</v>
       </c>
       <c r="F30">
-        <v>0.610996748530634</v>
+        <v>0.547602580794708</v>
       </c>
       <c r="G30">
-        <v>4.3519745347601</v>
+        <v>4.06966767228786</v>
       </c>
       <c r="H30">
-        <v>7.35747001816129</v>
+        <v>6.61025852295855</v>
       </c>
       <c r="I30">
-        <v>2.97817968427913</v>
+        <v>2.67554260452983</v>
       </c>
       <c r="J30">
-        <v>18.5042074846419</v>
+        <v>16.9502330637648</v>
       </c>
       <c r="K30">
-        <v>22.9847898801443</v>
+        <v>20.6531490947031</v>
       </c>
       <c r="L30">
-        <v>46.0192385356361</v>
+        <v>41.5119707616311</v>
       </c>
       <c r="M30">
-        <v>12.2812528411706</v>
+        <v>11.0298411502183</v>
       </c>
       <c r="N30">
-        <v>17.559747117094</v>
+        <v>16.0981560180182</v>
       </c>
       <c r="O30">
-        <v>627.385350849105</v>
+        <v>567.924599331462</v>
       </c>
       <c r="P30">
-        <v>8.422000962201899</v>
+        <v>7.56807202568803</v>
       </c>
     </row>
     <row r="31">
@@ -1954,49 +1954,49 @@
         </is>
       </c>
       <c r="B31">
-        <v>864.94524029515</v>
+        <v>1416.52253834526</v>
       </c>
       <c r="C31">
-        <v>56.7824594812724</v>
+        <v>50.6903825221046</v>
       </c>
       <c r="D31">
-        <v>65.82834665443789</v>
+        <v>59.1109237094523</v>
       </c>
       <c r="E31">
-        <v>28.4696384013829</v>
+        <v>25.6200413960435</v>
       </c>
       <c r="F31">
-        <v>10.7839301533217</v>
+        <v>9.547250059534409</v>
       </c>
       <c r="G31">
-        <v>173.390074523962</v>
+        <v>155.192484499096</v>
       </c>
       <c r="H31">
-        <v>32.9006155892251</v>
+        <v>29.5443233434808</v>
       </c>
       <c r="I31">
-        <v>34.2197861177012</v>
+        <v>31.1350409176447</v>
       </c>
       <c r="J31">
-        <v>50.8008324376285</v>
+        <v>44.9713719617553</v>
       </c>
       <c r="K31">
-        <v>53.6526404593018</v>
+        <v>47.4927040865106</v>
       </c>
       <c r="L31">
-        <v>73.2497157029884</v>
+        <v>65.25649948325059</v>
       </c>
       <c r="M31">
-        <v>33.4973498695757</v>
+        <v>30.0658377555024</v>
       </c>
       <c r="N31">
-        <v>81.9489099802355</v>
+        <v>72.5412472771939</v>
       </c>
       <c r="O31">
-        <v>4467.8552867431</v>
+        <v>3991.80434796961</v>
       </c>
       <c r="P31">
-        <v>10.2490159970328</v>
+        <v>9.07885158490814</v>
       </c>
     </row>
     <row r="32">
@@ -2006,49 +2006,49 @@
         </is>
       </c>
       <c r="B32">
-        <v>205.859594684385</v>
+        <v>347.501403045607</v>
       </c>
       <c r="C32">
-        <v>5.4713063028722</v>
+        <v>4.6860197772975</v>
       </c>
       <c r="D32">
-        <v>3.39457784777976</v>
+        <v>3.30558955324121</v>
       </c>
       <c r="E32">
-        <v>3.6538256043023</v>
+        <v>3.12704404051275</v>
       </c>
       <c r="F32">
-        <v>38.2333432451389</v>
+        <v>32.8076865520459</v>
       </c>
       <c r="G32">
-        <v>2.48223777111956</v>
+        <v>2.13027889786302</v>
       </c>
       <c r="H32">
-        <v>3.02480655692366</v>
+        <v>2.58681103341938</v>
       </c>
       <c r="I32">
-        <v>3.48192206279384</v>
+        <v>2.97474291288707</v>
       </c>
       <c r="J32">
-        <v>3.81703139851371</v>
+        <v>3.27304325223402</v>
       </c>
       <c r="K32">
-        <v>6.84314417450601</v>
+        <v>5.8535414452795</v>
       </c>
       <c r="L32">
-        <v>18.1206773037223</v>
+        <v>15.4804687208459</v>
       </c>
       <c r="M32">
-        <v>4.87024372827404</v>
+        <v>4.17314556931131</v>
       </c>
       <c r="N32">
-        <v>15.1586860111801</v>
+        <v>12.9425327634238</v>
       </c>
       <c r="O32">
-        <v>919.520417781468</v>
+        <v>795.356952009175</v>
       </c>
       <c r="P32">
-        <v>29.2403090044655</v>
+        <v>26.972864503352</v>
       </c>
     </row>
     <row r="33">
@@ -2058,49 +2058,49 @@
         </is>
       </c>
       <c r="B33">
-        <v>2262.33517541645</v>
+        <v>3716.97622638988</v>
       </c>
       <c r="C33">
-        <v>99.64987600214801</v>
+        <v>86.88151336220589</v>
       </c>
       <c r="D33">
-        <v>183.394226831733</v>
+        <v>159.991669558534</v>
       </c>
       <c r="E33">
-        <v>47.8791375988364</v>
+        <v>41.2998941733168</v>
       </c>
       <c r="F33">
-        <v>13.876083491248</v>
+        <v>11.97613631183</v>
       </c>
       <c r="G33">
-        <v>88.4391264637128</v>
+        <v>77.6973147575719</v>
       </c>
       <c r="H33">
-        <v>49.3994612159389</v>
+        <v>44.0090200003215</v>
       </c>
       <c r="I33">
-        <v>43.5837723129861</v>
+        <v>39.463450934628</v>
       </c>
       <c r="J33">
-        <v>125.724449740857</v>
+        <v>110.301896976244</v>
       </c>
       <c r="K33">
-        <v>140.828339437228</v>
+        <v>121.903605414272</v>
       </c>
       <c r="L33">
-        <v>180.575679756131</v>
+        <v>157.124847957109</v>
       </c>
       <c r="M33">
-        <v>102.31493916492</v>
+        <v>88.2586994545437</v>
       </c>
       <c r="N33">
-        <v>242.96520812713</v>
+        <v>210.886080438328</v>
       </c>
       <c r="O33">
-        <v>9944.04738221325</v>
+        <v>8667.750330113369</v>
       </c>
       <c r="P33">
-        <v>72.8071798845742</v>
+        <v>63.299351489758</v>
       </c>
     </row>
     <row r="34">
@@ -2110,49 +2110,49 @@
         </is>
       </c>
       <c r="B34">
-        <v>673.315060611047</v>
+        <v>1343.80866573539</v>
       </c>
       <c r="C34">
-        <v>107.096203527564</v>
+        <v>91.82544317695459</v>
       </c>
       <c r="D34">
-        <v>274.221867553923</v>
+        <v>237.740439687151</v>
       </c>
       <c r="E34">
-        <v>68.698774409401</v>
+        <v>59.79093113887</v>
       </c>
       <c r="F34">
-        <v>6.94596676937622</v>
+        <v>5.9655036303807</v>
       </c>
       <c r="G34">
-        <v>84.8775261280839</v>
+        <v>74.11870544281931</v>
       </c>
       <c r="H34">
-        <v>60.2549508081519</v>
+        <v>52.096614648101</v>
       </c>
       <c r="I34">
-        <v>27.3855942107298</v>
+        <v>23.4811674254887</v>
       </c>
       <c r="J34">
-        <v>72.772283293437</v>
+        <v>62.3957389557105</v>
       </c>
       <c r="K34">
-        <v>100.515426921609</v>
+        <v>86.61973725618439</v>
       </c>
       <c r="L34">
-        <v>157.618427667054</v>
+        <v>136.026001603287</v>
       </c>
       <c r="M34">
-        <v>61.3525503035589</v>
+        <v>53.0620336217656</v>
       </c>
       <c r="N34">
-        <v>154.515466144703</v>
+        <v>133.813034634273</v>
       </c>
       <c r="O34">
-        <v>3714.89094211629</v>
+        <v>3213.95513562043</v>
       </c>
       <c r="P34">
-        <v>84.6231709951894</v>
+        <v>74.385061498204</v>
       </c>
     </row>
     <row r="35">
@@ -2162,49 +2162,49 @@
         </is>
       </c>
       <c r="B35">
-        <v>39.1300326560588</v>
+        <v>75.0810578537896</v>
       </c>
       <c r="C35">
-        <v>5.63514842331697</v>
+        <v>5.09957349116968</v>
       </c>
       <c r="D35">
-        <v>0.871888145707472</v>
+        <v>0.788863249652717</v>
       </c>
       <c r="E35">
-        <v>3.54380547569342</v>
+        <v>3.28039688947869</v>
       </c>
       <c r="F35">
-        <v>5.81799578319735</v>
+        <v>5.33818202567532</v>
       </c>
       <c r="G35">
-        <v>0.338641573848681</v>
+        <v>0.305701362153362</v>
       </c>
       <c r="H35">
-        <v>0.714924304735109</v>
+        <v>0.64695390100721</v>
       </c>
       <c r="I35">
-        <v>1.6019780493122</v>
+        <v>1.44969050608027</v>
       </c>
       <c r="J35">
-        <v>2.10425734486149</v>
+        <v>1.90335043219543</v>
       </c>
       <c r="K35">
-        <v>7.79336398901595</v>
+        <v>7.05289093700113</v>
       </c>
       <c r="L35">
-        <v>3.57096062059269</v>
+        <v>3.23001177435794</v>
       </c>
       <c r="M35">
-        <v>2.24412395861162</v>
+        <v>2.10355178148345</v>
       </c>
       <c r="N35">
-        <v>2.55252508757015</v>
+        <v>2.30907274417022</v>
       </c>
       <c r="O35">
-        <v>332.015122549449</v>
+        <v>302.374437438253</v>
       </c>
       <c r="P35">
-        <v>44.3998242219168</v>
+        <v>41.3709092599202</v>
       </c>
     </row>
     <row r="36">
@@ -2214,49 +2214,49 @@
         </is>
       </c>
       <c r="B36">
-        <v>1043.55232426328</v>
+        <v>1910.98322654044</v>
       </c>
       <c r="C36">
-        <v>73.83266919458271</v>
+        <v>64.05780678127481</v>
       </c>
       <c r="D36">
-        <v>20.8809327709613</v>
+        <v>18.1132211910107</v>
       </c>
       <c r="E36">
-        <v>66.00993108802071</v>
+        <v>57.2640079103326</v>
       </c>
       <c r="F36">
-        <v>45.6005239576015</v>
+        <v>40.4382452830454</v>
       </c>
       <c r="G36">
-        <v>130.192272528687</v>
+        <v>113.824697655218</v>
       </c>
       <c r="H36">
-        <v>134.719683773098</v>
+        <v>117.746885345474</v>
       </c>
       <c r="I36">
-        <v>55.6547244168473</v>
+        <v>49.1618716008763</v>
       </c>
       <c r="J36">
-        <v>266.267352257864</v>
+        <v>232.312535309779</v>
       </c>
       <c r="K36">
-        <v>220.819318981034</v>
+        <v>193.769702502</v>
       </c>
       <c r="L36">
-        <v>127.632292334456</v>
+        <v>111.177012857852</v>
       </c>
       <c r="M36">
-        <v>263.252241618276</v>
+        <v>231.466978710285</v>
       </c>
       <c r="N36">
-        <v>111.401223953514</v>
+        <v>97.0904896063285</v>
       </c>
       <c r="O36">
-        <v>5467.24012257937</v>
+        <v>4794.09412988476</v>
       </c>
       <c r="P36">
-        <v>57.1920530141142</v>
+        <v>52.7472214783964</v>
       </c>
     </row>
     <row r="37">
@@ -2266,49 +2266,49 @@
         </is>
       </c>
       <c r="B37">
-        <v>338.259894594115</v>
+        <v>640.228005670884</v>
       </c>
       <c r="C37">
-        <v>27.7881745614097</v>
+        <v>23.3584446443436</v>
       </c>
       <c r="D37">
-        <v>14.5365151103413</v>
+        <v>12.5641457425433</v>
       </c>
       <c r="E37">
-        <v>22.0339664540475</v>
+        <v>18.5126765056977</v>
       </c>
       <c r="F37">
-        <v>52.4040337053188</v>
+        <v>44.3656884544782</v>
       </c>
       <c r="G37">
-        <v>10.0685306852724</v>
+        <v>8.477329867506009</v>
       </c>
       <c r="H37">
-        <v>29.5419473250205</v>
+        <v>24.8107937146845</v>
       </c>
       <c r="I37">
-        <v>20.8439253597144</v>
+        <v>18.1969818439729</v>
       </c>
       <c r="J37">
-        <v>42.860681801478</v>
+        <v>36.7011332470826</v>
       </c>
       <c r="K37">
-        <v>51.0079603333051</v>
+        <v>43.1981384023074</v>
       </c>
       <c r="L37">
-        <v>32.7909279945705</v>
+        <v>27.5718015125589</v>
       </c>
       <c r="M37">
-        <v>35.2340213177564</v>
+        <v>29.974160446074</v>
       </c>
       <c r="N37">
-        <v>20.9386745042299</v>
+        <v>17.9524243374332</v>
       </c>
       <c r="O37">
-        <v>1645.471370688</v>
+        <v>1406.67596430135</v>
       </c>
       <c r="P37">
-        <v>70.4548268769182</v>
+        <v>61.648024394015</v>
       </c>
     </row>
     <row r="38">
@@ -2318,49 +2318,49 @@
         </is>
       </c>
       <c r="B38">
-        <v>356.944552424953</v>
+        <v>582.783797180606</v>
       </c>
       <c r="C38">
-        <v>34.4655759185308</v>
+        <v>30.3447069990682</v>
       </c>
       <c r="D38">
-        <v>16.3445235512585</v>
+        <v>14.3914550493542</v>
       </c>
       <c r="E38">
-        <v>58.6273558123822</v>
+        <v>52.4316612234898</v>
       </c>
       <c r="F38">
-        <v>3.74907084342327</v>
+        <v>3.30361880919433</v>
       </c>
       <c r="G38">
-        <v>10.1673841244682</v>
+        <v>8.951903209654461</v>
       </c>
       <c r="H38">
-        <v>8.13587659519682</v>
+        <v>7.16268623565163</v>
       </c>
       <c r="I38">
-        <v>6.32033808642046</v>
+        <v>5.56455550901413</v>
       </c>
       <c r="J38">
-        <v>38.2060228662198</v>
+        <v>34.0467182682238</v>
       </c>
       <c r="K38">
-        <v>22.4106034926355</v>
+        <v>20.1389153236241</v>
       </c>
       <c r="L38">
-        <v>75.39226143735949</v>
+        <v>67.59796890645811</v>
       </c>
       <c r="M38">
-        <v>30.7005873233136</v>
+        <v>27.0392077715371</v>
       </c>
       <c r="N38">
-        <v>31.4400254763595</v>
+        <v>28.0887162765522</v>
       </c>
       <c r="O38">
-        <v>1669.14984809148</v>
+        <v>1489.35715794936</v>
       </c>
       <c r="P38">
-        <v>80.1107850363677</v>
+        <v>70.96183901759839</v>
       </c>
     </row>
     <row r="39">
@@ -2370,49 +2370,49 @@
         </is>
       </c>
       <c r="B39">
-        <v>1225.16804362219</v>
+        <v>2118.23576350468</v>
       </c>
       <c r="C39">
-        <v>153.319024982589</v>
+        <v>135.077353617664</v>
       </c>
       <c r="D39">
-        <v>80.9737449645975</v>
+        <v>71.74722775924771</v>
       </c>
       <c r="E39">
-        <v>96.7639011298661</v>
+        <v>85.1303393959777</v>
       </c>
       <c r="F39">
-        <v>32.7406926830881</v>
+        <v>28.6570966557027</v>
       </c>
       <c r="G39">
-        <v>147.177821686882</v>
+        <v>129.702644982354</v>
       </c>
       <c r="H39">
-        <v>58.7460722983748</v>
+        <v>51.4165596158853</v>
       </c>
       <c r="I39">
-        <v>64.0028168592365</v>
+        <v>56.9001380586492</v>
       </c>
       <c r="J39">
-        <v>203.521242181429</v>
+        <v>179.013893855958</v>
       </c>
       <c r="K39">
-        <v>165.23225266622</v>
+        <v>145.49620130467</v>
       </c>
       <c r="L39">
-        <v>161.883429284069</v>
+        <v>142.129786134327</v>
       </c>
       <c r="M39">
-        <v>86.6031834058975</v>
+        <v>76.2467093973016</v>
       </c>
       <c r="N39">
-        <v>132.819353824866</v>
+        <v>117.128905088655</v>
       </c>
       <c r="O39">
-        <v>6117.35403555371</v>
+        <v>5398.56561127953</v>
       </c>
       <c r="P39">
-        <v>73.52898567162551</v>
+        <v>64.38670808802139</v>
       </c>
     </row>
     <row r="40">
@@ -2422,49 +2422,49 @@
         </is>
       </c>
       <c r="B40">
-        <v>84.232031280334</v>
+        <v>163.619982726026</v>
       </c>
       <c r="C40">
-        <v>4.02898763603224</v>
+        <v>3.51787258794429</v>
       </c>
       <c r="D40">
-        <v>13.0057528604635</v>
+        <v>11.3529089282471</v>
       </c>
       <c r="E40">
-        <v>2.16808492179988</v>
+        <v>2.04011549652263</v>
       </c>
       <c r="F40">
-        <v>0.718415195904144</v>
+        <v>0.627304411616469</v>
       </c>
       <c r="G40">
-        <v>6.37112089446287</v>
+        <v>5.56242449807679</v>
       </c>
       <c r="H40">
-        <v>11.3898709383029</v>
+        <v>9.942437230639699</v>
       </c>
       <c r="I40">
-        <v>1.7400439329765</v>
+        <v>1.51950938471458</v>
       </c>
       <c r="J40">
-        <v>14.341707090816</v>
+        <v>12.6679622541716</v>
       </c>
       <c r="K40">
-        <v>12.3350766628848</v>
+        <v>10.7690133510061</v>
       </c>
       <c r="L40">
-        <v>15.0303557149119</v>
+        <v>13.1232954689385</v>
       </c>
       <c r="M40">
-        <v>8.951637432608241</v>
+        <v>8.109255210076711</v>
       </c>
       <c r="N40">
-        <v>35.162880461467</v>
+        <v>30.8424185112813</v>
       </c>
       <c r="O40">
-        <v>530.251192160404</v>
+        <v>466.351676779845</v>
       </c>
       <c r="P40">
-        <v>2.53790088401293</v>
+        <v>2.21883344697563</v>
       </c>
     </row>
     <row r="41">
@@ -2474,49 +2474,49 @@
         </is>
       </c>
       <c r="B41">
-        <v>338.250031888481</v>
+        <v>727.901030371285</v>
       </c>
       <c r="C41">
-        <v>15.0680351125245</v>
+        <v>13.0769915827248</v>
       </c>
       <c r="D41">
-        <v>134.469955302226</v>
+        <v>112.322484051204</v>
       </c>
       <c r="E41">
-        <v>55.9173615078051</v>
+        <v>46.5061299139704</v>
       </c>
       <c r="F41">
-        <v>4.6240761113406</v>
+        <v>3.85921686763177</v>
       </c>
       <c r="G41">
-        <v>53.3138285312459</v>
+        <v>44.8545441941218</v>
       </c>
       <c r="H41">
-        <v>48.7526456613782</v>
+        <v>40.5354434012361</v>
       </c>
       <c r="I41">
-        <v>15.1770076233872</v>
+        <v>13.1413387973547</v>
       </c>
       <c r="J41">
-        <v>61.5854693464107</v>
+        <v>51.7374033231302</v>
       </c>
       <c r="K41">
-        <v>70.2831635634215</v>
+        <v>58.4495965191083</v>
       </c>
       <c r="L41">
-        <v>37.0866494393686</v>
+        <v>30.8711541781039</v>
       </c>
       <c r="M41">
-        <v>45.1141089296711</v>
+        <v>37.5438611551915</v>
       </c>
       <c r="N41">
-        <v>28.8571738545155</v>
+        <v>25.0551929876</v>
       </c>
       <c r="O41">
-        <v>1846.17911218342</v>
+        <v>1554.03741955001</v>
       </c>
       <c r="P41">
-        <v>31.2190064758728</v>
+        <v>26.0056046178615</v>
       </c>
     </row>
     <row r="42">
@@ -2526,49 +2526,49 @@
         </is>
       </c>
       <c r="B42">
-        <v>40.3130374728521</v>
+        <v>82.26280954947001</v>
       </c>
       <c r="C42">
-        <v>9.281676011718901</v>
+        <v>8.474048617299809</v>
       </c>
       <c r="D42">
-        <v>2.35724393251822</v>
+        <v>2.2129886301285</v>
       </c>
       <c r="E42">
-        <v>5.19048804543805</v>
+        <v>4.69117183239828</v>
       </c>
       <c r="F42">
-        <v>2.25939846097811</v>
+        <v>2.04197102768837</v>
       </c>
       <c r="G42">
-        <v>1.63309051256581</v>
+        <v>1.47532837315416</v>
       </c>
       <c r="H42">
-        <v>1.59728878008293</v>
+        <v>1.44379258558142</v>
       </c>
       <c r="I42">
-        <v>1.01003116995612</v>
+        <v>0.912552039046285</v>
       </c>
       <c r="J42">
-        <v>5.06419275769273</v>
+        <v>4.57681100019763</v>
       </c>
       <c r="K42">
-        <v>8.99163281219978</v>
+        <v>8.12844800533075</v>
       </c>
       <c r="L42">
-        <v>10.0125285482025</v>
+        <v>9.04987678076416</v>
       </c>
       <c r="M42">
-        <v>4.34179838648161</v>
+        <v>3.9211031548985</v>
       </c>
       <c r="N42">
-        <v>8.969495746132891</v>
+        <v>8.10634722117539</v>
       </c>
       <c r="O42">
-        <v>381.714991902052</v>
+        <v>348.909052346876</v>
       </c>
       <c r="P42">
-        <v>43.2005959338816</v>
+        <v>39.7312127146565</v>
       </c>
     </row>
     <row r="43">
@@ -2578,49 +2578,49 @@
         </is>
       </c>
       <c r="B43">
-        <v>553.500031215416</v>
+        <v>1083.81275148896</v>
       </c>
       <c r="C43">
-        <v>38.1474466147739</v>
+        <v>32.0075195128264</v>
       </c>
       <c r="D43">
-        <v>71.87037077029621</v>
+        <v>62.0803609252899</v>
       </c>
       <c r="E43">
-        <v>50.9665838297546</v>
+        <v>43.3469305302994</v>
       </c>
       <c r="F43">
-        <v>15.1430410167783</v>
+        <v>12.7109147151942</v>
       </c>
       <c r="G43">
-        <v>34.8045263342259</v>
+        <v>29.2004179517161</v>
       </c>
       <c r="H43">
-        <v>32.4316949174173</v>
+        <v>27.1962800994397</v>
       </c>
       <c r="I43">
-        <v>31.4288727498414</v>
+        <v>26.3556389394601</v>
       </c>
       <c r="J43">
-        <v>64.15983915745559</v>
+        <v>55.0247792958626</v>
       </c>
       <c r="K43">
-        <v>82.0853559102613</v>
+        <v>68.83728334272151</v>
       </c>
       <c r="L43">
-        <v>62.871574138165</v>
+        <v>53.3496409508602</v>
       </c>
       <c r="M43">
-        <v>97.8479118820389</v>
+        <v>83.2780249537927</v>
       </c>
       <c r="N43">
-        <v>106.532898847447</v>
+        <v>89.9326485953742</v>
       </c>
       <c r="O43">
-        <v>2743.2390260605</v>
+        <v>2324.91247108155</v>
       </c>
       <c r="P43">
-        <v>69.956485868475</v>
+        <v>62.9401662117344</v>
       </c>
     </row>
     <row r="44">
@@ -2630,49 +2630,49 @@
         </is>
       </c>
       <c r="B44">
-        <v>2219.51276478052</v>
+        <v>3391.51584148015</v>
       </c>
       <c r="C44">
-        <v>199.771788763191</v>
+        <v>178.929955535878</v>
       </c>
       <c r="D44">
-        <v>89.2724704407422</v>
+        <v>80.88308063604519</v>
       </c>
       <c r="E44">
-        <v>88.38916830686431</v>
+        <v>79.4757577229108</v>
       </c>
       <c r="F44">
-        <v>278.341650640914</v>
+        <v>252.786976208756</v>
       </c>
       <c r="G44">
-        <v>182.261395559693</v>
+        <v>163.934693093484</v>
       </c>
       <c r="H44">
-        <v>62.6850034195397</v>
+        <v>57.1635161458613</v>
       </c>
       <c r="I44">
-        <v>60.9337043109464</v>
+        <v>55.001150129409</v>
       </c>
       <c r="J44">
-        <v>166.270504191387</v>
+        <v>150.247455030791</v>
       </c>
       <c r="K44">
-        <v>179.26922845253</v>
+        <v>160.634312145015</v>
       </c>
       <c r="L44">
-        <v>298.455418596874</v>
+        <v>267.051659281453</v>
       </c>
       <c r="M44">
-        <v>143.569787443786</v>
+        <v>129.979733275143</v>
       </c>
       <c r="N44">
-        <v>110.647766935427</v>
+        <v>99.9742357358938</v>
       </c>
       <c r="O44">
-        <v>9816.44758559368</v>
+        <v>8850.126286410959</v>
       </c>
       <c r="P44">
-        <v>296.166700247956</v>
+        <v>274.29005815637</v>
       </c>
     </row>
     <row r="45">
@@ -2682,49 +2682,49 @@
         </is>
       </c>
       <c r="B45">
-        <v>215.3807657862</v>
+        <v>324.303438701666</v>
       </c>
       <c r="C45">
-        <v>17.4104033908149</v>
+        <v>16.0598156988536</v>
       </c>
       <c r="D45">
-        <v>6.77713516114162</v>
+        <v>6.15302796439068</v>
       </c>
       <c r="E45">
-        <v>7.65971237680022</v>
+        <v>6.95335719300868</v>
       </c>
       <c r="F45">
-        <v>26.2961612165626</v>
+        <v>23.904906860991</v>
       </c>
       <c r="G45">
-        <v>10.2329467338816</v>
+        <v>9.29672793733204</v>
       </c>
       <c r="H45">
-        <v>5.0217380964775</v>
+        <v>4.56067426007231</v>
       </c>
       <c r="I45">
-        <v>6.858066176365</v>
+        <v>6.2313502432156</v>
       </c>
       <c r="J45">
-        <v>24.0289252475108</v>
+        <v>21.8372844468179</v>
       </c>
       <c r="K45">
-        <v>12.7521531756873</v>
+        <v>11.5854958458211</v>
       </c>
       <c r="L45">
-        <v>25.3224812530205</v>
+        <v>23.0055572636123</v>
       </c>
       <c r="M45">
-        <v>28.0154548032963</v>
+        <v>25.9406366689411</v>
       </c>
       <c r="N45">
-        <v>33.1044309665211</v>
+        <v>30.0927764160042</v>
       </c>
       <c r="O45">
-        <v>1052.86942928247</v>
+        <v>962.825877992651</v>
       </c>
       <c r="P45">
-        <v>19.1810663640853</v>
+        <v>18.1599211285649</v>
       </c>
     </row>
     <row r="46">
@@ -2734,49 +2734,49 @@
         </is>
       </c>
       <c r="B46">
-        <v>41.5177806379953</v>
+        <v>81.04678755304251</v>
       </c>
       <c r="C46">
-        <v>5.22036818122693</v>
+        <v>4.73175767812593</v>
       </c>
       <c r="D46">
-        <v>2.45746111451603</v>
+        <v>2.18543813358117</v>
       </c>
       <c r="E46">
-        <v>6.88122070670275</v>
+        <v>6.20945817415713</v>
       </c>
       <c r="F46">
-        <v>1.8139395020682</v>
+        <v>1.61401948129061</v>
       </c>
       <c r="G46">
-        <v>1.94093328678454</v>
+        <v>1.726426867849</v>
       </c>
       <c r="H46">
-        <v>2.71173331178981</v>
+        <v>2.41229211371157</v>
       </c>
       <c r="I46">
-        <v>2.80170569300623</v>
+        <v>2.66788288716665</v>
       </c>
       <c r="J46">
-        <v>5.04192334423595</v>
+        <v>4.48553725346334</v>
       </c>
       <c r="K46">
-        <v>5.63896196231884</v>
+        <v>5.01584594291695</v>
       </c>
       <c r="L46">
-        <v>15.2183442155689</v>
+        <v>13.7137020489965</v>
       </c>
       <c r="M46">
-        <v>4.76519833010433</v>
+        <v>4.23831101750805</v>
       </c>
       <c r="N46">
-        <v>9.32990494061818</v>
+        <v>8.298980081483281</v>
       </c>
       <c r="O46">
-        <v>317.149984108607</v>
+        <v>285.0911031188</v>
       </c>
       <c r="P46">
-        <v>9.397222603633571</v>
+        <v>8.449171310527429</v>
       </c>
     </row>
     <row r="47">
@@ -2786,49 +2786,49 @@
         </is>
       </c>
       <c r="B47">
-        <v>628.545776518394</v>
+        <v>1167.38081844342</v>
       </c>
       <c r="C47">
-        <v>78.95649829244159</v>
+        <v>71.1741268950651</v>
       </c>
       <c r="D47">
-        <v>48.4788229874024</v>
+        <v>42.7109700747957</v>
       </c>
       <c r="E47">
-        <v>50.0896695357006</v>
+        <v>43.4416589261726</v>
       </c>
       <c r="F47">
-        <v>11.5451406519851</v>
+        <v>10.6854308620966</v>
       </c>
       <c r="G47">
-        <v>41.7698453144015</v>
+        <v>37.5767799601221</v>
       </c>
       <c r="H47">
-        <v>21.8262140671538</v>
+        <v>18.929360103052</v>
       </c>
       <c r="I47">
-        <v>19.9844081509485</v>
+        <v>17.335394755409</v>
       </c>
       <c r="J47">
-        <v>64.60492750169389</v>
+        <v>56.7079552231042</v>
       </c>
       <c r="K47">
-        <v>38.2395873633083</v>
+        <v>33.8433577079509</v>
       </c>
       <c r="L47">
-        <v>65.8300275512495</v>
+        <v>57.1081230698061</v>
       </c>
       <c r="M47">
-        <v>88.73005037646711</v>
+        <v>76.96561755268149</v>
       </c>
       <c r="N47">
-        <v>46.1412507769817</v>
+        <v>40.0310776239392</v>
       </c>
       <c r="O47">
-        <v>3692.70954255294</v>
+        <v>3228.92731451192</v>
       </c>
       <c r="P47">
-        <v>45.8181363219341</v>
+        <v>40.4515191831308</v>
       </c>
     </row>
     <row r="48">
@@ -2838,49 +2838,49 @@
         </is>
       </c>
       <c r="B48">
-        <v>597.443681112598</v>
+        <v>984.831727606628</v>
       </c>
       <c r="C48">
-        <v>20.988490940896</v>
+        <v>18.508694117012</v>
       </c>
       <c r="D48">
-        <v>19.806194599355</v>
+        <v>17.4588245406286</v>
       </c>
       <c r="E48">
-        <v>79.783578524234</v>
+        <v>71.657931593458</v>
       </c>
       <c r="F48">
-        <v>19.5333853391229</v>
+        <v>17.222853274386</v>
       </c>
       <c r="G48">
-        <v>18.1303682543484</v>
+        <v>15.9838033906098</v>
       </c>
       <c r="H48">
-        <v>8.77123407598044</v>
+        <v>7.73257175044885</v>
       </c>
       <c r="I48">
-        <v>22.3129849369228</v>
+        <v>19.6666621236342</v>
       </c>
       <c r="J48">
-        <v>35.323799705967</v>
+        <v>31.8078225513808</v>
       </c>
       <c r="K48">
-        <v>30.5556333605732</v>
+        <v>26.9407205093592</v>
       </c>
       <c r="L48">
-        <v>52.9974315034312</v>
+        <v>46.7296191311198</v>
       </c>
       <c r="M48">
-        <v>170.261018679365</v>
+        <v>152.06997470351</v>
       </c>
       <c r="N48">
-        <v>29.4459275058283</v>
+        <v>25.9626414830863</v>
       </c>
       <c r="O48">
-        <v>2935.12194152302</v>
+        <v>2614.28066656186</v>
       </c>
       <c r="P48">
-        <v>110.324324435799</v>
+        <v>99.9452725756852</v>
       </c>
     </row>
     <row r="49">
@@ -2890,49 +2890,49 @@
         </is>
       </c>
       <c r="B49">
-        <v>270.950198914901</v>
+        <v>473.818765534795</v>
       </c>
       <c r="C49">
-        <v>6.65164206041345</v>
+        <v>5.33482031868133</v>
       </c>
       <c r="D49">
-        <v>8.68794725294522</v>
+        <v>6.95944318913841</v>
       </c>
       <c r="E49">
-        <v>18.4826598345902</v>
+        <v>14.7772432885319</v>
       </c>
       <c r="F49">
-        <v>48.3868980912953</v>
+        <v>38.8482210031684</v>
       </c>
       <c r="G49">
-        <v>25.8114766758742</v>
+        <v>21.2362661492527</v>
       </c>
       <c r="H49">
-        <v>4.51402606570359</v>
+        <v>3.61867699064871</v>
       </c>
       <c r="I49">
-        <v>13.0285371833878</v>
+        <v>10.6149591384418</v>
       </c>
       <c r="J49">
-        <v>28.5358125075324</v>
+        <v>22.819567512787</v>
       </c>
       <c r="K49">
-        <v>13.3217726213712</v>
+        <v>10.6677399141959</v>
       </c>
       <c r="L49">
-        <v>4.2267094719003</v>
+        <v>3.40640738961334</v>
       </c>
       <c r="M49">
-        <v>8.063129461700839</v>
+        <v>6.47334186830336</v>
       </c>
       <c r="N49">
-        <v>4.91158255592386</v>
+        <v>3.9484916459429</v>
       </c>
       <c r="O49">
-        <v>879.313259363626</v>
+        <v>713.523969821788</v>
       </c>
       <c r="P49">
-        <v>8.92737843918589</v>
+        <v>7.76518115694295</v>
       </c>
     </row>
     <row r="50">
@@ -2942,49 +2942,49 @@
         </is>
       </c>
       <c r="B50">
-        <v>339.72357363116</v>
+        <v>684.818091584522</v>
       </c>
       <c r="C50">
-        <v>93.2399018057627</v>
+        <v>83.7709517124174</v>
       </c>
       <c r="D50">
-        <v>14.8658552207124</v>
+        <v>13.2553810434901</v>
       </c>
       <c r="E50">
-        <v>117.9016429343</v>
+        <v>105.225387088906</v>
       </c>
       <c r="F50">
-        <v>4.61464002591025</v>
+        <v>4.118260698562</v>
       </c>
       <c r="G50">
-        <v>38.3789793007334</v>
+        <v>34.8047005260523</v>
       </c>
       <c r="H50">
-        <v>36.3598959632509</v>
+        <v>32.4491628471332</v>
       </c>
       <c r="I50">
-        <v>21.3689740151756</v>
+        <v>19.6242607014402</v>
       </c>
       <c r="J50">
-        <v>112.574628734401</v>
+        <v>102.133443923903</v>
       </c>
       <c r="K50">
-        <v>145.545032007166</v>
+        <v>132.119501474016</v>
       </c>
       <c r="L50">
-        <v>102.291059895463</v>
+        <v>91.2905127057392</v>
       </c>
       <c r="M50">
-        <v>35.6716868768322</v>
+        <v>31.8288296893003</v>
       </c>
       <c r="N50">
-        <v>89.62774238207661</v>
+        <v>79.990945943154</v>
       </c>
       <c r="O50">
-        <v>2554.63190422886</v>
+        <v>2299.28478083488</v>
       </c>
       <c r="P50">
-        <v>84.1173381948114</v>
+        <v>76.19823984181321</v>
       </c>
     </row>
     <row r="51">
@@ -2994,49 +2994,49 @@
         </is>
       </c>
       <c r="B51">
-        <v>43.3610690504556</v>
+        <v>74.309083787323</v>
       </c>
       <c r="C51">
-        <v>2.03350211629632</v>
+        <v>1.86300896810883</v>
       </c>
       <c r="D51">
-        <v>0.54106170247832</v>
+        <v>0.480412045546993</v>
       </c>
       <c r="E51">
-        <v>1.58965431271618</v>
+        <v>1.4108946854963</v>
       </c>
       <c r="F51">
-        <v>28.8713873540288</v>
+        <v>25.7389979173671</v>
       </c>
       <c r="G51">
-        <v>1.04870545828516</v>
+        <v>0.931173027094758</v>
       </c>
       <c r="H51">
-        <v>0.30862086907146</v>
+        <v>0.274192543882136</v>
       </c>
       <c r="I51">
-        <v>1.13301752638202</v>
+        <v>1.0058321348926</v>
       </c>
       <c r="J51">
-        <v>2.05935122080031</v>
+        <v>1.82819604556888</v>
       </c>
       <c r="K51">
-        <v>1.53080594306682</v>
+        <v>1.35974792324982</v>
       </c>
       <c r="L51">
-        <v>0.810647488319701</v>
+        <v>0.721499549588404</v>
       </c>
       <c r="M51">
-        <v>0.6910328228757761</v>
+        <v>0.614580297854044</v>
       </c>
       <c r="N51">
-        <v>1.51940857205975</v>
+        <v>1.34954456344495</v>
       </c>
       <c r="O51">
-        <v>242.196997889045</v>
+        <v>217.478081108056</v>
       </c>
       <c r="P51">
-        <v>18.4389374984634</v>
+        <v>16.7689905871227</v>
       </c>
     </row>
     <row r="52">

</xml_diff>

<commit_message>
cps annual matching and cps+cps_supp
</commit_message>
<xml_diff>
--- a/1-Data-Codes/2-Final_Data/L_1999.xlsx
+++ b/1-Data-Codes/2-Final_Data/L_1999.xlsx
@@ -446,49 +446,49 @@
         </is>
       </c>
       <c r="B2">
-        <v>880.626869372828</v>
+        <v>1169.80662325887</v>
       </c>
       <c r="C2">
-        <v>32.9909579140803</v>
+        <v>40.3885188932118</v>
       </c>
       <c r="D2">
-        <v>70.8827548295604</v>
+        <v>92.07100750786771</v>
       </c>
       <c r="E2">
-        <v>78.45011750803489</v>
+        <v>68.49600481491829</v>
       </c>
       <c r="F2">
-        <v>18.0610184063369</v>
+        <v>15.8527736626304</v>
       </c>
       <c r="G2">
-        <v>25.0685985958796</v>
+        <v>22.1616101595343</v>
       </c>
       <c r="H2">
-        <v>38.1171766202186</v>
+        <v>24.7955694748319</v>
       </c>
       <c r="I2">
-        <v>19.3528069798599</v>
+        <v>14.5473839856517</v>
       </c>
       <c r="J2">
-        <v>72.1265509522174</v>
+        <v>73.79667632284961</v>
       </c>
       <c r="K2">
-        <v>23.4458519567515</v>
+        <v>25.5405741857225</v>
       </c>
       <c r="L2">
-        <v>36.3640469687735</v>
+        <v>37.187294585555</v>
       </c>
       <c r="M2">
-        <v>49.1197621695025</v>
+        <v>38.8907652269414</v>
       </c>
       <c r="N2">
-        <v>29.416542064031</v>
+        <v>30.9597871246405</v>
       </c>
       <c r="O2">
-        <v>1729.41044535951</v>
+        <v>1445.40134261463</v>
       </c>
       <c r="P2">
-        <v>47.1555427693103</v>
+        <v>50.7103474436891</v>
       </c>
     </row>
     <row r="3">
@@ -498,49 +498,49 @@
         </is>
       </c>
       <c r="B3">
-        <v>99.87958678024791</v>
+        <v>124.356542777432</v>
       </c>
       <c r="C3">
-        <v>3.1310697155839</v>
+        <v>5.84361325084831</v>
       </c>
       <c r="D3">
-        <v>0.481454533742216</v>
+        <v>0.532778615332813</v>
       </c>
       <c r="E3">
-        <v>1.54140807849281</v>
+        <v>1.67723919848077</v>
       </c>
       <c r="F3">
-        <v>10.2812471614954</v>
+        <v>9.651803808627349</v>
       </c>
       <c r="G3">
-        <v>0.989668329299163</v>
+        <v>0.496406046965805</v>
       </c>
       <c r="H3">
-        <v>0.237845091980672</v>
+        <v>0.185386558819401</v>
       </c>
       <c r="I3">
-        <v>0.691656023427396</v>
+        <v>0.185512128061022</v>
       </c>
       <c r="J3">
-        <v>0.608622775176926</v>
+        <v>0.541351773273659</v>
       </c>
       <c r="K3">
-        <v>0.6558604586874081</v>
+        <v>0.401563425613806</v>
       </c>
       <c r="L3">
-        <v>0.38345854974616</v>
+        <v>0.32683074279789</v>
       </c>
       <c r="M3">
-        <v>1.39754100682496</v>
+        <v>1.12981794609696</v>
       </c>
       <c r="N3">
-        <v>1.13378547992054</v>
+        <v>0.732003263256041</v>
       </c>
       <c r="O3">
-        <v>273.702657320687</v>
+        <v>249.321559707904</v>
       </c>
       <c r="P3">
-        <v>10.9782647915221</v>
+        <v>10.7076008331701</v>
       </c>
     </row>
     <row r="4">
@@ -550,49 +550,49 @@
         </is>
       </c>
       <c r="B4">
-        <v>910.368958813005</v>
+        <v>1270.67108467159</v>
       </c>
       <c r="C4">
-        <v>16.768934296197</v>
+        <v>15.1623803792313</v>
       </c>
       <c r="D4">
-        <v>9.491005270082811</v>
+        <v>11.989135427276</v>
       </c>
       <c r="E4">
-        <v>13.4598550333781</v>
+        <v>17.3646601594878</v>
       </c>
       <c r="F4">
-        <v>9.819518341323819</v>
+        <v>20.7557037485372</v>
       </c>
       <c r="G4">
-        <v>14.4227631604536</v>
+        <v>13.9531453821672</v>
       </c>
       <c r="H4">
-        <v>5.56493731579996</v>
+        <v>8.18802786203536</v>
       </c>
       <c r="I4">
-        <v>8.98995925864066</v>
+        <v>6.96783600063118</v>
       </c>
       <c r="J4">
-        <v>28.0111262689024</v>
+        <v>26.028666516929</v>
       </c>
       <c r="K4">
-        <v>11.7945400585141</v>
+        <v>9.267967282567041</v>
       </c>
       <c r="L4">
-        <v>96.31585328265901</v>
+        <v>92.70368251624571</v>
       </c>
       <c r="M4">
-        <v>63.7780385587697</v>
+        <v>56.8223507638853</v>
       </c>
       <c r="N4">
-        <v>38.2667782115534</v>
+        <v>21.9870426240282</v>
       </c>
       <c r="O4">
-        <v>2273.94114297833</v>
+        <v>1930.94336823436</v>
       </c>
       <c r="P4">
-        <v>38.0231732392639</v>
+        <v>36.1800154365612</v>
       </c>
     </row>
     <row r="5">
@@ -602,49 +602,49 @@
         </is>
       </c>
       <c r="B5">
-        <v>519.660985662407</v>
+        <v>687.250183822308</v>
       </c>
       <c r="C5">
-        <v>57.9454516682765</v>
+        <v>59.1193931481618</v>
       </c>
       <c r="D5">
-        <v>19.7978917932569</v>
+        <v>14.9047762775098</v>
       </c>
       <c r="E5">
-        <v>31.6548562224411</v>
+        <v>45.0638232850824</v>
       </c>
       <c r="F5">
-        <v>2.4270840885265</v>
+        <v>4.51217888027607</v>
       </c>
       <c r="G5">
-        <v>11.5423881087472</v>
+        <v>14.7894579942568</v>
       </c>
       <c r="H5">
-        <v>13.2824799246698</v>
+        <v>15.5915817889997</v>
       </c>
       <c r="I5">
-        <v>9.897171797936309</v>
+        <v>7.49840241540469</v>
       </c>
       <c r="J5">
-        <v>38.456006681837</v>
+        <v>39.1073451160403</v>
       </c>
       <c r="K5">
-        <v>28.1456104440175</v>
+        <v>26.1747653365326</v>
       </c>
       <c r="L5">
-        <v>27.9389976906553</v>
+        <v>23.354973572804</v>
       </c>
       <c r="M5">
-        <v>16.5911908315753</v>
+        <v>20.5526038927974</v>
       </c>
       <c r="N5">
-        <v>19.9125323455726</v>
+        <v>19.1841569925131</v>
       </c>
       <c r="O5">
-        <v>1027.50192034216</v>
+        <v>827.823423057903</v>
       </c>
       <c r="P5">
-        <v>44.7333825895591</v>
+        <v>64.5721197648826</v>
       </c>
     </row>
     <row r="6">
@@ -654,49 +654,49 @@
         </is>
       </c>
       <c r="B6">
-        <v>5996.69404674058</v>
+        <v>8232.893646179609</v>
       </c>
       <c r="C6">
-        <v>192.70692038665</v>
+        <v>214.493971836629</v>
       </c>
       <c r="D6">
-        <v>313.74734107682</v>
+        <v>246.958047741748</v>
       </c>
       <c r="E6">
-        <v>116.296902150511</v>
+        <v>145.280928951152</v>
       </c>
       <c r="F6">
-        <v>59.4553704754713</v>
+        <v>49.6138360696182</v>
       </c>
       <c r="G6">
-        <v>128.407269089246</v>
+        <v>108.258902536894</v>
       </c>
       <c r="H6">
-        <v>80.02307233803489</v>
+        <v>69.1830961582674</v>
       </c>
       <c r="I6">
-        <v>61.6287385347997</v>
+        <v>55.0399989814105</v>
       </c>
       <c r="J6">
-        <v>211.447505772444</v>
+        <v>195.64598911656</v>
       </c>
       <c r="K6">
-        <v>175.205600103884</v>
+        <v>138.445616452083</v>
       </c>
       <c r="L6">
-        <v>565.772430070455</v>
+        <v>583.238311005987</v>
       </c>
       <c r="M6">
-        <v>377.959606451273</v>
+        <v>321.024784025261</v>
       </c>
       <c r="N6">
-        <v>370.188362569557</v>
+        <v>303.848233616888</v>
       </c>
       <c r="O6">
-        <v>14519.4691901651</v>
+        <v>12463.5662511451</v>
       </c>
       <c r="P6">
-        <v>281.655597878665</v>
+        <v>323.342677958546</v>
       </c>
     </row>
     <row r="7">
@@ -706,49 +706,49 @@
         </is>
       </c>
       <c r="B7">
-        <v>595.546369672757</v>
+        <v>825.788159088176</v>
       </c>
       <c r="C7">
-        <v>34.933619092928</v>
+        <v>33.9039909785586</v>
       </c>
       <c r="D7">
-        <v>6.09708359714507</v>
+        <v>5.87593527686245</v>
       </c>
       <c r="E7">
-        <v>14.2989887756996</v>
+        <v>19.771828774842</v>
       </c>
       <c r="F7">
-        <v>18.2776185660558</v>
+        <v>18.6855331421006</v>
       </c>
       <c r="G7">
-        <v>10.8031727648949</v>
+        <v>10.149117160222</v>
       </c>
       <c r="H7">
-        <v>11.0136620590001</v>
+        <v>9.441492763744741</v>
       </c>
       <c r="I7">
-        <v>10.9418232246552</v>
+        <v>11.5870576714173</v>
       </c>
       <c r="J7">
-        <v>23.120520984079</v>
+        <v>18.0237835886683</v>
       </c>
       <c r="K7">
-        <v>26.4542131806825</v>
+        <v>17.2674850316021</v>
       </c>
       <c r="L7">
-        <v>70.63250611858121</v>
+        <v>68.2724845758132</v>
       </c>
       <c r="M7">
-        <v>24.721089358147</v>
+        <v>20.8757045276163</v>
       </c>
       <c r="N7">
-        <v>40.069820607378</v>
+        <v>28.1446336103064</v>
       </c>
       <c r="O7">
-        <v>2109.72088513858</v>
+        <v>1895.02697820488</v>
       </c>
       <c r="P7">
-        <v>26.1237166209137</v>
+        <v>39.8181561527282</v>
       </c>
     </row>
     <row r="8">
@@ -758,49 +758,49 @@
         </is>
       </c>
       <c r="B8">
-        <v>480.541030086974</v>
+        <v>728.975487337692</v>
       </c>
       <c r="C8">
-        <v>17.1396514165494</v>
+        <v>16.5858908063122</v>
       </c>
       <c r="D8">
-        <v>9.316977391856771</v>
+        <v>9.31431656426737</v>
       </c>
       <c r="E8">
-        <v>13.3764806062381</v>
+        <v>23.5985356398191</v>
       </c>
       <c r="F8">
-        <v>2.8933745692754</v>
+        <v>0.944301494087143</v>
       </c>
       <c r="G8">
-        <v>34.288450969646</v>
+        <v>29.7623832409898</v>
       </c>
       <c r="H8">
-        <v>14.6607347854669</v>
+        <v>12.2100401574013</v>
       </c>
       <c r="I8">
-        <v>2.02864669497607</v>
+        <v>2.92599351877837</v>
       </c>
       <c r="J8">
-        <v>46.9909980511296</v>
+        <v>52.403815056161</v>
       </c>
       <c r="K8">
-        <v>46.9748460106991</v>
+        <v>36.6602005924526</v>
       </c>
       <c r="L8">
-        <v>45.0097607812675</v>
+        <v>41.6285519149974</v>
       </c>
       <c r="M8">
-        <v>70.75720444612981</v>
+        <v>66.0074481011247</v>
       </c>
       <c r="N8">
-        <v>46.2549817345791</v>
+        <v>30.5108465253586</v>
       </c>
       <c r="O8">
-        <v>1574.08598332351</v>
+        <v>1351.84285902865</v>
       </c>
       <c r="P8">
-        <v>6.50836525532381</v>
+        <v>7.46673951804276</v>
       </c>
     </row>
     <row r="9">
@@ -810,49 +810,49 @@
         </is>
       </c>
       <c r="B9">
-        <v>120.323835799842</v>
+        <v>170.215475037224</v>
       </c>
       <c r="C9">
-        <v>7.77883512021922</v>
+        <v>10.0468659969272</v>
       </c>
       <c r="D9">
-        <v>1.71285511502378</v>
+        <v>2.02897381867205</v>
       </c>
       <c r="E9">
-        <v>4.19053516875917</v>
+        <v>5.28643778822353</v>
       </c>
       <c r="F9">
-        <v>2.43298438201349</v>
+        <v>2.37088365795269</v>
       </c>
       <c r="G9">
-        <v>24.6381490739067</v>
+        <v>22.8367023545677</v>
       </c>
       <c r="H9">
-        <v>3.82179671062446</v>
+        <v>4.2627974923656</v>
       </c>
       <c r="I9">
-        <v>0.742122702190297</v>
+        <v>0.281512285665513</v>
       </c>
       <c r="J9">
-        <v>3.34837820807518</v>
+        <v>3.08256530770771</v>
       </c>
       <c r="K9">
-        <v>4.01551225726424</v>
+        <v>3.66884025228682</v>
       </c>
       <c r="L9">
-        <v>3.29912678050639</v>
+        <v>2.00101870521672</v>
       </c>
       <c r="M9">
-        <v>9.053620318312159</v>
+        <v>7.97241323003273</v>
       </c>
       <c r="N9">
-        <v>5.07379343271493</v>
+        <v>4.53573255879267</v>
       </c>
       <c r="O9">
-        <v>354.289117816761</v>
+        <v>307.183411505851</v>
       </c>
       <c r="P9">
-        <v>6.04007008582979</v>
+        <v>4.97966487149367</v>
       </c>
     </row>
     <row r="10">
@@ -862,49 +862,49 @@
         </is>
       </c>
       <c r="B10">
-        <v>2922.3197780863</v>
+        <v>4261.93824010483</v>
       </c>
       <c r="C10">
-        <v>63.7647807652841</v>
+        <v>54.3653554772369</v>
       </c>
       <c r="D10">
-        <v>49.4087402680209</v>
+        <v>44.2096746481746</v>
       </c>
       <c r="E10">
-        <v>49.0266326424347</v>
+        <v>66.28995457891909</v>
       </c>
       <c r="F10">
-        <v>10.2120844845851</v>
+        <v>11.9688277586096</v>
       </c>
       <c r="G10">
-        <v>46.3140031821666</v>
+        <v>47.2010752234275</v>
       </c>
       <c r="H10">
-        <v>26.7295613696293</v>
+        <v>21.2743674597964</v>
       </c>
       <c r="I10">
-        <v>43.3536493701569</v>
+        <v>29.1826005058623</v>
       </c>
       <c r="J10">
-        <v>54.240070660702</v>
+        <v>47.9640092637999</v>
       </c>
       <c r="K10">
-        <v>58.9052741638122</v>
+        <v>48.0134885652165</v>
       </c>
       <c r="L10">
-        <v>144.4464558569</v>
+        <v>117.008168082801</v>
       </c>
       <c r="M10">
-        <v>104.759874144099</v>
+        <v>90.7591761545398</v>
       </c>
       <c r="N10">
-        <v>114.869550370995</v>
+        <v>107.00386778567</v>
       </c>
       <c r="O10">
-        <v>7734.83247631022</v>
+        <v>6466.94096422243</v>
       </c>
       <c r="P10">
-        <v>93.4515373249847</v>
+        <v>102.010482868437</v>
       </c>
     </row>
     <row r="11">
@@ -914,49 +914,49 @@
         </is>
       </c>
       <c r="B11">
-        <v>1325.24094592297</v>
+        <v>1786.44400435144</v>
       </c>
       <c r="C11">
-        <v>73.882054419531</v>
+        <v>75.1973502665811</v>
       </c>
       <c r="D11">
-        <v>181.774724156334</v>
+        <v>164.983048661863</v>
       </c>
       <c r="E11">
-        <v>103.970154958801</v>
+        <v>110.445397485562</v>
       </c>
       <c r="F11">
-        <v>9.51769287565074</v>
+        <v>13.3020658495239</v>
       </c>
       <c r="G11">
-        <v>39.4989903842233</v>
+        <v>47.7107919203053</v>
       </c>
       <c r="H11">
-        <v>22.1371808142329</v>
+        <v>26.4190749999304</v>
       </c>
       <c r="I11">
-        <v>19.0776520893582</v>
+        <v>24.9867902087537</v>
       </c>
       <c r="J11">
-        <v>56.5430065568769</v>
+        <v>50.2675061415569</v>
       </c>
       <c r="K11">
-        <v>54.3841164828221</v>
+        <v>53.4375056168645</v>
       </c>
       <c r="L11">
-        <v>78.013596009998</v>
+        <v>67.67465031232329</v>
       </c>
       <c r="M11">
-        <v>58.2163600024796</v>
+        <v>70.5773106400581</v>
       </c>
       <c r="N11">
-        <v>64.7277122831393</v>
+        <v>59.4670079175509</v>
       </c>
       <c r="O11">
-        <v>3550.40769025899</v>
+        <v>3066.06255582342</v>
       </c>
       <c r="P11">
-        <v>38.0300389316832</v>
+        <v>58.3857026185594</v>
       </c>
     </row>
     <row r="12">
@@ -966,49 +966,49 @@
         </is>
       </c>
       <c r="B12">
-        <v>196.659707752949</v>
+        <v>293.894801548589</v>
       </c>
       <c r="C12">
-        <v>11.9745800454517</v>
+        <v>8.24366152523246</v>
       </c>
       <c r="D12">
-        <v>4.04648422342273</v>
+        <v>4.95104782331318</v>
       </c>
       <c r="E12">
-        <v>0.816252806555824</v>
+        <v>1.03352752802699</v>
       </c>
       <c r="F12">
-        <v>1.26040316531491</v>
+        <v>0.720301243024804</v>
       </c>
       <c r="G12">
-        <v>1.00202072317796</v>
+        <v>1.16755512601945</v>
       </c>
       <c r="H12">
-        <v>0.324106183104064</v>
+        <v>0.93490403284755</v>
       </c>
       <c r="I12">
-        <v>1.69778358735847</v>
+        <v>1.45200553295133</v>
       </c>
       <c r="J12">
-        <v>1.11854014011125</v>
+        <v>0.82240239156423</v>
       </c>
       <c r="K12">
-        <v>0.679380169298104</v>
+        <v>0.635667646294615</v>
       </c>
       <c r="L12">
-        <v>1.00890013650881</v>
+        <v>1.98686900115808</v>
       </c>
       <c r="M12">
-        <v>5.18582426524184</v>
+        <v>3.7068392636537</v>
       </c>
       <c r="N12">
-        <v>3.80715123922989</v>
+        <v>2.77269146731101</v>
       </c>
       <c r="O12">
-        <v>603.607857297338</v>
+        <v>510.904485786853</v>
       </c>
       <c r="P12">
-        <v>20.4313030617076</v>
+        <v>20.3996871667631</v>
       </c>
     </row>
     <row r="13">
@@ -1018,49 +1018,49 @@
         </is>
       </c>
       <c r="B13">
-        <v>198.121546975493</v>
+        <v>280.199002432048</v>
       </c>
       <c r="C13">
-        <v>27.3351568897384</v>
+        <v>26.6074225667637</v>
       </c>
       <c r="D13">
-        <v>2.12136120194854</v>
+        <v>2.47475266473497</v>
       </c>
       <c r="E13">
-        <v>15.8958667734533</v>
+        <v>20.4860833026574</v>
       </c>
       <c r="F13">
-        <v>5.16640168467483</v>
+        <v>6.53959069250594</v>
       </c>
       <c r="G13">
-        <v>5.51940527616049</v>
+        <v>5.32272345432399</v>
       </c>
       <c r="H13">
-        <v>2.26927567228706</v>
+        <v>2.27719514841413</v>
       </c>
       <c r="I13">
-        <v>2.14810757581839</v>
+        <v>1.8690311277285</v>
       </c>
       <c r="J13">
-        <v>5.94235979288646</v>
+        <v>4.97443516863315</v>
       </c>
       <c r="K13">
-        <v>4.96982278396638</v>
+        <v>2.9535304096612</v>
       </c>
       <c r="L13">
-        <v>28.0932669217353</v>
+        <v>21.1828602352311</v>
       </c>
       <c r="M13">
-        <v>4.67993563878822</v>
+        <v>4.88119723057878</v>
       </c>
       <c r="N13">
-        <v>6.87021538399899</v>
+        <v>7.27133118218478</v>
       </c>
       <c r="O13">
-        <v>533.4171594384191</v>
+        <v>462.372807287483</v>
       </c>
       <c r="P13">
-        <v>49.1817806350607</v>
+        <v>42.3427999496964</v>
       </c>
     </row>
     <row r="14">
@@ -1070,49 +1070,49 @@
         </is>
       </c>
       <c r="B14">
-        <v>1927.56779707315</v>
+        <v>2685.94779577808</v>
       </c>
       <c r="C14">
-        <v>126.784990628812</v>
+        <v>114.826254044976</v>
       </c>
       <c r="D14">
-        <v>20.3755751182095</v>
+        <v>20.5048266270638</v>
       </c>
       <c r="E14">
-        <v>63.1830810756283</v>
+        <v>97.45622549265261</v>
       </c>
       <c r="F14">
-        <v>17.3357605370785</v>
+        <v>25.3537312202551</v>
       </c>
       <c r="G14">
-        <v>115.974981500317</v>
+        <v>99.69155326737869</v>
       </c>
       <c r="H14">
-        <v>62.046876173648</v>
+        <v>64.84960826139761</v>
       </c>
       <c r="I14">
-        <v>37.292601766527</v>
+        <v>32.0190517410773</v>
       </c>
       <c r="J14">
-        <v>150.999347704135</v>
+        <v>186.565006944813</v>
       </c>
       <c r="K14">
-        <v>208.468365585892</v>
+        <v>181.383615494039</v>
       </c>
       <c r="L14">
-        <v>179.815018050927</v>
+        <v>172.392244472769</v>
       </c>
       <c r="M14">
-        <v>99.5792257257807</v>
+        <v>100.50082668854</v>
       </c>
       <c r="N14">
-        <v>102.684668399769</v>
+        <v>103.009342009149</v>
       </c>
       <c r="O14">
-        <v>5609.05174601724</v>
+        <v>4791.53816655745</v>
       </c>
       <c r="P14">
-        <v>39.390970477924</v>
+        <v>84.4777120232045</v>
       </c>
     </row>
     <row r="15">
@@ -1122,49 +1122,49 @@
         </is>
       </c>
       <c r="B15">
-        <v>947.433184502429</v>
+        <v>1298.89704470066</v>
       </c>
       <c r="C15">
-        <v>34.4086180631402</v>
+        <v>42.6477855809541</v>
       </c>
       <c r="D15">
-        <v>15.8690461158909</v>
+        <v>15.2714157564213</v>
       </c>
       <c r="E15">
-        <v>58.5162172267104</v>
+        <v>67.759472475587</v>
       </c>
       <c r="F15">
-        <v>14.2453903641304</v>
+        <v>13.3585069822928</v>
       </c>
       <c r="G15">
-        <v>47.3415112955349</v>
+        <v>47.3609754202629</v>
       </c>
       <c r="H15">
-        <v>51.661034487475</v>
+        <v>52.3487487127116</v>
       </c>
       <c r="I15">
-        <v>47.5687882969829</v>
+        <v>33.0650875775596</v>
       </c>
       <c r="J15">
-        <v>200.476069137659</v>
+        <v>177.830554140287</v>
       </c>
       <c r="K15">
-        <v>111.326648381254</v>
+        <v>89.6863503282009</v>
       </c>
       <c r="L15">
-        <v>71.66427387001799</v>
+        <v>83.8648197116266</v>
       </c>
       <c r="M15">
-        <v>162.379906831843</v>
+        <v>187.319596955542</v>
       </c>
       <c r="N15">
-        <v>100.720191404153</v>
+        <v>70.9075472774195</v>
       </c>
       <c r="O15">
-        <v>2383.96939774711</v>
+        <v>2076.37071068164</v>
       </c>
       <c r="P15">
-        <v>47.6428069096457</v>
+        <v>38.5766160613724</v>
       </c>
     </row>
     <row r="16">
@@ -1174,49 +1174,49 @@
         </is>
       </c>
       <c r="B16">
-        <v>334.014791003096</v>
+        <v>534.497205250248</v>
       </c>
       <c r="C16">
-        <v>65.3586681723006</v>
+        <v>60.6773462589503</v>
       </c>
       <c r="D16">
-        <v>16.0645463924195</v>
+        <v>10.9382316983721</v>
       </c>
       <c r="E16">
-        <v>16.1575315359967</v>
+        <v>25.8928923153384</v>
       </c>
       <c r="F16">
-        <v>4.77262665244336</v>
+        <v>4.00502068017659</v>
       </c>
       <c r="G16">
-        <v>15.8039386015776</v>
+        <v>13.8419381235624</v>
       </c>
       <c r="H16">
-        <v>15.053460585439</v>
+        <v>14.9254099771511</v>
       </c>
       <c r="I16">
-        <v>11.0320240129759</v>
+        <v>14.8260033783125</v>
       </c>
       <c r="J16">
-        <v>45.0169460897291</v>
+        <v>48.111837122349</v>
       </c>
       <c r="K16">
-        <v>55.6367233620095</v>
+        <v>49.6377641966877</v>
       </c>
       <c r="L16">
-        <v>32.6855241761649</v>
+        <v>38.5470704649172</v>
       </c>
       <c r="M16">
-        <v>14.7788097336027</v>
+        <v>23.5437063863778</v>
       </c>
       <c r="N16">
-        <v>29.558460996696</v>
+        <v>23.3705302444889</v>
       </c>
       <c r="O16">
-        <v>1312.10370414818</v>
+        <v>1116.19289059643</v>
       </c>
       <c r="P16">
-        <v>95.2165300168148</v>
+        <v>84.27738009737411</v>
       </c>
     </row>
     <row r="17">
@@ -1226,49 +1226,49 @@
         </is>
       </c>
       <c r="B17">
-        <v>354.118436693893</v>
+        <v>523.967681230208</v>
       </c>
       <c r="C17">
-        <v>27.4930425509592</v>
+        <v>31.607815069463</v>
       </c>
       <c r="D17">
-        <v>8.027592137719891</v>
+        <v>6.44760992918903</v>
       </c>
       <c r="E17">
-        <v>9.715500851299209</v>
+        <v>15.2421749228039</v>
       </c>
       <c r="F17">
-        <v>13.0143011403895</v>
+        <v>15.0705887854177</v>
       </c>
       <c r="G17">
-        <v>12.4711187378769</v>
+        <v>11.9034612897312</v>
       </c>
       <c r="H17">
-        <v>8.657249488025229</v>
+        <v>15.2932048022965</v>
       </c>
       <c r="I17">
-        <v>7.94405551882832</v>
+        <v>8.09642526085373</v>
       </c>
       <c r="J17">
-        <v>20.4849316858812</v>
+        <v>21.3341256343883</v>
       </c>
       <c r="K17">
-        <v>25.1178273075355</v>
+        <v>27.3375617235326</v>
       </c>
       <c r="L17">
-        <v>14.156652696269</v>
+        <v>16.5827482800561</v>
       </c>
       <c r="M17">
-        <v>79.08275177754589</v>
+        <v>74.9675946840127</v>
       </c>
       <c r="N17">
-        <v>16.3583470321655</v>
+        <v>17.1003783471084</v>
       </c>
       <c r="O17">
-        <v>1226.63042760495</v>
+        <v>1023.69025904723</v>
       </c>
       <c r="P17">
-        <v>58.7664870858442</v>
+        <v>73.4478891102937</v>
       </c>
     </row>
     <row r="18">
@@ -1278,49 +1278,49 @@
         </is>
       </c>
       <c r="B18">
-        <v>839.14776350022</v>
+        <v>1046.90990988774</v>
       </c>
       <c r="C18">
-        <v>32.5520903361579</v>
+        <v>34.9148624220921</v>
       </c>
       <c r="D18">
-        <v>18.5103252527292</v>
+        <v>30.8559832949836</v>
       </c>
       <c r="E18">
-        <v>30.351636034262</v>
+        <v>42.2595389541995</v>
       </c>
       <c r="F18">
-        <v>40.6263072121668</v>
+        <v>35.5687823641702</v>
       </c>
       <c r="G18">
-        <v>32.9905227833032</v>
+        <v>29.0926827426063</v>
       </c>
       <c r="H18">
-        <v>21.0551609636316</v>
+        <v>24.6239537731645</v>
       </c>
       <c r="I18">
-        <v>9.541441526527009</v>
+        <v>8.997022308455311</v>
       </c>
       <c r="J18">
-        <v>32.246398546898</v>
+        <v>45.5368344809074</v>
       </c>
       <c r="K18">
-        <v>38.1872555986806</v>
+        <v>39.957087574057</v>
       </c>
       <c r="L18">
-        <v>46.4703593380309</v>
+        <v>48.7855416936223</v>
       </c>
       <c r="M18">
-        <v>58.7227117583695</v>
+        <v>65.5967754006965</v>
       </c>
       <c r="N18">
-        <v>22.3615843147832</v>
+        <v>29.152925071816</v>
       </c>
       <c r="O18">
-        <v>1623.34265454442</v>
+        <v>1369.58839121828</v>
       </c>
       <c r="P18">
-        <v>48.9067233638985</v>
+        <v>43.2015466589629</v>
       </c>
     </row>
     <row r="19">
@@ -1330,49 +1330,49 @@
         </is>
       </c>
       <c r="B19">
-        <v>914.082123620849</v>
+        <v>1169.84266274599</v>
       </c>
       <c r="C19">
-        <v>29.2245753872958</v>
+        <v>24.9744061602189</v>
       </c>
       <c r="D19">
-        <v>17.1051421055931</v>
+        <v>18.1765026575804</v>
       </c>
       <c r="E19">
-        <v>24.023479670697</v>
+        <v>39.9590721268225</v>
       </c>
       <c r="F19">
-        <v>96.0301099301853</v>
+        <v>71.5988260307292</v>
       </c>
       <c r="G19">
-        <v>43.0037095628364</v>
+        <v>43.7801760216017</v>
       </c>
       <c r="H19">
-        <v>6.28146006319015</v>
+        <v>6.01933105047655</v>
       </c>
       <c r="I19">
-        <v>8.228509623541029</v>
+        <v>7.62535125961992</v>
       </c>
       <c r="J19">
-        <v>13.6429414149605</v>
+        <v>20.0429182978859</v>
       </c>
       <c r="K19">
-        <v>14.1589314015608</v>
+        <v>12.7177983016376</v>
       </c>
       <c r="L19">
-        <v>8.955013198010111</v>
+        <v>12.3117606581055</v>
       </c>
       <c r="M19">
-        <v>27.1378029127332</v>
+        <v>27.5400099857348</v>
       </c>
       <c r="N19">
-        <v>10.1461408753343</v>
+        <v>13.0955648263722</v>
       </c>
       <c r="O19">
-        <v>1827.93361602091</v>
+        <v>1571.13502608026</v>
       </c>
       <c r="P19">
-        <v>39.3786296577106</v>
+        <v>40.5124771485005</v>
       </c>
     </row>
     <row r="20">
@@ -1382,49 +1382,49 @@
         </is>
       </c>
       <c r="B20">
-        <v>201.378971010919</v>
+        <v>293.462197631221</v>
       </c>
       <c r="C20">
-        <v>9.365039611076149</v>
+        <v>8.136679711711221</v>
       </c>
       <c r="D20">
-        <v>18.4177024306412</v>
+        <v>16.9008236423214</v>
       </c>
       <c r="E20">
-        <v>32.4280578632098</v>
+        <v>34.1762785272218</v>
       </c>
       <c r="F20">
-        <v>0.689078879378622</v>
+        <v>0.26273761668546</v>
       </c>
       <c r="G20">
-        <v>1.44366432813385</v>
+        <v>1.86580325640495</v>
       </c>
       <c r="H20">
-        <v>4.31386041274117</v>
+        <v>3.26319755949231</v>
       </c>
       <c r="I20">
-        <v>0.879587283620681</v>
+        <v>1.16652060187282</v>
       </c>
       <c r="J20">
-        <v>3.48698269628341</v>
+        <v>6.76898733938144</v>
       </c>
       <c r="K20">
-        <v>5.27104975375041</v>
+        <v>5.43412651206477</v>
       </c>
       <c r="L20">
-        <v>9.61149560809611</v>
+        <v>10.5816510901135</v>
       </c>
       <c r="M20">
-        <v>22.2088643137272</v>
+        <v>17.8295794977926</v>
       </c>
       <c r="N20">
-        <v>5.29291015138251</v>
+        <v>5.83772418192329</v>
       </c>
       <c r="O20">
-        <v>582.918692080631</v>
+        <v>490.126313486207</v>
       </c>
       <c r="P20">
-        <v>22.4401685282581</v>
+        <v>24.3481487440958</v>
       </c>
     </row>
     <row r="21">
@@ -1434,49 +1434,49 @@
         </is>
       </c>
       <c r="B21">
-        <v>839.039684615126</v>
+        <v>1077.43123261643</v>
       </c>
       <c r="C21">
-        <v>32.0951581235593</v>
+        <v>30.9005935509151</v>
       </c>
       <c r="D21">
-        <v>10.7517649835086</v>
+        <v>13.9377193983874</v>
       </c>
       <c r="E21">
-        <v>19.3885786529658</v>
+        <v>33.9218456653992</v>
       </c>
       <c r="F21">
-        <v>3.37496289729722</v>
+        <v>5.08979301085637</v>
       </c>
       <c r="G21">
-        <v>22.4313915003937</v>
+        <v>13.7503518743044</v>
       </c>
       <c r="H21">
-        <v>10.8611507230871</v>
+        <v>21.2857910733231</v>
       </c>
       <c r="I21">
-        <v>9.26195844816591</v>
+        <v>9.45591801076932</v>
       </c>
       <c r="J21">
-        <v>21.1408438026066</v>
+        <v>16.358435554809</v>
       </c>
       <c r="K21">
-        <v>18.7921080515391</v>
+        <v>17.6468650963224</v>
       </c>
       <c r="L21">
-        <v>30.291323394083</v>
+        <v>39.1127468738507</v>
       </c>
       <c r="M21">
-        <v>38.3927753795673</v>
+        <v>38.1832674019375</v>
       </c>
       <c r="N21">
-        <v>18.9154100606515</v>
+        <v>19.4497761691559</v>
       </c>
       <c r="O21">
-        <v>2622.35987584634</v>
+        <v>2366.48378453545</v>
       </c>
       <c r="P21">
-        <v>25.4623555759288</v>
+        <v>19.5951588858586</v>
       </c>
     </row>
     <row r="22">
@@ -1486,49 +1486,49 @@
         </is>
       </c>
       <c r="B22">
-        <v>948.118627037897</v>
+        <v>1339.50948416087</v>
       </c>
       <c r="C22">
-        <v>21.939177866103</v>
+        <v>25.884881657114</v>
       </c>
       <c r="D22">
-        <v>37.2519051181855</v>
+        <v>37.5185398334899</v>
       </c>
       <c r="E22">
-        <v>30.207788158726</v>
+        <v>38.3760695404797</v>
       </c>
       <c r="F22">
-        <v>3.42214774517</v>
+        <v>2.78280569100777</v>
       </c>
       <c r="G22">
-        <v>35.7757424184891</v>
+        <v>27.0865196777349</v>
       </c>
       <c r="H22">
-        <v>33.9109595802639</v>
+        <v>29.0190977433709</v>
       </c>
       <c r="I22">
-        <v>9.889006029960409</v>
+        <v>11.1006074005778</v>
       </c>
       <c r="J22">
-        <v>58.3793766255936</v>
+        <v>60.6488098177626</v>
       </c>
       <c r="K22">
-        <v>53.6604932339116</v>
+        <v>45.7345894122181</v>
       </c>
       <c r="L22">
-        <v>133.393081444068</v>
+        <v>133.78669221209</v>
       </c>
       <c r="M22">
-        <v>23.7895461993814</v>
+        <v>24.3231061998333</v>
       </c>
       <c r="N22">
-        <v>100.476721970467</v>
+        <v>81.65355891883471</v>
       </c>
       <c r="O22">
-        <v>3048.2067669042</v>
+        <v>2683.67750717556</v>
       </c>
       <c r="P22">
-        <v>21.6795842878557</v>
+        <v>19.0193947340342</v>
       </c>
     </row>
     <row r="23">
@@ -1538,49 +1538,49 @@
         </is>
       </c>
       <c r="B23">
-        <v>1622.72451377556</v>
+        <v>2259.4187103394</v>
       </c>
       <c r="C23">
-        <v>52.569487289442</v>
+        <v>50.4928820684313</v>
       </c>
       <c r="D23">
-        <v>17.1916509474503</v>
+        <v>19.1705037749862</v>
       </c>
       <c r="E23">
-        <v>39.1011918870334</v>
+        <v>65.3385897979186</v>
       </c>
       <c r="F23">
-        <v>4.12544239150013</v>
+        <v>5.61844446975169</v>
       </c>
       <c r="G23">
-        <v>68.1829529701774</v>
+        <v>64.2356529154482</v>
       </c>
       <c r="H23">
-        <v>71.1903106234081</v>
+        <v>65.4416628562585</v>
       </c>
       <c r="I23">
-        <v>23.3059147059899</v>
+        <v>22.4878021545648</v>
       </c>
       <c r="J23">
-        <v>167.153667737721</v>
+        <v>178.171326552623</v>
       </c>
       <c r="K23">
-        <v>157.509112593937</v>
+        <v>132.560795779804</v>
       </c>
       <c r="L23">
-        <v>55.7499113106022</v>
+        <v>56.7832739681505</v>
       </c>
       <c r="M23">
-        <v>616.954736008991</v>
+        <v>532.296324073191</v>
       </c>
       <c r="N23">
-        <v>106.870679718288</v>
+        <v>94.629831641053</v>
       </c>
       <c r="O23">
-        <v>3964.49721238944</v>
+        <v>3393.20695985529</v>
       </c>
       <c r="P23">
-        <v>43.5650617302365</v>
+        <v>70.8389871020707</v>
       </c>
     </row>
     <row r="24">
@@ -1590,49 +1590,49 @@
         </is>
       </c>
       <c r="B24">
-        <v>566.460542245841</v>
+        <v>865.2026153199651</v>
       </c>
       <c r="C24">
-        <v>45.7309228151562</v>
+        <v>71.8871081403139</v>
       </c>
       <c r="D24">
-        <v>13.7094547959318</v>
+        <v>8.205752972459569</v>
       </c>
       <c r="E24">
-        <v>42.7285289236648</v>
+        <v>67.044682932017</v>
       </c>
       <c r="F24">
-        <v>16.0536317488587</v>
+        <v>18.3692868684119</v>
       </c>
       <c r="G24">
-        <v>27.7314396215158</v>
+        <v>17.3923409446076</v>
       </c>
       <c r="H24">
-        <v>23.7819399801807</v>
+        <v>28.9470656174223</v>
       </c>
       <c r="I24">
-        <v>15.5573406721035</v>
+        <v>10.1293210780359</v>
       </c>
       <c r="J24">
-        <v>40.1267388495266</v>
+        <v>58.6709696318547</v>
       </c>
       <c r="K24">
-        <v>98.6633781603317</v>
+        <v>62.1990682577345</v>
       </c>
       <c r="L24">
-        <v>68.5445160233035</v>
+        <v>77.6702159068402</v>
       </c>
       <c r="M24">
-        <v>20.108825168259</v>
+        <v>22.1242136427015</v>
       </c>
       <c r="N24">
-        <v>88.94693247575481</v>
+        <v>63.5015693239902</v>
       </c>
       <c r="O24">
-        <v>2296.19188245015</v>
+        <v>1964.79003067697</v>
       </c>
       <c r="P24">
-        <v>92.7306544809347</v>
+        <v>120.954118002462</v>
       </c>
     </row>
     <row r="25">
@@ -1642,49 +1642,49 @@
         </is>
       </c>
       <c r="B25">
-        <v>539.385026097631</v>
+        <v>735.618888391426</v>
       </c>
       <c r="C25">
-        <v>46.518841542389</v>
+        <v>35.2100861037667</v>
       </c>
       <c r="D25">
-        <v>19.4577660142224</v>
+        <v>28.6337109795753</v>
       </c>
       <c r="E25">
-        <v>39.9189883291451</v>
+        <v>34.4970565580722</v>
       </c>
       <c r="F25">
-        <v>27.4283450604598</v>
+        <v>17.9049016266198</v>
       </c>
       <c r="G25">
-        <v>10.3878071526179</v>
+        <v>12.4161701621486</v>
       </c>
       <c r="H25">
-        <v>16.5092530489047</v>
+        <v>16.7514013455531</v>
       </c>
       <c r="I25">
-        <v>5.35568890154511</v>
+        <v>4.978841556205</v>
       </c>
       <c r="J25">
-        <v>19.8640422235227</v>
+        <v>21.9051777990684</v>
       </c>
       <c r="K25">
-        <v>22.6051898374343</v>
+        <v>18.7810283289994</v>
       </c>
       <c r="L25">
-        <v>29.5678561473986</v>
+        <v>34.1510724440874</v>
       </c>
       <c r="M25">
-        <v>34.5020664362315</v>
+        <v>26.1757039218367</v>
       </c>
       <c r="N25">
-        <v>30.5434465793455</v>
+        <v>45.9962115087641</v>
       </c>
       <c r="O25">
-        <v>1055.01721036501</v>
+        <v>870.790118786016</v>
       </c>
       <c r="P25">
-        <v>46.2923913502756</v>
+        <v>39.5232937405508</v>
       </c>
     </row>
     <row r="26">
@@ -1694,49 +1694,49 @@
         </is>
       </c>
       <c r="B26">
-        <v>808.305760752846</v>
+        <v>1216.78381990952</v>
       </c>
       <c r="C26">
-        <v>65.6489635658512</v>
+        <v>61.1430995333746</v>
       </c>
       <c r="D26">
-        <v>16.6689414873</v>
+        <v>17.8015068774224</v>
       </c>
       <c r="E26">
-        <v>38.5434779604663</v>
+        <v>50.7099100726775</v>
       </c>
       <c r="F26">
-        <v>7.38526672977478</v>
+        <v>4.19368662271761</v>
       </c>
       <c r="G26">
-        <v>46.9619887546387</v>
+        <v>35.9260711545228</v>
       </c>
       <c r="H26">
-        <v>20.8029442195974</v>
+        <v>25.5937636651417</v>
       </c>
       <c r="I26">
-        <v>16.4844045802342</v>
+        <v>17.8978675294592</v>
       </c>
       <c r="J26">
-        <v>60.0636141435348</v>
+        <v>63.1871191828055</v>
       </c>
       <c r="K26">
-        <v>59.4012337450077</v>
+        <v>51.9145295354277</v>
       </c>
       <c r="L26">
-        <v>34.9002288991616</v>
+        <v>42.8993913529518</v>
       </c>
       <c r="M26">
-        <v>75.8773583158338</v>
+        <v>88.91232691530131</v>
       </c>
       <c r="N26">
-        <v>40.977920812906</v>
+        <v>41.4211495719713</v>
       </c>
       <c r="O26">
-        <v>2600.31751223387</v>
+        <v>2151.28435922654</v>
       </c>
       <c r="P26">
-        <v>50.5532270552522</v>
+        <v>73.23356483204969</v>
       </c>
     </row>
     <row r="27">
@@ -1746,49 +1746,49 @@
         </is>
       </c>
       <c r="B27">
-        <v>140.573751363302</v>
+        <v>199.076684209529</v>
       </c>
       <c r="C27">
-        <v>3.96124892551835</v>
+        <v>3.1370211119833</v>
       </c>
       <c r="D27">
-        <v>1.09112742918001</v>
+        <v>1.53794594244035</v>
       </c>
       <c r="E27">
-        <v>12.0415246270566</v>
+        <v>11.4907424452274</v>
       </c>
       <c r="F27">
-        <v>6.70618606602504</v>
+        <v>8.72397641430674</v>
       </c>
       <c r="G27">
-        <v>0.702513597448498</v>
+        <v>0.768433781165237</v>
       </c>
       <c r="H27">
-        <v>0.366534921712657</v>
+        <v>0.303443517505309</v>
       </c>
       <c r="I27">
-        <v>2.28920924558393</v>
+        <v>1.57305524261065</v>
       </c>
       <c r="J27">
-        <v>4.94638886359155</v>
+        <v>4.45888189705332</v>
       </c>
       <c r="K27">
-        <v>2.01042806832806</v>
+        <v>1.68845471479037</v>
       </c>
       <c r="L27">
-        <v>2.48192501502413</v>
+        <v>1.72482228053544</v>
       </c>
       <c r="M27">
-        <v>1.51664672801614</v>
+        <v>1.15521744790459</v>
       </c>
       <c r="N27">
-        <v>6.19796791347159</v>
+        <v>4.94520638208155</v>
       </c>
       <c r="O27">
-        <v>415.685674299533</v>
+        <v>355.530094040322</v>
       </c>
       <c r="P27">
-        <v>42.1487680913994</v>
+        <v>46.5993375546977</v>
       </c>
     </row>
     <row r="28">
@@ -1798,49 +1798,49 @@
         </is>
       </c>
       <c r="B28">
-        <v>189.496183339868</v>
+        <v>308.062913142309</v>
       </c>
       <c r="C28">
-        <v>28.0044262889178</v>
+        <v>33.67085720315</v>
       </c>
       <c r="D28">
-        <v>2.99106869478376</v>
+        <v>1.9835425354511</v>
       </c>
       <c r="E28">
-        <v>5.65711782095564</v>
+        <v>8.46678932217529</v>
       </c>
       <c r="F28">
-        <v>2.61335902780851</v>
+        <v>1.9394799093711</v>
       </c>
       <c r="G28">
-        <v>7.5107813907564</v>
+        <v>5.30727530483647</v>
       </c>
       <c r="H28">
-        <v>8.581816203238869</v>
+        <v>7.55810185464167</v>
       </c>
       <c r="I28">
-        <v>4.43833831919274</v>
+        <v>4.8628231902685</v>
       </c>
       <c r="J28">
-        <v>15.5840992373442</v>
+        <v>17.8240752091484</v>
       </c>
       <c r="K28">
-        <v>16.7069225200633</v>
+        <v>16.5402209008487</v>
       </c>
       <c r="L28">
-        <v>13.7912766564364</v>
+        <v>10.5527934210211</v>
       </c>
       <c r="M28">
-        <v>6.98234176006313</v>
+        <v>8.07768973266921</v>
       </c>
       <c r="N28">
-        <v>12.172800429456</v>
+        <v>11.4057484576783</v>
       </c>
       <c r="O28">
-        <v>795.746234688734</v>
+        <v>668.959151628356</v>
       </c>
       <c r="P28">
-        <v>85.39655381116459</v>
+        <v>90.4753626937172</v>
       </c>
     </row>
     <row r="29">
@@ -1850,49 +1850,49 @@
         </is>
       </c>
       <c r="B29">
-        <v>322.452310021209</v>
+        <v>452.45145814494</v>
       </c>
       <c r="C29">
-        <v>5.45250198631043</v>
+        <v>6.5501464481183</v>
       </c>
       <c r="D29">
-        <v>3.64742965904264</v>
+        <v>3.36258719392007</v>
       </c>
       <c r="E29">
-        <v>2.33507973463641</v>
+        <v>5.52023663330243</v>
       </c>
       <c r="F29">
-        <v>15.9938694462648</v>
+        <v>16.9309334014761</v>
       </c>
       <c r="G29">
-        <v>2.6773584003731</v>
+        <v>2.25777430336111</v>
       </c>
       <c r="H29">
-        <v>2.55391189689644</v>
+        <v>2.44346327199796</v>
       </c>
       <c r="I29">
-        <v>5.54833434169032</v>
+        <v>4.91278342435096</v>
       </c>
       <c r="J29">
-        <v>5.26161220750469</v>
+        <v>7.18960929293192</v>
       </c>
       <c r="K29">
-        <v>3.88885634670775</v>
+        <v>2.58489846547419</v>
       </c>
       <c r="L29">
-        <v>4.87254420530103</v>
+        <v>5.69715193394456</v>
       </c>
       <c r="M29">
-        <v>2.35725257758319</v>
+        <v>3.00477412406027</v>
       </c>
       <c r="N29">
-        <v>10.7795449654614</v>
+        <v>14.0174155156279</v>
       </c>
       <c r="O29">
-        <v>997.859455673869</v>
+        <v>857.813310589323</v>
       </c>
       <c r="P29">
-        <v>3.81360584686136</v>
+        <v>4.80766353206247</v>
       </c>
     </row>
     <row r="30">
@@ -1902,49 +1902,49 @@
         </is>
       </c>
       <c r="B30">
-        <v>163.635815401152</v>
+        <v>235.381801910105</v>
       </c>
       <c r="C30">
-        <v>5.05843142382786</v>
+        <v>3.77494986993697</v>
       </c>
       <c r="D30">
-        <v>7.85311698486403</v>
+        <v>5.74920759548003</v>
       </c>
       <c r="E30">
-        <v>8.808196704673479</v>
+        <v>14.6070869924591</v>
       </c>
       <c r="F30">
-        <v>0.547602580794708</v>
+        <v>0.936210633301014</v>
       </c>
       <c r="G30">
-        <v>4.06966767228786</v>
+        <v>5.15705791744963</v>
       </c>
       <c r="H30">
-        <v>6.61025852295855</v>
+        <v>5.89778643073005</v>
       </c>
       <c r="I30">
-        <v>2.67554260452983</v>
+        <v>2.31906094395044</v>
       </c>
       <c r="J30">
-        <v>16.9502330637648</v>
+        <v>19.5892595370797</v>
       </c>
       <c r="K30">
-        <v>20.6531490947031</v>
+        <v>12.6864260054867</v>
       </c>
       <c r="L30">
-        <v>41.5119707616311</v>
+        <v>42.5973046068522</v>
       </c>
       <c r="M30">
-        <v>11.0298411502183</v>
+        <v>10.6227255859435</v>
       </c>
       <c r="N30">
-        <v>16.0981560180182</v>
+        <v>15.7836705456432</v>
       </c>
       <c r="O30">
-        <v>567.924599331462</v>
+        <v>497.848841105928</v>
       </c>
       <c r="P30">
-        <v>7.56807202568803</v>
+        <v>8.051487239930591</v>
       </c>
     </row>
     <row r="31">
@@ -1954,49 +1954,49 @@
         </is>
       </c>
       <c r="B31">
-        <v>1416.52253834526</v>
+        <v>1989.99311756414</v>
       </c>
       <c r="C31">
-        <v>50.6903825221046</v>
+        <v>47.5844604183837</v>
       </c>
       <c r="D31">
-        <v>59.1109237094523</v>
+        <v>49.6902589846837</v>
       </c>
       <c r="E31">
-        <v>25.6200413960435</v>
+        <v>31.9946487662315</v>
       </c>
       <c r="F31">
-        <v>9.547250059534409</v>
+        <v>13.1945067190421</v>
       </c>
       <c r="G31">
-        <v>155.192484499096</v>
+        <v>150.490754967827</v>
       </c>
       <c r="H31">
-        <v>29.5443233434808</v>
+        <v>30.7511337766412</v>
       </c>
       <c r="I31">
-        <v>31.1350409176447</v>
+        <v>26.2866947821393</v>
       </c>
       <c r="J31">
-        <v>44.9713719617553</v>
+        <v>40.7848700046967</v>
       </c>
       <c r="K31">
-        <v>47.4927040865106</v>
+        <v>42.2554412721478</v>
       </c>
       <c r="L31">
-        <v>65.25649948325059</v>
+        <v>60.3677917726294</v>
       </c>
       <c r="M31">
-        <v>30.0658377555024</v>
+        <v>30.3465238482269</v>
       </c>
       <c r="N31">
-        <v>72.5412472771939</v>
+        <v>71.0102554651713</v>
       </c>
       <c r="O31">
-        <v>3991.80434796961</v>
+        <v>3442.53778776368</v>
       </c>
       <c r="P31">
-        <v>9.07885158490814</v>
+        <v>11.2882497267854</v>
       </c>
     </row>
     <row r="32">
@@ -2006,49 +2006,49 @@
         </is>
       </c>
       <c r="B32">
-        <v>347.501403045607</v>
+        <v>469.86017838227</v>
       </c>
       <c r="C32">
-        <v>4.6860197772975</v>
+        <v>4.68117043310382</v>
       </c>
       <c r="D32">
-        <v>3.30558955324121</v>
+        <v>4.12815043320869</v>
       </c>
       <c r="E32">
-        <v>3.12704404051275</v>
+        <v>2.71470113740485</v>
       </c>
       <c r="F32">
-        <v>32.8076865520459</v>
+        <v>22.4266553640703</v>
       </c>
       <c r="G32">
-        <v>2.13027889786302</v>
+        <v>2.28731990324421</v>
       </c>
       <c r="H32">
-        <v>2.58681103341938</v>
+        <v>1.2909772103003</v>
       </c>
       <c r="I32">
-        <v>2.97474291288707</v>
+        <v>3.47941489738063</v>
       </c>
       <c r="J32">
-        <v>3.27304325223402</v>
+        <v>1.82110608286975</v>
       </c>
       <c r="K32">
-        <v>5.8535414452795</v>
+        <v>4.64025007658797</v>
       </c>
       <c r="L32">
-        <v>15.4804687208459</v>
+        <v>14.2198435764762</v>
       </c>
       <c r="M32">
-        <v>4.17314556931131</v>
+        <v>5.39289236376901</v>
       </c>
       <c r="N32">
-        <v>12.9425327634238</v>
+        <v>10.7727623588742</v>
       </c>
       <c r="O32">
-        <v>795.356952009175</v>
+        <v>684.955237653412</v>
       </c>
       <c r="P32">
-        <v>26.972864503352</v>
+        <v>30.5132521017565</v>
       </c>
     </row>
     <row r="33">
@@ -2058,49 +2058,49 @@
         </is>
       </c>
       <c r="B33">
-        <v>3716.97622638988</v>
+        <v>4966.1271442769</v>
       </c>
       <c r="C33">
-        <v>86.88151336220589</v>
+        <v>83.0467069988069</v>
       </c>
       <c r="D33">
-        <v>159.991669558534</v>
+        <v>140.958268069453</v>
       </c>
       <c r="E33">
-        <v>41.2998941733168</v>
+        <v>86.0021449413394</v>
       </c>
       <c r="F33">
-        <v>11.97613631183</v>
+        <v>11.4561960123759</v>
       </c>
       <c r="G33">
-        <v>77.6973147575719</v>
+        <v>81.6600824960163</v>
       </c>
       <c r="H33">
-        <v>44.0090200003215</v>
+        <v>49.3893159183442</v>
       </c>
       <c r="I33">
-        <v>39.463450934628</v>
+        <v>46.2394858751952</v>
       </c>
       <c r="J33">
-        <v>110.301896976244</v>
+        <v>120.308220225919</v>
       </c>
       <c r="K33">
-        <v>121.903605414272</v>
+        <v>123.473493111889</v>
       </c>
       <c r="L33">
-        <v>157.124847957109</v>
+        <v>150.139134577737</v>
       </c>
       <c r="M33">
-        <v>88.2586994545437</v>
+        <v>90.89892055836199</v>
       </c>
       <c r="N33">
-        <v>210.886080438328</v>
+        <v>154.902199151613</v>
       </c>
       <c r="O33">
-        <v>8667.750330113369</v>
+        <v>7407.27167725685</v>
       </c>
       <c r="P33">
-        <v>63.299351489758</v>
+        <v>86.08198844794561</v>
       </c>
     </row>
     <row r="34">
@@ -2110,49 +2110,49 @@
         </is>
       </c>
       <c r="B34">
-        <v>1343.80866573539</v>
+        <v>1761.14392675455</v>
       </c>
       <c r="C34">
-        <v>91.82544317695459</v>
+        <v>80.7591783470438</v>
       </c>
       <c r="D34">
-        <v>237.740439687151</v>
+        <v>227.347173200802</v>
       </c>
       <c r="E34">
-        <v>59.79093113887</v>
+        <v>83.5487411073368</v>
       </c>
       <c r="F34">
-        <v>5.9655036303807</v>
+        <v>6.82360527421301</v>
       </c>
       <c r="G34">
-        <v>74.11870544281931</v>
+        <v>71.1318921968619</v>
       </c>
       <c r="H34">
-        <v>52.096614648101</v>
+        <v>47.9370509255264</v>
       </c>
       <c r="I34">
-        <v>23.4811674254887</v>
+        <v>30.3982447634987</v>
       </c>
       <c r="J34">
-        <v>62.3957389557105</v>
+        <v>56.4343771572463</v>
       </c>
       <c r="K34">
-        <v>86.61973725618439</v>
+        <v>62.8953056525506</v>
       </c>
       <c r="L34">
-        <v>136.026001603287</v>
+        <v>115.07116548162</v>
       </c>
       <c r="M34">
-        <v>53.0620336217656</v>
+        <v>53.188200170489</v>
       </c>
       <c r="N34">
-        <v>133.813034634273</v>
+        <v>140.545603065836</v>
       </c>
       <c r="O34">
-        <v>3213.95513562043</v>
+        <v>2848.379446076</v>
       </c>
       <c r="P34">
-        <v>74.385061498204</v>
+        <v>63.4713812305307</v>
       </c>
     </row>
     <row r="35">
@@ -2162,49 +2162,49 @@
         </is>
       </c>
       <c r="B35">
-        <v>75.0810578537896</v>
+        <v>126.248993981484</v>
       </c>
       <c r="C35">
-        <v>5.09957349116968</v>
+        <v>6.83545228747081</v>
       </c>
       <c r="D35">
-        <v>0.788863249652717</v>
+        <v>1.02706732601107</v>
       </c>
       <c r="E35">
-        <v>3.28039688947869</v>
+        <v>1.6917637399754</v>
       </c>
       <c r="F35">
-        <v>5.33818202567532</v>
+        <v>5.41393379689693</v>
       </c>
       <c r="G35">
-        <v>0.305701362153362</v>
+        <v>0.419551273257561</v>
       </c>
       <c r="H35">
-        <v>0.64695390100721</v>
+        <v>0.620314146396964</v>
       </c>
       <c r="I35">
-        <v>1.44969050608027</v>
+        <v>1.00716913073822</v>
       </c>
       <c r="J35">
-        <v>1.90335043219543</v>
+        <v>1.69625688801694</v>
       </c>
       <c r="K35">
-        <v>7.05289093700113</v>
+        <v>5.97414531729449</v>
       </c>
       <c r="L35">
-        <v>3.23001177435794</v>
+        <v>2.55375865361182</v>
       </c>
       <c r="M35">
-        <v>2.10355178148345</v>
+        <v>1.9249342837492</v>
       </c>
       <c r="N35">
-        <v>2.30907274417022</v>
+        <v>2.44161830713658</v>
       </c>
       <c r="O35">
-        <v>302.374437438253</v>
+        <v>250.085115709754</v>
       </c>
       <c r="P35">
-        <v>41.3709092599202</v>
+        <v>44.3921528241118</v>
       </c>
     </row>
     <row r="36">
@@ -2214,49 +2214,49 @@
         </is>
       </c>
       <c r="B36">
-        <v>1910.98322654044</v>
+        <v>2556.36989788166</v>
       </c>
       <c r="C36">
-        <v>64.05780678127481</v>
+        <v>67.3397912445316</v>
       </c>
       <c r="D36">
-        <v>18.1132211910107</v>
+        <v>22.6421134567218</v>
       </c>
       <c r="E36">
-        <v>57.2640079103326</v>
+        <v>91.1689809903488</v>
       </c>
       <c r="F36">
-        <v>40.4382452830454</v>
+        <v>30.8144542688797</v>
       </c>
       <c r="G36">
-        <v>113.824697655218</v>
+        <v>96.1970697451881</v>
       </c>
       <c r="H36">
-        <v>117.746885345474</v>
+        <v>123.615883411363</v>
       </c>
       <c r="I36">
-        <v>49.1618716008763</v>
+        <v>48.682710999187</v>
       </c>
       <c r="J36">
-        <v>232.312535309779</v>
+        <v>275.467535752717</v>
       </c>
       <c r="K36">
-        <v>193.769702502</v>
+        <v>159.428627040276</v>
       </c>
       <c r="L36">
-        <v>111.177012857852</v>
+        <v>112.303335879875</v>
       </c>
       <c r="M36">
-        <v>231.466978710285</v>
+        <v>257.780608195348</v>
       </c>
       <c r="N36">
-        <v>97.0904896063285</v>
+        <v>88.47822101933301</v>
       </c>
       <c r="O36">
-        <v>4794.09412988476</v>
+        <v>4087.99412236794</v>
       </c>
       <c r="P36">
-        <v>52.7472214783964</v>
+        <v>66.01225008471761</v>
       </c>
     </row>
     <row r="37">
@@ -2266,49 +2266,49 @@
         </is>
       </c>
       <c r="B37">
-        <v>640.228005670884</v>
+        <v>857.173304215656</v>
       </c>
       <c r="C37">
-        <v>23.3584446443436</v>
+        <v>21.864261819586</v>
       </c>
       <c r="D37">
-        <v>12.5641457425433</v>
+        <v>15.6050319428567</v>
       </c>
       <c r="E37">
-        <v>18.5126765056977</v>
+        <v>19.0027572503999</v>
       </c>
       <c r="F37">
-        <v>44.3656884544782</v>
+        <v>46.3688100268896</v>
       </c>
       <c r="G37">
-        <v>8.477329867506009</v>
+        <v>5.00217605919258</v>
       </c>
       <c r="H37">
-        <v>24.8107937146845</v>
+        <v>20.8565218848826</v>
       </c>
       <c r="I37">
-        <v>18.1969818439729</v>
+        <v>12.3023158302319</v>
       </c>
       <c r="J37">
-        <v>36.7011332470826</v>
+        <v>36.4113462311357</v>
       </c>
       <c r="K37">
-        <v>43.1981384023074</v>
+        <v>30.0598045278922</v>
       </c>
       <c r="L37">
-        <v>27.5718015125589</v>
+        <v>28.4562506235384</v>
       </c>
       <c r="M37">
-        <v>29.974160446074</v>
+        <v>32.7571952974448</v>
       </c>
       <c r="N37">
-        <v>17.9524243374332</v>
+        <v>21.0305742201052</v>
       </c>
       <c r="O37">
-        <v>1406.67596430135</v>
+        <v>1203.50311544067</v>
       </c>
       <c r="P37">
-        <v>61.648024394015</v>
+        <v>63.847164493231</v>
       </c>
     </row>
     <row r="38">
@@ -2318,49 +2318,49 @@
         </is>
       </c>
       <c r="B38">
-        <v>582.783797180606</v>
+        <v>772.051898696871</v>
       </c>
       <c r="C38">
-        <v>30.3447069990682</v>
+        <v>29.7895043458816</v>
       </c>
       <c r="D38">
-        <v>14.3914550493542</v>
+        <v>11.2630383736204</v>
       </c>
       <c r="E38">
-        <v>52.4316612234898</v>
+        <v>62.7064910392325</v>
       </c>
       <c r="F38">
-        <v>3.30361880919433</v>
+        <v>1.98122358851233</v>
       </c>
       <c r="G38">
-        <v>8.951903209654461</v>
+        <v>7.95570993301583</v>
       </c>
       <c r="H38">
-        <v>7.16268623565163</v>
+        <v>8.162360276007311</v>
       </c>
       <c r="I38">
-        <v>5.56455550901413</v>
+        <v>6.56855464186928</v>
       </c>
       <c r="J38">
-        <v>34.0467182682238</v>
+        <v>31.695730764417</v>
       </c>
       <c r="K38">
-        <v>20.1389153236241</v>
+        <v>18.8193307196791</v>
       </c>
       <c r="L38">
-        <v>67.59796890645811</v>
+        <v>61.2526012438656</v>
       </c>
       <c r="M38">
-        <v>27.0392077715371</v>
+        <v>25.4785693873662</v>
       </c>
       <c r="N38">
-        <v>28.0887162765522</v>
+        <v>26.0827985009203</v>
       </c>
       <c r="O38">
-        <v>1489.35715794936</v>
+        <v>1308.66394515761</v>
       </c>
       <c r="P38">
-        <v>70.96183901759839</v>
+        <v>69.6609811677781</v>
       </c>
     </row>
     <row r="39">
@@ -2370,49 +2370,49 @@
         </is>
       </c>
       <c r="B39">
-        <v>2118.23576350468</v>
+        <v>3003.59457762485</v>
       </c>
       <c r="C39">
-        <v>135.077353617664</v>
+        <v>112.125730706106</v>
       </c>
       <c r="D39">
-        <v>71.74722775924771</v>
+        <v>69.2922911795751</v>
       </c>
       <c r="E39">
-        <v>85.1303393959777</v>
+        <v>112.328092143654</v>
       </c>
       <c r="F39">
-        <v>28.6570966557027</v>
+        <v>38.6774430463974</v>
       </c>
       <c r="G39">
-        <v>129.702644982354</v>
+        <v>114.109216841931</v>
       </c>
       <c r="H39">
-        <v>51.4165596158853</v>
+        <v>58.8858825349836</v>
       </c>
       <c r="I39">
-        <v>56.9001380586492</v>
+        <v>61.087783878804</v>
       </c>
       <c r="J39">
-        <v>179.013893855958</v>
+        <v>212.384242961497</v>
       </c>
       <c r="K39">
-        <v>145.49620130467</v>
+        <v>116.996053146758</v>
       </c>
       <c r="L39">
-        <v>142.129786134327</v>
+        <v>139.749485813656</v>
       </c>
       <c r="M39">
-        <v>76.2467093973016</v>
+        <v>88.8063106462789</v>
       </c>
       <c r="N39">
-        <v>117.128905088655</v>
+        <v>101.723030432901</v>
       </c>
       <c r="O39">
-        <v>5398.56561127953</v>
+        <v>4491.34313179065</v>
       </c>
       <c r="P39">
-        <v>64.38670808802139</v>
+        <v>78.7200045578399</v>
       </c>
     </row>
     <row r="40">
@@ -2422,49 +2422,49 @@
         </is>
       </c>
       <c r="B40">
-        <v>163.619982726026</v>
+        <v>245.495981027687</v>
       </c>
       <c r="C40">
-        <v>3.51787258794429</v>
+        <v>3.74072210302383</v>
       </c>
       <c r="D40">
-        <v>11.3529089282471</v>
+        <v>10.5561603277532</v>
       </c>
       <c r="E40">
-        <v>2.04011549652263</v>
+        <v>3.77179343860779</v>
       </c>
       <c r="F40">
-        <v>0.627304411616469</v>
+        <v>1.4048433048906</v>
       </c>
       <c r="G40">
-        <v>5.56242449807679</v>
+        <v>3.40657360031914</v>
       </c>
       <c r="H40">
-        <v>9.942437230639699</v>
+        <v>7.0926202283456</v>
       </c>
       <c r="I40">
-        <v>1.51950938471458</v>
+        <v>2.2098457760382</v>
       </c>
       <c r="J40">
-        <v>12.6679622541716</v>
+        <v>12.5130350855538</v>
       </c>
       <c r="K40">
-        <v>10.7690133510061</v>
+        <v>5.95836671678774</v>
       </c>
       <c r="L40">
-        <v>13.1232954689385</v>
+        <v>16.3919512306929</v>
       </c>
       <c r="M40">
-        <v>8.109255210076711</v>
+        <v>9.50870817767016</v>
       </c>
       <c r="N40">
-        <v>30.8424185112813</v>
+        <v>26.364802432494</v>
       </c>
       <c r="O40">
-        <v>466.351676779845</v>
+        <v>391.571075803498</v>
       </c>
       <c r="P40">
-        <v>2.21883344697563</v>
+        <v>2.28694858923544</v>
       </c>
     </row>
     <row r="41">
@@ -2474,49 +2474,49 @@
         </is>
       </c>
       <c r="B41">
-        <v>727.901030371285</v>
+        <v>939.7667967327631</v>
       </c>
       <c r="C41">
-        <v>13.0769915827248</v>
+        <v>17.3313582245488</v>
       </c>
       <c r="D41">
-        <v>112.322484051204</v>
+        <v>116.084142760799</v>
       </c>
       <c r="E41">
-        <v>46.5061299139704</v>
+        <v>53.8586876635712</v>
       </c>
       <c r="F41">
-        <v>3.85921686763177</v>
+        <v>2.93909401135507</v>
       </c>
       <c r="G41">
-        <v>44.8545441941218</v>
+        <v>37.6721481555986</v>
       </c>
       <c r="H41">
-        <v>40.5354434012361</v>
+        <v>35.1088510023125</v>
       </c>
       <c r="I41">
-        <v>13.1413387973547</v>
+        <v>8.42147693928667</v>
       </c>
       <c r="J41">
-        <v>51.7374033231302</v>
+        <v>46.0055991984422</v>
       </c>
       <c r="K41">
-        <v>58.4495965191083</v>
+        <v>48.826649820072</v>
       </c>
       <c r="L41">
-        <v>30.8711541781039</v>
+        <v>27.8634466313022</v>
       </c>
       <c r="M41">
-        <v>37.5438611551915</v>
+        <v>39.4500150948236</v>
       </c>
       <c r="N41">
-        <v>25.0551929876</v>
+        <v>25.2928677875102</v>
       </c>
       <c r="O41">
-        <v>1554.03741955001</v>
+        <v>1364.73013555117</v>
       </c>
       <c r="P41">
-        <v>26.0056046178615</v>
+        <v>22.5207791197253</v>
       </c>
     </row>
     <row r="42">
@@ -2526,49 +2526,49 @@
         </is>
       </c>
       <c r="B42">
-        <v>82.26280954947001</v>
+        <v>141.031621902772</v>
       </c>
       <c r="C42">
-        <v>8.474048617299809</v>
+        <v>9.098506772978711</v>
       </c>
       <c r="D42">
-        <v>2.2129886301285</v>
+        <v>2.17649649712067</v>
       </c>
       <c r="E42">
-        <v>4.69117183239828</v>
+        <v>5.00081893082992</v>
       </c>
       <c r="F42">
-        <v>2.04197102768837</v>
+        <v>1.81926523156168</v>
       </c>
       <c r="G42">
-        <v>1.47532837315416</v>
+        <v>0.900229583978941</v>
       </c>
       <c r="H42">
-        <v>1.44379258558142</v>
+        <v>1.8005237010903</v>
       </c>
       <c r="I42">
-        <v>0.912552039046285</v>
+        <v>1.04567612352603</v>
       </c>
       <c r="J42">
-        <v>4.57681100019763</v>
+        <v>3.81370223720151</v>
       </c>
       <c r="K42">
-        <v>8.12844800533075</v>
+        <v>7.35970381725568</v>
       </c>
       <c r="L42">
-        <v>9.04987678076416</v>
+        <v>7.87673124160456</v>
       </c>
       <c r="M42">
-        <v>3.9211031548985</v>
+        <v>2.86874865354254</v>
       </c>
       <c r="N42">
-        <v>8.10634722117539</v>
+        <v>8.5183710723161</v>
       </c>
       <c r="O42">
-        <v>348.909052346876</v>
+        <v>286.755698356636</v>
       </c>
       <c r="P42">
-        <v>39.7312127146565</v>
+        <v>45.8666032569146</v>
       </c>
     </row>
     <row r="43">
@@ -2578,49 +2578,49 @@
         </is>
       </c>
       <c r="B43">
-        <v>1083.81275148896</v>
+        <v>1377.82733294947</v>
       </c>
       <c r="C43">
-        <v>32.0075195128264</v>
+        <v>41.7336042324832</v>
       </c>
       <c r="D43">
-        <v>62.0803609252899</v>
+        <v>56.2851595667943</v>
       </c>
       <c r="E43">
-        <v>43.3469305302994</v>
+        <v>74.35972086171211</v>
       </c>
       <c r="F43">
-        <v>12.7109147151942</v>
+        <v>10.1266489242354</v>
       </c>
       <c r="G43">
-        <v>29.2004179517161</v>
+        <v>32.9521459871658</v>
       </c>
       <c r="H43">
-        <v>27.1962800994397</v>
+        <v>40.6042069756287</v>
       </c>
       <c r="I43">
-        <v>26.3556389394601</v>
+        <v>22.6509438014535</v>
       </c>
       <c r="J43">
-        <v>55.0247792958626</v>
+        <v>73.9036199070098</v>
       </c>
       <c r="K43">
-        <v>68.83728334272151</v>
+        <v>51.4184251420576</v>
       </c>
       <c r="L43">
-        <v>53.3496409508602</v>
+        <v>57.897152278559</v>
       </c>
       <c r="M43">
-        <v>83.2780249537927</v>
+        <v>92.3323045625196</v>
       </c>
       <c r="N43">
-        <v>89.9326485953742</v>
+        <v>71.11780568039571</v>
       </c>
       <c r="O43">
-        <v>2324.91247108155</v>
+        <v>2005.4179010925</v>
       </c>
       <c r="P43">
-        <v>62.9401662117344</v>
+        <v>46.3729261344152</v>
       </c>
     </row>
     <row r="44">
@@ -2630,49 +2630,49 @@
         </is>
       </c>
       <c r="B44">
-        <v>3391.51584148015</v>
+        <v>4722.79339179212</v>
       </c>
       <c r="C44">
-        <v>178.929955535878</v>
+        <v>162.911617801448</v>
       </c>
       <c r="D44">
-        <v>80.88308063604519</v>
+        <v>79.7387388731936</v>
       </c>
       <c r="E44">
-        <v>79.4757577229108</v>
+        <v>100.293349022177</v>
       </c>
       <c r="F44">
-        <v>252.786976208756</v>
+        <v>210.581819613956</v>
       </c>
       <c r="G44">
-        <v>163.934693093484</v>
+        <v>125.409498367957</v>
       </c>
       <c r="H44">
-        <v>57.1635161458613</v>
+        <v>65.1091948499738</v>
       </c>
       <c r="I44">
-        <v>55.001150129409</v>
+        <v>53.1067267053528</v>
       </c>
       <c r="J44">
-        <v>150.247455030791</v>
+        <v>159.041504096005</v>
       </c>
       <c r="K44">
-        <v>160.634312145015</v>
+        <v>140.093769860706</v>
       </c>
       <c r="L44">
-        <v>267.051659281453</v>
+        <v>255.251090947673</v>
       </c>
       <c r="M44">
-        <v>129.979733275143</v>
+        <v>147.967393277581</v>
       </c>
       <c r="N44">
-        <v>99.9742357358938</v>
+        <v>108.905810674888</v>
       </c>
       <c r="O44">
-        <v>8850.126286410959</v>
+        <v>7630.87843917498</v>
       </c>
       <c r="P44">
-        <v>274.29005815637</v>
+        <v>229.959046382133</v>
       </c>
     </row>
     <row r="45">
@@ -2682,49 +2682,49 @@
         </is>
       </c>
       <c r="B45">
-        <v>324.303438701666</v>
+        <v>434.959883685712</v>
       </c>
       <c r="C45">
-        <v>16.0598156988536</v>
+        <v>18.4048877453908</v>
       </c>
       <c r="D45">
-        <v>6.15302796439068</v>
+        <v>5.0042076163227</v>
       </c>
       <c r="E45">
-        <v>6.95335719300868</v>
+        <v>11.260885352413</v>
       </c>
       <c r="F45">
-        <v>23.904906860991</v>
+        <v>19.1356262684842</v>
       </c>
       <c r="G45">
-        <v>9.29672793733204</v>
+        <v>9.58971188435679</v>
       </c>
       <c r="H45">
-        <v>4.56067426007231</v>
+        <v>4.08063967365446</v>
       </c>
       <c r="I45">
-        <v>6.2313502432156</v>
+        <v>6.2981583611143</v>
       </c>
       <c r="J45">
-        <v>21.8372844468179</v>
+        <v>19.3209694780232</v>
       </c>
       <c r="K45">
-        <v>11.5854958458211</v>
+        <v>13.5272425947446</v>
       </c>
       <c r="L45">
-        <v>23.0055572636123</v>
+        <v>23.8477485432449</v>
       </c>
       <c r="M45">
-        <v>25.9406366689411</v>
+        <v>27.7399605043389</v>
       </c>
       <c r="N45">
-        <v>30.0927764160042</v>
+        <v>26.5581288415731</v>
       </c>
       <c r="O45">
-        <v>962.825877992651</v>
+        <v>852.679782270642</v>
       </c>
       <c r="P45">
-        <v>18.1599211285649</v>
+        <v>18.5076768302115</v>
       </c>
     </row>
     <row r="46">
@@ -2734,49 +2734,49 @@
         </is>
       </c>
       <c r="B46">
-        <v>81.04678755304251</v>
+        <v>114.821989745671</v>
       </c>
       <c r="C46">
-        <v>4.73175767812593</v>
+        <v>4.8488150280236</v>
       </c>
       <c r="D46">
-        <v>2.18543813358117</v>
+        <v>1.75718884655115</v>
       </c>
       <c r="E46">
-        <v>6.20945817415713</v>
+        <v>7.31927273371963</v>
       </c>
       <c r="F46">
-        <v>1.61401948129061</v>
+        <v>0.955492401926225</v>
       </c>
       <c r="G46">
-        <v>1.726426867849</v>
+        <v>1.06220919307587</v>
       </c>
       <c r="H46">
-        <v>2.41229211371157</v>
+        <v>1.2859992032592</v>
       </c>
       <c r="I46">
-        <v>2.66788288716665</v>
+        <v>2.39774473768199</v>
       </c>
       <c r="J46">
-        <v>4.48553725346334</v>
+        <v>5.22780221540604</v>
       </c>
       <c r="K46">
-        <v>5.01584594291695</v>
+        <v>4.28644350213336</v>
       </c>
       <c r="L46">
-        <v>13.7137020489965</v>
+        <v>10.9045066964943</v>
       </c>
       <c r="M46">
-        <v>4.23831101750805</v>
+        <v>4.89678710861229</v>
       </c>
       <c r="N46">
-        <v>8.298980081483281</v>
+        <v>7.07635941425569</v>
       </c>
       <c r="O46">
-        <v>285.0911031188</v>
+        <v>252.789776495531</v>
       </c>
       <c r="P46">
-        <v>8.449171310527429</v>
+        <v>12.2628126013651</v>
       </c>
     </row>
     <row r="47">
@@ -2786,49 +2786,49 @@
         </is>
       </c>
       <c r="B47">
-        <v>1167.38081844342</v>
+        <v>1532.38150772466</v>
       </c>
       <c r="C47">
-        <v>71.1741268950651</v>
+        <v>63.464454047052</v>
       </c>
       <c r="D47">
-        <v>42.7109700747957</v>
+        <v>49.9632781548595</v>
       </c>
       <c r="E47">
-        <v>43.4416589261726</v>
+        <v>67.0104995145181</v>
       </c>
       <c r="F47">
-        <v>10.6854308620966</v>
+        <v>14.2973087951848</v>
       </c>
       <c r="G47">
-        <v>37.5767799601221</v>
+        <v>34.1622729369113</v>
       </c>
       <c r="H47">
-        <v>18.929360103052</v>
+        <v>28.422448318368</v>
       </c>
       <c r="I47">
-        <v>17.335394755409</v>
+        <v>16.3460464268271</v>
       </c>
       <c r="J47">
-        <v>56.7079552231042</v>
+        <v>47.7820485415386</v>
       </c>
       <c r="K47">
-        <v>33.8433577079509</v>
+        <v>40.886781333909</v>
       </c>
       <c r="L47">
-        <v>57.1081230698061</v>
+        <v>53.3156407455881</v>
       </c>
       <c r="M47">
-        <v>76.96561755268149</v>
+        <v>80.8734047474404</v>
       </c>
       <c r="N47">
-        <v>40.0310776239392</v>
+        <v>51.5079642420247</v>
       </c>
       <c r="O47">
-        <v>3228.92731451192</v>
+        <v>2815.61505623256</v>
       </c>
       <c r="P47">
-        <v>40.4515191831308</v>
+        <v>47.1981070369037</v>
       </c>
     </row>
     <row r="48">
@@ -2838,49 +2838,49 @@
         </is>
       </c>
       <c r="B48">
-        <v>984.831727606628</v>
+        <v>1307.21993647225</v>
       </c>
       <c r="C48">
-        <v>18.508694117012</v>
+        <v>26.117790758769</v>
       </c>
       <c r="D48">
-        <v>17.4588245406286</v>
+        <v>12.04665237474</v>
       </c>
       <c r="E48">
-        <v>71.657931593458</v>
+        <v>69.1863163624504</v>
       </c>
       <c r="F48">
-        <v>17.222853274386</v>
+        <v>12.8489034405886</v>
       </c>
       <c r="G48">
-        <v>15.9838033906098</v>
+        <v>18.2471818464743</v>
       </c>
       <c r="H48">
-        <v>7.73257175044885</v>
+        <v>8.30210124161502</v>
       </c>
       <c r="I48">
-        <v>19.6666621236342</v>
+        <v>11.9668864709299</v>
       </c>
       <c r="J48">
-        <v>31.8078225513808</v>
+        <v>34.8025225474609</v>
       </c>
       <c r="K48">
-        <v>26.9407205093592</v>
+        <v>19.9982607228663</v>
       </c>
       <c r="L48">
-        <v>46.7296191311198</v>
+        <v>47.1953848466505</v>
       </c>
       <c r="M48">
-        <v>152.06997470351</v>
+        <v>156.293903551672</v>
       </c>
       <c r="N48">
-        <v>25.9626414830863</v>
+        <v>23.7926111575796</v>
       </c>
       <c r="O48">
-        <v>2614.28066656186</v>
+        <v>2293.99886078354</v>
       </c>
       <c r="P48">
-        <v>99.9452725756852</v>
+        <v>108.848110595914</v>
       </c>
     </row>
     <row r="49">
@@ -2890,49 +2890,49 @@
         </is>
       </c>
       <c r="B49">
-        <v>473.818765534795</v>
+        <v>585.259274081977</v>
       </c>
       <c r="C49">
-        <v>5.33482031868133</v>
+        <v>8.540797477153561</v>
       </c>
       <c r="D49">
-        <v>6.95944318913841</v>
+        <v>5.61192432315581</v>
       </c>
       <c r="E49">
-        <v>14.7772432885319</v>
+        <v>12.7040821977381</v>
       </c>
       <c r="F49">
-        <v>38.8482210031684</v>
+        <v>34.1051447048124</v>
       </c>
       <c r="G49">
-        <v>21.2362661492527</v>
+        <v>16.9463049900563</v>
       </c>
       <c r="H49">
-        <v>3.61867699064871</v>
+        <v>5.49081324206701</v>
       </c>
       <c r="I49">
-        <v>10.6149591384418</v>
+        <v>9.418270365996991</v>
       </c>
       <c r="J49">
-        <v>22.819567512787</v>
+        <v>22.0355957926245</v>
       </c>
       <c r="K49">
-        <v>10.6677399141959</v>
+        <v>9.5803685736361</v>
       </c>
       <c r="L49">
-        <v>3.40640738961334</v>
+        <v>4.79851313386701</v>
       </c>
       <c r="M49">
-        <v>6.47334186830336</v>
+        <v>7.80429339290863</v>
       </c>
       <c r="N49">
-        <v>3.9484916459429</v>
+        <v>4.83987037620063</v>
       </c>
       <c r="O49">
-        <v>713.523969821788</v>
+        <v>606.9964670481839</v>
       </c>
       <c r="P49">
-        <v>7.76518115694295</v>
+        <v>9.67825371795672</v>
       </c>
     </row>
     <row r="50">
@@ -2942,49 +2942,49 @@
         </is>
       </c>
       <c r="B50">
-        <v>684.818091584522</v>
+        <v>1000.74087231162</v>
       </c>
       <c r="C50">
-        <v>83.7709517124174</v>
+        <v>90.0099542326325</v>
       </c>
       <c r="D50">
-        <v>13.2553810434901</v>
+        <v>10.1819293006756</v>
       </c>
       <c r="E50">
-        <v>105.225387088906</v>
+        <v>131.955374860309</v>
       </c>
       <c r="F50">
-        <v>4.118260698562</v>
+        <v>4.40731926194103</v>
       </c>
       <c r="G50">
-        <v>34.8047005260523</v>
+        <v>21.5660267411229</v>
       </c>
       <c r="H50">
-        <v>32.4491628471332</v>
+        <v>37.306516964585</v>
       </c>
       <c r="I50">
-        <v>19.6242607014402</v>
+        <v>21.9151027152787</v>
       </c>
       <c r="J50">
-        <v>102.133443923903</v>
+        <v>114.288247218406</v>
       </c>
       <c r="K50">
-        <v>132.119501474016</v>
+        <v>123.579494068705</v>
       </c>
       <c r="L50">
-        <v>91.2905127057392</v>
+        <v>84.49135429598211</v>
       </c>
       <c r="M50">
-        <v>31.8288296893003</v>
+        <v>48.9618372392033</v>
       </c>
       <c r="N50">
-        <v>79.990945943154</v>
+        <v>69.0166047636764</v>
       </c>
       <c r="O50">
-        <v>2299.28478083488</v>
+        <v>1895.54143665812</v>
       </c>
       <c r="P50">
-        <v>76.19823984181321</v>
+        <v>136.949326086744</v>
       </c>
     </row>
     <row r="51">
@@ -2994,49 +2994,49 @@
         </is>
       </c>
       <c r="B51">
-        <v>74.309083787323</v>
+        <v>102.010940715634</v>
       </c>
       <c r="C51">
-        <v>1.86300896810883</v>
+        <v>1.48641324042074</v>
       </c>
       <c r="D51">
-        <v>0.480412045546993</v>
+        <v>0.549827253239673</v>
       </c>
       <c r="E51">
-        <v>1.4108946854963</v>
+        <v>1.82116021100414</v>
       </c>
       <c r="F51">
-        <v>25.7389979173671</v>
+        <v>24.2460878527584</v>
       </c>
       <c r="G51">
-        <v>0.931173027094758</v>
+        <v>2.27249589696597</v>
       </c>
       <c r="H51">
-        <v>0.274192543882136</v>
+        <v>0.320203584553521</v>
       </c>
       <c r="I51">
-        <v>1.0058321348926</v>
+        <v>0.814772441165003</v>
       </c>
       <c r="J51">
-        <v>1.82819604556888</v>
+        <v>1.78620790578585</v>
       </c>
       <c r="K51">
-        <v>1.35974792324982</v>
+        <v>0.996666601637859</v>
       </c>
       <c r="L51">
-        <v>0.721499549588404</v>
+        <v>0.501491320782666</v>
       </c>
       <c r="M51">
-        <v>0.614580297854044</v>
+        <v>0.940712656253801</v>
       </c>
       <c r="N51">
-        <v>1.34954456344495</v>
+        <v>1.6372004598346</v>
       </c>
       <c r="O51">
-        <v>217.478081108056</v>
+        <v>192.083819725898</v>
       </c>
       <c r="P51">
-        <v>16.7689905871227</v>
+        <v>14.6648526698888</v>
       </c>
     </row>
     <row r="52">

</xml_diff>

<commit_message>
diag zero value correction cps
</commit_message>
<xml_diff>
--- a/1-Data-Codes/2-Final_Data/L_1999.xlsx
+++ b/1-Data-Codes/2-Final_Data/L_1999.xlsx
@@ -446,49 +446,49 @@
         </is>
       </c>
       <c r="B2">
-        <v>1169.80662325887</v>
+        <v>1169.80658334613</v>
       </c>
       <c r="C2">
-        <v>40.3885188932118</v>
+        <v>40.3885177371109</v>
       </c>
       <c r="D2">
-        <v>92.07100750786771</v>
+        <v>92.07100683174269</v>
       </c>
       <c r="E2">
-        <v>68.49600481491829</v>
+        <v>68.4961355440167</v>
       </c>
       <c r="F2">
-        <v>15.8527736626304</v>
+        <v>15.8527735903268</v>
       </c>
       <c r="G2">
-        <v>22.1616101595343</v>
+        <v>22.1616100282479</v>
       </c>
       <c r="H2">
-        <v>24.7955694748319</v>
+        <v>24.7956361518259</v>
       </c>
       <c r="I2">
-        <v>14.5473839856517</v>
+        <v>14.5473837908715</v>
       </c>
       <c r="J2">
-        <v>73.79667632284961</v>
+        <v>73.7966911823771</v>
       </c>
       <c r="K2">
-        <v>25.5405741857225</v>
+        <v>25.5405741319049</v>
       </c>
       <c r="L2">
-        <v>37.187294585555</v>
+        <v>37.187497507836</v>
       </c>
       <c r="M2">
-        <v>38.8907652269414</v>
+        <v>38.8907647569356</v>
       </c>
       <c r="N2">
-        <v>30.9597871246405</v>
+        <v>30.9597868075987</v>
       </c>
       <c r="O2">
-        <v>1445.40134261463</v>
+        <v>1445.40119399736</v>
       </c>
       <c r="P2">
-        <v>50.7103474436891</v>
+        <v>50.7103446417472</v>
       </c>
     </row>
     <row r="3">
@@ -498,49 +498,49 @@
         </is>
       </c>
       <c r="B3">
-        <v>124.356542777432</v>
+        <v>124.357550472118</v>
       </c>
       <c r="C3">
-        <v>5.84361325084831</v>
+        <v>5.84370033476064</v>
       </c>
       <c r="D3">
-        <v>0.532778615332813</v>
+        <v>0.532784308889151</v>
       </c>
       <c r="E3">
-        <v>1.67723919848077</v>
+        <v>1.67726037209228</v>
       </c>
       <c r="F3">
-        <v>9.651803808627349</v>
+        <v>9.65195306873</v>
       </c>
       <c r="G3">
-        <v>0.496406046965805</v>
+        <v>0.49641180029835</v>
       </c>
       <c r="H3">
-        <v>0.185386558819401</v>
+        <v>0.182884941233513</v>
       </c>
       <c r="I3">
-        <v>0.185512128061022</v>
+        <v>0.185514054694753</v>
       </c>
       <c r="J3">
-        <v>0.541351773273659</v>
+        <v>0.541151839499823</v>
       </c>
       <c r="K3">
-        <v>0.401563425613806</v>
+        <v>0.4015671202925</v>
       </c>
       <c r="L3">
-        <v>0.32683074279789</v>
+        <v>0.326647535925599</v>
       </c>
       <c r="M3">
-        <v>1.12981794609696</v>
+        <v>1.12982931393969</v>
       </c>
       <c r="N3">
-        <v>0.732003263256041</v>
+        <v>0.731585279185888</v>
       </c>
       <c r="O3">
-        <v>249.321559707904</v>
+        <v>249.322956221572</v>
       </c>
       <c r="P3">
-        <v>10.7076008331701</v>
+        <v>10.7077622567879</v>
       </c>
     </row>
     <row r="4">
@@ -550,49 +550,49 @@
         </is>
       </c>
       <c r="B4">
-        <v>1270.67108467159</v>
+        <v>1270.67089668933</v>
       </c>
       <c r="C4">
-        <v>15.1623803792313</v>
+        <v>15.1623739767493</v>
       </c>
       <c r="D4">
-        <v>11.989135427276</v>
+        <v>11.9891329728222</v>
       </c>
       <c r="E4">
-        <v>17.3646601594878</v>
+        <v>17.3651171933868</v>
       </c>
       <c r="F4">
-        <v>20.7557037485372</v>
+        <v>20.7556994966667</v>
       </c>
       <c r="G4">
-        <v>13.9531453821672</v>
+        <v>13.9531447490499</v>
       </c>
       <c r="H4">
-        <v>8.18802786203536</v>
+        <v>8.18838299524197</v>
       </c>
       <c r="I4">
-        <v>6.96783600063118</v>
+        <v>6.96783528534483</v>
       </c>
       <c r="J4">
-        <v>26.028666516929</v>
+        <v>26.028780260979</v>
       </c>
       <c r="K4">
-        <v>9.267967282567041</v>
+        <v>9.26796696256198</v>
       </c>
       <c r="L4">
-        <v>92.70368251624571</v>
+        <v>92.7044380303486</v>
       </c>
       <c r="M4">
-        <v>56.8223507638853</v>
+        <v>56.822348883009</v>
       </c>
       <c r="N4">
-        <v>21.9870426240282</v>
+        <v>21.9870184580025</v>
       </c>
       <c r="O4">
-        <v>1930.94336823436</v>
+        <v>1930.94275110412</v>
       </c>
       <c r="P4">
-        <v>36.1800154365612</v>
+        <v>36.1800011856351</v>
       </c>
     </row>
     <row r="5">
@@ -602,49 +602,49 @@
         </is>
       </c>
       <c r="B5">
-        <v>687.250183822308</v>
+        <v>687.25015946441</v>
       </c>
       <c r="C5">
-        <v>59.1193931481618</v>
+        <v>59.1193920169989</v>
       </c>
       <c r="D5">
-        <v>14.9047762775098</v>
+        <v>14.904776222328</v>
       </c>
       <c r="E5">
-        <v>45.0638232850824</v>
+        <v>45.0638230118399</v>
       </c>
       <c r="F5">
-        <v>4.51217888027607</v>
+        <v>4.51217689412204</v>
       </c>
       <c r="G5">
-        <v>14.7894579942568</v>
+        <v>14.7894579246355</v>
       </c>
       <c r="H5">
-        <v>15.5915817889997</v>
+        <v>15.591629581667</v>
       </c>
       <c r="I5">
-        <v>7.49840241540469</v>
+        <v>7.49840238964256</v>
       </c>
       <c r="J5">
-        <v>39.1073451160403</v>
+        <v>39.1073759720611</v>
       </c>
       <c r="K5">
-        <v>26.1747653365326</v>
+        <v>26.1747652953947</v>
       </c>
       <c r="L5">
-        <v>23.354973572804</v>
+        <v>23.3549962188541</v>
       </c>
       <c r="M5">
-        <v>20.5526038927974</v>
+        <v>20.552603737132</v>
       </c>
       <c r="N5">
-        <v>19.1841569925131</v>
+        <v>19.1841566450878</v>
       </c>
       <c r="O5">
-        <v>827.823423057903</v>
+        <v>827.823373580546</v>
       </c>
       <c r="P5">
-        <v>64.5721197648826</v>
+        <v>64.5721176168867</v>
       </c>
     </row>
     <row r="6">
@@ -654,49 +654,49 @@
         </is>
       </c>
       <c r="B6">
-        <v>8232.893646179609</v>
+        <v>8232.892281271241</v>
       </c>
       <c r="C6">
-        <v>214.493971836629</v>
+        <v>214.493928974541</v>
       </c>
       <c r="D6">
-        <v>246.958047741748</v>
+        <v>246.958026561414</v>
       </c>
       <c r="E6">
-        <v>145.280928951152</v>
+        <v>145.285030028191</v>
       </c>
       <c r="F6">
-        <v>49.6138360696182</v>
+        <v>49.6138233646019</v>
       </c>
       <c r="G6">
-        <v>108.258902536894</v>
+        <v>108.258897788129</v>
       </c>
       <c r="H6">
-        <v>69.1830961582674</v>
+        <v>69.1853109948791</v>
       </c>
       <c r="I6">
-        <v>55.0399989814105</v>
+        <v>55.0399928723042</v>
       </c>
       <c r="J6">
-        <v>195.64598911656</v>
+        <v>195.646619743145</v>
       </c>
       <c r="K6">
-        <v>138.445616452083</v>
+        <v>138.445614457053</v>
       </c>
       <c r="L6">
-        <v>583.238311005987</v>
+        <v>583.244798520158</v>
       </c>
       <c r="M6">
-        <v>321.024784025261</v>
+        <v>321.024768538684</v>
       </c>
       <c r="N6">
-        <v>303.848233616888</v>
+        <v>303.848098744927</v>
       </c>
       <c r="O6">
-        <v>12463.5662511451</v>
+        <v>12463.5613454583</v>
       </c>
       <c r="P6">
-        <v>323.342677958546</v>
+        <v>323.342578320321</v>
       </c>
     </row>
     <row r="7">
@@ -706,49 +706,49 @@
         </is>
       </c>
       <c r="B7">
-        <v>825.788159088176</v>
+        <v>825.7879441115369</v>
       </c>
       <c r="C7">
-        <v>33.9039909785586</v>
+        <v>33.9039818193791</v>
       </c>
       <c r="D7">
-        <v>5.87593527686245</v>
+        <v>5.87593414137867</v>
       </c>
       <c r="E7">
-        <v>19.771828774842</v>
+        <v>19.7719575551981</v>
       </c>
       <c r="F7">
-        <v>18.6855331421006</v>
+        <v>18.6855187512718</v>
       </c>
       <c r="G7">
-        <v>10.149117160222</v>
+        <v>10.1491164618991</v>
       </c>
       <c r="H7">
-        <v>9.441492763744741</v>
+        <v>9.442473396592479</v>
       </c>
       <c r="I7">
-        <v>11.5870576714173</v>
+        <v>11.5870572800848</v>
       </c>
       <c r="J7">
-        <v>18.0237835886683</v>
+        <v>18.0240144703635</v>
       </c>
       <c r="K7">
-        <v>17.2674850316021</v>
+        <v>17.2674845978249</v>
       </c>
       <c r="L7">
-        <v>68.2724845758132</v>
+        <v>68.27284611371731</v>
       </c>
       <c r="M7">
-        <v>20.8757045276163</v>
+        <v>20.8757030116514</v>
       </c>
       <c r="N7">
-        <v>28.1446336103064</v>
+        <v>28.1445470951437</v>
       </c>
       <c r="O7">
-        <v>1895.02697820488</v>
+        <v>1895.02647963785</v>
       </c>
       <c r="P7">
-        <v>39.8181561527282</v>
+        <v>39.8181376986202</v>
       </c>
     </row>
     <row r="8">
@@ -758,49 +758,49 @@
         </is>
       </c>
       <c r="B8">
-        <v>728.975487337692</v>
+        <v>728.975428976144</v>
       </c>
       <c r="C8">
-        <v>16.5858908063122</v>
+        <v>16.5858890469144</v>
       </c>
       <c r="D8">
-        <v>9.31431656426737</v>
+        <v>9.3143155642025</v>
       </c>
       <c r="E8">
-        <v>23.5985356398191</v>
+        <v>23.5987317308589</v>
       </c>
       <c r="F8">
-        <v>0.944301494087143</v>
+        <v>0.944301387837727</v>
       </c>
       <c r="G8">
-        <v>29.7623832409898</v>
+        <v>29.7623830229073</v>
       </c>
       <c r="H8">
-        <v>12.2100401574013</v>
+        <v>12.2101443260948</v>
       </c>
       <c r="I8">
-        <v>2.92599351877837</v>
+        <v>2.92599322503371</v>
       </c>
       <c r="J8">
-        <v>52.403815056161</v>
+        <v>52.4038373563136</v>
       </c>
       <c r="K8">
-        <v>36.6602005924526</v>
+        <v>36.6602005077404</v>
       </c>
       <c r="L8">
-        <v>41.6285519149974</v>
+        <v>41.6288562191887</v>
       </c>
       <c r="M8">
-        <v>66.0074481011247</v>
+        <v>66.0074474003907</v>
       </c>
       <c r="N8">
-        <v>30.5108465253586</v>
+        <v>30.5108293012019</v>
       </c>
       <c r="O8">
-        <v>1351.84285902865</v>
+        <v>1351.8426376654</v>
       </c>
       <c r="P8">
-        <v>7.46673951804276</v>
+        <v>7.46673525326738</v>
       </c>
     </row>
     <row r="9">
@@ -810,49 +810,49 @@
         </is>
       </c>
       <c r="B9">
-        <v>170.215475037224</v>
+        <v>170.215458422665</v>
       </c>
       <c r="C9">
-        <v>10.0468659969272</v>
+        <v>10.0468652364138</v>
       </c>
       <c r="D9">
-        <v>2.02897381867205</v>
+        <v>2.02897377985051</v>
       </c>
       <c r="E9">
-        <v>5.28643778822353</v>
+        <v>5.28643761112095</v>
       </c>
       <c r="F9">
-        <v>2.37088365795269</v>
+        <v>2.37088233168719</v>
       </c>
       <c r="G9">
-        <v>22.8367023545677</v>
+        <v>22.8367023051447</v>
       </c>
       <c r="H9">
-        <v>4.2627974923656</v>
+        <v>4.26282014598123</v>
       </c>
       <c r="I9">
-        <v>0.281512285665513</v>
+        <v>0.281512270681961</v>
       </c>
       <c r="J9">
-        <v>3.08256530770771</v>
+        <v>3.08258588222266</v>
       </c>
       <c r="K9">
-        <v>3.66884025228682</v>
+        <v>3.66884021751272</v>
       </c>
       <c r="L9">
-        <v>2.00101870521672</v>
+        <v>2.001033817619</v>
       </c>
       <c r="M9">
-        <v>7.97241323003273</v>
+        <v>7.97241312033409</v>
       </c>
       <c r="N9">
-        <v>4.53573255879267</v>
+        <v>4.53573231878199</v>
       </c>
       <c r="O9">
-        <v>307.183411505851</v>
+        <v>307.183378108415</v>
       </c>
       <c r="P9">
-        <v>4.97966487149367</v>
+        <v>4.97966343686703</v>
       </c>
     </row>
     <row r="10">
@@ -862,49 +862,49 @@
         </is>
       </c>
       <c r="B10">
-        <v>4261.93824010483</v>
+        <v>4261.93801809132</v>
       </c>
       <c r="C10">
-        <v>54.3653554772369</v>
+        <v>54.3653476820336</v>
       </c>
       <c r="D10">
-        <v>44.2096746481746</v>
+        <v>44.2096717488047</v>
       </c>
       <c r="E10">
-        <v>66.28995457891909</v>
+        <v>66.290476818692</v>
       </c>
       <c r="F10">
-        <v>11.9688277586096</v>
+        <v>11.9688221140249</v>
       </c>
       <c r="G10">
-        <v>47.2010752234275</v>
+        <v>47.2010744156521</v>
       </c>
       <c r="H10">
-        <v>21.2743674597964</v>
+        <v>21.2747578751097</v>
       </c>
       <c r="I10">
-        <v>29.1826005058623</v>
+        <v>29.1825996772191</v>
       </c>
       <c r="J10">
-        <v>47.9640092637999</v>
+        <v>47.9641509293239</v>
       </c>
       <c r="K10">
-        <v>48.0134885652165</v>
+        <v>48.0134881982321</v>
       </c>
       <c r="L10">
-        <v>117.008168082801</v>
+        <v>117.009040075187</v>
       </c>
       <c r="M10">
-        <v>90.7591761545398</v>
+        <v>90.75917372655751</v>
       </c>
       <c r="N10">
-        <v>107.00386778567</v>
+        <v>107.003843243042</v>
       </c>
       <c r="O10">
-        <v>6466.94096422243</v>
+        <v>6466.94024178293</v>
       </c>
       <c r="P10">
-        <v>102.010482868437</v>
+        <v>102.010465756654</v>
       </c>
     </row>
     <row r="11">
@@ -914,49 +914,49 @@
         </is>
       </c>
       <c r="B11">
-        <v>1786.44400435144</v>
+        <v>1786.44386673282</v>
       </c>
       <c r="C11">
-        <v>75.1973502665811</v>
+        <v>75.19734747968521</v>
       </c>
       <c r="D11">
-        <v>164.983048661863</v>
+        <v>164.98304509186</v>
       </c>
       <c r="E11">
-        <v>110.445397485562</v>
+        <v>110.445592208079</v>
       </c>
       <c r="F11">
-        <v>13.3020658495239</v>
+        <v>13.3020597424875</v>
       </c>
       <c r="G11">
-        <v>47.7107919203053</v>
+        <v>47.7107908711939</v>
       </c>
       <c r="H11">
-        <v>26.4190749999304</v>
+        <v>26.4193049630904</v>
       </c>
       <c r="I11">
-        <v>24.9867902087537</v>
+        <v>24.9867898050001</v>
       </c>
       <c r="J11">
-        <v>50.2675061415569</v>
+        <v>50.2676238852541</v>
       </c>
       <c r="K11">
-        <v>53.4375056168645</v>
+        <v>53.4375009592185</v>
       </c>
       <c r="L11">
-        <v>67.67465031232329</v>
+        <v>67.67502020982781</v>
       </c>
       <c r="M11">
-        <v>70.5773106400581</v>
+        <v>70.5773098622238</v>
       </c>
       <c r="N11">
-        <v>59.4670079175509</v>
+        <v>59.4669945000274</v>
       </c>
       <c r="O11">
-        <v>3066.06255582342</v>
+        <v>3066.06232890034</v>
       </c>
       <c r="P11">
-        <v>58.3857026185594</v>
+        <v>58.3856895226025</v>
       </c>
     </row>
     <row r="12">
@@ -966,49 +966,49 @@
         </is>
       </c>
       <c r="B12">
-        <v>293.894801548589</v>
+        <v>293.898518031205</v>
       </c>
       <c r="C12">
-        <v>8.24366152523246</v>
+        <v>8.243548149700841</v>
       </c>
       <c r="D12">
-        <v>4.95104782331318</v>
+        <v>4.9511105629907</v>
       </c>
       <c r="E12">
-        <v>1.03352752802699</v>
+        <v>1.35025506932098</v>
       </c>
       <c r="F12">
-        <v>0.720301243024804</v>
+        <v>0.7203029963900101</v>
       </c>
       <c r="G12">
-        <v>1.16755512601945</v>
+        <v>1.16756830833161</v>
       </c>
       <c r="H12">
-        <v>0.93490403284755</v>
+        <v>0.9298496055566951</v>
       </c>
       <c r="I12">
-        <v>1.45200553295133</v>
+        <v>1.45202371101633</v>
       </c>
       <c r="J12">
-        <v>0.82240239156423</v>
+        <v>0.822372464066726</v>
       </c>
       <c r="K12">
-        <v>0.635667646294615</v>
+        <v>0.635673116210003</v>
       </c>
       <c r="L12">
-        <v>1.98686900115808</v>
+        <v>1.96716634747312</v>
       </c>
       <c r="M12">
-        <v>3.7068392636537</v>
+        <v>3.70688386938709</v>
       </c>
       <c r="N12">
-        <v>2.77269146731101</v>
+        <v>2.77272261386823</v>
       </c>
       <c r="O12">
-        <v>510.904485786853</v>
+        <v>510.58830439622</v>
       </c>
       <c r="P12">
-        <v>20.3996871667631</v>
+        <v>20.399954668965</v>
       </c>
     </row>
     <row r="13">
@@ -1018,49 +1018,49 @@
         </is>
       </c>
       <c r="B13">
-        <v>280.199002432048</v>
+        <v>280.19895813844</v>
       </c>
       <c r="C13">
-        <v>26.6074225667637</v>
+        <v>26.6074252997116</v>
       </c>
       <c r="D13">
-        <v>2.47475266473497</v>
+        <v>2.47475253553602</v>
       </c>
       <c r="E13">
-        <v>20.4860833026574</v>
+        <v>20.4860825714956</v>
       </c>
       <c r="F13">
-        <v>6.53959069250594</v>
+        <v>6.53958762401606</v>
       </c>
       <c r="G13">
-        <v>5.32272345432399</v>
+        <v>5.32272344029195</v>
       </c>
       <c r="H13">
-        <v>2.27719514841413</v>
+        <v>2.27741464948492</v>
       </c>
       <c r="I13">
-        <v>1.8690311277285</v>
+        <v>1.86903099020986</v>
       </c>
       <c r="J13">
-        <v>4.97443516863315</v>
+        <v>4.97448619541873</v>
       </c>
       <c r="K13">
-        <v>2.9535304096612</v>
+        <v>2.95353009081102</v>
       </c>
       <c r="L13">
-        <v>21.1828602352311</v>
+        <v>21.1829026760906</v>
       </c>
       <c r="M13">
-        <v>4.88119723057878</v>
+        <v>4.88119655566553</v>
       </c>
       <c r="N13">
-        <v>7.27133118218478</v>
+        <v>7.27128597698296</v>
       </c>
       <c r="O13">
-        <v>462.372807287483</v>
+        <v>462.372722075598</v>
       </c>
       <c r="P13">
-        <v>42.3427999496964</v>
+        <v>42.3427940116002</v>
       </c>
     </row>
     <row r="14">
@@ -1070,49 +1070,49 @@
         </is>
       </c>
       <c r="B14">
-        <v>2685.94779577808</v>
+        <v>2685.94820263025</v>
       </c>
       <c r="C14">
-        <v>114.826254044976</v>
+        <v>114.826256380769</v>
       </c>
       <c r="D14">
-        <v>20.5048266270638</v>
+        <v>20.5048258399779</v>
       </c>
       <c r="E14">
-        <v>97.45622549265261</v>
+        <v>97.4564215711507</v>
       </c>
       <c r="F14">
-        <v>25.3537312202551</v>
+        <v>25.3537323210084</v>
       </c>
       <c r="G14">
-        <v>99.69155326737869</v>
+        <v>99.6915524478008</v>
       </c>
       <c r="H14">
-        <v>64.84960826139761</v>
+        <v>64.8498081155292</v>
       </c>
       <c r="I14">
-        <v>32.0190517410773</v>
+        <v>32.0190545531076</v>
       </c>
       <c r="J14">
-        <v>186.565006944813</v>
+        <v>186.56507540075</v>
       </c>
       <c r="K14">
-        <v>181.383615494039</v>
+        <v>181.383652675082</v>
       </c>
       <c r="L14">
-        <v>172.392244472769</v>
+        <v>172.392554929164</v>
       </c>
       <c r="M14">
-        <v>100.50082668854</v>
+        <v>100.500818683141</v>
       </c>
       <c r="N14">
-        <v>103.009342009149</v>
+        <v>103.009334712207</v>
       </c>
       <c r="O14">
-        <v>4791.53816655745</v>
+        <v>4791.53838045126</v>
       </c>
       <c r="P14">
-        <v>84.4777120232045</v>
+        <v>84.47770459145011</v>
       </c>
     </row>
     <row r="15">
@@ -1122,49 +1122,49 @@
         </is>
       </c>
       <c r="B15">
-        <v>1298.89704470066</v>
+        <v>1298.89712551691</v>
       </c>
       <c r="C15">
-        <v>42.6477855809541</v>
+        <v>42.6477853907428</v>
       </c>
       <c r="D15">
-        <v>15.2714157564213</v>
+        <v>15.2714163434774</v>
       </c>
       <c r="E15">
-        <v>67.759472475587</v>
+        <v>67.75959999207539</v>
       </c>
       <c r="F15">
-        <v>13.3585069822928</v>
+        <v>13.3585056344745</v>
       </c>
       <c r="G15">
-        <v>47.3609754202629</v>
+        <v>47.3609768903868</v>
       </c>
       <c r="H15">
-        <v>52.3487487127116</v>
+        <v>52.3488624316659</v>
       </c>
       <c r="I15">
-        <v>33.0650875775596</v>
+        <v>33.0650861540076</v>
       </c>
       <c r="J15">
-        <v>177.830554140287</v>
+        <v>177.830627087415</v>
       </c>
       <c r="K15">
-        <v>89.6863503282009</v>
+        <v>89.68634772104031</v>
       </c>
       <c r="L15">
-        <v>83.8648197116266</v>
+        <v>83.86504250720751</v>
       </c>
       <c r="M15">
-        <v>187.319596955542</v>
+        <v>187.31955532459</v>
       </c>
       <c r="N15">
-        <v>70.9075472774195</v>
+        <v>70.9075376341622</v>
       </c>
       <c r="O15">
-        <v>2076.37071068164</v>
+        <v>2076.37048450973</v>
       </c>
       <c r="P15">
-        <v>38.5766160613724</v>
+        <v>38.5766102652578</v>
       </c>
     </row>
     <row r="16">
@@ -1174,49 +1174,49 @@
         </is>
       </c>
       <c r="B16">
-        <v>534.497205250248</v>
+        <v>534.497201078873</v>
       </c>
       <c r="C16">
-        <v>60.6773462589503</v>
+        <v>60.6773452999063</v>
       </c>
       <c r="D16">
-        <v>10.9382316983721</v>
+        <v>10.9382309349508</v>
       </c>
       <c r="E16">
-        <v>25.8928923153384</v>
+        <v>25.8928939480104</v>
       </c>
       <c r="F16">
-        <v>4.00502068017659</v>
+        <v>4.00502017666425</v>
       </c>
       <c r="G16">
-        <v>13.8419381235624</v>
+        <v>13.841937975177</v>
       </c>
       <c r="H16">
-        <v>14.9254099771511</v>
+        <v>14.9254448806247</v>
       </c>
       <c r="I16">
-        <v>14.8260033783125</v>
+        <v>14.8260023763905</v>
       </c>
       <c r="J16">
-        <v>48.111837122349</v>
+        <v>48.1118499969667</v>
       </c>
       <c r="K16">
-        <v>49.6377641966877</v>
+        <v>49.6377603292954</v>
       </c>
       <c r="L16">
-        <v>38.5470704649172</v>
+        <v>38.5470764804919</v>
       </c>
       <c r="M16">
-        <v>23.5437063863778</v>
+        <v>23.5437084187309</v>
       </c>
       <c r="N16">
-        <v>23.3705302444889</v>
+        <v>23.3705194515426</v>
       </c>
       <c r="O16">
-        <v>1116.19289059643</v>
+        <v>1116.19282014054</v>
       </c>
       <c r="P16">
-        <v>84.27738009737411</v>
+        <v>84.27738126017771</v>
       </c>
     </row>
     <row r="17">
@@ -1226,49 +1226,49 @@
         </is>
       </c>
       <c r="B17">
-        <v>523.967681230208</v>
+        <v>523.9677234865291</v>
       </c>
       <c r="C17">
-        <v>31.607815069463</v>
+        <v>31.6078104836265</v>
       </c>
       <c r="D17">
-        <v>6.44760992918903</v>
+        <v>6.44760958203473</v>
       </c>
       <c r="E17">
-        <v>15.2421749228039</v>
+        <v>15.2421712026926</v>
       </c>
       <c r="F17">
-        <v>15.0705887854177</v>
+        <v>15.070586464942</v>
       </c>
       <c r="G17">
-        <v>11.9034612897312</v>
+        <v>11.9034617764983</v>
       </c>
       <c r="H17">
-        <v>15.2932048022965</v>
+        <v>15.2933140829635</v>
       </c>
       <c r="I17">
-        <v>8.09642526085373</v>
+        <v>8.09642484671244</v>
       </c>
       <c r="J17">
-        <v>21.3341256343883</v>
+        <v>21.3341280234123</v>
       </c>
       <c r="K17">
-        <v>27.3375617235326</v>
+        <v>27.3375583110808</v>
       </c>
       <c r="L17">
-        <v>16.5827482800561</v>
+        <v>16.5827479895797</v>
       </c>
       <c r="M17">
-        <v>74.9675946840127</v>
+        <v>74.96759397989371</v>
       </c>
       <c r="N17">
-        <v>17.1003783471084</v>
+        <v>17.1003450757004</v>
       </c>
       <c r="O17">
-        <v>1023.69025904723</v>
+        <v>1023.69026784869</v>
       </c>
       <c r="P17">
-        <v>73.4478891102937</v>
+        <v>73.447884377626</v>
       </c>
     </row>
     <row r="18">
@@ -1278,49 +1278,49 @@
         </is>
       </c>
       <c r="B18">
-        <v>1046.90990988774</v>
+        <v>1046.90985586985</v>
       </c>
       <c r="C18">
-        <v>34.9148624220921</v>
+        <v>34.9148626931801</v>
       </c>
       <c r="D18">
-        <v>30.8559832949836</v>
+        <v>30.8559831873363</v>
       </c>
       <c r="E18">
-        <v>42.2595389541995</v>
+        <v>42.2597339784343</v>
       </c>
       <c r="F18">
-        <v>35.5687823641702</v>
+        <v>35.5687835241003</v>
       </c>
       <c r="G18">
-        <v>29.0926827426063</v>
+        <v>29.0926859055207</v>
       </c>
       <c r="H18">
-        <v>24.6239537731645</v>
+        <v>24.6241004614492</v>
       </c>
       <c r="I18">
-        <v>8.997022308455311</v>
+        <v>8.99702151646361</v>
       </c>
       <c r="J18">
-        <v>45.5368344809074</v>
+        <v>45.5368778916199</v>
       </c>
       <c r="K18">
-        <v>39.957087574057</v>
+        <v>39.9570910203189</v>
       </c>
       <c r="L18">
-        <v>48.7855416936223</v>
+        <v>48.7858612671896</v>
       </c>
       <c r="M18">
-        <v>65.5967754006965</v>
+        <v>65.5967742773497</v>
       </c>
       <c r="N18">
-        <v>29.152925071816</v>
+        <v>29.1529256621694</v>
       </c>
       <c r="O18">
-        <v>1369.58839121828</v>
+        <v>1369.58836746886</v>
       </c>
       <c r="P18">
-        <v>43.2015466589629</v>
+        <v>43.2015391353503</v>
       </c>
     </row>
     <row r="19">
@@ -1330,49 +1330,49 @@
         </is>
       </c>
       <c r="B19">
-        <v>1169.84266274599</v>
+        <v>1169.84263248826</v>
       </c>
       <c r="C19">
-        <v>24.9744061602189</v>
+        <v>24.9744077020973</v>
       </c>
       <c r="D19">
-        <v>18.1765026575804</v>
+        <v>18.1765021441543</v>
       </c>
       <c r="E19">
-        <v>39.9590721268225</v>
+        <v>39.9592053458883</v>
       </c>
       <c r="F19">
-        <v>71.5988260307292</v>
+        <v>71.5988245375582</v>
       </c>
       <c r="G19">
-        <v>43.7801760216017</v>
+        <v>43.7801778395548</v>
       </c>
       <c r="H19">
-        <v>6.01933105047655</v>
+        <v>6.01946960267989</v>
       </c>
       <c r="I19">
-        <v>7.62535125961992</v>
+        <v>7.62535084935924</v>
       </c>
       <c r="J19">
-        <v>20.0429182978859</v>
+        <v>20.0429550791438</v>
       </c>
       <c r="K19">
-        <v>12.7177983016376</v>
+        <v>12.7177976615325</v>
       </c>
       <c r="L19">
-        <v>12.3117606581055</v>
+        <v>12.3119784690176</v>
       </c>
       <c r="M19">
-        <v>27.5400099857348</v>
+        <v>27.5400091411257</v>
       </c>
       <c r="N19">
-        <v>13.0955648263722</v>
+        <v>13.0955583296096</v>
       </c>
       <c r="O19">
-        <v>1571.13502608026</v>
+        <v>1571.13499494794</v>
       </c>
       <c r="P19">
-        <v>40.5124771485005</v>
+        <v>40.5124765910107</v>
       </c>
     </row>
     <row r="20">
@@ -1382,49 +1382,49 @@
         </is>
       </c>
       <c r="B20">
-        <v>293.462197631221</v>
+        <v>293.462226718812</v>
       </c>
       <c r="C20">
-        <v>8.136679711711221</v>
+        <v>8.136679022963319</v>
       </c>
       <c r="D20">
-        <v>16.9008236423214</v>
+        <v>16.900823338119</v>
       </c>
       <c r="E20">
-        <v>34.1762785272218</v>
+        <v>34.1762832231737</v>
       </c>
       <c r="F20">
-        <v>0.26273761668546</v>
+        <v>0.262736919583967</v>
       </c>
       <c r="G20">
-        <v>1.86580325640495</v>
+        <v>1.86580323374386</v>
       </c>
       <c r="H20">
-        <v>3.26319755949231</v>
+        <v>3.26320887260769</v>
       </c>
       <c r="I20">
-        <v>1.16652060187282</v>
+        <v>1.16652059529631</v>
       </c>
       <c r="J20">
-        <v>6.76898733938144</v>
+        <v>6.76899755831113</v>
       </c>
       <c r="K20">
-        <v>5.43412651206477</v>
+        <v>5.43412612273316</v>
       </c>
       <c r="L20">
-        <v>10.5816510901135</v>
+        <v>10.5816586169763</v>
       </c>
       <c r="M20">
-        <v>17.8295794977926</v>
+        <v>17.8295781656015</v>
       </c>
       <c r="N20">
-        <v>5.83772418192329</v>
+        <v>5.83772438809814</v>
       </c>
       <c r="O20">
-        <v>490.126313486207</v>
+        <v>490.126263035197</v>
       </c>
       <c r="P20">
-        <v>24.3481487440958</v>
+        <v>24.3481526101184</v>
       </c>
     </row>
     <row r="21">
@@ -1434,49 +1434,49 @@
         </is>
       </c>
       <c r="B21">
-        <v>1077.43123261643</v>
+        <v>1077.43121718162</v>
       </c>
       <c r="C21">
-        <v>30.9005935509151</v>
+        <v>30.9005883930164</v>
       </c>
       <c r="D21">
-        <v>13.9377193983874</v>
+        <v>13.9377192521587</v>
       </c>
       <c r="E21">
-        <v>33.9218456653992</v>
+        <v>33.9219116552185</v>
       </c>
       <c r="F21">
-        <v>5.08979301085637</v>
+        <v>5.08979131604493</v>
       </c>
       <c r="G21">
-        <v>13.7503518743044</v>
+        <v>13.7503524687969</v>
       </c>
       <c r="H21">
-        <v>21.2857910733231</v>
+        <v>21.2858683879468</v>
       </c>
       <c r="I21">
-        <v>9.45591801076932</v>
+        <v>9.455918664646511</v>
       </c>
       <c r="J21">
-        <v>16.358435554809</v>
+        <v>16.3584745478528</v>
       </c>
       <c r="K21">
-        <v>17.6468650963224</v>
+        <v>17.6468651105093</v>
       </c>
       <c r="L21">
-        <v>39.1127468738507</v>
+        <v>39.1128742458654</v>
       </c>
       <c r="M21">
-        <v>38.1832674019375</v>
+        <v>38.1832719064899</v>
       </c>
       <c r="N21">
-        <v>19.4497761691559</v>
+        <v>19.4497638815289</v>
       </c>
       <c r="O21">
-        <v>2366.48378453545</v>
+        <v>2366.48313856001</v>
       </c>
       <c r="P21">
-        <v>19.5951588858586</v>
+        <v>19.5951567901529</v>
       </c>
     </row>
     <row r="22">
@@ -1486,49 +1486,49 @@
         </is>
       </c>
       <c r="B22">
-        <v>1339.50948416087</v>
+        <v>1339.50945838194</v>
       </c>
       <c r="C22">
-        <v>25.884881657114</v>
+        <v>25.8848726950015</v>
       </c>
       <c r="D22">
-        <v>37.5185398334899</v>
+        <v>37.5185377346484</v>
       </c>
       <c r="E22">
-        <v>38.3760695404797</v>
+        <v>38.3763942206816</v>
       </c>
       <c r="F22">
-        <v>2.78280569100777</v>
+        <v>2.78280244358686</v>
       </c>
       <c r="G22">
-        <v>27.0865196777349</v>
+        <v>27.0865203174987</v>
       </c>
       <c r="H22">
-        <v>29.0190977433709</v>
+        <v>29.0193001558003</v>
       </c>
       <c r="I22">
-        <v>11.1006074005778</v>
+        <v>11.1006072204702</v>
       </c>
       <c r="J22">
-        <v>60.6488098177626</v>
+        <v>60.6489028790574</v>
       </c>
       <c r="K22">
-        <v>45.7345894122181</v>
+        <v>45.734587033864</v>
       </c>
       <c r="L22">
-        <v>133.78669221209</v>
+        <v>133.787231584676</v>
       </c>
       <c r="M22">
-        <v>24.3231061998333</v>
+        <v>24.3231049624807</v>
       </c>
       <c r="N22">
-        <v>81.65355891883471</v>
+        <v>81.6535592598425</v>
       </c>
       <c r="O22">
-        <v>2683.67750717556</v>
+        <v>2683.67668177074</v>
       </c>
       <c r="P22">
-        <v>19.0193947340342</v>
+        <v>19.0193885455058</v>
       </c>
     </row>
     <row r="23">
@@ -1538,49 +1538,49 @@
         </is>
       </c>
       <c r="B23">
-        <v>2259.4187103394</v>
+        <v>2259.4182273964</v>
       </c>
       <c r="C23">
-        <v>50.4928820684313</v>
+        <v>50.4928841279873</v>
       </c>
       <c r="D23">
-        <v>19.1705037749862</v>
+        <v>19.1705032961356</v>
       </c>
       <c r="E23">
-        <v>65.3385897979186</v>
+        <v>65.3386562403839</v>
       </c>
       <c r="F23">
-        <v>5.61844446975169</v>
+        <v>5.61844202833703</v>
       </c>
       <c r="G23">
-        <v>64.2356529154482</v>
+        <v>64.235653828419</v>
       </c>
       <c r="H23">
-        <v>65.4416628562585</v>
+        <v>65.44181220038701</v>
       </c>
       <c r="I23">
-        <v>22.4878021545648</v>
+        <v>22.4878037213956</v>
       </c>
       <c r="J23">
-        <v>178.171326552623</v>
+        <v>178.171410036847</v>
       </c>
       <c r="K23">
-        <v>132.560795779804</v>
+        <v>132.560804201498</v>
       </c>
       <c r="L23">
-        <v>56.7832739681505</v>
+        <v>56.7834088177219</v>
       </c>
       <c r="M23">
-        <v>532.296324073191</v>
+        <v>532.296328122667</v>
       </c>
       <c r="N23">
-        <v>94.629831641053</v>
+        <v>94.6298170399366</v>
       </c>
       <c r="O23">
-        <v>3393.20695985529</v>
+        <v>3393.20684232216</v>
       </c>
       <c r="P23">
-        <v>70.8389871020707</v>
+        <v>70.8389875777158</v>
       </c>
     </row>
     <row r="24">
@@ -1590,49 +1590,49 @@
         </is>
       </c>
       <c r="B24">
-        <v>865.2026153199651</v>
+        <v>865.2024700819441</v>
       </c>
       <c r="C24">
-        <v>71.8871081403139</v>
+        <v>71.8871030916098</v>
       </c>
       <c r="D24">
-        <v>8.205752972459569</v>
+        <v>8.20575131611972</v>
       </c>
       <c r="E24">
-        <v>67.044682932017</v>
+        <v>67.0449432139001</v>
       </c>
       <c r="F24">
-        <v>18.3692868684119</v>
+        <v>18.3692866559402</v>
       </c>
       <c r="G24">
-        <v>17.3923409446076</v>
+        <v>17.392340433467</v>
       </c>
       <c r="H24">
-        <v>28.9470656174223</v>
+        <v>28.9473462299088</v>
       </c>
       <c r="I24">
-        <v>10.1293210780359</v>
+        <v>10.1293207779831</v>
       </c>
       <c r="J24">
-        <v>58.6709696318547</v>
+        <v>58.6710696494283</v>
       </c>
       <c r="K24">
-        <v>62.1990682577345</v>
+        <v>62.1990680083238</v>
       </c>
       <c r="L24">
-        <v>77.6702159068402</v>
+        <v>77.6706726182008</v>
       </c>
       <c r="M24">
-        <v>22.1242136427015</v>
+        <v>22.1242155414529</v>
       </c>
       <c r="N24">
-        <v>63.5015693239902</v>
+        <v>63.5015296511757</v>
       </c>
       <c r="O24">
-        <v>1964.79003067697</v>
+        <v>1964.78982370835</v>
       </c>
       <c r="P24">
-        <v>120.954118002462</v>
+        <v>120.954113748132</v>
       </c>
     </row>
     <row r="25">
@@ -1642,49 +1642,49 @@
         </is>
       </c>
       <c r="B25">
-        <v>735.618888391426</v>
+        <v>735.618794714958</v>
       </c>
       <c r="C25">
-        <v>35.2100861037667</v>
+        <v>35.2100873418215</v>
       </c>
       <c r="D25">
-        <v>28.6337109795753</v>
+        <v>28.6337095956052</v>
       </c>
       <c r="E25">
-        <v>34.4970565580722</v>
+        <v>34.4971917647894</v>
       </c>
       <c r="F25">
-        <v>17.9049016266198</v>
+        <v>17.9048983733968</v>
       </c>
       <c r="G25">
-        <v>12.4161701621486</v>
+        <v>12.4161708168332</v>
       </c>
       <c r="H25">
-        <v>16.7514013455531</v>
+        <v>16.7514794519602</v>
       </c>
       <c r="I25">
-        <v>4.978841556205</v>
+        <v>4.9788414886734</v>
       </c>
       <c r="J25">
-        <v>21.9051777990684</v>
+        <v>21.9052002225357</v>
       </c>
       <c r="K25">
-        <v>18.7810283289994</v>
+        <v>18.7810337257313</v>
       </c>
       <c r="L25">
-        <v>34.1510724440874</v>
+        <v>34.1512811485723</v>
       </c>
       <c r="M25">
-        <v>26.1757039218367</v>
+        <v>26.175698469465</v>
       </c>
       <c r="N25">
-        <v>45.9962115087641</v>
+        <v>45.9962122237637</v>
       </c>
       <c r="O25">
-        <v>870.790118786016</v>
+        <v>870.789994176729</v>
       </c>
       <c r="P25">
-        <v>39.5232937405508</v>
+        <v>39.5232954219409</v>
       </c>
     </row>
     <row r="26">
@@ -1694,49 +1694,49 @@
         </is>
       </c>
       <c r="B26">
-        <v>1216.78381990952</v>
+        <v>1216.78329997945</v>
       </c>
       <c r="C26">
-        <v>61.1430995333746</v>
+        <v>61.1430979027072</v>
       </c>
       <c r="D26">
-        <v>17.8015068774224</v>
+        <v>17.8015093079094</v>
       </c>
       <c r="E26">
-        <v>50.7099100726775</v>
+        <v>50.710042657853</v>
       </c>
       <c r="F26">
-        <v>4.19368662271761</v>
+        <v>4.19368549706325</v>
       </c>
       <c r="G26">
-        <v>35.9260711545228</v>
+        <v>35.9260730220993</v>
       </c>
       <c r="H26">
-        <v>25.5937636651417</v>
+        <v>25.5938571118155</v>
       </c>
       <c r="I26">
-        <v>17.8978675294592</v>
+        <v>17.8978653829385</v>
       </c>
       <c r="J26">
-        <v>63.1871191828055</v>
+        <v>63.1871596369294</v>
       </c>
       <c r="K26">
-        <v>51.9145295354277</v>
+        <v>51.9145264204457</v>
       </c>
       <c r="L26">
-        <v>42.8993913529518</v>
+        <v>42.8996152171226</v>
       </c>
       <c r="M26">
-        <v>88.91232691530131</v>
+        <v>88.9123262482079</v>
       </c>
       <c r="N26">
-        <v>41.4211495719713</v>
+        <v>41.4211467801769</v>
       </c>
       <c r="O26">
-        <v>2151.28435922654</v>
+        <v>2151.2842062865</v>
       </c>
       <c r="P26">
-        <v>73.23356483204969</v>
+        <v>73.2335653469229</v>
       </c>
     </row>
     <row r="27">
@@ -1746,49 +1746,49 @@
         </is>
       </c>
       <c r="B27">
-        <v>199.076684209529</v>
+        <v>199.076625406625</v>
       </c>
       <c r="C27">
-        <v>3.1370211119833</v>
+        <v>3.13701937958451</v>
       </c>
       <c r="D27">
-        <v>1.53794594244035</v>
+        <v>1.53794593580651</v>
       </c>
       <c r="E27">
-        <v>11.4907424452274</v>
+        <v>11.490743191972</v>
       </c>
       <c r="F27">
-        <v>8.72397641430674</v>
+        <v>8.723973979424679</v>
       </c>
       <c r="G27">
-        <v>0.768433781165237</v>
+        <v>0.7684336286479601</v>
       </c>
       <c r="H27">
-        <v>0.303443517505309</v>
+        <v>0.341393470165284</v>
       </c>
       <c r="I27">
-        <v>1.57305524261065</v>
+        <v>1.57305522183479</v>
       </c>
       <c r="J27">
-        <v>4.45888189705332</v>
+        <v>4.45892372388156</v>
       </c>
       <c r="K27">
-        <v>1.68845471479037</v>
+        <v>1.6884546567951</v>
       </c>
       <c r="L27">
-        <v>1.72482228053544</v>
+        <v>1.72485299543346</v>
       </c>
       <c r="M27">
-        <v>1.15521744790459</v>
+        <v>1.1552172356787</v>
       </c>
       <c r="N27">
-        <v>4.94520638208155</v>
+        <v>4.91467001280897</v>
       </c>
       <c r="O27">
-        <v>355.530094040322</v>
+        <v>355.52241191255</v>
       </c>
       <c r="P27">
-        <v>46.5993375546977</v>
+        <v>46.5993348823864</v>
       </c>
     </row>
     <row r="28">
@@ -1798,49 +1798,49 @@
         </is>
       </c>
       <c r="B28">
-        <v>308.062913142309</v>
+        <v>308.062891171096</v>
       </c>
       <c r="C28">
-        <v>33.67085720315</v>
+        <v>33.6708613087766</v>
       </c>
       <c r="D28">
-        <v>1.9835425354511</v>
+        <v>1.98354225040809</v>
       </c>
       <c r="E28">
-        <v>8.46678932217529</v>
+        <v>8.46685480342383</v>
       </c>
       <c r="F28">
-        <v>1.9394799093711</v>
+        <v>1.93947865946416</v>
       </c>
       <c r="G28">
-        <v>5.30727530483647</v>
+        <v>5.30727609246022</v>
       </c>
       <c r="H28">
-        <v>7.55810185464167</v>
+        <v>7.55830522203061</v>
       </c>
       <c r="I28">
-        <v>4.8628231902685</v>
+        <v>4.8628229756396</v>
       </c>
       <c r="J28">
-        <v>17.8240752091484</v>
+        <v>17.8240990062558</v>
       </c>
       <c r="K28">
-        <v>16.5402209008487</v>
+        <v>16.540223475719</v>
       </c>
       <c r="L28">
-        <v>10.5527934210211</v>
+        <v>10.5529105755307</v>
       </c>
       <c r="M28">
-        <v>8.07768973266921</v>
+        <v>8.077688906846319</v>
       </c>
       <c r="N28">
-        <v>11.4057484576783</v>
+        <v>11.4057369559657</v>
       </c>
       <c r="O28">
-        <v>668.959151628356</v>
+        <v>668.959088444833</v>
       </c>
       <c r="P28">
-        <v>90.4753626937172</v>
+        <v>90.47536309665129</v>
       </c>
     </row>
     <row r="29">
@@ -1850,49 +1850,49 @@
         </is>
       </c>
       <c r="B29">
-        <v>452.45145814494</v>
+        <v>452.451317127841</v>
       </c>
       <c r="C29">
-        <v>6.5501464481183</v>
+        <v>6.55014149872212</v>
       </c>
       <c r="D29">
-        <v>3.36258719392007</v>
+        <v>3.36258543924484</v>
       </c>
       <c r="E29">
-        <v>5.52023663330243</v>
+        <v>5.52056263806955</v>
       </c>
       <c r="F29">
-        <v>16.9309334014761</v>
+        <v>16.930926585493</v>
       </c>
       <c r="G29">
-        <v>2.25777430336111</v>
+        <v>2.25777388659164</v>
       </c>
       <c r="H29">
-        <v>2.44346327199796</v>
+        <v>2.44374595354489</v>
       </c>
       <c r="I29">
-        <v>4.91278342435096</v>
+        <v>4.91278281857887</v>
       </c>
       <c r="J29">
-        <v>7.18960929293192</v>
+        <v>7.18969809029582</v>
       </c>
       <c r="K29">
-        <v>2.58489846547419</v>
+        <v>2.58489831285419</v>
       </c>
       <c r="L29">
-        <v>5.69715193394456</v>
+        <v>5.69769636080658</v>
       </c>
       <c r="M29">
-        <v>3.00477412406027</v>
+        <v>3.0047723755418</v>
       </c>
       <c r="N29">
-        <v>14.0174155156279</v>
+        <v>14.017397307573</v>
       </c>
       <c r="O29">
-        <v>857.813310589323</v>
+        <v>857.812904172844</v>
       </c>
       <c r="P29">
-        <v>4.80766353206247</v>
+        <v>4.80765274064585</v>
       </c>
     </row>
     <row r="30">
@@ -1902,49 +1902,49 @@
         </is>
       </c>
       <c r="B30">
-        <v>235.381801910105</v>
+        <v>235.381821755915</v>
       </c>
       <c r="C30">
-        <v>3.77494986993697</v>
+        <v>3.77495016264634</v>
       </c>
       <c r="D30">
-        <v>5.74920759548003</v>
+        <v>5.74920755019004</v>
       </c>
       <c r="E30">
-        <v>14.6070869924591</v>
+        <v>14.6070840533885</v>
       </c>
       <c r="F30">
-        <v>0.936210633301014</v>
+        <v>0.936210644235205</v>
       </c>
       <c r="G30">
-        <v>5.15705791744963</v>
+        <v>5.15705782219808</v>
       </c>
       <c r="H30">
-        <v>5.89778643073005</v>
+        <v>5.89778663222827</v>
       </c>
       <c r="I30">
-        <v>2.31906094395044</v>
+        <v>2.31906107505363</v>
       </c>
       <c r="J30">
-        <v>19.5892595370797</v>
+        <v>19.5892592518846</v>
       </c>
       <c r="K30">
-        <v>12.6864260054867</v>
+        <v>12.6864255354231</v>
       </c>
       <c r="L30">
-        <v>42.5973046068522</v>
+        <v>42.5973040207252</v>
       </c>
       <c r="M30">
-        <v>10.6227255859435</v>
+        <v>10.6227254618775</v>
       </c>
       <c r="N30">
-        <v>15.7836705456432</v>
+        <v>15.7836712265567</v>
       </c>
       <c r="O30">
-        <v>497.848841105928</v>
+        <v>497.848806291683</v>
       </c>
       <c r="P30">
-        <v>8.051487239930591</v>
+        <v>8.05148675958935</v>
       </c>
     </row>
     <row r="31">
@@ -1954,49 +1954,49 @@
         </is>
       </c>
       <c r="B31">
-        <v>1989.99311756414</v>
+        <v>1989.9929992055</v>
       </c>
       <c r="C31">
-        <v>47.5844604183837</v>
+        <v>47.5844535142313</v>
       </c>
       <c r="D31">
-        <v>49.6902589846837</v>
+        <v>49.6902584348024</v>
       </c>
       <c r="E31">
-        <v>31.9946487662315</v>
+        <v>31.9947839431414</v>
       </c>
       <c r="F31">
-        <v>13.1945067190421</v>
+        <v>13.1945064151482</v>
       </c>
       <c r="G31">
-        <v>150.490754967827</v>
+        <v>150.490760848881</v>
       </c>
       <c r="H31">
-        <v>30.7511337766412</v>
+        <v>30.7511944789835</v>
       </c>
       <c r="I31">
-        <v>26.2866947821393</v>
+        <v>26.2866933976378</v>
       </c>
       <c r="J31">
-        <v>40.7848700046967</v>
+        <v>40.784890602391</v>
       </c>
       <c r="K31">
-        <v>42.2554412721478</v>
+        <v>42.2554416701562</v>
       </c>
       <c r="L31">
-        <v>60.3677917726294</v>
+        <v>60.3680068858599</v>
       </c>
       <c r="M31">
-        <v>30.3465238482269</v>
+        <v>30.3465226014686</v>
       </c>
       <c r="N31">
-        <v>71.0102554651713</v>
+        <v>71.01025696168919</v>
       </c>
       <c r="O31">
-        <v>3442.53778776368</v>
+        <v>3442.53778172323</v>
       </c>
       <c r="P31">
-        <v>11.2882497267854</v>
+        <v>11.288246325478</v>
       </c>
     </row>
     <row r="32">
@@ -2006,49 +2006,49 @@
         </is>
       </c>
       <c r="B32">
-        <v>469.86017838227</v>
+        <v>469.860053461902</v>
       </c>
       <c r="C32">
-        <v>4.68117043310382</v>
+        <v>4.68116451580685</v>
       </c>
       <c r="D32">
-        <v>4.12815043320869</v>
+        <v>4.12814996802828</v>
       </c>
       <c r="E32">
-        <v>2.71470113740485</v>
+        <v>2.71483100237447</v>
       </c>
       <c r="F32">
-        <v>22.4266553640703</v>
+        <v>22.4266517801364</v>
       </c>
       <c r="G32">
-        <v>2.28731990324421</v>
+        <v>2.28731949694278</v>
       </c>
       <c r="H32">
-        <v>1.2909772103003</v>
+        <v>1.29126264058699</v>
       </c>
       <c r="I32">
-        <v>3.47941489738063</v>
+        <v>3.47941409502772</v>
       </c>
       <c r="J32">
-        <v>1.82110608286975</v>
+        <v>1.82124422496368</v>
       </c>
       <c r="K32">
-        <v>4.64025007658797</v>
+        <v>4.64024929139458</v>
       </c>
       <c r="L32">
-        <v>14.2198435764762</v>
+        <v>14.2201374074414</v>
       </c>
       <c r="M32">
-        <v>5.39289236376901</v>
+        <v>5.39289150215322</v>
       </c>
       <c r="N32">
-        <v>10.7727623588742</v>
+        <v>10.7727331514795</v>
       </c>
       <c r="O32">
-        <v>684.955237653412</v>
+        <v>684.954849562393</v>
       </c>
       <c r="P32">
-        <v>30.5132521017565</v>
+        <v>30.5132437499727</v>
       </c>
     </row>
     <row r="33">
@@ -2058,49 +2058,49 @@
         </is>
       </c>
       <c r="B33">
-        <v>4966.1271442769</v>
+        <v>4966.12706843955</v>
       </c>
       <c r="C33">
-        <v>83.0467069988069</v>
+        <v>83.0466988715572</v>
       </c>
       <c r="D33">
-        <v>140.958268069453</v>
+        <v>140.958264724002</v>
       </c>
       <c r="E33">
-        <v>86.0021449413394</v>
+        <v>86.0022763066679</v>
       </c>
       <c r="F33">
-        <v>11.4561960123759</v>
+        <v>11.4561924883977</v>
       </c>
       <c r="G33">
-        <v>81.6600824960163</v>
+        <v>81.66008833448841</v>
       </c>
       <c r="H33">
-        <v>49.3893159183442</v>
+        <v>49.3894481600266</v>
       </c>
       <c r="I33">
-        <v>46.2394858751952</v>
+        <v>46.2394889983433</v>
       </c>
       <c r="J33">
-        <v>120.308220225919</v>
+        <v>120.308284690323</v>
       </c>
       <c r="K33">
-        <v>123.473493111889</v>
+        <v>123.473495657889</v>
       </c>
       <c r="L33">
-        <v>150.139134577737</v>
+        <v>150.13937749966</v>
       </c>
       <c r="M33">
-        <v>90.89892055836199</v>
+        <v>90.89891279929481</v>
       </c>
       <c r="N33">
-        <v>154.902199151613</v>
+        <v>154.902200090536</v>
       </c>
       <c r="O33">
-        <v>7407.27167725685</v>
+        <v>7407.27067478601</v>
       </c>
       <c r="P33">
-        <v>86.08198844794561</v>
+        <v>86.0819794742979</v>
       </c>
     </row>
     <row r="34">
@@ -2110,49 +2110,49 @@
         </is>
       </c>
       <c r="B34">
-        <v>1761.14392675455</v>
+        <v>1761.1436883192</v>
       </c>
       <c r="C34">
-        <v>80.7591783470438</v>
+        <v>80.75918364119821</v>
       </c>
       <c r="D34">
-        <v>227.347173200802</v>
+        <v>227.347157387304</v>
       </c>
       <c r="E34">
-        <v>83.5487411073368</v>
+        <v>83.54926750786819</v>
       </c>
       <c r="F34">
-        <v>6.82360527421301</v>
+        <v>6.82360271882618</v>
       </c>
       <c r="G34">
-        <v>71.1318921968619</v>
+        <v>71.13189588183749</v>
       </c>
       <c r="H34">
-        <v>47.9370509255264</v>
+        <v>47.9373433131552</v>
       </c>
       <c r="I34">
-        <v>30.3982447634987</v>
+        <v>30.3982416083516</v>
       </c>
       <c r="J34">
-        <v>56.4343771572463</v>
+        <v>56.4344821663147</v>
       </c>
       <c r="K34">
-        <v>62.8953056525506</v>
+        <v>62.8953088522118</v>
       </c>
       <c r="L34">
-        <v>115.07116548162</v>
+        <v>115.072011144529</v>
       </c>
       <c r="M34">
-        <v>53.188200170489</v>
+        <v>53.1881966993836</v>
       </c>
       <c r="N34">
-        <v>140.545603065836</v>
+        <v>140.545584208165</v>
       </c>
       <c r="O34">
-        <v>2848.379446076</v>
+        <v>2848.37925970663</v>
       </c>
       <c r="P34">
-        <v>63.4713812305307</v>
+        <v>63.4713706178447</v>
       </c>
     </row>
     <row r="35">
@@ -2162,49 +2162,49 @@
         </is>
       </c>
       <c r="B35">
-        <v>126.248993981484</v>
+        <v>126.248981436026</v>
       </c>
       <c r="C35">
-        <v>6.83545228747081</v>
+        <v>6.83545134691101</v>
       </c>
       <c r="D35">
-        <v>1.02706732601107</v>
+        <v>1.02706731725004</v>
       </c>
       <c r="E35">
-        <v>1.6917637399754</v>
+        <v>1.69176353089817</v>
       </c>
       <c r="F35">
-        <v>5.41393379689693</v>
+        <v>5.41393269503226</v>
       </c>
       <c r="G35">
-        <v>0.419551273257561</v>
+        <v>0.419551272299675</v>
       </c>
       <c r="H35">
-        <v>0.620314146396964</v>
+        <v>0.620389272577663</v>
       </c>
       <c r="I35">
-        <v>1.00716913073822</v>
+        <v>1.00716918226573</v>
       </c>
       <c r="J35">
-        <v>1.69625688801694</v>
+        <v>1.69627745947915</v>
       </c>
       <c r="K35">
-        <v>5.97414531729449</v>
+        <v>5.97414483270686</v>
       </c>
       <c r="L35">
-        <v>2.55375865361182</v>
+        <v>2.5537737555654</v>
       </c>
       <c r="M35">
-        <v>1.9249342837492</v>
+        <v>1.9249346562159</v>
       </c>
       <c r="N35">
-        <v>2.44161830713658</v>
+        <v>2.44160119565735</v>
       </c>
       <c r="O35">
-        <v>250.085115709754</v>
+        <v>250.085055302987</v>
       </c>
       <c r="P35">
-        <v>44.3921528241118</v>
+        <v>44.392154471283</v>
       </c>
     </row>
     <row r="36">
@@ -2214,49 +2214,49 @@
         </is>
       </c>
       <c r="B36">
-        <v>2556.36989788166</v>
+        <v>2556.36955858577</v>
       </c>
       <c r="C36">
-        <v>67.3397912445316</v>
+        <v>67.33978767951621</v>
       </c>
       <c r="D36">
-        <v>22.6421134567218</v>
+        <v>22.6421118746591</v>
       </c>
       <c r="E36">
-        <v>91.1689809903488</v>
+        <v>91.16910818157319</v>
       </c>
       <c r="F36">
-        <v>30.8144542688797</v>
+        <v>30.814448817189</v>
       </c>
       <c r="G36">
-        <v>96.1970697451881</v>
+        <v>96.19706738133689</v>
       </c>
       <c r="H36">
-        <v>123.615883411363</v>
+        <v>123.615992755821</v>
       </c>
       <c r="I36">
-        <v>48.682710999187</v>
+        <v>48.6827153111993</v>
       </c>
       <c r="J36">
-        <v>275.467535752717</v>
+        <v>275.467561606113</v>
       </c>
       <c r="K36">
-        <v>159.428627040276</v>
+        <v>159.428642897749</v>
       </c>
       <c r="L36">
-        <v>112.303335879875</v>
+        <v>112.30355109895</v>
       </c>
       <c r="M36">
-        <v>257.780608195348</v>
+        <v>257.780636915077</v>
       </c>
       <c r="N36">
-        <v>88.47822101933301</v>
+        <v>88.47820932703161</v>
       </c>
       <c r="O36">
-        <v>4087.99412236794</v>
+        <v>4087.99412296406</v>
       </c>
       <c r="P36">
-        <v>66.01225008471761</v>
+        <v>66.0122385611983</v>
       </c>
     </row>
     <row r="37">
@@ -2266,49 +2266,49 @@
         </is>
       </c>
       <c r="B37">
-        <v>857.173304215656</v>
+        <v>857.173274561684</v>
       </c>
       <c r="C37">
-        <v>21.864261819586</v>
+        <v>21.864257396813</v>
       </c>
       <c r="D37">
-        <v>15.6050319428567</v>
+        <v>15.6050322982173</v>
       </c>
       <c r="E37">
-        <v>19.0027572503999</v>
+        <v>19.0028228938311</v>
       </c>
       <c r="F37">
-        <v>46.3688100268896</v>
+        <v>46.3688058505594</v>
       </c>
       <c r="G37">
-        <v>5.00217605919258</v>
+        <v>5.00217590527145</v>
       </c>
       <c r="H37">
-        <v>20.8565218848826</v>
+        <v>20.8566878109395</v>
       </c>
       <c r="I37">
-        <v>12.3023158302319</v>
+        <v>12.302315510137</v>
       </c>
       <c r="J37">
-        <v>36.4113462311357</v>
+        <v>36.411386763176</v>
       </c>
       <c r="K37">
-        <v>30.0598045278922</v>
+        <v>30.0598059165814</v>
       </c>
       <c r="L37">
-        <v>28.4562506235384</v>
+        <v>28.4563797118336</v>
       </c>
       <c r="M37">
-        <v>32.7571952974448</v>
+        <v>32.757199468739</v>
       </c>
       <c r="N37">
-        <v>21.0305742201052</v>
+        <v>21.0305572383274</v>
       </c>
       <c r="O37">
-        <v>1203.50311544067</v>
+        <v>1203.50298605801</v>
       </c>
       <c r="P37">
-        <v>63.847164493231</v>
+        <v>63.8471615875058</v>
       </c>
     </row>
     <row r="38">
@@ -2318,49 +2318,49 @@
         </is>
       </c>
       <c r="B38">
-        <v>772.051898696871</v>
+        <v>772.051733006203</v>
       </c>
       <c r="C38">
-        <v>29.7895043458816</v>
+        <v>29.7894934966724</v>
       </c>
       <c r="D38">
-        <v>11.2630383736204</v>
+        <v>11.2630361477915</v>
       </c>
       <c r="E38">
-        <v>62.7064910392325</v>
+        <v>62.7067561079008</v>
       </c>
       <c r="F38">
-        <v>1.98122358851233</v>
+        <v>1.98121486244247</v>
       </c>
       <c r="G38">
-        <v>7.95570993301583</v>
+        <v>7.95570923827349</v>
       </c>
       <c r="H38">
-        <v>8.162360276007311</v>
+        <v>8.16280721499581</v>
       </c>
       <c r="I38">
-        <v>6.56855464186928</v>
+        <v>6.56855396966426</v>
       </c>
       <c r="J38">
-        <v>31.695730764417</v>
+        <v>31.6958997142784</v>
       </c>
       <c r="K38">
-        <v>18.8193307196791</v>
+        <v>18.8193307976107</v>
       </c>
       <c r="L38">
-        <v>61.2526012438656</v>
+        <v>61.2531052492542</v>
       </c>
       <c r="M38">
-        <v>25.4785693873662</v>
+        <v>25.4785690364833</v>
       </c>
       <c r="N38">
-        <v>26.0827985009203</v>
+        <v>26.0827407770678</v>
       </c>
       <c r="O38">
-        <v>1308.66394515761</v>
+        <v>1308.6630674891</v>
       </c>
       <c r="P38">
-        <v>69.6609811677781</v>
+        <v>69.6609598744877</v>
       </c>
     </row>
     <row r="39">
@@ -2370,49 +2370,49 @@
         </is>
       </c>
       <c r="B39">
-        <v>3003.59457762485</v>
+        <v>3003.59418024676</v>
       </c>
       <c r="C39">
-        <v>112.125730706106</v>
+        <v>112.12572982682</v>
       </c>
       <c r="D39">
-        <v>69.2922911795751</v>
+        <v>69.29228679229971</v>
       </c>
       <c r="E39">
-        <v>112.328092143654</v>
+        <v>112.328223834066</v>
       </c>
       <c r="F39">
-        <v>38.6774430463974</v>
+        <v>38.6774388762997</v>
       </c>
       <c r="G39">
-        <v>114.109216841931</v>
+        <v>114.109220416101</v>
       </c>
       <c r="H39">
-        <v>58.8858825349836</v>
+        <v>58.8859664249207</v>
       </c>
       <c r="I39">
-        <v>61.087783878804</v>
+        <v>61.0877817641274</v>
       </c>
       <c r="J39">
-        <v>212.384242961497</v>
+        <v>212.384269397333</v>
       </c>
       <c r="K39">
-        <v>116.996053146758</v>
+        <v>116.996055177214</v>
       </c>
       <c r="L39">
-        <v>139.749485813656</v>
+        <v>139.749702127907</v>
       </c>
       <c r="M39">
-        <v>88.8063106462789</v>
+        <v>88.80631368835721</v>
       </c>
       <c r="N39">
-        <v>101.723030432901</v>
+        <v>101.723018903966</v>
       </c>
       <c r="O39">
-        <v>4491.34313179065</v>
+        <v>4491.34264781785</v>
       </c>
       <c r="P39">
-        <v>78.7200045578399</v>
+        <v>78.7199989301718</v>
       </c>
     </row>
     <row r="40">
@@ -2422,49 +2422,49 @@
         </is>
       </c>
       <c r="B40">
-        <v>245.495981027687</v>
+        <v>245.495914191527</v>
       </c>
       <c r="C40">
-        <v>3.74072210302383</v>
+        <v>3.74072180504489</v>
       </c>
       <c r="D40">
-        <v>10.5561603277532</v>
+        <v>10.5561601150241</v>
       </c>
       <c r="E40">
-        <v>3.77179343860779</v>
+        <v>3.77185826962841</v>
       </c>
       <c r="F40">
-        <v>1.4048433048906</v>
+        <v>1.40484320146478</v>
       </c>
       <c r="G40">
-        <v>3.40657360031914</v>
+        <v>3.4065734822127</v>
       </c>
       <c r="H40">
-        <v>7.0926202283456</v>
+        <v>7.0926461267981</v>
       </c>
       <c r="I40">
-        <v>2.2098457760382</v>
+        <v>2.20984576554684</v>
       </c>
       <c r="J40">
-        <v>12.5130350855538</v>
+        <v>12.5130426439611</v>
       </c>
       <c r="K40">
-        <v>5.95836671678774</v>
+        <v>5.95836646205664</v>
       </c>
       <c r="L40">
-        <v>16.3919512306929</v>
+        <v>16.3920548712676</v>
       </c>
       <c r="M40">
-        <v>9.50870817767016</v>
+        <v>9.508707017581161</v>
       </c>
       <c r="N40">
-        <v>26.364802432494</v>
+        <v>26.3648064385926</v>
       </c>
       <c r="O40">
-        <v>391.571075803498</v>
+        <v>391.570976435481</v>
       </c>
       <c r="P40">
-        <v>2.28694858923544</v>
+        <v>2.28694696244195</v>
       </c>
     </row>
     <row r="41">
@@ -2474,49 +2474,49 @@
         </is>
       </c>
       <c r="B41">
-        <v>939.7667967327631</v>
+        <v>939.76666380018</v>
       </c>
       <c r="C41">
-        <v>17.3313582245488</v>
+        <v>17.3313531058462</v>
       </c>
       <c r="D41">
-        <v>116.084142760799</v>
+        <v>116.0841370828</v>
       </c>
       <c r="E41">
-        <v>53.8586876635712</v>
+        <v>53.8591449367659</v>
       </c>
       <c r="F41">
-        <v>2.93909401135507</v>
+        <v>2.93909208711169</v>
       </c>
       <c r="G41">
-        <v>37.6721481555986</v>
+        <v>37.6721474115891</v>
       </c>
       <c r="H41">
-        <v>35.1088510023125</v>
+        <v>35.1090704670667</v>
       </c>
       <c r="I41">
-        <v>8.42147693928667</v>
+        <v>8.42147683611703</v>
       </c>
       <c r="J41">
-        <v>46.0055991984422</v>
+        <v>46.0056716943536</v>
       </c>
       <c r="K41">
-        <v>48.826649820072</v>
+        <v>48.8266434183651</v>
       </c>
       <c r="L41">
-        <v>27.8634466313022</v>
+        <v>27.8641715868304</v>
       </c>
       <c r="M41">
-        <v>39.4500150948236</v>
+        <v>39.4500151898565</v>
       </c>
       <c r="N41">
-        <v>25.2928677875102</v>
+        <v>25.2928617645337</v>
       </c>
       <c r="O41">
-        <v>1364.73013555117</v>
+        <v>1364.72956090763</v>
       </c>
       <c r="P41">
-        <v>22.5207791197253</v>
+        <v>22.5207706495914</v>
       </c>
     </row>
     <row r="42">
@@ -2526,49 +2526,49 @@
         </is>
       </c>
       <c r="B42">
-        <v>141.031621902772</v>
+        <v>141.031606631375</v>
       </c>
       <c r="C42">
-        <v>9.098506772978711</v>
+        <v>9.098506254681199</v>
       </c>
       <c r="D42">
-        <v>2.17649649712067</v>
+        <v>2.17649636379483</v>
       </c>
       <c r="E42">
-        <v>5.00081893082992</v>
+        <v>5.00081885489675</v>
       </c>
       <c r="F42">
-        <v>1.81926523156168</v>
+        <v>1.81926418147472</v>
       </c>
       <c r="G42">
-        <v>0.900229583978941</v>
+        <v>0.900229448681772</v>
       </c>
       <c r="H42">
-        <v>1.8005237010903</v>
+        <v>1.80064021807196</v>
       </c>
       <c r="I42">
-        <v>1.04567612352603</v>
+        <v>1.04567611169635</v>
       </c>
       <c r="J42">
-        <v>3.81370223720151</v>
+        <v>3.81372319937037</v>
       </c>
       <c r="K42">
-        <v>7.35970381725568</v>
+        <v>7.35970344438214</v>
       </c>
       <c r="L42">
-        <v>7.87673124160456</v>
+        <v>7.87674563964963</v>
       </c>
       <c r="M42">
-        <v>2.86874865354254</v>
+        <v>2.86874858180991</v>
       </c>
       <c r="N42">
-        <v>8.5183710723161</v>
+        <v>8.51835401981374</v>
       </c>
       <c r="O42">
-        <v>286.755698356636</v>
+        <v>286.755664088248</v>
       </c>
       <c r="P42">
-        <v>45.8666032569146</v>
+        <v>45.8665980646321</v>
       </c>
     </row>
     <row r="43">
@@ -2578,49 +2578,49 @@
         </is>
       </c>
       <c r="B43">
-        <v>1377.82733294947</v>
+        <v>1377.8269294258</v>
       </c>
       <c r="C43">
-        <v>41.7336042324832</v>
+        <v>41.7335984308369</v>
       </c>
       <c r="D43">
-        <v>56.2851595667943</v>
+        <v>56.2851539932729</v>
       </c>
       <c r="E43">
-        <v>74.35972086171211</v>
+        <v>74.35978630067839</v>
       </c>
       <c r="F43">
-        <v>10.1266489242354</v>
+        <v>10.1266450914262</v>
       </c>
       <c r="G43">
-        <v>32.9521459871658</v>
+        <v>32.9521454018165</v>
       </c>
       <c r="H43">
-        <v>40.6042069756287</v>
+        <v>40.6043016105551</v>
       </c>
       <c r="I43">
-        <v>22.6509438014535</v>
+        <v>22.6509486617368</v>
       </c>
       <c r="J43">
-        <v>73.9036199070098</v>
+        <v>73.90369067152891</v>
       </c>
       <c r="K43">
-        <v>51.4184251420576</v>
+        <v>51.4184267487581</v>
       </c>
       <c r="L43">
-        <v>57.897152278559</v>
+        <v>57.8972958795635</v>
       </c>
       <c r="M43">
-        <v>92.3323045625196</v>
+        <v>92.3323010020701</v>
       </c>
       <c r="N43">
-        <v>71.11780568039571</v>
+        <v>71.1178092688409</v>
       </c>
       <c r="O43">
-        <v>2005.4179010925</v>
+        <v>2005.41756155371</v>
       </c>
       <c r="P43">
-        <v>46.3729261344152</v>
+        <v>46.3729269425919</v>
       </c>
     </row>
     <row r="44">
@@ -2630,49 +2630,49 @@
         </is>
       </c>
       <c r="B44">
-        <v>4722.79339179212</v>
+        <v>4722.7931527464</v>
       </c>
       <c r="C44">
-        <v>162.911617801448</v>
+        <v>162.911604345394</v>
       </c>
       <c r="D44">
-        <v>79.7387388731936</v>
+        <v>79.7387384664794</v>
       </c>
       <c r="E44">
-        <v>100.293349022177</v>
+        <v>100.293944328126</v>
       </c>
       <c r="F44">
-        <v>210.581819613956</v>
+        <v>210.581827931959</v>
       </c>
       <c r="G44">
-        <v>125.409498367957</v>
+        <v>125.409501369499</v>
       </c>
       <c r="H44">
-        <v>65.1091948499738</v>
+        <v>65.1099174691096</v>
       </c>
       <c r="I44">
-        <v>53.1067267053528</v>
+        <v>53.1067256933746</v>
       </c>
       <c r="J44">
-        <v>159.041504096005</v>
+        <v>159.041709878801</v>
       </c>
       <c r="K44">
-        <v>140.093769860706</v>
+        <v>140.093764015411</v>
       </c>
       <c r="L44">
-        <v>255.251090947673</v>
+        <v>255.25206440322</v>
       </c>
       <c r="M44">
-        <v>147.967393277581</v>
+        <v>147.967387695134</v>
       </c>
       <c r="N44">
-        <v>108.905810674888</v>
+        <v>108.905767496086</v>
       </c>
       <c r="O44">
-        <v>7630.87843917498</v>
+        <v>7630.8771711608</v>
       </c>
       <c r="P44">
-        <v>229.959046382133</v>
+        <v>229.958978855737</v>
       </c>
     </row>
     <row r="45">
@@ -2682,49 +2682,49 @@
         </is>
       </c>
       <c r="B45">
-        <v>434.959883685712</v>
+        <v>434.959827530795</v>
       </c>
       <c r="C45">
-        <v>18.4048877453908</v>
+        <v>18.4048789962158</v>
       </c>
       <c r="D45">
-        <v>5.0042076163227</v>
+        <v>5.00420678276139</v>
       </c>
       <c r="E45">
-        <v>11.260885352413</v>
+        <v>11.261014847555</v>
       </c>
       <c r="F45">
-        <v>19.1356262684842</v>
+        <v>19.1356188514603</v>
       </c>
       <c r="G45">
-        <v>9.58971188435679</v>
+        <v>9.589712376039371</v>
       </c>
       <c r="H45">
-        <v>4.08063967365446</v>
+        <v>4.08112497239236</v>
       </c>
       <c r="I45">
-        <v>6.2981583611143</v>
+        <v>6.2981579745765</v>
       </c>
       <c r="J45">
-        <v>19.3209694780232</v>
+        <v>19.321044460705</v>
       </c>
       <c r="K45">
-        <v>13.5272425947446</v>
+        <v>13.5272431646146</v>
       </c>
       <c r="L45">
-        <v>23.8477485432449</v>
+        <v>23.847994340557</v>
       </c>
       <c r="M45">
-        <v>27.7399605043389</v>
+        <v>27.73995782481</v>
       </c>
       <c r="N45">
-        <v>26.5581288415731</v>
+        <v>26.5581053755874</v>
       </c>
       <c r="O45">
-        <v>852.679782270642</v>
+        <v>852.679482167822</v>
       </c>
       <c r="P45">
-        <v>18.5076768302115</v>
+        <v>18.5076738892494</v>
       </c>
     </row>
     <row r="46">
@@ -2734,49 +2734,49 @@
         </is>
       </c>
       <c r="B46">
-        <v>114.821989745671</v>
+        <v>114.821986318857</v>
       </c>
       <c r="C46">
-        <v>4.8488150280236</v>
+        <v>4.84881495976353</v>
       </c>
       <c r="D46">
-        <v>1.75718884655115</v>
+        <v>1.75718844160258</v>
       </c>
       <c r="E46">
-        <v>7.31927273371963</v>
+        <v>7.31927251911312</v>
       </c>
       <c r="F46">
-        <v>0.955492401926225</v>
+        <v>0.955492332184371</v>
       </c>
       <c r="G46">
-        <v>1.06220919307587</v>
+        <v>1.06220928286379</v>
       </c>
       <c r="H46">
-        <v>1.2859992032592</v>
+        <v>1.28599923802037</v>
       </c>
       <c r="I46">
-        <v>2.39774473768199</v>
+        <v>2.39774465990439</v>
       </c>
       <c r="J46">
-        <v>5.22780221540604</v>
+        <v>5.22780210793862</v>
       </c>
       <c r="K46">
-        <v>4.28644350213336</v>
+        <v>4.28644390597106</v>
       </c>
       <c r="L46">
-        <v>10.9045066964943</v>
+        <v>10.9045066969151</v>
       </c>
       <c r="M46">
-        <v>4.89678710861229</v>
+        <v>4.89678746102619</v>
       </c>
       <c r="N46">
-        <v>7.07635941425569</v>
+        <v>7.07636019439841</v>
       </c>
       <c r="O46">
-        <v>252.789776495531</v>
+        <v>252.789731981686</v>
       </c>
       <c r="P46">
-        <v>12.2628126013651</v>
+        <v>12.2628131517192</v>
       </c>
     </row>
     <row r="47">
@@ -2786,49 +2786,49 @@
         </is>
       </c>
       <c r="B47">
-        <v>1532.38150772466</v>
+        <v>1532.38134927773</v>
       </c>
       <c r="C47">
-        <v>63.464454047052</v>
+        <v>63.4644449940746</v>
       </c>
       <c r="D47">
-        <v>49.9632781548595</v>
+        <v>49.963279178611</v>
       </c>
       <c r="E47">
-        <v>67.0104995145181</v>
+        <v>67.0108959319623</v>
       </c>
       <c r="F47">
-        <v>14.2973087951848</v>
+        <v>14.2973011939436</v>
       </c>
       <c r="G47">
-        <v>34.1622729369113</v>
+        <v>34.1622764525952</v>
       </c>
       <c r="H47">
-        <v>28.422448318368</v>
+        <v>28.4227120233401</v>
       </c>
       <c r="I47">
-        <v>16.3460464268271</v>
+        <v>16.3460474920829</v>
       </c>
       <c r="J47">
-        <v>47.7820485415386</v>
+        <v>47.7821462616798</v>
       </c>
       <c r="K47">
-        <v>40.886781333909</v>
+        <v>40.8867778425807</v>
       </c>
       <c r="L47">
-        <v>53.3156407455881</v>
+        <v>53.3162845511088</v>
       </c>
       <c r="M47">
-        <v>80.8734047474404</v>
+        <v>80.8734000952698</v>
       </c>
       <c r="N47">
-        <v>51.5079642420247</v>
+        <v>51.5079433410541</v>
       </c>
       <c r="O47">
-        <v>2815.61505623256</v>
+        <v>2815.61420493311</v>
       </c>
       <c r="P47">
-        <v>47.1981070369037</v>
+        <v>47.1980962755977</v>
       </c>
     </row>
     <row r="48">
@@ -2838,49 +2838,49 @@
         </is>
       </c>
       <c r="B48">
-        <v>1307.21993647225</v>
+        <v>1307.21934979317</v>
       </c>
       <c r="C48">
-        <v>26.117790758769</v>
+        <v>26.1177712916949</v>
       </c>
       <c r="D48">
-        <v>12.04665237474</v>
+        <v>12.0466442846058</v>
       </c>
       <c r="E48">
-        <v>69.1863163624504</v>
+        <v>69.1876817370822</v>
       </c>
       <c r="F48">
-        <v>12.8489034405886</v>
+        <v>12.8488900634503</v>
       </c>
       <c r="G48">
-        <v>18.2471818464743</v>
+        <v>18.2471811910835</v>
       </c>
       <c r="H48">
-        <v>8.30210124161502</v>
+        <v>8.303071346775649</v>
       </c>
       <c r="I48">
-        <v>11.9668864709299</v>
+        <v>11.9668842267262</v>
       </c>
       <c r="J48">
-        <v>34.8025225474609</v>
+        <v>34.8028702627806</v>
       </c>
       <c r="K48">
-        <v>19.9982607228663</v>
+        <v>19.9982604516169</v>
       </c>
       <c r="L48">
-        <v>47.1953848466505</v>
+        <v>47.1976566237413</v>
       </c>
       <c r="M48">
-        <v>156.293903551672</v>
+        <v>156.293887624662</v>
       </c>
       <c r="N48">
-        <v>23.7926111575796</v>
+        <v>23.7925292978254</v>
       </c>
       <c r="O48">
-        <v>2293.99886078354</v>
+        <v>2293.9967923795</v>
       </c>
       <c r="P48">
-        <v>108.848110595914</v>
+        <v>108.848068308877</v>
       </c>
     </row>
     <row r="49">
@@ -2890,49 +2890,49 @@
         </is>
       </c>
       <c r="B49">
-        <v>585.259274081977</v>
+        <v>585.259263835327</v>
       </c>
       <c r="C49">
-        <v>8.540797477153561</v>
+        <v>8.540797689200071</v>
       </c>
       <c r="D49">
-        <v>5.61192432315581</v>
+        <v>5.6119241975008</v>
       </c>
       <c r="E49">
-        <v>12.7040821977381</v>
+        <v>12.7040823071204</v>
       </c>
       <c r="F49">
-        <v>34.1051447048124</v>
+        <v>34.1051469813377</v>
       </c>
       <c r="G49">
-        <v>16.9463049900563</v>
+        <v>16.9463091887906</v>
       </c>
       <c r="H49">
-        <v>5.49081324206701</v>
+        <v>5.49081293544106</v>
       </c>
       <c r="I49">
-        <v>9.418270365996991</v>
+        <v>9.41827041119851</v>
       </c>
       <c r="J49">
-        <v>22.0355957926245</v>
+        <v>22.0355930069578</v>
       </c>
       <c r="K49">
-        <v>9.5803685736361</v>
+        <v>9.580368066356281</v>
       </c>
       <c r="L49">
-        <v>4.79851313386701</v>
+        <v>4.7985131683095</v>
       </c>
       <c r="M49">
-        <v>7.80429339290863</v>
+        <v>7.8042934434358</v>
       </c>
       <c r="N49">
-        <v>4.83987037620063</v>
+        <v>4.83987065896193</v>
       </c>
       <c r="O49">
-        <v>606.9964670481839</v>
+        <v>606.996487194141</v>
       </c>
       <c r="P49">
-        <v>9.67825371795672</v>
+        <v>9.678253993831371</v>
       </c>
     </row>
     <row r="50">
@@ -2942,49 +2942,49 @@
         </is>
       </c>
       <c r="B50">
-        <v>1000.74087231162</v>
+        <v>1000.74072684121</v>
       </c>
       <c r="C50">
-        <v>90.0099542326325</v>
+        <v>90.0099396714859</v>
       </c>
       <c r="D50">
-        <v>10.1819293006756</v>
+        <v>10.1819278346505</v>
       </c>
       <c r="E50">
-        <v>131.955374860309</v>
+        <v>131.955670766602</v>
       </c>
       <c r="F50">
-        <v>4.40731926194103</v>
+        <v>4.40731304292922</v>
       </c>
       <c r="G50">
-        <v>21.5660267411229</v>
+        <v>21.5660262314134</v>
       </c>
       <c r="H50">
-        <v>37.306516964585</v>
+        <v>37.306737501811</v>
       </c>
       <c r="I50">
-        <v>21.9151027152787</v>
+        <v>21.915105050253</v>
       </c>
       <c r="J50">
-        <v>114.288247218406</v>
+        <v>114.28837000573</v>
       </c>
       <c r="K50">
-        <v>123.579494068705</v>
+        <v>123.579499763213</v>
       </c>
       <c r="L50">
-        <v>84.49135429598211</v>
+        <v>84.49183142289471</v>
       </c>
       <c r="M50">
-        <v>48.9618372392033</v>
+        <v>48.9618354868699</v>
       </c>
       <c r="N50">
-        <v>69.0166047636764</v>
+        <v>69.0166043798193</v>
       </c>
       <c r="O50">
-        <v>1895.54143665812</v>
+        <v>1895.54148814618</v>
       </c>
       <c r="P50">
-        <v>136.949326086744</v>
+        <v>136.949307591834</v>
       </c>
     </row>
     <row r="51">
@@ -2994,49 +2994,49 @@
         </is>
       </c>
       <c r="B51">
-        <v>102.010940715634</v>
+        <v>102.010884606508</v>
       </c>
       <c r="C51">
-        <v>1.48641324042074</v>
+        <v>1.4864110388683</v>
       </c>
       <c r="D51">
-        <v>0.549827253239673</v>
+        <v>0.549826567915813</v>
       </c>
       <c r="E51">
-        <v>1.82116021100414</v>
+        <v>1.82129102705149</v>
       </c>
       <c r="F51">
-        <v>24.2460878527584</v>
+        <v>24.2460844751734</v>
       </c>
       <c r="G51">
-        <v>2.27249589696597</v>
+        <v>2.27249631356316</v>
       </c>
       <c r="H51">
-        <v>0.320203584553521</v>
+        <v>0.317301054689828</v>
       </c>
       <c r="I51">
-        <v>0.814772441165003</v>
+        <v>0.814772243149075</v>
       </c>
       <c r="J51">
-        <v>1.78620790578585</v>
+        <v>1.78625370591146</v>
       </c>
       <c r="K51">
-        <v>0.996666601637859</v>
+        <v>0.99666657955296</v>
       </c>
       <c r="L51">
-        <v>0.501491320782666</v>
+        <v>0.501716868741798</v>
       </c>
       <c r="M51">
-        <v>0.940712656253801</v>
+        <v>0.940712053149664</v>
       </c>
       <c r="N51">
-        <v>1.6372004598346</v>
+        <v>1.63714966187816</v>
       </c>
       <c r="O51">
-        <v>192.083819725898</v>
+        <v>192.083618910183</v>
       </c>
       <c r="P51">
-        <v>14.6648526698888</v>
+        <v>14.6648514606004</v>
       </c>
     </row>
     <row r="52">

</xml_diff>

<commit_message>
rolling +-2 and no <10 obs correction
</commit_message>
<xml_diff>
--- a/1-Data-Codes/2-Final_Data/L_1999.xlsx
+++ b/1-Data-Codes/2-Final_Data/L_1999.xlsx
@@ -446,49 +446,49 @@
         </is>
       </c>
       <c r="B2">
-        <v>1169.80658334613</v>
+        <v>1155.90748771602</v>
       </c>
       <c r="C2">
-        <v>40.3885177371109</v>
+        <v>42.5518281165067</v>
       </c>
       <c r="D2">
-        <v>92.07100683174269</v>
+        <v>85.6491836812769</v>
       </c>
       <c r="E2">
-        <v>68.4961355440167</v>
+        <v>68.81797049805959</v>
       </c>
       <c r="F2">
-        <v>15.8527735903268</v>
+        <v>15.3292926268959</v>
       </c>
       <c r="G2">
-        <v>22.1616100282479</v>
+        <v>23.6467315157155</v>
       </c>
       <c r="H2">
-        <v>24.7956361518259</v>
+        <v>24.6424681408457</v>
       </c>
       <c r="I2">
-        <v>14.5473837908715</v>
+        <v>14.3040110169016</v>
       </c>
       <c r="J2">
-        <v>73.7966911823771</v>
+        <v>71.74352964427089</v>
       </c>
       <c r="K2">
-        <v>25.5405741319049</v>
+        <v>26.9991765463656</v>
       </c>
       <c r="L2">
-        <v>37.187497507836</v>
+        <v>33.5312994362337</v>
       </c>
       <c r="M2">
-        <v>38.8907647569356</v>
+        <v>42.7861239973732</v>
       </c>
       <c r="N2">
-        <v>30.9597868075987</v>
+        <v>32.3365875210218</v>
       </c>
       <c r="O2">
-        <v>1445.40119399736</v>
+        <v>1463.42846971546</v>
       </c>
       <c r="P2">
-        <v>50.7103446417472</v>
+        <v>49.9705833731624</v>
       </c>
     </row>
     <row r="3">
@@ -498,49 +498,49 @@
         </is>
       </c>
       <c r="B3">
-        <v>124.357550472118</v>
+        <v>124.13982065645</v>
       </c>
       <c r="C3">
-        <v>5.84370033476064</v>
+        <v>5.93322455567343</v>
       </c>
       <c r="D3">
-        <v>0.532784308889151</v>
+        <v>0.465192664940686</v>
       </c>
       <c r="E3">
-        <v>1.67726037209228</v>
+        <v>1.58848431825929</v>
       </c>
       <c r="F3">
-        <v>9.65195306873</v>
+        <v>10.1068682646592</v>
       </c>
       <c r="G3">
-        <v>0.49641180029835</v>
+        <v>0.479474569053615</v>
       </c>
       <c r="H3">
-        <v>0.182884941233513</v>
+        <v>0.16336366977054</v>
       </c>
       <c r="I3">
-        <v>0.185514054694753</v>
+        <v>0.233525542226655</v>
       </c>
       <c r="J3">
-        <v>0.541151839499823</v>
+        <v>0.908501083371814</v>
       </c>
       <c r="K3">
-        <v>0.4015671202925</v>
+        <v>0.330939710350803</v>
       </c>
       <c r="L3">
-        <v>0.326647535925599</v>
+        <v>0.450050260865235</v>
       </c>
       <c r="M3">
-        <v>1.12982931393969</v>
+        <v>1.10903121344896</v>
       </c>
       <c r="N3">
-        <v>0.731585279185888</v>
+        <v>0.547480059528962</v>
       </c>
       <c r="O3">
-        <v>249.322956221572</v>
+        <v>250.057100875365</v>
       </c>
       <c r="P3">
-        <v>10.7077622567879</v>
+        <v>10.4167249204277</v>
       </c>
     </row>
     <row r="4">
@@ -550,49 +550,49 @@
         </is>
       </c>
       <c r="B4">
-        <v>1270.67089668933</v>
+        <v>1270.0299312172</v>
       </c>
       <c r="C4">
-        <v>15.1623739767493</v>
+        <v>16.5725577514139</v>
       </c>
       <c r="D4">
-        <v>11.9891329728222</v>
+        <v>11.1018116763272</v>
       </c>
       <c r="E4">
-        <v>17.3651171933868</v>
+        <v>21.6157539453895</v>
       </c>
       <c r="F4">
-        <v>20.7556994966667</v>
+        <v>21.0762153673323</v>
       </c>
       <c r="G4">
-        <v>13.9531447490499</v>
+        <v>14.3827241404247</v>
       </c>
       <c r="H4">
-        <v>8.18838299524197</v>
+        <v>6.27622190516132</v>
       </c>
       <c r="I4">
-        <v>6.96783528534483</v>
+        <v>7.39607496030093</v>
       </c>
       <c r="J4">
-        <v>26.028780260979</v>
+        <v>22.9605302662463</v>
       </c>
       <c r="K4">
-        <v>9.26796696256198</v>
+        <v>13.8667983485207</v>
       </c>
       <c r="L4">
-        <v>92.7044380303486</v>
+        <v>89.6453005757415</v>
       </c>
       <c r="M4">
-        <v>56.822348883009</v>
+        <v>60.7505952133282</v>
       </c>
       <c r="N4">
-        <v>21.9870184580025</v>
+        <v>23.2888172353501</v>
       </c>
       <c r="O4">
-        <v>1930.94275110412</v>
+        <v>1926.85990817774</v>
       </c>
       <c r="P4">
-        <v>36.1800011856351</v>
+        <v>36.1169318801539</v>
       </c>
     </row>
     <row r="5">
@@ -602,49 +602,49 @@
         </is>
       </c>
       <c r="B5">
-        <v>687.25015946441</v>
+        <v>684.321206264305</v>
       </c>
       <c r="C5">
-        <v>59.1193920169989</v>
+        <v>60.7011239459622</v>
       </c>
       <c r="D5">
-        <v>14.904776222328</v>
+        <v>16.5602844728313</v>
       </c>
       <c r="E5">
-        <v>45.0638230118399</v>
+        <v>44.6121560833013</v>
       </c>
       <c r="F5">
-        <v>4.51217689412204</v>
+        <v>5.95437063899369</v>
       </c>
       <c r="G5">
-        <v>14.7894579246355</v>
+        <v>13.6308813801756</v>
       </c>
       <c r="H5">
-        <v>15.591629581667</v>
+        <v>16.0047669532262</v>
       </c>
       <c r="I5">
-        <v>7.49840238964256</v>
+        <v>6.77103546936564</v>
       </c>
       <c r="J5">
-        <v>39.1073759720611</v>
+        <v>36.6247396877504</v>
       </c>
       <c r="K5">
-        <v>26.1747652953947</v>
+        <v>25.8816468790771</v>
       </c>
       <c r="L5">
-        <v>23.3549962188541</v>
+        <v>23.7854879952975</v>
       </c>
       <c r="M5">
-        <v>20.552603737132</v>
+        <v>20.3284459132498</v>
       </c>
       <c r="N5">
-        <v>19.1841566450878</v>
+        <v>19.4943331631262</v>
       </c>
       <c r="O5">
-        <v>827.823373580546</v>
+        <v>834.239538551086</v>
       </c>
       <c r="P5">
-        <v>64.5721176168867</v>
+        <v>61.1178698596417</v>
       </c>
     </row>
     <row r="6">
@@ -654,49 +654,49 @@
         </is>
       </c>
       <c r="B6">
-        <v>8232.892281271241</v>
+        <v>8180.58129993061</v>
       </c>
       <c r="C6">
-        <v>214.493928974541</v>
+        <v>226.021036302625</v>
       </c>
       <c r="D6">
-        <v>246.958026561414</v>
+        <v>243.202889156251</v>
       </c>
       <c r="E6">
-        <v>145.285030028191</v>
+        <v>135.008823461821</v>
       </c>
       <c r="F6">
-        <v>49.6138233646019</v>
+        <v>52.2351540978841</v>
       </c>
       <c r="G6">
-        <v>108.258897788129</v>
+        <v>112.10418623004</v>
       </c>
       <c r="H6">
-        <v>69.1853109948791</v>
+        <v>67.58721866810031</v>
       </c>
       <c r="I6">
-        <v>55.0399928723042</v>
+        <v>58.9928782932245</v>
       </c>
       <c r="J6">
-        <v>195.646619743145</v>
+        <v>197.494545138821</v>
       </c>
       <c r="K6">
-        <v>138.445614457053</v>
+        <v>138.215098993353</v>
       </c>
       <c r="L6">
-        <v>583.244798520158</v>
+        <v>592.309740581594</v>
       </c>
       <c r="M6">
-        <v>321.024768538684</v>
+        <v>309.145083396598</v>
       </c>
       <c r="N6">
-        <v>303.848098744927</v>
+        <v>312.718852331678</v>
       </c>
       <c r="O6">
-        <v>12463.5613454583</v>
+        <v>12536.1790878006</v>
       </c>
       <c r="P6">
-        <v>323.342578320321</v>
+        <v>316.14145987825</v>
       </c>
     </row>
     <row r="7">
@@ -706,49 +706,49 @@
         </is>
       </c>
       <c r="B7">
-        <v>825.7879441115369</v>
+        <v>827.507782466098</v>
       </c>
       <c r="C7">
-        <v>33.9039818193791</v>
+        <v>36.8803412713503</v>
       </c>
       <c r="D7">
-        <v>5.87593414137867</v>
+        <v>6.35797216532079</v>
       </c>
       <c r="E7">
-        <v>19.7719575551981</v>
+        <v>18.3213172652257</v>
       </c>
       <c r="F7">
-        <v>18.6855187512718</v>
+        <v>21.8615979506178</v>
       </c>
       <c r="G7">
-        <v>10.1491164618991</v>
+        <v>10.1141884603223</v>
       </c>
       <c r="H7">
-        <v>9.442473396592479</v>
+        <v>8.114004771371761</v>
       </c>
       <c r="I7">
-        <v>11.5870572800848</v>
+        <v>10.9842281216013</v>
       </c>
       <c r="J7">
-        <v>18.0240144703635</v>
+        <v>19.5383027764453</v>
       </c>
       <c r="K7">
-        <v>17.2674845978249</v>
+        <v>20.9789828296881</v>
       </c>
       <c r="L7">
-        <v>68.27284611371731</v>
+        <v>73.39344844072861</v>
       </c>
       <c r="M7">
-        <v>20.8757030116514</v>
+        <v>19.3812768646707</v>
       </c>
       <c r="N7">
-        <v>28.1445470951437</v>
+        <v>29.0561443129126</v>
       </c>
       <c r="O7">
-        <v>1895.02647963785</v>
+        <v>1891.85264894205</v>
       </c>
       <c r="P7">
-        <v>39.8181376986202</v>
+        <v>43.5251795552418</v>
       </c>
     </row>
     <row r="8">
@@ -758,49 +758,49 @@
         </is>
       </c>
       <c r="B8">
-        <v>728.975428976144</v>
+        <v>725.82448550622</v>
       </c>
       <c r="C8">
-        <v>16.5858890469144</v>
+        <v>13.045287811315</v>
       </c>
       <c r="D8">
-        <v>9.3143155642025</v>
+        <v>8.795138314000949</v>
       </c>
       <c r="E8">
-        <v>23.5987317308589</v>
+        <v>23.0422033518841</v>
       </c>
       <c r="F8">
-        <v>0.944301387837727</v>
+        <v>0.9502356434435481</v>
       </c>
       <c r="G8">
-        <v>29.7623830229073</v>
+        <v>27.6397749163253</v>
       </c>
       <c r="H8">
-        <v>12.2101443260948</v>
+        <v>11.7631671234572</v>
       </c>
       <c r="I8">
-        <v>2.92599322503371</v>
+        <v>3.16623457036267</v>
       </c>
       <c r="J8">
-        <v>52.4038373563136</v>
+        <v>50.0810363525876</v>
       </c>
       <c r="K8">
-        <v>36.6602005077404</v>
+        <v>35.3251571772438</v>
       </c>
       <c r="L8">
-        <v>41.6288562191887</v>
+        <v>39.7978433676137</v>
       </c>
       <c r="M8">
-        <v>66.0074474003907</v>
+        <v>64.194025196173</v>
       </c>
       <c r="N8">
-        <v>30.5108293012019</v>
+        <v>31.1942649949048</v>
       </c>
       <c r="O8">
-        <v>1351.8426376654</v>
+        <v>1369.39289312655</v>
       </c>
       <c r="P8">
-        <v>7.46673525326738</v>
+        <v>7.6748594833174</v>
       </c>
     </row>
     <row r="9">
@@ -810,49 +810,49 @@
         </is>
       </c>
       <c r="B9">
-        <v>170.215458422665</v>
+        <v>168.076966978008</v>
       </c>
       <c r="C9">
-        <v>10.0468652364138</v>
+        <v>9.36316598759586</v>
       </c>
       <c r="D9">
-        <v>2.02897377985051</v>
+        <v>2.06681665294493</v>
       </c>
       <c r="E9">
-        <v>5.28643761112095</v>
+        <v>4.90027695703681</v>
       </c>
       <c r="F9">
-        <v>2.37088233168719</v>
+        <v>2.34309123893235</v>
       </c>
       <c r="G9">
-        <v>22.8367023051447</v>
+        <v>22.5041199675104</v>
       </c>
       <c r="H9">
-        <v>4.26282014598123</v>
+        <v>3.77829176627828</v>
       </c>
       <c r="I9">
-        <v>0.281512270681961</v>
+        <v>0.682018248730845</v>
       </c>
       <c r="J9">
-        <v>3.08258588222266</v>
+        <v>3.50930497284795</v>
       </c>
       <c r="K9">
-        <v>3.66884021751272</v>
+        <v>3.52046588950351</v>
       </c>
       <c r="L9">
-        <v>2.001033817619</v>
+        <v>1.99900134608019</v>
       </c>
       <c r="M9">
-        <v>7.97241312033409</v>
+        <v>7.45478995312183</v>
       </c>
       <c r="N9">
-        <v>4.53573231878199</v>
+        <v>4.5903437215371</v>
       </c>
       <c r="O9">
-        <v>307.183378108415</v>
+        <v>310.045584055496</v>
       </c>
       <c r="P9">
-        <v>4.97966343686703</v>
+        <v>4.96099009126937</v>
       </c>
     </row>
     <row r="10">
@@ -862,49 +862,49 @@
         </is>
       </c>
       <c r="B10">
-        <v>4261.93801809132</v>
+        <v>4247.01224733223</v>
       </c>
       <c r="C10">
-        <v>54.3653476820336</v>
+        <v>51.9189114423029</v>
       </c>
       <c r="D10">
-        <v>44.2096717488047</v>
+        <v>44.9749274584861</v>
       </c>
       <c r="E10">
-        <v>66.290476818692</v>
+        <v>61.1163055607174</v>
       </c>
       <c r="F10">
-        <v>11.9688221140249</v>
+        <v>12.376635699315</v>
       </c>
       <c r="G10">
-        <v>47.2010744156521</v>
+        <v>47.1561051150154</v>
       </c>
       <c r="H10">
-        <v>21.2747578751097</v>
+        <v>20.6366030988897</v>
       </c>
       <c r="I10">
-        <v>29.1825996772191</v>
+        <v>29.5552299488828</v>
       </c>
       <c r="J10">
-        <v>47.9641509293239</v>
+        <v>49.1327351469161</v>
       </c>
       <c r="K10">
-        <v>48.0134881982321</v>
+        <v>46.1581656339009</v>
       </c>
       <c r="L10">
-        <v>117.009040075187</v>
+        <v>119.246312724892</v>
       </c>
       <c r="M10">
-        <v>90.75917372655751</v>
+        <v>92.267547909103</v>
       </c>
       <c r="N10">
-        <v>107.003843243042</v>
+        <v>107.934834921247</v>
       </c>
       <c r="O10">
-        <v>6466.94024178293</v>
+        <v>6486.46873200435</v>
       </c>
       <c r="P10">
-        <v>102.010465756654</v>
+        <v>94.14922009304421</v>
       </c>
     </row>
     <row r="11">
@@ -914,49 +914,49 @@
         </is>
       </c>
       <c r="B11">
-        <v>1786.44386673282</v>
+        <v>1775.65065432996</v>
       </c>
       <c r="C11">
-        <v>75.19734747968521</v>
+        <v>75.99455717885439</v>
       </c>
       <c r="D11">
-        <v>164.98304509186</v>
+        <v>162.464172478673</v>
       </c>
       <c r="E11">
-        <v>110.445592208079</v>
+        <v>103.435282077454</v>
       </c>
       <c r="F11">
-        <v>13.3020597424875</v>
+        <v>12.8540001728789</v>
       </c>
       <c r="G11">
-        <v>47.7107908711939</v>
+        <v>44.5863949980092</v>
       </c>
       <c r="H11">
-        <v>26.4193049630904</v>
+        <v>32.2797898103184</v>
       </c>
       <c r="I11">
-        <v>24.9867898050001</v>
+        <v>24.7459036380201</v>
       </c>
       <c r="J11">
-        <v>50.2676238852541</v>
+        <v>52.4821322060096</v>
       </c>
       <c r="K11">
-        <v>53.4375009592185</v>
+        <v>53.6028549666202</v>
       </c>
       <c r="L11">
-        <v>67.67502020982781</v>
+        <v>70.6679819076315</v>
       </c>
       <c r="M11">
-        <v>70.5773098622238</v>
+        <v>75.8367011096253</v>
       </c>
       <c r="N11">
-        <v>59.4669945000274</v>
+        <v>58.9642840610286</v>
       </c>
       <c r="O11">
-        <v>3066.06232890034</v>
+        <v>3069.44433803004</v>
       </c>
       <c r="P11">
-        <v>58.3856895226025</v>
+        <v>54.293953164181</v>
       </c>
     </row>
     <row r="12">
@@ -966,49 +966,49 @@
         </is>
       </c>
       <c r="B12">
-        <v>293.898518031205</v>
+        <v>290.01577744885</v>
       </c>
       <c r="C12">
-        <v>8.243548149700841</v>
+        <v>7.50266699596209</v>
       </c>
       <c r="D12">
-        <v>4.9511105629907</v>
+        <v>4.74590898940546</v>
       </c>
       <c r="E12">
-        <v>1.35025506932098</v>
+        <v>2.5631536257844</v>
       </c>
       <c r="F12">
-        <v>0.7203029963900101</v>
+        <v>0.667711605295335</v>
       </c>
       <c r="G12">
-        <v>1.16756830833161</v>
+        <v>1.04704191783243</v>
       </c>
       <c r="H12">
-        <v>0.9298496055566951</v>
+        <v>0.709561319468104</v>
       </c>
       <c r="I12">
-        <v>1.45202371101633</v>
+        <v>1.31144573207453</v>
       </c>
       <c r="J12">
-        <v>0.822372464066726</v>
+        <v>0.996819184412412</v>
       </c>
       <c r="K12">
-        <v>0.635673116210003</v>
+        <v>0.822923251893628</v>
       </c>
       <c r="L12">
-        <v>1.96716634747312</v>
+        <v>1.91893121096981</v>
       </c>
       <c r="M12">
-        <v>3.70688386938709</v>
+        <v>3.74388966137734</v>
       </c>
       <c r="N12">
-        <v>2.77272261386823</v>
+        <v>3.25864856466091</v>
       </c>
       <c r="O12">
-        <v>510.58830439622</v>
+        <v>511.773522861485</v>
       </c>
       <c r="P12">
-        <v>20.399954668965</v>
+        <v>18.5095317359322</v>
       </c>
     </row>
     <row r="13">
@@ -1018,49 +1018,49 @@
         </is>
       </c>
       <c r="B13">
-        <v>280.19895813844</v>
+        <v>279.570245472812</v>
       </c>
       <c r="C13">
-        <v>26.6074252997116</v>
+        <v>26.4132144918427</v>
       </c>
       <c r="D13">
-        <v>2.47475253553602</v>
+        <v>2.11914084329854</v>
       </c>
       <c r="E13">
-        <v>20.4860825714956</v>
+        <v>18.9164006850812</v>
       </c>
       <c r="F13">
-        <v>6.53958762401606</v>
+        <v>5.59410636599248</v>
       </c>
       <c r="G13">
-        <v>5.32272344029195</v>
+        <v>5.67304104020605</v>
       </c>
       <c r="H13">
-        <v>2.27741464948492</v>
+        <v>2.12610525693736</v>
       </c>
       <c r="I13">
-        <v>1.86903099020986</v>
+        <v>2.12481324134198</v>
       </c>
       <c r="J13">
-        <v>4.97448619541873</v>
+        <v>4.97420107773667</v>
       </c>
       <c r="K13">
-        <v>2.95353009081102</v>
+        <v>2.95228575952579</v>
       </c>
       <c r="L13">
-        <v>21.1829026760906</v>
+        <v>22.7636983314187</v>
       </c>
       <c r="M13">
-        <v>4.88119655566553</v>
+        <v>4.5459166421022</v>
       </c>
       <c r="N13">
-        <v>7.27128597698296</v>
+        <v>7.13495957134708</v>
       </c>
       <c r="O13">
-        <v>462.372722075598</v>
+        <v>463.812475658323</v>
       </c>
       <c r="P13">
-        <v>42.3427940116002</v>
+        <v>42.8829915304118</v>
       </c>
     </row>
     <row r="14">
@@ -1070,49 +1070,49 @@
         </is>
       </c>
       <c r="B14">
-        <v>2685.94820263025</v>
+        <v>2674.67041221932</v>
       </c>
       <c r="C14">
-        <v>114.826256380769</v>
+        <v>112.25845241948</v>
       </c>
       <c r="D14">
-        <v>20.5048258399779</v>
+        <v>18.7421963458165</v>
       </c>
       <c r="E14">
-        <v>97.4564215711507</v>
+        <v>96.6663828654266</v>
       </c>
       <c r="F14">
-        <v>25.3537323210084</v>
+        <v>27.3293323880705</v>
       </c>
       <c r="G14">
-        <v>99.6915524478008</v>
+        <v>96.4354357077422</v>
       </c>
       <c r="H14">
-        <v>64.8498081155292</v>
+        <v>66.8895346612815</v>
       </c>
       <c r="I14">
-        <v>32.0190545531076</v>
+        <v>32.2328129267682</v>
       </c>
       <c r="J14">
-        <v>186.56507540075</v>
+        <v>186.333611126867</v>
       </c>
       <c r="K14">
-        <v>181.383652675082</v>
+        <v>185.343836838617</v>
       </c>
       <c r="L14">
-        <v>172.392554929164</v>
+        <v>172.513452603414</v>
       </c>
       <c r="M14">
-        <v>100.500818683141</v>
+        <v>103.305989564246</v>
       </c>
       <c r="N14">
-        <v>103.009334712207</v>
+        <v>109.96666181027</v>
       </c>
       <c r="O14">
-        <v>4791.53838045126</v>
+        <v>4797.67540343431</v>
       </c>
       <c r="P14">
-        <v>84.47770459145011</v>
+        <v>85.3333388854291</v>
       </c>
     </row>
     <row r="15">
@@ -1122,49 +1122,49 @@
         </is>
       </c>
       <c r="B15">
-        <v>1298.89712551691</v>
+        <v>1283.18538417007</v>
       </c>
       <c r="C15">
-        <v>42.6477853907428</v>
+        <v>38.3404509569308</v>
       </c>
       <c r="D15">
-        <v>15.2714163434774</v>
+        <v>15.7225984493849</v>
       </c>
       <c r="E15">
-        <v>67.75959999207539</v>
+        <v>67.9377693931132</v>
       </c>
       <c r="F15">
-        <v>13.3585056344745</v>
+        <v>12.5481245237197</v>
       </c>
       <c r="G15">
-        <v>47.3609768903868</v>
+        <v>47.6810000883377</v>
       </c>
       <c r="H15">
-        <v>52.3488624316659</v>
+        <v>53.5148624276557</v>
       </c>
       <c r="I15">
-        <v>33.0650861540076</v>
+        <v>30.8895076977699</v>
       </c>
       <c r="J15">
-        <v>177.830627087415</v>
+        <v>174.228119883896</v>
       </c>
       <c r="K15">
-        <v>89.68634772104031</v>
+        <v>93.7939005628178</v>
       </c>
       <c r="L15">
-        <v>83.86504250720751</v>
+        <v>75.54191973360329</v>
       </c>
       <c r="M15">
-        <v>187.31955532459</v>
+        <v>185.831631267017</v>
       </c>
       <c r="N15">
-        <v>70.9075376341622</v>
+        <v>80.3532005541135</v>
       </c>
       <c r="O15">
-        <v>2076.37048450973</v>
+        <v>2079.64940757015</v>
       </c>
       <c r="P15">
-        <v>38.5766102652578</v>
+        <v>44.2306992129769</v>
       </c>
     </row>
     <row r="16">
@@ -1174,49 +1174,49 @@
         </is>
       </c>
       <c r="B16">
-        <v>534.497201078873</v>
+        <v>532.650307134125</v>
       </c>
       <c r="C16">
-        <v>60.6773452999063</v>
+        <v>65.529432065739</v>
       </c>
       <c r="D16">
-        <v>10.9382309349508</v>
+        <v>11.277008985418</v>
       </c>
       <c r="E16">
-        <v>25.8928939480104</v>
+        <v>21.77183171631</v>
       </c>
       <c r="F16">
-        <v>4.00502017666425</v>
+        <v>4.03774041708282</v>
       </c>
       <c r="G16">
-        <v>13.841937975177</v>
+        <v>12.7966339871533</v>
       </c>
       <c r="H16">
-        <v>14.9254448806247</v>
+        <v>17.3898679319101</v>
       </c>
       <c r="I16">
-        <v>14.8260023763905</v>
+        <v>12.6843219596077</v>
       </c>
       <c r="J16">
-        <v>48.1118499969667</v>
+        <v>50.7500046436628</v>
       </c>
       <c r="K16">
-        <v>49.6377603292954</v>
+        <v>48.9745822618077</v>
       </c>
       <c r="L16">
-        <v>38.5470764804919</v>
+        <v>40.8463720051137</v>
       </c>
       <c r="M16">
-        <v>23.5437084187309</v>
+        <v>24.2253761450492</v>
       </c>
       <c r="N16">
-        <v>23.3705194515426</v>
+        <v>24.3546264813168</v>
       </c>
       <c r="O16">
-        <v>1116.19282014054</v>
+        <v>1112.93134737563</v>
       </c>
       <c r="P16">
-        <v>84.27738126017771</v>
+        <v>84.60494637368061</v>
       </c>
     </row>
     <row r="17">
@@ -1226,49 +1226,49 @@
         </is>
       </c>
       <c r="B17">
-        <v>523.9677234865291</v>
+        <v>527.985799706767</v>
       </c>
       <c r="C17">
-        <v>31.6078104836265</v>
+        <v>32.7162529751404</v>
       </c>
       <c r="D17">
-        <v>6.44760958203473</v>
+        <v>6.46080743344533</v>
       </c>
       <c r="E17">
-        <v>15.2421712026926</v>
+        <v>16.6856804913797</v>
       </c>
       <c r="F17">
-        <v>15.070586464942</v>
+        <v>15.8700208020937</v>
       </c>
       <c r="G17">
-        <v>11.9034617764983</v>
+        <v>13.5720929329116</v>
       </c>
       <c r="H17">
-        <v>15.2933140829635</v>
+        <v>15.2125953362325</v>
       </c>
       <c r="I17">
-        <v>8.09642484671244</v>
+        <v>6.72628819144011</v>
       </c>
       <c r="J17">
-        <v>21.3341280234123</v>
+        <v>22.3507499653717</v>
       </c>
       <c r="K17">
-        <v>27.3375583110808</v>
+        <v>25.8996013051531</v>
       </c>
       <c r="L17">
-        <v>16.5827479895797</v>
+        <v>18.810595380907</v>
       </c>
       <c r="M17">
-        <v>74.96759397989371</v>
+        <v>80.1030380307501</v>
       </c>
       <c r="N17">
-        <v>17.1003450757004</v>
+        <v>15.6292961282159</v>
       </c>
       <c r="O17">
-        <v>1023.69026784869</v>
+        <v>1007.38774074012</v>
       </c>
       <c r="P17">
-        <v>73.447884377626</v>
+        <v>71.97833817211151</v>
       </c>
     </row>
     <row r="18">
@@ -1278,49 +1278,49 @@
         </is>
       </c>
       <c r="B18">
-        <v>1046.90985586985</v>
+        <v>1050.0165630308</v>
       </c>
       <c r="C18">
-        <v>34.9148626931801</v>
+        <v>31.5279628539996</v>
       </c>
       <c r="D18">
-        <v>30.8559831873363</v>
+        <v>28.9226206607104</v>
       </c>
       <c r="E18">
-        <v>42.2597339784343</v>
+        <v>41.2881898675767</v>
       </c>
       <c r="F18">
-        <v>35.5687835241003</v>
+        <v>34.7258149545363</v>
       </c>
       <c r="G18">
-        <v>29.0926859055207</v>
+        <v>28.7029749361716</v>
       </c>
       <c r="H18">
-        <v>24.6241004614492</v>
+        <v>25.2723284921006</v>
       </c>
       <c r="I18">
-        <v>8.99702151646361</v>
+        <v>11.9579405738242</v>
       </c>
       <c r="J18">
-        <v>45.5368778916199</v>
+        <v>46.1004859018471</v>
       </c>
       <c r="K18">
-        <v>39.9570910203189</v>
+        <v>40.800079824706</v>
       </c>
       <c r="L18">
-        <v>48.7858612671896</v>
+        <v>43.8056233429995</v>
       </c>
       <c r="M18">
-        <v>65.5967742773497</v>
+        <v>65.6516084871913</v>
       </c>
       <c r="N18">
-        <v>29.1529256621694</v>
+        <v>27.9657142298688</v>
       </c>
       <c r="O18">
-        <v>1369.58836746886</v>
+        <v>1375.2617857225</v>
       </c>
       <c r="P18">
-        <v>43.2015391353503</v>
+        <v>40.7325136979494</v>
       </c>
     </row>
     <row r="19">
@@ -1330,49 +1330,49 @@
         </is>
       </c>
       <c r="B19">
-        <v>1169.84263248826</v>
+        <v>1182.62452100269</v>
       </c>
       <c r="C19">
-        <v>24.9744077020973</v>
+        <v>23.1994517142424</v>
       </c>
       <c r="D19">
-        <v>18.1765021441543</v>
+        <v>15.3738932396323</v>
       </c>
       <c r="E19">
-        <v>39.9592053458883</v>
+        <v>39.4282593653923</v>
       </c>
       <c r="F19">
-        <v>71.5988245375582</v>
+        <v>72.4370890081664</v>
       </c>
       <c r="G19">
-        <v>43.7801778395548</v>
+        <v>45.5863230874482</v>
       </c>
       <c r="H19">
-        <v>6.01946960267989</v>
+        <v>6.88043947943602</v>
       </c>
       <c r="I19">
-        <v>7.62535084935924</v>
+        <v>7.51411183803995</v>
       </c>
       <c r="J19">
-        <v>20.0429550791438</v>
+        <v>17.9785512561699</v>
       </c>
       <c r="K19">
-        <v>12.7177976615325</v>
+        <v>14.3752530249318</v>
       </c>
       <c r="L19">
-        <v>12.3119784690176</v>
+        <v>10.503556545512</v>
       </c>
       <c r="M19">
-        <v>27.5400091411257</v>
+        <v>32.5059139672898</v>
       </c>
       <c r="N19">
-        <v>13.0955583296096</v>
+        <v>12.2973050935925</v>
       </c>
       <c r="O19">
-        <v>1571.13499494794</v>
+        <v>1562.25549152341</v>
       </c>
       <c r="P19">
-        <v>40.5124765910107</v>
+        <v>40.2543151946458</v>
       </c>
     </row>
     <row r="20">
@@ -1382,49 +1382,49 @@
         </is>
       </c>
       <c r="B20">
-        <v>293.462226718812</v>
+        <v>290.372216376173</v>
       </c>
       <c r="C20">
-        <v>8.136679022963319</v>
+        <v>7.77353841812932</v>
       </c>
       <c r="D20">
-        <v>16.900823338119</v>
+        <v>18.2185590551544</v>
       </c>
       <c r="E20">
-        <v>34.1762832231737</v>
+        <v>34.2369115160832</v>
       </c>
       <c r="F20">
-        <v>0.262736919583967</v>
+        <v>0.263208742621594</v>
       </c>
       <c r="G20">
-        <v>1.86580323374386</v>
+        <v>1.71712184102401</v>
       </c>
       <c r="H20">
-        <v>3.26320887260769</v>
+        <v>3.25832879562404</v>
       </c>
       <c r="I20">
-        <v>1.16652059529631</v>
+        <v>1.22596158637976</v>
       </c>
       <c r="J20">
-        <v>6.76899755831113</v>
+        <v>7.78140947962672</v>
       </c>
       <c r="K20">
-        <v>5.43412612273316</v>
+        <v>5.42819884800172</v>
       </c>
       <c r="L20">
-        <v>10.5816586169763</v>
+        <v>9.232300658611541</v>
       </c>
       <c r="M20">
-        <v>17.8295781656015</v>
+        <v>17.0902925193104</v>
       </c>
       <c r="N20">
-        <v>5.83772438809814</v>
+        <v>5.77512776688749</v>
       </c>
       <c r="O20">
-        <v>490.126263035197</v>
+        <v>492.797688231353</v>
       </c>
       <c r="P20">
-        <v>24.3481526101184</v>
+        <v>24.4687798919781</v>
       </c>
     </row>
     <row r="21">
@@ -1434,49 +1434,49 @@
         </is>
       </c>
       <c r="B21">
-        <v>1077.43121718162</v>
+        <v>1069.4705960726</v>
       </c>
       <c r="C21">
-        <v>30.9005883930164</v>
+        <v>26.9859812029134</v>
       </c>
       <c r="D21">
-        <v>13.9377192521587</v>
+        <v>15.1215551969442</v>
       </c>
       <c r="E21">
-        <v>33.9219116552185</v>
+        <v>33.3761609226067</v>
       </c>
       <c r="F21">
-        <v>5.08979131604493</v>
+        <v>4.74684894081636</v>
       </c>
       <c r="G21">
-        <v>13.7503524687969</v>
+        <v>18.596654982032</v>
       </c>
       <c r="H21">
-        <v>21.2858683879468</v>
+        <v>17.8342769480457</v>
       </c>
       <c r="I21">
-        <v>9.455918664646511</v>
+        <v>6.47747115155455</v>
       </c>
       <c r="J21">
-        <v>16.3584745478528</v>
+        <v>19.6641942758974</v>
       </c>
       <c r="K21">
-        <v>17.6468651105093</v>
+        <v>21.6885207166019</v>
       </c>
       <c r="L21">
-        <v>39.1128742458654</v>
+        <v>34.5154945870962</v>
       </c>
       <c r="M21">
-        <v>38.1832719064899</v>
+        <v>39.8162306766658</v>
       </c>
       <c r="N21">
-        <v>19.4497638815289</v>
+        <v>16.6702548685866</v>
       </c>
       <c r="O21">
-        <v>2366.48313856001</v>
+        <v>2381.27963246908</v>
       </c>
       <c r="P21">
-        <v>19.5951567901529</v>
+        <v>19.9326403241562</v>
       </c>
     </row>
     <row r="22">
@@ -1486,49 +1486,49 @@
         </is>
       </c>
       <c r="B22">
-        <v>1339.50945838194</v>
+        <v>1327.62299552956</v>
       </c>
       <c r="C22">
-        <v>25.8848726950015</v>
+        <v>24.0742650768671</v>
       </c>
       <c r="D22">
-        <v>37.5185377346484</v>
+        <v>36.5969490062855</v>
       </c>
       <c r="E22">
-        <v>38.3763942206816</v>
+        <v>39.3192683199679</v>
       </c>
       <c r="F22">
-        <v>2.78280244358686</v>
+        <v>2.89086647628153</v>
       </c>
       <c r="G22">
-        <v>27.0865203174987</v>
+        <v>26.4489974301897</v>
       </c>
       <c r="H22">
-        <v>29.0193001558003</v>
+        <v>28.7074338415236</v>
       </c>
       <c r="I22">
-        <v>11.1006072204702</v>
+        <v>12.0512635792135</v>
       </c>
       <c r="J22">
-        <v>60.6489028790574</v>
+        <v>59.916992700201</v>
       </c>
       <c r="K22">
-        <v>45.734587033864</v>
+        <v>45.4328206297474</v>
       </c>
       <c r="L22">
-        <v>133.787231584676</v>
+        <v>125.012269223179</v>
       </c>
       <c r="M22">
-        <v>24.3231049624807</v>
+        <v>23.2081417337602</v>
       </c>
       <c r="N22">
-        <v>81.6535592598425</v>
+        <v>86.22555629395529</v>
       </c>
       <c r="O22">
-        <v>2683.67668177074</v>
+        <v>2712.87568201259</v>
       </c>
       <c r="P22">
-        <v>19.0193885455058</v>
+        <v>18.9726144551501</v>
       </c>
     </row>
     <row r="23">
@@ -1538,49 +1538,49 @@
         </is>
       </c>
       <c r="B23">
-        <v>2259.4182273964</v>
+        <v>2237.24925665277</v>
       </c>
       <c r="C23">
-        <v>50.4928841279873</v>
+        <v>48.0057562139088</v>
       </c>
       <c r="D23">
-        <v>19.1705032961356</v>
+        <v>18.0687563656199</v>
       </c>
       <c r="E23">
-        <v>65.3386562403839</v>
+        <v>65.7179734221221</v>
       </c>
       <c r="F23">
-        <v>5.61844202833703</v>
+        <v>7.76412143659329</v>
       </c>
       <c r="G23">
-        <v>64.235653828419</v>
+        <v>62.7417299375564</v>
       </c>
       <c r="H23">
-        <v>65.44181220038701</v>
+        <v>64.5625253238551</v>
       </c>
       <c r="I23">
-        <v>22.4878037213956</v>
+        <v>23.9321212691051</v>
       </c>
       <c r="J23">
-        <v>178.171410036847</v>
+        <v>175.021685797056</v>
       </c>
       <c r="K23">
-        <v>132.560804201498</v>
+        <v>140.95006379164</v>
       </c>
       <c r="L23">
-        <v>56.7834088177219</v>
+        <v>57.6844774418885</v>
       </c>
       <c r="M23">
-        <v>532.296328122667</v>
+        <v>532.21408760421</v>
       </c>
       <c r="N23">
-        <v>94.6298170399366</v>
+        <v>91.9845047712969</v>
       </c>
       <c r="O23">
-        <v>3393.20684232216</v>
+        <v>3422.03453745256</v>
       </c>
       <c r="P23">
-        <v>70.8389875777158</v>
+        <v>70.11384841927379</v>
       </c>
     </row>
     <row r="24">
@@ -1590,49 +1590,49 @@
         </is>
       </c>
       <c r="B24">
-        <v>865.2024700819441</v>
+        <v>842.796356524924</v>
       </c>
       <c r="C24">
-        <v>71.8871030916098</v>
+        <v>69.80455251447739</v>
       </c>
       <c r="D24">
-        <v>8.20575131611972</v>
+        <v>9.233668568180899</v>
       </c>
       <c r="E24">
-        <v>67.0449432139001</v>
+        <v>61.8610161047064</v>
       </c>
       <c r="F24">
-        <v>18.3692866559402</v>
+        <v>17.5837410080113</v>
       </c>
       <c r="G24">
-        <v>17.392340433467</v>
+        <v>18.7340850014634</v>
       </c>
       <c r="H24">
-        <v>28.9473462299088</v>
+        <v>30.4305732600902</v>
       </c>
       <c r="I24">
-        <v>10.1293207779831</v>
+        <v>11.8542299750312</v>
       </c>
       <c r="J24">
-        <v>58.6710696494283</v>
+        <v>59.3155249288565</v>
       </c>
       <c r="K24">
-        <v>62.1990680083238</v>
+        <v>64.51098366966291</v>
       </c>
       <c r="L24">
-        <v>77.6706726182008</v>
+        <v>78.2366466589957</v>
       </c>
       <c r="M24">
-        <v>22.1242155414529</v>
+        <v>22.8940765365901</v>
       </c>
       <c r="N24">
-        <v>63.5015296511757</v>
+        <v>65.1987582029855</v>
       </c>
       <c r="O24">
-        <v>1964.78982370835</v>
+        <v>1978.34963137788</v>
       </c>
       <c r="P24">
-        <v>120.954113748132</v>
+        <v>125.841533271921</v>
       </c>
     </row>
     <row r="25">
@@ -1642,49 +1642,49 @@
         </is>
       </c>
       <c r="B25">
-        <v>735.618794714958</v>
+        <v>742.78519377955</v>
       </c>
       <c r="C25">
-        <v>35.2100873418215</v>
+        <v>35.5422583479333</v>
       </c>
       <c r="D25">
-        <v>28.6337095956052</v>
+        <v>26.7051826627291</v>
       </c>
       <c r="E25">
-        <v>34.4971917647894</v>
+        <v>34.9480514644058</v>
       </c>
       <c r="F25">
-        <v>17.9048983733968</v>
+        <v>16.5719782071363</v>
       </c>
       <c r="G25">
-        <v>12.4161708168332</v>
+        <v>11.239505382851</v>
       </c>
       <c r="H25">
-        <v>16.7514794519602</v>
+        <v>16.3706757696871</v>
       </c>
       <c r="I25">
-        <v>4.9788414886734</v>
+        <v>4.96403898259472</v>
       </c>
       <c r="J25">
-        <v>21.9052002225357</v>
+        <v>21.6206164454553</v>
       </c>
       <c r="K25">
-        <v>18.7810337257313</v>
+        <v>18.3562280955871</v>
       </c>
       <c r="L25">
-        <v>34.1512811485723</v>
+        <v>33.8162412174103</v>
       </c>
       <c r="M25">
-        <v>26.175698469465</v>
+        <v>27.166164726166</v>
       </c>
       <c r="N25">
-        <v>45.9962122237637</v>
+        <v>47.573600205351</v>
       </c>
       <c r="O25">
-        <v>870.789994176729</v>
+        <v>868.1345459641281</v>
       </c>
       <c r="P25">
-        <v>39.5232954219409</v>
+        <v>40.7076741781858</v>
       </c>
     </row>
     <row r="26">
@@ -1694,49 +1694,49 @@
         </is>
       </c>
       <c r="B26">
-        <v>1216.78329997945</v>
+        <v>1219.08443094606</v>
       </c>
       <c r="C26">
-        <v>61.1430979027072</v>
+        <v>58.7609157124583</v>
       </c>
       <c r="D26">
-        <v>17.8015093079094</v>
+        <v>17.4325328661624</v>
       </c>
       <c r="E26">
-        <v>50.710042657853</v>
+        <v>52.6522077567204</v>
       </c>
       <c r="F26">
-        <v>4.19368549706325</v>
+        <v>3.75041692666702</v>
       </c>
       <c r="G26">
-        <v>35.9260730220993</v>
+        <v>38.9617907698757</v>
       </c>
       <c r="H26">
-        <v>25.5938571118155</v>
+        <v>23.0660803251662</v>
       </c>
       <c r="I26">
-        <v>17.8978653829385</v>
+        <v>15.7648625263643</v>
       </c>
       <c r="J26">
-        <v>63.1871596369294</v>
+        <v>59.2549000039295</v>
       </c>
       <c r="K26">
-        <v>51.9145264204457</v>
+        <v>51.4579779100724</v>
       </c>
       <c r="L26">
-        <v>42.8996152171226</v>
+        <v>53.6992419317954</v>
       </c>
       <c r="M26">
-        <v>88.9123262482079</v>
+        <v>88.6635145067455</v>
       </c>
       <c r="N26">
-        <v>41.4211467801769</v>
+        <v>39.8236408485684</v>
       </c>
       <c r="O26">
-        <v>2151.2842062865</v>
+        <v>2148.98490791069</v>
       </c>
       <c r="P26">
-        <v>73.2335653469229</v>
+        <v>76.276919730773</v>
       </c>
     </row>
     <row r="27">
@@ -1746,49 +1746,49 @@
         </is>
       </c>
       <c r="B27">
-        <v>199.076625406625</v>
+        <v>200.744600384505</v>
       </c>
       <c r="C27">
-        <v>3.13701937958451</v>
+        <v>2.90105441120513</v>
       </c>
       <c r="D27">
-        <v>1.53794593580651</v>
+        <v>1.25797615302641</v>
       </c>
       <c r="E27">
-        <v>11.490743191972</v>
+        <v>10.9809619679777</v>
       </c>
       <c r="F27">
-        <v>8.723973979424679</v>
+        <v>8.395725140833489</v>
       </c>
       <c r="G27">
-        <v>0.7684336286479601</v>
+        <v>0.772272084073371</v>
       </c>
       <c r="H27">
-        <v>0.341393470165284</v>
+        <v>0.519160826518464</v>
       </c>
       <c r="I27">
-        <v>1.57305522183479</v>
+        <v>1.32693871394504</v>
       </c>
       <c r="J27">
-        <v>4.45892372388156</v>
+        <v>4.6131384895411</v>
       </c>
       <c r="K27">
-        <v>1.6884546567951</v>
+        <v>1.67183680882689</v>
       </c>
       <c r="L27">
-        <v>1.72485299543346</v>
+        <v>2.04847923182377</v>
       </c>
       <c r="M27">
-        <v>1.1552172356787</v>
+        <v>1.06557326472868</v>
       </c>
       <c r="N27">
-        <v>4.91467001280897</v>
+        <v>4.5777710252635</v>
       </c>
       <c r="O27">
-        <v>355.52241191255</v>
+        <v>351.67174379185</v>
       </c>
       <c r="P27">
-        <v>46.5993348823864</v>
+        <v>45.6170748596869</v>
       </c>
     </row>
     <row r="28">
@@ -1798,49 +1798,49 @@
         </is>
       </c>
       <c r="B28">
-        <v>308.062891171096</v>
+        <v>305.662838983048</v>
       </c>
       <c r="C28">
-        <v>33.6708613087766</v>
+        <v>33.9843362381911</v>
       </c>
       <c r="D28">
-        <v>1.98354225040809</v>
+        <v>1.79402013645833</v>
       </c>
       <c r="E28">
-        <v>8.46685480342383</v>
+        <v>7.55203394506621</v>
       </c>
       <c r="F28">
-        <v>1.93947865946416</v>
+        <v>2.10668470894927</v>
       </c>
       <c r="G28">
-        <v>5.30727609246022</v>
+        <v>4.9075560951749</v>
       </c>
       <c r="H28">
-        <v>7.55830522203061</v>
+        <v>7.61485547387417</v>
       </c>
       <c r="I28">
-        <v>4.8628229756396</v>
+        <v>4.78549771839121</v>
       </c>
       <c r="J28">
-        <v>17.8240990062558</v>
+        <v>17.7214099593195</v>
       </c>
       <c r="K28">
-        <v>16.540223475719</v>
+        <v>17.6473216547729</v>
       </c>
       <c r="L28">
-        <v>10.5529105755307</v>
+        <v>12.6243878743702</v>
       </c>
       <c r="M28">
-        <v>8.077688906846319</v>
+        <v>10.060045622811</v>
       </c>
       <c r="N28">
-        <v>11.4057369559657</v>
+        <v>11.2413401190931</v>
       </c>
       <c r="O28">
-        <v>668.959088444833</v>
+        <v>668.205126819076</v>
       </c>
       <c r="P28">
-        <v>90.47536309665129</v>
+        <v>90.7789474154014</v>
       </c>
     </row>
     <row r="29">
@@ -1850,49 +1850,49 @@
         </is>
       </c>
       <c r="B29">
-        <v>452.451317127841</v>
+        <v>459.357809269112</v>
       </c>
       <c r="C29">
-        <v>6.55014149872212</v>
+        <v>6.18172200340556</v>
       </c>
       <c r="D29">
-        <v>3.36258543924484</v>
+        <v>2.46515567610891</v>
       </c>
       <c r="E29">
-        <v>5.52056263806955</v>
+        <v>6.38600959262967</v>
       </c>
       <c r="F29">
-        <v>16.930926585493</v>
+        <v>16.7306605890075</v>
       </c>
       <c r="G29">
-        <v>2.25777388659164</v>
+        <v>3.0052642782115</v>
       </c>
       <c r="H29">
-        <v>2.44374595354489</v>
+        <v>2.43045037199739</v>
       </c>
       <c r="I29">
-        <v>4.91278281857887</v>
+        <v>4.6018509258705</v>
       </c>
       <c r="J29">
-        <v>7.18969809029582</v>
+        <v>7.98550749469173</v>
       </c>
       <c r="K29">
-        <v>2.58489831285419</v>
+        <v>3.89262062171539</v>
       </c>
       <c r="L29">
-        <v>5.69769636080658</v>
+        <v>6.12621250839574</v>
       </c>
       <c r="M29">
-        <v>3.0047723755418</v>
+        <v>2.57741991724912</v>
       </c>
       <c r="N29">
-        <v>14.017397307573</v>
+        <v>11.8930636398841</v>
       </c>
       <c r="O29">
-        <v>857.812904172844</v>
+        <v>860.871863638923</v>
       </c>
       <c r="P29">
-        <v>4.80765274064585</v>
+        <v>5.04581011651747</v>
       </c>
     </row>
     <row r="30">
@@ -1902,49 +1902,49 @@
         </is>
       </c>
       <c r="B30">
-        <v>235.381821755915</v>
+        <v>226.749084521377</v>
       </c>
       <c r="C30">
-        <v>3.77495016264634</v>
+        <v>4.20704992978002</v>
       </c>
       <c r="D30">
-        <v>5.74920755019004</v>
+        <v>5.41073495737029</v>
       </c>
       <c r="E30">
-        <v>14.6070840533885</v>
+        <v>13.4348310613761</v>
       </c>
       <c r="F30">
-        <v>0.936210644235205</v>
+        <v>0.700780284776182</v>
       </c>
       <c r="G30">
-        <v>5.15705782219808</v>
+        <v>5.03507264803216</v>
       </c>
       <c r="H30">
-        <v>5.89778663222827</v>
+        <v>6.16047089808915</v>
       </c>
       <c r="I30">
-        <v>2.31906107505363</v>
+        <v>2.0069412299088</v>
       </c>
       <c r="J30">
-        <v>19.5892592518846</v>
+        <v>19.5185284570598</v>
       </c>
       <c r="K30">
-        <v>12.6864255354231</v>
+        <v>14.784108808065</v>
       </c>
       <c r="L30">
-        <v>42.5973040207252</v>
+        <v>43.9108373632867</v>
       </c>
       <c r="M30">
-        <v>10.6227254618775</v>
+        <v>10.3104298577904</v>
       </c>
       <c r="N30">
-        <v>15.7836712265567</v>
+        <v>16.9445042432983</v>
       </c>
       <c r="O30">
-        <v>497.848806291683</v>
+        <v>502.663201672947</v>
       </c>
       <c r="P30">
-        <v>8.05148675958935</v>
+        <v>7.37955867475769</v>
       </c>
     </row>
     <row r="31">
@@ -1954,49 +1954,49 @@
         </is>
       </c>
       <c r="B31">
-        <v>1989.9929992055</v>
+        <v>1956.16438398493</v>
       </c>
       <c r="C31">
-        <v>47.5844535142313</v>
+        <v>50.0858832922281</v>
       </c>
       <c r="D31">
-        <v>49.6902584348024</v>
+        <v>48.1739442067156</v>
       </c>
       <c r="E31">
-        <v>31.9947839431414</v>
+        <v>35.2824860852174</v>
       </c>
       <c r="F31">
-        <v>13.1945064151482</v>
+        <v>11.5590782546921</v>
       </c>
       <c r="G31">
-        <v>150.490760848881</v>
+        <v>147.626672516345</v>
       </c>
       <c r="H31">
-        <v>30.7511944789835</v>
+        <v>29.8594577334319</v>
       </c>
       <c r="I31">
-        <v>26.2866933976378</v>
+        <v>24.3892079449946</v>
       </c>
       <c r="J31">
-        <v>40.784890602391</v>
+        <v>46.8894495380341</v>
       </c>
       <c r="K31">
-        <v>42.2554416701562</v>
+        <v>43.5858301129604</v>
       </c>
       <c r="L31">
-        <v>60.3680068858599</v>
+        <v>65.28688936774461</v>
       </c>
       <c r="M31">
-        <v>30.3465226014686</v>
+        <v>33.8418374056134</v>
       </c>
       <c r="N31">
-        <v>71.01025696168919</v>
+        <v>69.4188387279418</v>
       </c>
       <c r="O31">
-        <v>3442.53778172323</v>
+        <v>3461.28256597285</v>
       </c>
       <c r="P31">
-        <v>11.288246325478</v>
+        <v>12.9681354553658</v>
       </c>
     </row>
     <row r="32">
@@ -2006,49 +2006,49 @@
         </is>
       </c>
       <c r="B32">
-        <v>469.860053461902</v>
+        <v>468.432170908557</v>
       </c>
       <c r="C32">
-        <v>4.68116451580685</v>
+        <v>4.57688787453954</v>
       </c>
       <c r="D32">
-        <v>4.12814996802828</v>
+        <v>3.91437702446431</v>
       </c>
       <c r="E32">
-        <v>2.71483100237447</v>
+        <v>4.76999180297106</v>
       </c>
       <c r="F32">
-        <v>22.4266517801364</v>
+        <v>23.0745777105139</v>
       </c>
       <c r="G32">
-        <v>2.28731949694278</v>
+        <v>2.0730050339173</v>
       </c>
       <c r="H32">
-        <v>1.29126264058699</v>
+        <v>1.07065109239605</v>
       </c>
       <c r="I32">
-        <v>3.47941409502772</v>
+        <v>3.68455550385468</v>
       </c>
       <c r="J32">
-        <v>1.82124422496368</v>
+        <v>2.39679606244615</v>
       </c>
       <c r="K32">
-        <v>4.64024929139458</v>
+        <v>4.63742217939964</v>
       </c>
       <c r="L32">
-        <v>14.2201374074414</v>
+        <v>14.6674711123281</v>
       </c>
       <c r="M32">
-        <v>5.39289150215322</v>
+        <v>5.12956032324501</v>
       </c>
       <c r="N32">
-        <v>10.7727331514795</v>
+        <v>12.3334973003257</v>
       </c>
       <c r="O32">
-        <v>684.954849562393</v>
+        <v>677.6319120557751</v>
       </c>
       <c r="P32">
-        <v>30.5132437499727</v>
+        <v>27.8215768209428</v>
       </c>
     </row>
     <row r="33">
@@ -2058,49 +2058,49 @@
         </is>
       </c>
       <c r="B33">
-        <v>4966.12706843955</v>
+        <v>4909.46079214075</v>
       </c>
       <c r="C33">
-        <v>83.0466988715572</v>
+        <v>86.39799978660341</v>
       </c>
       <c r="D33">
-        <v>140.958264724002</v>
+        <v>138.851852441689</v>
       </c>
       <c r="E33">
-        <v>86.0022763066679</v>
+        <v>86.8988213418385</v>
       </c>
       <c r="F33">
-        <v>11.4561924883977</v>
+        <v>13.6323107824493</v>
       </c>
       <c r="G33">
-        <v>81.66008833448841</v>
+        <v>87.72497671971939</v>
       </c>
       <c r="H33">
-        <v>49.3894481600266</v>
+        <v>47.3889098921297</v>
       </c>
       <c r="I33">
-        <v>46.2394889983433</v>
+        <v>46.0931589614087</v>
       </c>
       <c r="J33">
-        <v>120.308284690323</v>
+        <v>123.744042050845</v>
       </c>
       <c r="K33">
-        <v>123.473495657889</v>
+        <v>124.866963310515</v>
       </c>
       <c r="L33">
-        <v>150.13937749966</v>
+        <v>155.258556534165</v>
       </c>
       <c r="M33">
-        <v>90.89891279929481</v>
+        <v>90.8861169327616</v>
       </c>
       <c r="N33">
-        <v>154.902200090536</v>
+        <v>150.916458915792</v>
       </c>
       <c r="O33">
-        <v>7407.27067478601</v>
+        <v>7434.49586040378</v>
       </c>
       <c r="P33">
-        <v>86.0819794742979</v>
+        <v>84.3382895457051</v>
       </c>
     </row>
     <row r="34">
@@ -2110,49 +2110,49 @@
         </is>
       </c>
       <c r="B34">
-        <v>1761.1436883192</v>
+        <v>1745.54010811914</v>
       </c>
       <c r="C34">
-        <v>80.75918364119821</v>
+        <v>79.8208622284771</v>
       </c>
       <c r="D34">
-        <v>227.347157387304</v>
+        <v>226.410869331526</v>
       </c>
       <c r="E34">
-        <v>83.54926750786819</v>
+        <v>85.295711739422</v>
       </c>
       <c r="F34">
-        <v>6.82360271882618</v>
+        <v>7.08592233116567</v>
       </c>
       <c r="G34">
-        <v>71.13189588183749</v>
+        <v>68.3609079300528</v>
       </c>
       <c r="H34">
-        <v>47.9373433131552</v>
+        <v>47.722128337101</v>
       </c>
       <c r="I34">
-        <v>30.3982416083516</v>
+        <v>28.8301856955953</v>
       </c>
       <c r="J34">
-        <v>56.4344821663147</v>
+        <v>60.4076999995961</v>
       </c>
       <c r="K34">
-        <v>62.8953088522118</v>
+        <v>66.5983788423558</v>
       </c>
       <c r="L34">
-        <v>115.072011144529</v>
+        <v>113.936318792367</v>
       </c>
       <c r="M34">
-        <v>53.1881966993836</v>
+        <v>57.8528286268327</v>
       </c>
       <c r="N34">
-        <v>140.545584208165</v>
+        <v>138.459172489997</v>
       </c>
       <c r="O34">
-        <v>2848.37925970663</v>
+        <v>2855.4248606175</v>
       </c>
       <c r="P34">
-        <v>63.4713706178447</v>
+        <v>67.37569528476929</v>
       </c>
     </row>
     <row r="35">
@@ -2162,49 +2162,49 @@
         </is>
       </c>
       <c r="B35">
-        <v>126.248981436026</v>
+        <v>125.210173401618</v>
       </c>
       <c r="C35">
-        <v>6.83545134691101</v>
+        <v>6.41747445000095</v>
       </c>
       <c r="D35">
-        <v>1.02706731725004</v>
+        <v>0.861492687093335</v>
       </c>
       <c r="E35">
-        <v>1.69176353089817</v>
+        <v>1.84335976509919</v>
       </c>
       <c r="F35">
-        <v>5.41393269503226</v>
+        <v>5.59281143308514</v>
       </c>
       <c r="G35">
-        <v>0.419551272299675</v>
+        <v>0.38774844238725</v>
       </c>
       <c r="H35">
-        <v>0.620389272577663</v>
+        <v>0.497780880018149</v>
       </c>
       <c r="I35">
-        <v>1.00716918226573</v>
+        <v>0.887563401892233</v>
       </c>
       <c r="J35">
-        <v>1.69627745947915</v>
+        <v>2.19712624555184</v>
       </c>
       <c r="K35">
-        <v>5.97414483270686</v>
+        <v>6.72756707053916</v>
       </c>
       <c r="L35">
-        <v>2.5537737555654</v>
+        <v>2.25939339803661</v>
       </c>
       <c r="M35">
-        <v>1.9249346562159</v>
+        <v>2.05722818474405</v>
       </c>
       <c r="N35">
-        <v>2.44160119565735</v>
+        <v>2.44002845719026</v>
       </c>
       <c r="O35">
-        <v>250.085055302987</v>
+        <v>248.127544435021</v>
       </c>
       <c r="P35">
-        <v>44.392154471283</v>
+        <v>43.8984898511149</v>
       </c>
     </row>
     <row r="36">
@@ -2214,49 +2214,49 @@
         </is>
       </c>
       <c r="B36">
-        <v>2556.36955858577</v>
+        <v>2547.81739382766</v>
       </c>
       <c r="C36">
-        <v>67.33978767951621</v>
+        <v>69.77037824684579</v>
       </c>
       <c r="D36">
-        <v>22.6421118746591</v>
+        <v>22.9881789001268</v>
       </c>
       <c r="E36">
-        <v>91.16910818157319</v>
+        <v>90.4897098843672</v>
       </c>
       <c r="F36">
-        <v>30.814448817189</v>
+        <v>30.0461354054688</v>
       </c>
       <c r="G36">
-        <v>96.19706738133689</v>
+        <v>92.2769492882077</v>
       </c>
       <c r="H36">
-        <v>123.615992755821</v>
+        <v>124.551216084465</v>
       </c>
       <c r="I36">
-        <v>48.6827153111993</v>
+        <v>49.784499007342</v>
       </c>
       <c r="J36">
-        <v>275.467561606113</v>
+        <v>274.126740222993</v>
       </c>
       <c r="K36">
-        <v>159.428642897749</v>
+        <v>164.306241669177</v>
       </c>
       <c r="L36">
-        <v>112.30355109895</v>
+        <v>112.476460511136</v>
       </c>
       <c r="M36">
-        <v>257.780636915077</v>
+        <v>256.853381349219</v>
       </c>
       <c r="N36">
-        <v>88.47820932703161</v>
+        <v>91.22100458763261</v>
       </c>
       <c r="O36">
-        <v>4087.99412296406</v>
+        <v>4088.48928181362</v>
       </c>
       <c r="P36">
-        <v>66.0122385611983</v>
+        <v>61.4695571909974</v>
       </c>
     </row>
     <row r="37">
@@ -2266,49 +2266,49 @@
         </is>
       </c>
       <c r="B37">
-        <v>857.173274561684</v>
+        <v>847.969036354373</v>
       </c>
       <c r="C37">
-        <v>21.864257396813</v>
+        <v>22.1032862876502</v>
       </c>
       <c r="D37">
-        <v>15.6050322982173</v>
+        <v>14.6812918253888</v>
       </c>
       <c r="E37">
-        <v>19.0028228938311</v>
+        <v>19.1914266071534</v>
       </c>
       <c r="F37">
-        <v>46.3688058505594</v>
+        <v>50.5391907724864</v>
       </c>
       <c r="G37">
-        <v>5.00217590527145</v>
+        <v>4.58895192315646</v>
       </c>
       <c r="H37">
-        <v>20.8566878109395</v>
+        <v>19.6137345032366</v>
       </c>
       <c r="I37">
-        <v>12.302315510137</v>
+        <v>12.058123804024</v>
       </c>
       <c r="J37">
-        <v>36.411386763176</v>
+        <v>35.2351487609228</v>
       </c>
       <c r="K37">
-        <v>30.0598059165814</v>
+        <v>32.4279772836772</v>
       </c>
       <c r="L37">
-        <v>28.4563797118336</v>
+        <v>24.9432354874981</v>
       </c>
       <c r="M37">
-        <v>32.757199468739</v>
+        <v>29.7289772673683</v>
       </c>
       <c r="N37">
-        <v>21.0305572383274</v>
+        <v>21.0622687867798</v>
       </c>
       <c r="O37">
-        <v>1203.50298605801</v>
+        <v>1211.25384940429</v>
       </c>
       <c r="P37">
-        <v>63.8471615875058</v>
+        <v>60.8921315632603</v>
       </c>
     </row>
     <row r="38">
@@ -2318,49 +2318,49 @@
         </is>
       </c>
       <c r="B38">
-        <v>772.051733006203</v>
+        <v>770.05049638699</v>
       </c>
       <c r="C38">
-        <v>29.7894934966724</v>
+        <v>31.436281515493</v>
       </c>
       <c r="D38">
-        <v>11.2630361477915</v>
+        <v>10.671931786589</v>
       </c>
       <c r="E38">
-        <v>62.7067561079008</v>
+        <v>61.3367426852909</v>
       </c>
       <c r="F38">
-        <v>1.98121486244247</v>
+        <v>2.23120618927668</v>
       </c>
       <c r="G38">
-        <v>7.95570923827349</v>
+        <v>9.39281920277803</v>
       </c>
       <c r="H38">
-        <v>8.16280721499581</v>
+        <v>7.45139931901234</v>
       </c>
       <c r="I38">
-        <v>6.56855396966426</v>
+        <v>7.55286665605764</v>
       </c>
       <c r="J38">
-        <v>31.6958997142784</v>
+        <v>30.8897329997375</v>
       </c>
       <c r="K38">
-        <v>18.8193307976107</v>
+        <v>20.2633612130203</v>
       </c>
       <c r="L38">
-        <v>61.2531052492542</v>
+        <v>63.3456599186116</v>
       </c>
       <c r="M38">
-        <v>25.4785690364833</v>
+        <v>24.8283770431573</v>
       </c>
       <c r="N38">
-        <v>26.0827407770678</v>
+        <v>26.1589960761185</v>
       </c>
       <c r="O38">
-        <v>1308.6630674891</v>
+        <v>1303.70231979793</v>
       </c>
       <c r="P38">
-        <v>69.6609598744877</v>
+        <v>68.7014644235657</v>
       </c>
     </row>
     <row r="39">
@@ -2370,49 +2370,49 @@
         </is>
       </c>
       <c r="B39">
-        <v>3003.59418024676</v>
+        <v>2974.16922277137</v>
       </c>
       <c r="C39">
-        <v>112.12572982682</v>
+        <v>110.13356615787</v>
       </c>
       <c r="D39">
-        <v>69.29228679229971</v>
+        <v>70.1158058730703</v>
       </c>
       <c r="E39">
-        <v>112.328223834066</v>
+        <v>117.325966911547</v>
       </c>
       <c r="F39">
-        <v>38.6774388762997</v>
+        <v>37.8573820034592</v>
       </c>
       <c r="G39">
-        <v>114.109220416101</v>
+        <v>109.65756578693</v>
       </c>
       <c r="H39">
-        <v>58.8859664249207</v>
+        <v>57.2883187039078</v>
       </c>
       <c r="I39">
-        <v>61.0877817641274</v>
+        <v>57.128835614034</v>
       </c>
       <c r="J39">
-        <v>212.384269397333</v>
+        <v>218.761716718808</v>
       </c>
       <c r="K39">
-        <v>116.996055177214</v>
+        <v>113.40241272497</v>
       </c>
       <c r="L39">
-        <v>139.749702127907</v>
+        <v>142.328284730144</v>
       </c>
       <c r="M39">
-        <v>88.80631368835721</v>
+        <v>85.7089786087208</v>
       </c>
       <c r="N39">
-        <v>101.723018903966</v>
+        <v>103.707655599721</v>
       </c>
       <c r="O39">
-        <v>4491.34264781785</v>
+        <v>4521.0868525875</v>
       </c>
       <c r="P39">
-        <v>78.7199989301718</v>
+        <v>83.16326434323391</v>
       </c>
     </row>
     <row r="40">
@@ -2422,49 +2422,49 @@
         </is>
       </c>
       <c r="B40">
-        <v>245.495914191527</v>
+        <v>242.733939213068</v>
       </c>
       <c r="C40">
-        <v>3.74072180504489</v>
+        <v>4.09334170238452</v>
       </c>
       <c r="D40">
-        <v>10.5561601150241</v>
+        <v>9.89155552296925</v>
       </c>
       <c r="E40">
-        <v>3.77185826962841</v>
+        <v>4.17442040305565</v>
       </c>
       <c r="F40">
-        <v>1.40484320146478</v>
+        <v>1.10804974457362</v>
       </c>
       <c r="G40">
-        <v>3.4065734822127</v>
+        <v>4.05422684144253</v>
       </c>
       <c r="H40">
-        <v>7.0926461267981</v>
+        <v>7.73423070654445</v>
       </c>
       <c r="I40">
-        <v>2.20984576554684</v>
+        <v>2.2580693008857</v>
       </c>
       <c r="J40">
-        <v>12.5130426439611</v>
+        <v>13.4386896894955</v>
       </c>
       <c r="K40">
-        <v>5.95836646205664</v>
+        <v>6.9624292885848</v>
       </c>
       <c r="L40">
-        <v>16.3920548712676</v>
+        <v>15.272540446086</v>
       </c>
       <c r="M40">
-        <v>9.508707017581161</v>
+        <v>8.33194557041667</v>
       </c>
       <c r="N40">
-        <v>26.3648064385926</v>
+        <v>25.9559481954561</v>
       </c>
       <c r="O40">
-        <v>391.570976435481</v>
+        <v>392.722643608512</v>
       </c>
       <c r="P40">
-        <v>2.28694696244195</v>
+        <v>2.58457606330136</v>
       </c>
     </row>
     <row r="41">
@@ -2474,49 +2474,49 @@
         </is>
       </c>
       <c r="B41">
-        <v>939.76666380018</v>
+        <v>942.344129461032</v>
       </c>
       <c r="C41">
-        <v>17.3313531058462</v>
+        <v>18.3366038835945</v>
       </c>
       <c r="D41">
-        <v>116.0841370828</v>
+        <v>112.478900164668</v>
       </c>
       <c r="E41">
-        <v>53.8591449367659</v>
+        <v>50.9428154063509</v>
       </c>
       <c r="F41">
-        <v>2.93909208711169</v>
+        <v>3.49810984593389</v>
       </c>
       <c r="G41">
-        <v>37.6721474115891</v>
+        <v>37.8538821871059</v>
       </c>
       <c r="H41">
-        <v>35.1090704670667</v>
+        <v>32.9253558618822</v>
       </c>
       <c r="I41">
-        <v>8.42147683611703</v>
+        <v>6.54263690254379</v>
       </c>
       <c r="J41">
-        <v>46.0056716943536</v>
+        <v>45.9725805405725</v>
       </c>
       <c r="K41">
-        <v>48.8266434183651</v>
+        <v>47.630689866631</v>
       </c>
       <c r="L41">
-        <v>27.8641715868304</v>
+        <v>31.4708940591114</v>
       </c>
       <c r="M41">
-        <v>39.4500151898565</v>
+        <v>42.3979999938718</v>
       </c>
       <c r="N41">
-        <v>25.2928617645337</v>
+        <v>23.7162542279589</v>
       </c>
       <c r="O41">
-        <v>1364.72956090763</v>
+        <v>1374.16524903778</v>
       </c>
       <c r="P41">
-        <v>22.5207706495914</v>
+        <v>19.4993580139839</v>
       </c>
     </row>
     <row r="42">
@@ -2526,49 +2526,49 @@
         </is>
       </c>
       <c r="B42">
-        <v>141.031606631375</v>
+        <v>138.191033623413</v>
       </c>
       <c r="C42">
-        <v>9.098506254681199</v>
+        <v>9.40158954947163</v>
       </c>
       <c r="D42">
-        <v>2.17649636379483</v>
+        <v>1.81438913946594</v>
       </c>
       <c r="E42">
-        <v>5.00081885489675</v>
+        <v>5.44956179992106</v>
       </c>
       <c r="F42">
-        <v>1.81926418147472</v>
+        <v>1.67608283085396</v>
       </c>
       <c r="G42">
-        <v>0.900229448681772</v>
+        <v>0.739838574810427</v>
       </c>
       <c r="H42">
-        <v>1.80064021807196</v>
+        <v>1.72745081133819</v>
       </c>
       <c r="I42">
-        <v>1.04567611169635</v>
+        <v>1.17832918159157</v>
       </c>
       <c r="J42">
-        <v>3.81372319937037</v>
+        <v>3.95950126068993</v>
       </c>
       <c r="K42">
-        <v>7.35970344438214</v>
+        <v>7.45671325403486</v>
       </c>
       <c r="L42">
-        <v>7.87674563964963</v>
+        <v>8.20204010833065</v>
       </c>
       <c r="M42">
-        <v>2.86874858180991</v>
+        <v>3.05106481684603</v>
       </c>
       <c r="N42">
-        <v>8.51835401981374</v>
+        <v>7.94715830768643</v>
       </c>
       <c r="O42">
-        <v>286.755664088248</v>
+        <v>286.675713528194</v>
       </c>
       <c r="P42">
-        <v>45.8665980646321</v>
+        <v>46.9344964644011</v>
       </c>
     </row>
     <row r="43">
@@ -2578,49 +2578,49 @@
         </is>
       </c>
       <c r="B43">
-        <v>1377.8269294258</v>
+        <v>1387.74610230064</v>
       </c>
       <c r="C43">
-        <v>41.7335984308369</v>
+        <v>43.0817405069454</v>
       </c>
       <c r="D43">
-        <v>56.2851539932729</v>
+        <v>55.9097326006064</v>
       </c>
       <c r="E43">
-        <v>74.35978630067839</v>
+        <v>67.7172317114801</v>
       </c>
       <c r="F43">
-        <v>10.1266450914262</v>
+        <v>9.65620844245858</v>
       </c>
       <c r="G43">
-        <v>32.9521454018165</v>
+        <v>32.3831577083187</v>
       </c>
       <c r="H43">
-        <v>40.6043016105551</v>
+        <v>33.8067181871739</v>
       </c>
       <c r="I43">
-        <v>22.6509486617368</v>
+        <v>21.4220005406247</v>
       </c>
       <c r="J43">
-        <v>73.90369067152891</v>
+        <v>76.728935242516</v>
       </c>
       <c r="K43">
-        <v>51.4184267487581</v>
+        <v>51.4238792970346</v>
       </c>
       <c r="L43">
-        <v>57.8972958795635</v>
+        <v>62.4724718081677</v>
       </c>
       <c r="M43">
-        <v>92.3323010020701</v>
+        <v>87.9800442180789</v>
       </c>
       <c r="N43">
-        <v>71.1178092688409</v>
+        <v>71.72177448866501</v>
       </c>
       <c r="O43">
-        <v>2005.41756155371</v>
+        <v>2009.01525494741</v>
       </c>
       <c r="P43">
-        <v>46.3729269425919</v>
+        <v>42.5091216120379</v>
       </c>
     </row>
     <row r="44">
@@ -2630,49 +2630,49 @@
         </is>
       </c>
       <c r="B44">
-        <v>4722.7931527464</v>
+        <v>4699.29531790275</v>
       </c>
       <c r="C44">
-        <v>162.911604345394</v>
+        <v>156.159359376929</v>
       </c>
       <c r="D44">
-        <v>79.7387384664794</v>
+        <v>79.0512449464604</v>
       </c>
       <c r="E44">
-        <v>100.293944328126</v>
+        <v>96.92377283811641</v>
       </c>
       <c r="F44">
-        <v>210.581827931959</v>
+        <v>220.848113176794</v>
       </c>
       <c r="G44">
-        <v>125.409501369499</v>
+        <v>133.224817676539</v>
       </c>
       <c r="H44">
-        <v>65.1099174691096</v>
+        <v>63.8872486386454</v>
       </c>
       <c r="I44">
-        <v>53.1067256933746</v>
+        <v>49.6764185157905</v>
       </c>
       <c r="J44">
-        <v>159.041709878801</v>
+        <v>158.304579243439</v>
       </c>
       <c r="K44">
-        <v>140.093764015411</v>
+        <v>137.012693618743</v>
       </c>
       <c r="L44">
-        <v>255.25206440322</v>
+        <v>259.385830299696</v>
       </c>
       <c r="M44">
-        <v>147.967387695134</v>
+        <v>143.904210628502</v>
       </c>
       <c r="N44">
-        <v>108.905767496086</v>
+        <v>108.422060237925</v>
       </c>
       <c r="O44">
-        <v>7630.8771711608</v>
+        <v>7660.60241845309</v>
       </c>
       <c r="P44">
-        <v>229.958978855737</v>
+        <v>227.137922775815</v>
       </c>
     </row>
     <row r="45">
@@ -2682,49 +2682,49 @@
         </is>
       </c>
       <c r="B45">
-        <v>434.959827530795</v>
+        <v>430.419728039053</v>
       </c>
       <c r="C45">
-        <v>18.4048789962158</v>
+        <v>17.2620159294939</v>
       </c>
       <c r="D45">
-        <v>5.00420678276139</v>
+        <v>4.39292862146293</v>
       </c>
       <c r="E45">
-        <v>11.261014847555</v>
+        <v>12.2768010426072</v>
       </c>
       <c r="F45">
-        <v>19.1356188514603</v>
+        <v>18.6631914734262</v>
       </c>
       <c r="G45">
-        <v>9.589712376039371</v>
+        <v>9.20344537469308</v>
       </c>
       <c r="H45">
-        <v>4.08112497239236</v>
+        <v>4.11434516173406</v>
       </c>
       <c r="I45">
-        <v>6.2981579745765</v>
+        <v>5.54045183962303</v>
       </c>
       <c r="J45">
-        <v>19.321044460705</v>
+        <v>19.1705654585232</v>
       </c>
       <c r="K45">
-        <v>13.5272431646146</v>
+        <v>12.1578495466486</v>
       </c>
       <c r="L45">
-        <v>23.847994340557</v>
+        <v>24.7193885882964</v>
       </c>
       <c r="M45">
-        <v>27.73995782481</v>
+        <v>28.3899709351547</v>
       </c>
       <c r="N45">
-        <v>26.5581053755874</v>
+        <v>26.7463633501647</v>
       </c>
       <c r="O45">
-        <v>852.679482167822</v>
+        <v>855.308635153836</v>
       </c>
       <c r="P45">
-        <v>18.5076738892494</v>
+        <v>19.3835513598183</v>
       </c>
     </row>
     <row r="46">
@@ -2734,49 +2734,49 @@
         </is>
       </c>
       <c r="B46">
-        <v>114.821986318857</v>
+        <v>115.312491138017</v>
       </c>
       <c r="C46">
-        <v>4.84881495976353</v>
+        <v>5.34576945466236</v>
       </c>
       <c r="D46">
-        <v>1.75718844160258</v>
+        <v>2.03213740922185</v>
       </c>
       <c r="E46">
-        <v>7.31927251911312</v>
+        <v>6.94458967932234</v>
       </c>
       <c r="F46">
-        <v>0.955492332184371</v>
+        <v>1.13129495858115</v>
       </c>
       <c r="G46">
-        <v>1.06220928286379</v>
+        <v>1.17773390535898</v>
       </c>
       <c r="H46">
-        <v>1.28599923802037</v>
+        <v>1.60022089662419</v>
       </c>
       <c r="I46">
-        <v>2.39774465990439</v>
+        <v>2.47115386329216</v>
       </c>
       <c r="J46">
-        <v>5.22780210793862</v>
+        <v>5.00632278297979</v>
       </c>
       <c r="K46">
-        <v>4.28644390597106</v>
+        <v>5.31474013385246</v>
       </c>
       <c r="L46">
-        <v>10.9045066969151</v>
+        <v>11.4383431298233</v>
       </c>
       <c r="M46">
-        <v>4.89678746102619</v>
+        <v>5.06141734306248</v>
       </c>
       <c r="N46">
-        <v>7.07636019439841</v>
+        <v>7.60478252525847</v>
       </c>
       <c r="O46">
-        <v>252.789731981686</v>
+        <v>253.080123908438</v>
       </c>
       <c r="P46">
-        <v>12.2628131517192</v>
+        <v>12.0432616761335</v>
       </c>
     </row>
     <row r="47">
@@ -2786,49 +2786,49 @@
         </is>
       </c>
       <c r="B47">
-        <v>1532.38134927773</v>
+        <v>1512.13383079534</v>
       </c>
       <c r="C47">
-        <v>63.4644449940746</v>
+        <v>60.8636668598535</v>
       </c>
       <c r="D47">
-        <v>49.963279178611</v>
+        <v>59.9265705563423</v>
       </c>
       <c r="E47">
-        <v>67.0108959319623</v>
+        <v>61.3068231587631</v>
       </c>
       <c r="F47">
-        <v>14.2973011939436</v>
+        <v>13.6470767082469</v>
       </c>
       <c r="G47">
-        <v>34.1622764525952</v>
+        <v>37.3353833874435</v>
       </c>
       <c r="H47">
-        <v>28.4227120233401</v>
+        <v>25.845557118516</v>
       </c>
       <c r="I47">
-        <v>16.3460474920829</v>
+        <v>17.9586616272523</v>
       </c>
       <c r="J47">
-        <v>47.7821462616798</v>
+        <v>51.158139837711</v>
       </c>
       <c r="K47">
-        <v>40.8867778425807</v>
+        <v>39.5633238637389</v>
       </c>
       <c r="L47">
-        <v>53.3162845511088</v>
+        <v>55.1799758919431</v>
       </c>
       <c r="M47">
-        <v>80.8734000952698</v>
+        <v>78.66876094028</v>
       </c>
       <c r="N47">
-        <v>51.5079433410541</v>
+        <v>51.550764196329</v>
       </c>
       <c r="O47">
-        <v>2815.61420493311</v>
+        <v>2818.17269149788</v>
       </c>
       <c r="P47">
-        <v>47.1980962755977</v>
+        <v>49.2172990247577</v>
       </c>
     </row>
     <row r="48">
@@ -2838,49 +2838,49 @@
         </is>
       </c>
       <c r="B48">
-        <v>1307.21934979317</v>
+        <v>1304.95167643689</v>
       </c>
       <c r="C48">
-        <v>26.1177712916949</v>
+        <v>32.6333428796819</v>
       </c>
       <c r="D48">
-        <v>12.0466442846058</v>
+        <v>10.4611317898874</v>
       </c>
       <c r="E48">
-        <v>69.1876817370822</v>
+        <v>68.9864280242972</v>
       </c>
       <c r="F48">
-        <v>12.8488900634503</v>
+        <v>12.0318330583885</v>
       </c>
       <c r="G48">
-        <v>18.2471811910835</v>
+        <v>16.2782428725178</v>
       </c>
       <c r="H48">
-        <v>8.303071346775649</v>
+        <v>8.447906097050231</v>
       </c>
       <c r="I48">
-        <v>11.9668842267262</v>
+        <v>12.6978394391713</v>
       </c>
       <c r="J48">
-        <v>34.8028702627806</v>
+        <v>33.2345374676928</v>
       </c>
       <c r="K48">
-        <v>19.9982604516169</v>
+        <v>20.3736567291805</v>
       </c>
       <c r="L48">
-        <v>47.1976566237413</v>
+        <v>43.4723003556404</v>
       </c>
       <c r="M48">
-        <v>156.293887624662</v>
+        <v>156.23354740627</v>
       </c>
       <c r="N48">
-        <v>23.7925292978254</v>
+        <v>29.1453411293756</v>
       </c>
       <c r="O48">
-        <v>2293.9967923795</v>
+        <v>2307.23026256629</v>
       </c>
       <c r="P48">
-        <v>108.848068308877</v>
+        <v>102.563240503927</v>
       </c>
     </row>
     <row r="49">
@@ -2890,49 +2890,49 @@
         </is>
       </c>
       <c r="B49">
-        <v>585.259263835327</v>
+        <v>579.612139209878</v>
       </c>
       <c r="C49">
-        <v>8.540797689200071</v>
+        <v>7.61171004614206</v>
       </c>
       <c r="D49">
-        <v>5.6119241975008</v>
+        <v>4.67055652389534</v>
       </c>
       <c r="E49">
-        <v>12.7040823071204</v>
+        <v>13.6496652525128</v>
       </c>
       <c r="F49">
-        <v>34.1051469813377</v>
+        <v>34.7906804084974</v>
       </c>
       <c r="G49">
-        <v>16.9463091887906</v>
+        <v>18.258861862978</v>
       </c>
       <c r="H49">
-        <v>5.49081293544106</v>
+        <v>5.1062681022837</v>
       </c>
       <c r="I49">
-        <v>9.41827041119851</v>
+        <v>10.3705840511869</v>
       </c>
       <c r="J49">
-        <v>22.0355930069578</v>
+        <v>21.2585343099507</v>
       </c>
       <c r="K49">
-        <v>9.580368066356281</v>
+        <v>8.430694966831529</v>
       </c>
       <c r="L49">
-        <v>4.7985131683095</v>
+        <v>4.44691827628946</v>
       </c>
       <c r="M49">
-        <v>7.8042934434358</v>
+        <v>7.78950829499113</v>
       </c>
       <c r="N49">
-        <v>4.83987065896193</v>
+        <v>4.38415639660243</v>
       </c>
       <c r="O49">
-        <v>606.996487194141</v>
+        <v>607.775351019022</v>
       </c>
       <c r="P49">
-        <v>9.678253993831371</v>
+        <v>10.1452466503585</v>
       </c>
     </row>
     <row r="50">
@@ -2942,49 +2942,49 @@
         </is>
       </c>
       <c r="B50">
-        <v>1000.74072684121</v>
+        <v>1003.55256317261</v>
       </c>
       <c r="C50">
-        <v>90.0099396714859</v>
+        <v>91.8574181440632</v>
       </c>
       <c r="D50">
-        <v>10.1819278346505</v>
+        <v>11.9557711775036</v>
       </c>
       <c r="E50">
-        <v>131.955670766602</v>
+        <v>127.060724483552</v>
       </c>
       <c r="F50">
-        <v>4.40731304292922</v>
+        <v>4.78370874972567</v>
       </c>
       <c r="G50">
-        <v>21.5660262314134</v>
+        <v>24.1285301318535</v>
       </c>
       <c r="H50">
-        <v>37.306737501811</v>
+        <v>38.6675910022056</v>
       </c>
       <c r="I50">
-        <v>21.915105050253</v>
+        <v>20.359620967135</v>
       </c>
       <c r="J50">
-        <v>114.28837000573</v>
+        <v>112.265511209106</v>
       </c>
       <c r="K50">
-        <v>123.579499763213</v>
+        <v>124.400413804633</v>
       </c>
       <c r="L50">
-        <v>84.49183142289471</v>
+        <v>85.29001484257731</v>
       </c>
       <c r="M50">
-        <v>48.9618354868699</v>
+        <v>50.1493075052888</v>
       </c>
       <c r="N50">
-        <v>69.0166043798193</v>
+        <v>69.9954063965839</v>
       </c>
       <c r="O50">
-        <v>1895.54148814618</v>
+        <v>1884.63985514212</v>
       </c>
       <c r="P50">
-        <v>136.949307591834</v>
+        <v>139.1538060251</v>
       </c>
     </row>
     <row r="51">
@@ -2994,49 +2994,49 @@
         </is>
       </c>
       <c r="B51">
-        <v>102.010884606508</v>
+        <v>101.664467338447</v>
       </c>
       <c r="C51">
-        <v>1.4864110388683</v>
+        <v>1.44859338008465</v>
       </c>
       <c r="D51">
-        <v>0.549826567915813</v>
+        <v>0.511862148025355</v>
       </c>
       <c r="E51">
-        <v>1.82129102705149</v>
+        <v>1.7678141193593</v>
       </c>
       <c r="F51">
-        <v>24.2460844751734</v>
+        <v>23.3481329851183</v>
       </c>
       <c r="G51">
-        <v>2.27249631356316</v>
+        <v>2.63064845072944</v>
       </c>
       <c r="H51">
-        <v>0.317301054689828</v>
+        <v>0.330357180306387</v>
       </c>
       <c r="I51">
-        <v>0.814772243149075</v>
+        <v>1.44704169109411</v>
       </c>
       <c r="J51">
-        <v>1.78625370591146</v>
+        <v>1.90174647672779</v>
       </c>
       <c r="K51">
-        <v>0.99666657955296</v>
+        <v>1.07467487568067</v>
       </c>
       <c r="L51">
-        <v>0.501716868741798</v>
+        <v>0.650947948079337</v>
       </c>
       <c r="M51">
-        <v>0.940712053149664</v>
+        <v>0.840523596887066</v>
       </c>
       <c r="N51">
-        <v>1.63714966187816</v>
+        <v>1.37739379972823</v>
       </c>
       <c r="O51">
-        <v>192.083618910183</v>
+        <v>194.821654581873</v>
       </c>
       <c r="P51">
-        <v>14.6648514606004</v>
+        <v>14.6423760472302</v>
       </c>
     </row>
     <row r="52">

</xml_diff>

<commit_message>
migration weights and roll 0
</commit_message>
<xml_diff>
--- a/1-Data-Codes/2-Final_Data/L_1999.xlsx
+++ b/1-Data-Codes/2-Final_Data/L_1999.xlsx
@@ -446,49 +446,49 @@
         </is>
       </c>
       <c r="B2">
-        <v>1184.18105309252</v>
+        <v>1331.49015420539</v>
       </c>
       <c r="C2">
-        <v>37.7312493768588</v>
+        <v>39.8338941871166</v>
       </c>
       <c r="D2">
-        <v>95.684480932073</v>
+        <v>76.874843794814</v>
       </c>
       <c r="E2">
-        <v>68.71961130274531</v>
+        <v>65.5638685097135</v>
       </c>
       <c r="F2">
-        <v>15.913070153695</v>
+        <v>13.4131309453317</v>
       </c>
       <c r="G2">
-        <v>22.4703301943731</v>
+        <v>18.6087733277311</v>
       </c>
       <c r="H2">
-        <v>25.2261904083649</v>
+        <v>19.6830948209711</v>
       </c>
       <c r="I2">
-        <v>13.7107487640636</v>
+        <v>13.8150233483087</v>
       </c>
       <c r="J2">
-        <v>75.6051229570654</v>
+        <v>66.4773975556646</v>
       </c>
       <c r="K2">
-        <v>24.7943761422538</v>
+        <v>24.3459696751203</v>
       </c>
       <c r="L2">
-        <v>35.5903726407172</v>
+        <v>39.6813922407968</v>
       </c>
       <c r="M2">
-        <v>39.2993878131648</v>
+        <v>40.5663186292598</v>
       </c>
       <c r="N2">
-        <v>29.0830719332653</v>
+        <v>30.7523850119298</v>
       </c>
       <c r="O2">
-        <v>1433.82540854526</v>
+        <v>1323.59471028054</v>
       </c>
       <c r="P2">
-        <v>50.7071562968583</v>
+        <v>50.4773752552674</v>
       </c>
     </row>
     <row r="3">
@@ -498,49 +498,49 @@
         </is>
       </c>
       <c r="B3">
-        <v>126.28149479713</v>
+        <v>132.676454105894</v>
       </c>
       <c r="C3">
-        <v>5.7566581932203</v>
+        <v>4.19231087428372</v>
       </c>
       <c r="D3">
-        <v>0.5181136109044811</v>
+        <v>0.572653992140574</v>
       </c>
       <c r="E3">
-        <v>1.8448985831021</v>
+        <v>2.66458217664028</v>
       </c>
       <c r="F3">
-        <v>9.55526719754943</v>
+        <v>8.69465253149955</v>
       </c>
       <c r="G3">
-        <v>0.499599156286716</v>
+        <v>0.431560371886344</v>
       </c>
       <c r="H3">
-        <v>0.151407685956579</v>
+        <v>0.289093540698095</v>
       </c>
       <c r="I3">
-        <v>0.151831436568474</v>
+        <v>0.358197680432521</v>
       </c>
       <c r="J3">
-        <v>0.6852537017514581</v>
+        <v>0.8404319129088</v>
       </c>
       <c r="K3">
-        <v>0.443147046849816</v>
+        <v>0.241630189380403</v>
       </c>
       <c r="L3">
-        <v>0.43018188877555</v>
+        <v>0.444476342823298</v>
       </c>
       <c r="M3">
-        <v>1.20472110363438</v>
+        <v>0.882349075239046</v>
       </c>
       <c r="N3">
-        <v>0.612818974206455</v>
+        <v>0.737329370458944</v>
       </c>
       <c r="O3">
-        <v>246.210821479239</v>
+        <v>234.055327462255</v>
       </c>
       <c r="P3">
-        <v>10.5104964627374</v>
+        <v>10.5940926133311</v>
       </c>
     </row>
     <row r="4">
@@ -550,49 +550,49 @@
         </is>
       </c>
       <c r="B4">
-        <v>1278.45756060157</v>
+        <v>1442.52725724205</v>
       </c>
       <c r="C4">
-        <v>16.4224269419738</v>
+        <v>11.991860422245</v>
       </c>
       <c r="D4">
-        <v>13.5981601877411</v>
+        <v>10.968287042175</v>
       </c>
       <c r="E4">
-        <v>18.7350177689622</v>
+        <v>15.5715369854421</v>
       </c>
       <c r="F4">
-        <v>19.9148361895876</v>
+        <v>19.428197463429</v>
       </c>
       <c r="G4">
-        <v>13.0789728582458</v>
+        <v>10.7773733110144</v>
       </c>
       <c r="H4">
-        <v>9.19625772766309</v>
+        <v>9.48535151683671</v>
       </c>
       <c r="I4">
-        <v>8.040898527654299</v>
+        <v>8.37636914753786</v>
       </c>
       <c r="J4">
-        <v>27.9760627746798</v>
+        <v>25.4314453955506</v>
       </c>
       <c r="K4">
-        <v>7.28414019499799</v>
+        <v>12.0017098110685</v>
       </c>
       <c r="L4">
-        <v>95.1802763816155</v>
+        <v>88.301166201877</v>
       </c>
       <c r="M4">
-        <v>56.7227470234972</v>
+        <v>56.1879010880926</v>
       </c>
       <c r="N4">
-        <v>22.1894418071616</v>
+        <v>15.7399062376146</v>
       </c>
       <c r="O4">
-        <v>1907.44700862473</v>
+        <v>1773.90606410085</v>
       </c>
       <c r="P4">
-        <v>38.2656259027017</v>
+        <v>34.2244429255395</v>
       </c>
     </row>
     <row r="5">
@@ -602,49 +602,49 @@
         </is>
       </c>
       <c r="B5">
-        <v>699.424859869128</v>
+        <v>780.305063171498</v>
       </c>
       <c r="C5">
-        <v>60.5811114770767</v>
+        <v>53.7320625547383</v>
       </c>
       <c r="D5">
-        <v>15.3751359842759</v>
+        <v>13.0641853743414</v>
       </c>
       <c r="E5">
-        <v>45.1005358171892</v>
+        <v>28.2983179468032</v>
       </c>
       <c r="F5">
-        <v>3.36141414505046</v>
+        <v>5.79783385316765</v>
       </c>
       <c r="G5">
-        <v>14.9631666500504</v>
+        <v>9.5906865443825</v>
       </c>
       <c r="H5">
-        <v>15.4349219361766</v>
+        <v>14.545019338243</v>
       </c>
       <c r="I5">
-        <v>8.11297049311071</v>
+        <v>10.3913068138562</v>
       </c>
       <c r="J5">
-        <v>39.390619372741</v>
+        <v>34.0746965588</v>
       </c>
       <c r="K5">
-        <v>27.4736473452091</v>
+        <v>27.1955340975446</v>
       </c>
       <c r="L5">
-        <v>22.1859921426408</v>
+        <v>22.7611423967049</v>
       </c>
       <c r="M5">
-        <v>19.5041502420764</v>
+        <v>20.0984386507713</v>
       </c>
       <c r="N5">
-        <v>17.8303868742086</v>
+        <v>16.9452102356054</v>
       </c>
       <c r="O5">
-        <v>819.230076398553</v>
+        <v>783.684488290127</v>
       </c>
       <c r="P5">
-        <v>63.3993512762447</v>
+        <v>56.8851330446934</v>
       </c>
     </row>
     <row r="6">
@@ -654,49 +654,49 @@
         </is>
       </c>
       <c r="B6">
-        <v>8319.875091511671</v>
+        <v>9565.261274005319</v>
       </c>
       <c r="C6">
-        <v>215.473046677271</v>
+        <v>178.22946788664</v>
       </c>
       <c r="D6">
-        <v>227.510391780223</v>
+        <v>198.95154263944</v>
       </c>
       <c r="E6">
-        <v>154.25531952515</v>
+        <v>145.772275148913</v>
       </c>
       <c r="F6">
-        <v>50.7806367664761</v>
+        <v>66.6816659325747</v>
       </c>
       <c r="G6">
-        <v>104.736171195071</v>
+        <v>93.0814644150485</v>
       </c>
       <c r="H6">
-        <v>68.6783542504126</v>
+        <v>40.1625991130467</v>
       </c>
       <c r="I6">
-        <v>56.9395690620835</v>
+        <v>52.6054204296298</v>
       </c>
       <c r="J6">
-        <v>203.594185932953</v>
+        <v>209.939122810866</v>
       </c>
       <c r="K6">
-        <v>140.553051426765</v>
+        <v>116.074994277833</v>
       </c>
       <c r="L6">
-        <v>611.74831678814</v>
+        <v>530.457334240518</v>
       </c>
       <c r="M6">
-        <v>308.395529207286</v>
+        <v>267.745599118003</v>
       </c>
       <c r="N6">
-        <v>314.540366100723</v>
+        <v>274.42020601792</v>
       </c>
       <c r="O6">
-        <v>12402.1904571266</v>
+        <v>11432.4085953563</v>
       </c>
       <c r="P6">
-        <v>349.339058302012</v>
+        <v>334.013299536302</v>
       </c>
     </row>
     <row r="7">
@@ -706,49 +706,49 @@
         </is>
       </c>
       <c r="B7">
-        <v>835.146427823938</v>
+        <v>952.019302862187</v>
       </c>
       <c r="C7">
-        <v>34.5520671661975</v>
+        <v>28.2489595754033</v>
       </c>
       <c r="D7">
-        <v>5.92304830389201</v>
+        <v>6.5189433458972</v>
       </c>
       <c r="E7">
-        <v>22.626285135918</v>
+        <v>23.4088386106682</v>
       </c>
       <c r="F7">
-        <v>18.1590262117981</v>
+        <v>24.0738556995617</v>
       </c>
       <c r="G7">
-        <v>9.173834685734709</v>
+        <v>17.8799505239627</v>
       </c>
       <c r="H7">
-        <v>9.54672257440418</v>
+        <v>5.31329824089102</v>
       </c>
       <c r="I7">
-        <v>11.8240049296039</v>
+        <v>11.0920306328974</v>
       </c>
       <c r="J7">
-        <v>18.2440314178694</v>
+        <v>24.0468656207423</v>
       </c>
       <c r="K7">
-        <v>15.7821903370926</v>
+        <v>16.3927961805511</v>
       </c>
       <c r="L7">
-        <v>67.69475044148039</v>
+        <v>61.1931615013352</v>
       </c>
       <c r="M7">
-        <v>20.8087777999332</v>
+        <v>23.1205507015726</v>
       </c>
       <c r="N7">
-        <v>26.6023500979878</v>
+        <v>15.4682510290836</v>
       </c>
       <c r="O7">
-        <v>1873.40063700653</v>
+        <v>1768.32789142905</v>
       </c>
       <c r="P7">
-        <v>39.7434680780375</v>
+        <v>26.1361151824489</v>
       </c>
     </row>
     <row r="8">
@@ -758,49 +758,49 @@
         </is>
       </c>
       <c r="B8">
-        <v>726.810619638754</v>
+        <v>860.0301988676</v>
       </c>
       <c r="C8">
-        <v>17.9745003905674</v>
+        <v>12.1678509135935</v>
       </c>
       <c r="D8">
-        <v>9.900862444121779</v>
+        <v>4.77626484179474</v>
       </c>
       <c r="E8">
-        <v>24.7224350036554</v>
+        <v>21.235268046991</v>
       </c>
       <c r="F8">
-        <v>0.963324739685245</v>
+        <v>0.718872230848903</v>
       </c>
       <c r="G8">
-        <v>31.1270861652849</v>
+        <v>25.7610037148164</v>
       </c>
       <c r="H8">
-        <v>11.0446985763124</v>
+        <v>14.9799271622353</v>
       </c>
       <c r="I8">
-        <v>3.00567713161428</v>
+        <v>1.64554129339211</v>
       </c>
       <c r="J8">
-        <v>50.995751767004</v>
+        <v>49.0420051362412</v>
       </c>
       <c r="K8">
-        <v>35.86149724132</v>
+        <v>35.1762097756319</v>
       </c>
       <c r="L8">
-        <v>42.4932893393781</v>
+        <v>39.2756115359313</v>
       </c>
       <c r="M8">
-        <v>66.94372204842971</v>
+        <v>68.3758863660487</v>
       </c>
       <c r="N8">
-        <v>28.9644361662272</v>
+        <v>20.7728838599334</v>
       </c>
       <c r="O8">
-        <v>1347.65584633206</v>
+        <v>1250.38804544899</v>
       </c>
       <c r="P8">
-        <v>7.56075279808984</v>
+        <v>8.695561471100501</v>
       </c>
     </row>
     <row r="9">
@@ -810,49 +810,49 @@
         </is>
       </c>
       <c r="B9">
-        <v>170.198020434754</v>
+        <v>205.21446043911</v>
       </c>
       <c r="C9">
-        <v>10.4751791158214</v>
+        <v>7.58350145145195</v>
       </c>
       <c r="D9">
-        <v>2.00555188373689</v>
+        <v>3.54482763934014</v>
       </c>
       <c r="E9">
-        <v>5.36715212701808</v>
+        <v>5.90895879974486</v>
       </c>
       <c r="F9">
-        <v>2.40943589723383</v>
+        <v>2.17028435818753</v>
       </c>
       <c r="G9">
-        <v>22.0016416613249</v>
+        <v>18.9045855600881</v>
       </c>
       <c r="H9">
-        <v>4.1935210289999</v>
+        <v>2.5596462648457</v>
       </c>
       <c r="I9">
-        <v>0.232237062165507</v>
+        <v>0.6070848503021</v>
       </c>
       <c r="J9">
-        <v>2.92250655329673</v>
+        <v>3.32008405361355</v>
       </c>
       <c r="K9">
-        <v>3.70688880540117</v>
+        <v>4.08447659763855</v>
       </c>
       <c r="L9">
-        <v>1.94827192393208</v>
+        <v>1.67940440332975</v>
       </c>
       <c r="M9">
-        <v>8.110327347207321</v>
+        <v>8.17243613391206</v>
       </c>
       <c r="N9">
-        <v>4.64247776099561</v>
+        <v>2.96405542842516</v>
       </c>
       <c r="O9">
-        <v>310.530356802868</v>
+        <v>284.29491488167</v>
       </c>
       <c r="P9">
-        <v>4.88466562700059</v>
+        <v>4.62184596992188</v>
       </c>
     </row>
     <row r="10">
@@ -862,49 +862,49 @@
         </is>
       </c>
       <c r="B10">
-        <v>4303.54971085694</v>
+        <v>4999.93989986026</v>
       </c>
       <c r="C10">
-        <v>57.2926923079952</v>
+        <v>44.7251422880344</v>
       </c>
       <c r="D10">
-        <v>45.6656371289964</v>
+        <v>33.4485923570905</v>
       </c>
       <c r="E10">
-        <v>71.284404808986</v>
+        <v>61.8097234389602</v>
       </c>
       <c r="F10">
-        <v>12.0786863976306</v>
+        <v>11.8415096640097</v>
       </c>
       <c r="G10">
-        <v>48.446056989966</v>
+        <v>44.0536968366579</v>
       </c>
       <c r="H10">
-        <v>17.9751683735803</v>
+        <v>22.3748791061129</v>
       </c>
       <c r="I10">
-        <v>28.6057853835648</v>
+        <v>32.1396599649676</v>
       </c>
       <c r="J10">
-        <v>44.4499832990247</v>
+        <v>46.9355197414036</v>
       </c>
       <c r="K10">
-        <v>49.493456113864</v>
+        <v>44.1674613343739</v>
       </c>
       <c r="L10">
-        <v>117.125707392211</v>
+        <v>79.4158462139298</v>
       </c>
       <c r="M10">
-        <v>92.7426371155147</v>
+        <v>80.110813987942</v>
       </c>
       <c r="N10">
-        <v>107.644182914592</v>
+        <v>83.39315410979</v>
       </c>
       <c r="O10">
-        <v>6433.05735360008</v>
+        <v>5852.88180821262</v>
       </c>
       <c r="P10">
-        <v>99.56892773239279</v>
+        <v>104.007621927199</v>
       </c>
     </row>
     <row r="11">
@@ -914,49 +914,49 @@
         </is>
       </c>
       <c r="B11">
-        <v>1806.66146959282</v>
+        <v>1997.74446950779</v>
       </c>
       <c r="C11">
-        <v>74.86847203366349</v>
+        <v>65.6167071976038</v>
       </c>
       <c r="D11">
-        <v>161.901978417888</v>
+        <v>120.296766421285</v>
       </c>
       <c r="E11">
-        <v>116.587414547519</v>
+        <v>106.551385540812</v>
       </c>
       <c r="F11">
-        <v>12.6607236307885</v>
+        <v>10.5622733043336</v>
       </c>
       <c r="G11">
-        <v>45.964969646048</v>
+        <v>37.1619958572508</v>
       </c>
       <c r="H11">
-        <v>25.5949065546656</v>
+        <v>25.6964606503791</v>
       </c>
       <c r="I11">
-        <v>26.0808158234067</v>
+        <v>14.9156241064528</v>
       </c>
       <c r="J11">
-        <v>52.0288896707677</v>
+        <v>51.7532951733682</v>
       </c>
       <c r="K11">
-        <v>51.8553610836126</v>
+        <v>41.2903494015771</v>
       </c>
       <c r="L11">
-        <v>66.3326692606999</v>
+        <v>46.4252073754524</v>
       </c>
       <c r="M11">
-        <v>69.9795236871387</v>
+        <v>78.4256155631858</v>
       </c>
       <c r="N11">
-        <v>56.2842949219039</v>
+        <v>48.8479876570234</v>
       </c>
       <c r="O11">
-        <v>3067.41568544058</v>
+        <v>2991.08227526564</v>
       </c>
       <c r="P11">
-        <v>57.3876082660749</v>
+        <v>58.6648453212775</v>
       </c>
     </row>
     <row r="12">
@@ -966,49 +966,49 @@
         </is>
       </c>
       <c r="B12">
-        <v>293.292790152106</v>
+        <v>334.772225262336</v>
       </c>
       <c r="C12">
-        <v>8.020900953442769</v>
+        <v>5.55695795346657</v>
       </c>
       <c r="D12">
-        <v>5.10721515395889</v>
+        <v>8.68382856816692</v>
       </c>
       <c r="E12">
-        <v>2.58665841687248</v>
+        <v>1.89618782903499</v>
       </c>
       <c r="F12">
-        <v>0.67099344192676</v>
+        <v>0.874101089386443</v>
       </c>
       <c r="G12">
-        <v>1.41888314823133</v>
+        <v>0.83810217252513</v>
       </c>
       <c r="H12">
-        <v>1.07930506722659</v>
+        <v>0.557926584826131</v>
       </c>
       <c r="I12">
-        <v>1.38828447573773</v>
+        <v>1.54673063879279</v>
       </c>
       <c r="J12">
-        <v>0.923323536138674</v>
+        <v>0.866069344819379</v>
       </c>
       <c r="K12">
-        <v>0.616189733429155</v>
+        <v>0.332674499243272</v>
       </c>
       <c r="L12">
-        <v>2.01879863379377</v>
+        <v>2.22356967255915</v>
       </c>
       <c r="M12">
-        <v>3.49138835946389</v>
+        <v>4.16098746951938</v>
       </c>
       <c r="N12">
-        <v>2.60454205897327</v>
+        <v>2.88756110662517</v>
       </c>
       <c r="O12">
-        <v>504.826667332035</v>
+        <v>458.566598526136</v>
       </c>
       <c r="P12">
-        <v>20.4110303335531</v>
+        <v>24.8028120754519</v>
       </c>
     </row>
     <row r="13">
@@ -1018,49 +1018,49 @@
         </is>
       </c>
       <c r="B13">
-        <v>278.754168361165</v>
+        <v>318.943303922679</v>
       </c>
       <c r="C13">
-        <v>27.5492821065653</v>
+        <v>23.988555950861</v>
       </c>
       <c r="D13">
-        <v>2.79235639526811</v>
+        <v>2.63764045382433</v>
       </c>
       <c r="E13">
-        <v>20.4814447383575</v>
+        <v>20.7099083998146</v>
       </c>
       <c r="F13">
-        <v>6.53268330857801</v>
+        <v>3.27514360493088</v>
       </c>
       <c r="G13">
-        <v>5.86223349697389</v>
+        <v>4.22738462911818</v>
       </c>
       <c r="H13">
-        <v>2.17102539400205</v>
+        <v>2.06064356798822</v>
       </c>
       <c r="I13">
-        <v>1.9268627177019</v>
+        <v>3.08622363973723</v>
       </c>
       <c r="J13">
-        <v>4.81088506341407</v>
+        <v>2.63164017543196</v>
       </c>
       <c r="K13">
-        <v>2.93205481473468</v>
+        <v>3.50375255122371</v>
       </c>
       <c r="L13">
-        <v>21.1353731278499</v>
+        <v>15.2241031838341</v>
       </c>
       <c r="M13">
-        <v>4.76824148215963</v>
+        <v>2.35367694921071</v>
       </c>
       <c r="N13">
-        <v>7.11451187908753</v>
+        <v>6.08595184245298</v>
       </c>
       <c r="O13">
-        <v>462.48667504132</v>
+        <v>429.26908343164</v>
       </c>
       <c r="P13">
-        <v>41.5298970637903</v>
+        <v>41.6950591672125</v>
       </c>
     </row>
     <row r="14">
@@ -1070,49 +1070,49 @@
         </is>
       </c>
       <c r="B14">
-        <v>2724.34706800646</v>
+        <v>3125.23734887412</v>
       </c>
       <c r="C14">
-        <v>117.179488719713</v>
+        <v>110.376057533739</v>
       </c>
       <c r="D14">
-        <v>21.932210253791</v>
+        <v>20.084308835452</v>
       </c>
       <c r="E14">
-        <v>100.714414893061</v>
+        <v>95.7052932461532</v>
       </c>
       <c r="F14">
-        <v>25.9220843183321</v>
+        <v>24.904166345985</v>
       </c>
       <c r="G14">
-        <v>98.6326221962462</v>
+        <v>61.6015522591</v>
       </c>
       <c r="H14">
-        <v>68.9328332326113</v>
+        <v>76.8656413348925</v>
       </c>
       <c r="I14">
-        <v>33.9843350970083</v>
+        <v>28.9190043460819</v>
       </c>
       <c r="J14">
-        <v>190.320613263575</v>
+        <v>162.146514085728</v>
       </c>
       <c r="K14">
-        <v>183.339250969925</v>
+        <v>151.583144773589</v>
       </c>
       <c r="L14">
-        <v>178.920571348383</v>
+        <v>158.752234415344</v>
       </c>
       <c r="M14">
-        <v>99.4207224252134</v>
+        <v>108.063052969163</v>
       </c>
       <c r="N14">
-        <v>104.308915060136</v>
+        <v>75.77375621310961</v>
       </c>
       <c r="O14">
-        <v>4725.3999079652</v>
+        <v>4462.90432976247</v>
       </c>
       <c r="P14">
-        <v>88.5844903554415</v>
+        <v>74.8698584053415</v>
       </c>
     </row>
     <row r="15">
@@ -1122,49 +1122,49 @@
         </is>
       </c>
       <c r="B15">
-        <v>1307.0194381584</v>
+        <v>1487.04034406289</v>
       </c>
       <c r="C15">
-        <v>45.0513572699827</v>
+        <v>32.7648014636365</v>
       </c>
       <c r="D15">
-        <v>15.1087505603228</v>
+        <v>10.5053443046768</v>
       </c>
       <c r="E15">
-        <v>70.757891118147</v>
+        <v>74.2279873572931</v>
       </c>
       <c r="F15">
-        <v>13.1787946218496</v>
+        <v>17.2895546467778</v>
       </c>
       <c r="G15">
-        <v>47.5903981401002</v>
+        <v>38.3794527496954</v>
       </c>
       <c r="H15">
-        <v>50.0865531307603</v>
+        <v>60.611268669778</v>
       </c>
       <c r="I15">
-        <v>33.7802221050491</v>
+        <v>23.3748324237274</v>
       </c>
       <c r="J15">
-        <v>176.441518988672</v>
+        <v>170.970598661421</v>
       </c>
       <c r="K15">
-        <v>89.0012509816595</v>
+        <v>79.215157664532</v>
       </c>
       <c r="L15">
-        <v>80.8254229655881</v>
+        <v>81.3534594539659</v>
       </c>
       <c r="M15">
-        <v>182.947077242327</v>
+        <v>185.269244321669</v>
       </c>
       <c r="N15">
-        <v>69.9605835752884</v>
+        <v>65.4510387640872</v>
       </c>
       <c r="O15">
-        <v>2072.70396660811</v>
+        <v>1947.03385702189</v>
       </c>
       <c r="P15">
-        <v>39.5751410006412</v>
+        <v>35.426609788896</v>
       </c>
     </row>
     <row r="16">
@@ -1174,49 +1174,49 @@
         </is>
       </c>
       <c r="B16">
-        <v>536.892608427248</v>
+        <v>657.58120227397</v>
       </c>
       <c r="C16">
-        <v>57.318005481793</v>
+        <v>59.9443660980051</v>
       </c>
       <c r="D16">
-        <v>11.1139241504929</v>
+        <v>10.1572254849056</v>
       </c>
       <c r="E16">
-        <v>28.4623485051637</v>
+        <v>24.9728898534227</v>
       </c>
       <c r="F16">
-        <v>4.00605243387668</v>
+        <v>7.07339770930818</v>
       </c>
       <c r="G16">
-        <v>13.4319281482711</v>
+        <v>13.6381033825872</v>
       </c>
       <c r="H16">
-        <v>14.2819073801684</v>
+        <v>15.0514263951086</v>
       </c>
       <c r="I16">
-        <v>14.9432816343442</v>
+        <v>8.90717365939534</v>
       </c>
       <c r="J16">
-        <v>48.209108593127</v>
+        <v>62.7642523258889</v>
       </c>
       <c r="K16">
-        <v>51.1854667888139</v>
+        <v>38.3884514035511</v>
       </c>
       <c r="L16">
-        <v>38.2499226771179</v>
+        <v>40.0312440964271</v>
       </c>
       <c r="M16">
-        <v>22.7641763639719</v>
+        <v>18.9410828539227</v>
       </c>
       <c r="N16">
-        <v>23.7020949440738</v>
+        <v>17.832118226474</v>
       </c>
       <c r="O16">
-        <v>1098.08514682237</v>
+        <v>994.586181263091</v>
       </c>
       <c r="P16">
-        <v>84.1669874929773</v>
+        <v>76.2426384115458</v>
       </c>
     </row>
     <row r="17">
@@ -1226,49 +1226,49 @@
         </is>
       </c>
       <c r="B17">
-        <v>524.0438538228081</v>
+        <v>613.0877370025401</v>
       </c>
       <c r="C17">
-        <v>31.4788495377213</v>
+        <v>29.4249261002647</v>
       </c>
       <c r="D17">
-        <v>6.13456830208344</v>
+        <v>8.7558314403732</v>
       </c>
       <c r="E17">
-        <v>14.6735762855872</v>
+        <v>11.5136791236643</v>
       </c>
       <c r="F17">
-        <v>14.5888586323115</v>
+        <v>13.3389278956407</v>
       </c>
       <c r="G17">
-        <v>12.0843042175136</v>
+        <v>13.9213115907467</v>
       </c>
       <c r="H17">
-        <v>14.651426647355</v>
+        <v>15.3959960738766</v>
       </c>
       <c r="I17">
-        <v>9.20770821295608</v>
+        <v>16.1361700790873</v>
       </c>
       <c r="J17">
-        <v>21.1554940811514</v>
+        <v>21.2884870629973</v>
       </c>
       <c r="K17">
-        <v>24.951562225466</v>
+        <v>28.1232560753277</v>
       </c>
       <c r="L17">
-        <v>16.3970577951996</v>
+        <v>8.86264134193042</v>
       </c>
       <c r="M17">
-        <v>74.1274260360554</v>
+        <v>72.1905393787705</v>
       </c>
       <c r="N17">
-        <v>17.8698096031599</v>
+        <v>5.53268600495756</v>
       </c>
       <c r="O17">
-        <v>1004.22679356742</v>
+        <v>935.702525078857</v>
       </c>
       <c r="P17">
-        <v>71.6497260695631</v>
+        <v>71.5014541301165</v>
       </c>
     </row>
     <row r="18">
@@ -1278,49 +1278,49 @@
         </is>
       </c>
       <c r="B18">
-        <v>1049.3121947003</v>
+        <v>1160.51847836368</v>
       </c>
       <c r="C18">
-        <v>34.8261732742588</v>
+        <v>35.5282035506526</v>
       </c>
       <c r="D18">
-        <v>31.1612618957766</v>
+        <v>29.3976309763685</v>
       </c>
       <c r="E18">
-        <v>44.8741806590517</v>
+        <v>46.5811087185976</v>
       </c>
       <c r="F18">
-        <v>37.1184103573107</v>
+        <v>38.5960757186734</v>
       </c>
       <c r="G18">
-        <v>29.2619520234073</v>
+        <v>27.3794644122176</v>
       </c>
       <c r="H18">
-        <v>26.3864958267487</v>
+        <v>14.7240606749598</v>
       </c>
       <c r="I18">
-        <v>9.908773832715481</v>
+        <v>10.1438686686076</v>
       </c>
       <c r="J18">
-        <v>44.482588663265</v>
+        <v>43.4626590066667</v>
       </c>
       <c r="K18">
-        <v>40.0184809667658</v>
+        <v>31.1868296127494</v>
       </c>
       <c r="L18">
-        <v>49.546845059047</v>
+        <v>49.2564270389272</v>
       </c>
       <c r="M18">
-        <v>65.1261635090068</v>
+        <v>62.1693948910064</v>
       </c>
       <c r="N18">
-        <v>30.1103404579689</v>
+        <v>23.6285620481528</v>
       </c>
       <c r="O18">
-        <v>1363.04967465128</v>
+        <v>1289.97602868549</v>
       </c>
       <c r="P18">
-        <v>43.0898331762976</v>
+        <v>42.1423671328424</v>
       </c>
     </row>
     <row r="19">
@@ -1330,49 +1330,49 @@
         </is>
       </c>
       <c r="B19">
-        <v>1173.09621402333</v>
+        <v>1339.14897653632</v>
       </c>
       <c r="C19">
-        <v>24.5502101431982</v>
+        <v>24.6739093553029</v>
       </c>
       <c r="D19">
-        <v>19.4508908684875</v>
+        <v>14.3327478860734</v>
       </c>
       <c r="E19">
-        <v>41.5018461704074</v>
+        <v>35.6065499696842</v>
       </c>
       <c r="F19">
-        <v>71.64152335955571</v>
+        <v>62.9321194092315</v>
       </c>
       <c r="G19">
-        <v>43.6582313619455</v>
+        <v>41.1496751040971</v>
       </c>
       <c r="H19">
-        <v>5.16612443878362</v>
+        <v>7.24295844686232</v>
       </c>
       <c r="I19">
-        <v>7.11695428591609</v>
+        <v>10.8082231126828</v>
       </c>
       <c r="J19">
-        <v>19.5979640308635</v>
+        <v>11.8371466593493</v>
       </c>
       <c r="K19">
-        <v>13.539867414862</v>
+        <v>12.2036968931862</v>
       </c>
       <c r="L19">
-        <v>12.1177500000471</v>
+        <v>11.6067717478273</v>
       </c>
       <c r="M19">
-        <v>26.5927131831128</v>
+        <v>25.5490553072897</v>
       </c>
       <c r="N19">
-        <v>12.5183343041293</v>
+        <v>15.2913801075718</v>
       </c>
       <c r="O19">
-        <v>1579.0697973635</v>
+        <v>1459.99363191564</v>
       </c>
       <c r="P19">
-        <v>38.793637442843</v>
+        <v>31.8246347669767</v>
       </c>
     </row>
     <row r="20">
@@ -1382,49 +1382,49 @@
         </is>
       </c>
       <c r="B20">
-        <v>293.534787309187</v>
+        <v>336.84233508701</v>
       </c>
       <c r="C20">
-        <v>8.152964093843901</v>
+        <v>7.61931131812218</v>
       </c>
       <c r="D20">
-        <v>17.7792180872363</v>
+        <v>12.9308152665299</v>
       </c>
       <c r="E20">
-        <v>35.3131658005604</v>
+        <v>32.0827548579053</v>
       </c>
       <c r="F20">
-        <v>0.302784263462114</v>
+        <v>0.338985516325318</v>
       </c>
       <c r="G20">
-        <v>1.84460918210795</v>
+        <v>3.43206638367455</v>
       </c>
       <c r="H20">
-        <v>3.43285854081779</v>
+        <v>3.38795926480715</v>
       </c>
       <c r="I20">
-        <v>1.30941522769341</v>
+        <v>3.09953343216395</v>
       </c>
       <c r="J20">
-        <v>7.04030978028419</v>
+        <v>5.68423664219114</v>
       </c>
       <c r="K20">
-        <v>5.07874414013995</v>
+        <v>7.52541577662344</v>
       </c>
       <c r="L20">
-        <v>10.9011919235776</v>
+        <v>9.084994864035179</v>
       </c>
       <c r="M20">
-        <v>17.8445366061672</v>
+        <v>18.2468108226036</v>
       </c>
       <c r="N20">
-        <v>5.33705168926546</v>
+        <v>5.13358644809207</v>
       </c>
       <c r="O20">
-        <v>484.043588599321</v>
+        <v>447.346180502174</v>
       </c>
       <c r="P20">
-        <v>24.2822993112754</v>
+        <v>24.5154845855287</v>
       </c>
     </row>
     <row r="21">
@@ -1434,49 +1434,49 @@
         </is>
       </c>
       <c r="B21">
-        <v>1094.65210446061</v>
+        <v>1251.29207091918</v>
       </c>
       <c r="C21">
-        <v>28.1052874890065</v>
+        <v>18.7033491055115</v>
       </c>
       <c r="D21">
-        <v>12.4956887118496</v>
+        <v>9.45297893040912</v>
       </c>
       <c r="E21">
-        <v>34.926891357326</v>
+        <v>26.1466455058971</v>
       </c>
       <c r="F21">
-        <v>4.32560135321767</v>
+        <v>4.25532907750121</v>
       </c>
       <c r="G21">
-        <v>13.7808034860173</v>
+        <v>15.743284980857</v>
       </c>
       <c r="H21">
-        <v>26.2194519362703</v>
+        <v>36.4209865704847</v>
       </c>
       <c r="I21">
-        <v>7.32849961092694</v>
+        <v>2.93998846101901</v>
       </c>
       <c r="J21">
-        <v>15.7226559828981</v>
+        <v>8.028628465399979</v>
       </c>
       <c r="K21">
-        <v>16.4658619927032</v>
+        <v>22.9833221858658</v>
       </c>
       <c r="L21">
-        <v>41.6536474395373</v>
+        <v>40.92577574982</v>
       </c>
       <c r="M21">
-        <v>39.411023176936</v>
+        <v>27.7845674457453</v>
       </c>
       <c r="N21">
-        <v>22.822258290942</v>
+        <v>17.096831714545</v>
       </c>
       <c r="O21">
-        <v>2334.93016398716</v>
+        <v>2231.50195890593</v>
       </c>
       <c r="P21">
-        <v>20.3250890434975</v>
+        <v>12.5383851685258</v>
       </c>
     </row>
     <row r="22">
@@ -1486,49 +1486,49 @@
         </is>
       </c>
       <c r="B22">
-        <v>1341.76078837971</v>
+        <v>1588.43943064075</v>
       </c>
       <c r="C22">
-        <v>25.2125234498989</v>
+        <v>19.3047905170377</v>
       </c>
       <c r="D22">
-        <v>37.6970009444894</v>
+        <v>34.1555895549705</v>
       </c>
       <c r="E22">
-        <v>41.5545719882011</v>
+        <v>29.402270680601</v>
       </c>
       <c r="F22">
-        <v>2.59713041378194</v>
+        <v>1.94955241070233</v>
       </c>
       <c r="G22">
-        <v>25.8039139756349</v>
+        <v>26.2830466161559</v>
       </c>
       <c r="H22">
-        <v>29.3130193860249</v>
+        <v>25.296446664389</v>
       </c>
       <c r="I22">
-        <v>11.3637472497707</v>
+        <v>14.8448320260519</v>
       </c>
       <c r="J22">
-        <v>60.5468092960385</v>
+        <v>39.2691254704963</v>
       </c>
       <c r="K22">
-        <v>45.8492393358763</v>
+        <v>40.2854340296007</v>
       </c>
       <c r="L22">
-        <v>135.378276918533</v>
+        <v>127.333733040636</v>
       </c>
       <c r="M22">
-        <v>24.3971760889289</v>
+        <v>19.4606083865982</v>
       </c>
       <c r="N22">
-        <v>82.9485141231166</v>
+        <v>78.9964098347162</v>
       </c>
       <c r="O22">
-        <v>2663.16705340831</v>
+        <v>2468.08918002124</v>
       </c>
       <c r="P22">
-        <v>18.9598302521315</v>
+        <v>23.8476727958016</v>
       </c>
     </row>
     <row r="23">
@@ -1538,49 +1538,49 @@
         </is>
       </c>
       <c r="B23">
-        <v>2285.7421778009</v>
+        <v>2618.17423592269</v>
       </c>
       <c r="C23">
-        <v>50.8224362729515</v>
+        <v>48.9581244135994</v>
       </c>
       <c r="D23">
-        <v>18.4288702884659</v>
+        <v>22.0909633485785</v>
       </c>
       <c r="E23">
-        <v>69.6314980433378</v>
+        <v>47.0554283028954</v>
       </c>
       <c r="F23">
-        <v>5.26596547216806</v>
+        <v>12.3216766458989</v>
       </c>
       <c r="G23">
-        <v>64.3822127117206</v>
+        <v>61.5174507218948</v>
       </c>
       <c r="H23">
-        <v>66.8490782116447</v>
+        <v>47.6278583834241</v>
       </c>
       <c r="I23">
-        <v>22.6710576738088</v>
+        <v>20.6571614433929</v>
       </c>
       <c r="J23">
-        <v>179.90454291734</v>
+        <v>172.956505610297</v>
       </c>
       <c r="K23">
-        <v>133.179141250589</v>
+        <v>123.382642209071</v>
       </c>
       <c r="L23">
-        <v>56.3031155439002</v>
+        <v>59.7089621258531</v>
       </c>
       <c r="M23">
-        <v>529.271226219534</v>
+        <v>491.726020481133</v>
       </c>
       <c r="N23">
-        <v>91.0792927917673</v>
+        <v>78.41283056962649</v>
       </c>
       <c r="O23">
-        <v>3356.87365562576</v>
+        <v>3114.26302432769</v>
       </c>
       <c r="P23">
-        <v>72.57216190144359</v>
+        <v>70.13402363929571</v>
       </c>
     </row>
     <row r="24">
@@ -1590,49 +1590,49 @@
         </is>
       </c>
       <c r="B24">
-        <v>869.3760073413951</v>
+        <v>1011.49159190342</v>
       </c>
       <c r="C24">
-        <v>72.1210779600722</v>
+        <v>65.6688881617546</v>
       </c>
       <c r="D24">
-        <v>7.19750735506032</v>
+        <v>6.26533032565399</v>
       </c>
       <c r="E24">
-        <v>70.31038796101061</v>
+        <v>73.43112613247691</v>
       </c>
       <c r="F24">
-        <v>17.7388564272555</v>
+        <v>16.3870936898719</v>
       </c>
       <c r="G24">
-        <v>17.116575788244</v>
+        <v>23.6654633357073</v>
       </c>
       <c r="H24">
-        <v>27.7684488715449</v>
+        <v>14.9875398490822</v>
       </c>
       <c r="I24">
-        <v>10.4620970280043</v>
+        <v>12.3170230060513</v>
       </c>
       <c r="J24">
-        <v>58.4757213470077</v>
+        <v>42.5518072698662</v>
       </c>
       <c r="K24">
-        <v>61.8563157234361</v>
+        <v>66.314554715138</v>
       </c>
       <c r="L24">
-        <v>77.7015791220459</v>
+        <v>67.957056498135</v>
       </c>
       <c r="M24">
-        <v>19.7032575208318</v>
+        <v>23.8558639083555</v>
       </c>
       <c r="N24">
-        <v>65.06397356733321</v>
+        <v>65.75067193666411</v>
       </c>
       <c r="O24">
-        <v>1962.79324302732</v>
+        <v>1851.24651715181</v>
       </c>
       <c r="P24">
-        <v>118.056675314928</v>
+        <v>120.995183372325</v>
       </c>
     </row>
     <row r="25">
@@ -1642,49 +1642,49 @@
         </is>
       </c>
       <c r="B25">
-        <v>735.1761180992351</v>
+        <v>839.852955780598</v>
       </c>
       <c r="C25">
-        <v>36.3057083205777</v>
+        <v>36.0019073239008</v>
       </c>
       <c r="D25">
-        <v>28.422154172089</v>
+        <v>20.219953073501</v>
       </c>
       <c r="E25">
-        <v>34.5293186788085</v>
+        <v>35.1815184663562</v>
       </c>
       <c r="F25">
-        <v>19.416939093047</v>
+        <v>16.2973846048247</v>
       </c>
       <c r="G25">
-        <v>12.7517100492074</v>
+        <v>13.3312739752272</v>
       </c>
       <c r="H25">
-        <v>15.048793238515</v>
+        <v>12.6094744538236</v>
       </c>
       <c r="I25">
-        <v>5.30626022583599</v>
+        <v>1.81689339934049</v>
       </c>
       <c r="J25">
-        <v>21.1598263653002</v>
+        <v>20.4154446907903</v>
       </c>
       <c r="K25">
-        <v>18.9683857669807</v>
+        <v>18.0021115392169</v>
       </c>
       <c r="L25">
-        <v>35.5343928903264</v>
+        <v>31.8881059710896</v>
       </c>
       <c r="M25">
-        <v>25.0265970817983</v>
+        <v>25.34875583906</v>
       </c>
       <c r="N25">
-        <v>47.1855593221854</v>
+        <v>51.9674443025398</v>
       </c>
       <c r="O25">
-        <v>872.14440591528</v>
+        <v>781.939150368202</v>
       </c>
       <c r="P25">
-        <v>39.5687650331761</v>
+        <v>33.5706092497366</v>
       </c>
     </row>
     <row r="26">
@@ -1694,49 +1694,49 @@
         </is>
       </c>
       <c r="B26">
-        <v>1220.04448263885</v>
+        <v>1389.23965682524</v>
       </c>
       <c r="C26">
-        <v>60.9691341216883</v>
+        <v>51.1542216607211</v>
       </c>
       <c r="D26">
-        <v>17.8920931464034</v>
+        <v>13.7779333855641</v>
       </c>
       <c r="E26">
-        <v>50.1224477226552</v>
+        <v>50.911435714627</v>
       </c>
       <c r="F26">
-        <v>4.57688180041449</v>
+        <v>10.3981378927185</v>
       </c>
       <c r="G26">
-        <v>38.1037960642479</v>
+        <v>39.2497722284959</v>
       </c>
       <c r="H26">
-        <v>25.6519390794479</v>
+        <v>22.5432874416696</v>
       </c>
       <c r="I26">
-        <v>18.4623143100801</v>
+        <v>20.0172501085827</v>
       </c>
       <c r="J26">
-        <v>65.0933861593996</v>
+        <v>66.5168112159315</v>
       </c>
       <c r="K26">
-        <v>52.2868180853586</v>
+        <v>41.1344422174171</v>
       </c>
       <c r="L26">
-        <v>39.3200384737351</v>
+        <v>27.6246247235138</v>
       </c>
       <c r="M26">
-        <v>87.58452959232901</v>
+        <v>74.57972771866341</v>
       </c>
       <c r="N26">
-        <v>45.8928568352622</v>
+        <v>37.9608140642795</v>
       </c>
       <c r="O26">
-        <v>2141.59088707405</v>
+        <v>2030.4703023787</v>
       </c>
       <c r="P26">
-        <v>76.1884390300478</v>
+        <v>65.4121593233986</v>
       </c>
     </row>
     <row r="27">
@@ -1746,49 +1746,49 @@
         </is>
       </c>
       <c r="B27">
-        <v>197.609011875795</v>
+        <v>235.919659084245</v>
       </c>
       <c r="C27">
-        <v>2.91805088037377</v>
+        <v>3.227921453644</v>
       </c>
       <c r="D27">
-        <v>1.52044646221438</v>
+        <v>1.69014637561541</v>
       </c>
       <c r="E27">
-        <v>11.8647712409764</v>
+        <v>10.6275066733532</v>
       </c>
       <c r="F27">
-        <v>8.756025970076999</v>
+        <v>7.55943787865488</v>
       </c>
       <c r="G27">
-        <v>0.826465635825786</v>
+        <v>0.479471350684927</v>
       </c>
       <c r="H27">
-        <v>0.500224188739828</v>
+        <v>0.830243579376054</v>
       </c>
       <c r="I27">
-        <v>1.66265114860403</v>
+        <v>1.05703418539769</v>
       </c>
       <c r="J27">
-        <v>4.28509400092575</v>
+        <v>5.06858062163096</v>
       </c>
       <c r="K27">
-        <v>1.64437399696971</v>
+        <v>0.336723273467707</v>
       </c>
       <c r="L27">
-        <v>1.79629044664661</v>
+        <v>1.80433166410322</v>
       </c>
       <c r="M27">
-        <v>1.24513067556602</v>
+        <v>1.08918310473335</v>
       </c>
       <c r="N27">
-        <v>5.05567307279888</v>
+        <v>4.52578620916391</v>
       </c>
       <c r="O27">
-        <v>355.322680888426</v>
+        <v>330.148332008112</v>
       </c>
       <c r="P27">
-        <v>46.781823875411</v>
+        <v>42.6711592651144</v>
       </c>
     </row>
     <row r="28">
@@ -1798,49 +1798,49 @@
         </is>
       </c>
       <c r="B28">
-        <v>311.968234637495</v>
+        <v>375.788257335698</v>
       </c>
       <c r="C28">
-        <v>32.7693163170842</v>
+        <v>30.3891856970369</v>
       </c>
       <c r="D28">
-        <v>1.7979529629042</v>
+        <v>2.37023816986682</v>
       </c>
       <c r="E28">
-        <v>9.147323714297651</v>
+        <v>8.31132212649902</v>
       </c>
       <c r="F28">
-        <v>1.82594242957091</v>
+        <v>1.84703282610392</v>
       </c>
       <c r="G28">
-        <v>5.04181927114217</v>
+        <v>4.33348795342448</v>
       </c>
       <c r="H28">
-        <v>7.44504378481012</v>
+        <v>7.09255204347739</v>
       </c>
       <c r="I28">
-        <v>4.84175769856777</v>
+        <v>5.27980958215033</v>
       </c>
       <c r="J28">
-        <v>16.7615627337135</v>
+        <v>18.104669434223</v>
       </c>
       <c r="K28">
-        <v>16.3873782042885</v>
+        <v>12.5776375388867</v>
       </c>
       <c r="L28">
-        <v>10.952362441397</v>
+        <v>10.2886338999463</v>
       </c>
       <c r="M28">
-        <v>7.94258597183249</v>
+        <v>8.14008150411847</v>
       </c>
       <c r="N28">
-        <v>11.9019680147365</v>
+        <v>9.5831396315292</v>
       </c>
       <c r="O28">
-        <v>664.741948663834</v>
+        <v>617.53605554532</v>
       </c>
       <c r="P28">
-        <v>91.04120735490101</v>
+        <v>88.85852665672731</v>
       </c>
     </row>
     <row r="29">
@@ -1850,49 +1850,49 @@
         </is>
       </c>
       <c r="B29">
-        <v>457.294268828525</v>
+        <v>509.25095103186</v>
       </c>
       <c r="C29">
-        <v>6.61035567013287</v>
+        <v>8.376528784073409</v>
       </c>
       <c r="D29">
-        <v>3.21016249075664</v>
+        <v>3.95163272195713</v>
       </c>
       <c r="E29">
-        <v>5.84074648871514</v>
+        <v>3.09407407323767</v>
       </c>
       <c r="F29">
-        <v>17.3118890026863</v>
+        <v>16.4395427563375</v>
       </c>
       <c r="G29">
-        <v>2.52882669918717</v>
+        <v>3.25679416852135</v>
       </c>
       <c r="H29">
-        <v>2.30362022372098</v>
+        <v>1.4761624355448</v>
       </c>
       <c r="I29">
-        <v>4.79472980489876</v>
+        <v>4.21868797002417</v>
       </c>
       <c r="J29">
-        <v>6.92362241738773</v>
+        <v>7.68300281649635</v>
       </c>
       <c r="K29">
-        <v>2.66065371033113</v>
+        <v>5.11822311806161</v>
       </c>
       <c r="L29">
-        <v>5.15000117939599</v>
+        <v>3.32935210764222</v>
       </c>
       <c r="M29">
-        <v>3.00320063320998</v>
+        <v>3.99757691293641</v>
       </c>
       <c r="N29">
-        <v>12.6875108805939</v>
+        <v>13.0694887494314</v>
       </c>
       <c r="O29">
-        <v>839.706397628284</v>
+        <v>772.685410877738</v>
       </c>
       <c r="P29">
-        <v>4.88209619225627</v>
+        <v>4.51975582533804</v>
       </c>
     </row>
     <row r="30">
@@ -1902,49 +1902,49 @@
         </is>
       </c>
       <c r="B30">
-        <v>238.642880120907</v>
+        <v>273.715249449492</v>
       </c>
       <c r="C30">
-        <v>3.63024180885036</v>
+        <v>3.74114341086937</v>
       </c>
       <c r="D30">
-        <v>5.71365778480317</v>
+        <v>3.2824882602077</v>
       </c>
       <c r="E30">
-        <v>15.2953955790166</v>
+        <v>15.4835213881129</v>
       </c>
       <c r="F30">
-        <v>1.27984135192145</v>
+        <v>1.94884534501563</v>
       </c>
       <c r="G30">
-        <v>5.12900959775889</v>
+        <v>4.45774210385011</v>
       </c>
       <c r="H30">
-        <v>6.04241999681927</v>
+        <v>7.15485294631908</v>
       </c>
       <c r="I30">
-        <v>2.44103531408558</v>
+        <v>2.52323229399379</v>
       </c>
       <c r="J30">
-        <v>19.1932765729743</v>
+        <v>18.0929896691453</v>
       </c>
       <c r="K30">
-        <v>12.8792722391933</v>
+        <v>12.9735475879937</v>
       </c>
       <c r="L30">
-        <v>44.7975303424017</v>
+        <v>39.5479088750247</v>
       </c>
       <c r="M30">
-        <v>10.8774180927892</v>
+        <v>11.8435444513531</v>
       </c>
       <c r="N30">
-        <v>14.8333306273958</v>
+        <v>11.9360549608928</v>
       </c>
       <c r="O30">
-        <v>494.844203654774</v>
+        <v>468.322334026876</v>
       </c>
       <c r="P30">
-        <v>7.70994607465328</v>
+        <v>6.5759432368554</v>
       </c>
     </row>
     <row r="31">
@@ -1954,49 +1954,49 @@
         </is>
       </c>
       <c r="B31">
-        <v>2013.36118967104</v>
+        <v>2341.51190889262</v>
       </c>
       <c r="C31">
-        <v>48.4723641482807</v>
+        <v>34.3651913825845</v>
       </c>
       <c r="D31">
-        <v>50.1578796749282</v>
+        <v>48.929238392491</v>
       </c>
       <c r="E31">
-        <v>31.0089629413327</v>
+        <v>19.1506245318903</v>
       </c>
       <c r="F31">
-        <v>12.6640924112532</v>
+        <v>4.53928834467387</v>
       </c>
       <c r="G31">
-        <v>153.816452636988</v>
+        <v>144.681666153988</v>
       </c>
       <c r="H31">
-        <v>30.2543692340789</v>
+        <v>28.0983665174497</v>
       </c>
       <c r="I31">
-        <v>27.2161656306248</v>
+        <v>23.1033271028439</v>
       </c>
       <c r="J31">
-        <v>41.2986907595629</v>
+        <v>61.2047811257363</v>
       </c>
       <c r="K31">
-        <v>42.1816858911589</v>
+        <v>35.3203526417977</v>
       </c>
       <c r="L31">
-        <v>62.0838949439208</v>
+        <v>57.7077526746936</v>
       </c>
       <c r="M31">
-        <v>32.8164917659235</v>
+        <v>24.8784185798862</v>
       </c>
       <c r="N31">
-        <v>73.4616643684699</v>
+        <v>67.17885198655161</v>
       </c>
       <c r="O31">
-        <v>3411.6557052288</v>
+        <v>3114.13957551483</v>
       </c>
       <c r="P31">
-        <v>11.9430345945625</v>
+        <v>15.4356532253774</v>
       </c>
     </row>
     <row r="32">
@@ -2006,49 +2006,49 @@
         </is>
       </c>
       <c r="B32">
-        <v>472.194927448305</v>
+        <v>544.806973147952</v>
       </c>
       <c r="C32">
-        <v>5.1252299979585</v>
+        <v>6.90463173478512</v>
       </c>
       <c r="D32">
-        <v>4.16775111158591</v>
+        <v>1.73115558616517</v>
       </c>
       <c r="E32">
-        <v>2.56057320092988</v>
+        <v>6.45495820009002</v>
       </c>
       <c r="F32">
-        <v>22.1924050487563</v>
+        <v>19.9456803481976</v>
       </c>
       <c r="G32">
-        <v>2.46434981852006</v>
+        <v>1.05049057098112</v>
       </c>
       <c r="H32">
-        <v>1.39559491329261</v>
+        <v>0.997706616178785</v>
       </c>
       <c r="I32">
-        <v>3.54213638452072</v>
+        <v>2.47960658258764</v>
       </c>
       <c r="J32">
-        <v>1.72141153352432</v>
+        <v>2.65398785559485</v>
       </c>
       <c r="K32">
-        <v>4.76381227386727</v>
+        <v>4.98411679389166</v>
       </c>
       <c r="L32">
-        <v>13.7395844067481</v>
+        <v>13.383781713661</v>
       </c>
       <c r="M32">
-        <v>6.10570904310519</v>
+        <v>5.95539061370651</v>
       </c>
       <c r="N32">
-        <v>11.4775860269267</v>
+        <v>13.048623315274</v>
       </c>
       <c r="O32">
-        <v>681.3548783172801</v>
+        <v>627.083856147735</v>
       </c>
       <c r="P32">
-        <v>37.0778649708015</v>
+        <v>23.5385791459215</v>
       </c>
     </row>
     <row r="33">
@@ -2058,49 +2058,49 @@
         </is>
       </c>
       <c r="B33">
-        <v>5012.597192907711</v>
+        <v>5752.49760211066</v>
       </c>
       <c r="C33">
-        <v>87.0874854488363</v>
+        <v>75.1201668443006</v>
       </c>
       <c r="D33">
-        <v>142.029140519144</v>
+        <v>94.7687900137968</v>
       </c>
       <c r="E33">
-        <v>92.102533480625</v>
+        <v>73.0417575410241</v>
       </c>
       <c r="F33">
-        <v>12.2237180255138</v>
+        <v>13.9961634337732</v>
       </c>
       <c r="G33">
-        <v>80.5499878083095</v>
+        <v>94.73252305010431</v>
       </c>
       <c r="H33">
-        <v>49.0205923544595</v>
+        <v>39.7906448363262</v>
       </c>
       <c r="I33">
-        <v>46.5828010850323</v>
+        <v>48.6299685872854</v>
       </c>
       <c r="J33">
-        <v>121.105592490636</v>
+        <v>128.191759830887</v>
       </c>
       <c r="K33">
-        <v>123.811795380308</v>
+        <v>110.717577743486</v>
       </c>
       <c r="L33">
-        <v>144.939428286565</v>
+        <v>137.514141846798</v>
       </c>
       <c r="M33">
-        <v>94.68629204525401</v>
+        <v>72.052211404349</v>
       </c>
       <c r="N33">
-        <v>157.522707838628</v>
+        <v>158.120060025903</v>
       </c>
       <c r="O33">
-        <v>7395.89272351457</v>
+        <v>6805.63174637968</v>
       </c>
       <c r="P33">
-        <v>87.1164208132151</v>
+        <v>74.05555179055639</v>
       </c>
     </row>
     <row r="34">
@@ -2110,49 +2110,49 @@
         </is>
       </c>
       <c r="B34">
-        <v>1768.56193966229</v>
+        <v>2035.94049069297</v>
       </c>
       <c r="C34">
-        <v>85.5114759413464</v>
+        <v>87.3232185615117</v>
       </c>
       <c r="D34">
-        <v>233.999622069114</v>
+        <v>204.675066073952</v>
       </c>
       <c r="E34">
-        <v>85.18613866198601</v>
+        <v>77.9248014381687</v>
       </c>
       <c r="F34">
-        <v>7.43878045499278</v>
+        <v>6.914745631755</v>
       </c>
       <c r="G34">
-        <v>72.6976509182274</v>
+        <v>45.8371381395963</v>
       </c>
       <c r="H34">
-        <v>49.0396544623566</v>
+        <v>51.0465912029942</v>
       </c>
       <c r="I34">
-        <v>30.5982142492891</v>
+        <v>36.3525372835738</v>
       </c>
       <c r="J34">
-        <v>56.8148671955168</v>
+        <v>46.3116834091425</v>
       </c>
       <c r="K34">
-        <v>63.7284428777263</v>
+        <v>49.3548237789891</v>
       </c>
       <c r="L34">
-        <v>113.199008458369</v>
+        <v>108.351905162913</v>
       </c>
       <c r="M34">
-        <v>58.6890593117381</v>
+        <v>53.4251862529864</v>
       </c>
       <c r="N34">
-        <v>137.697749634928</v>
+        <v>123.821438807033</v>
       </c>
       <c r="O34">
-        <v>2834.00831389223</v>
+        <v>2682.64404136704</v>
       </c>
       <c r="P34">
-        <v>61.9639821519707</v>
+        <v>57.2810088334396</v>
       </c>
     </row>
     <row r="35">
@@ -2162,49 +2162,49 @@
         </is>
       </c>
       <c r="B35">
-        <v>128.95036142207</v>
+        <v>158.657494105908</v>
       </c>
       <c r="C35">
-        <v>7.24089857981667</v>
+        <v>5.62892603959335</v>
       </c>
       <c r="D35">
-        <v>0.948363356050159</v>
+        <v>1.06978385152138</v>
       </c>
       <c r="E35">
-        <v>1.79271952655058</v>
+        <v>0.7629365038348031</v>
       </c>
       <c r="F35">
-        <v>5.49379777274914</v>
+        <v>5.78047047483491</v>
       </c>
       <c r="G35">
-        <v>0.445167024330014</v>
+        <v>0.783968513319689</v>
       </c>
       <c r="H35">
-        <v>0.609225537433419</v>
+        <v>0.461877098689284</v>
       </c>
       <c r="I35">
-        <v>1.05551563281556</v>
+        <v>0.777710694111396</v>
       </c>
       <c r="J35">
-        <v>1.64199691493016</v>
+        <v>2.09408786957575</v>
       </c>
       <c r="K35">
-        <v>6.02984532830725</v>
+        <v>5.02883979914715</v>
       </c>
       <c r="L35">
-        <v>2.78871408361419</v>
+        <v>2.89103164060593</v>
       </c>
       <c r="M35">
-        <v>1.99302712460928</v>
+        <v>1.77715664005682</v>
       </c>
       <c r="N35">
-        <v>2.53345519220419</v>
+        <v>2.03586545664026</v>
       </c>
       <c r="O35">
-        <v>250.855072089996</v>
+        <v>237.30251595353</v>
       </c>
       <c r="P35">
-        <v>44.5336200295281</v>
+        <v>39.1992446185905</v>
       </c>
     </row>
     <row r="36">
@@ -2214,49 +2214,49 @@
         </is>
       </c>
       <c r="B36">
-        <v>2592.16636489649</v>
+        <v>2918.03235297784</v>
       </c>
       <c r="C36">
-        <v>68.7500258475195</v>
+        <v>68.626274389537</v>
       </c>
       <c r="D36">
-        <v>24.1096645025117</v>
+        <v>14.1943014370054</v>
       </c>
       <c r="E36">
-        <v>88.0325203688637</v>
+        <v>79.43678292205919</v>
       </c>
       <c r="F36">
-        <v>32.4620866271299</v>
+        <v>33.9029463101044</v>
       </c>
       <c r="G36">
-        <v>94.67272886773201</v>
+        <v>88.2353786934584</v>
       </c>
       <c r="H36">
-        <v>129.021598759137</v>
+        <v>138.986479091093</v>
       </c>
       <c r="I36">
-        <v>45.0833465656789</v>
+        <v>36.3819405086144</v>
       </c>
       <c r="J36">
-        <v>282.556835214462</v>
+        <v>259.4936071402</v>
       </c>
       <c r="K36">
-        <v>157.655162840797</v>
+        <v>163.943663472377</v>
       </c>
       <c r="L36">
-        <v>114.680780981943</v>
+        <v>102.572671077242</v>
       </c>
       <c r="M36">
-        <v>257.896968103441</v>
+        <v>222.368541812484</v>
       </c>
       <c r="N36">
-        <v>84.5396801114574</v>
+        <v>95.3806382193402</v>
       </c>
       <c r="O36">
-        <v>4042.84871809497</v>
+        <v>3793.52260972815</v>
       </c>
       <c r="P36">
-        <v>69.8511915585388</v>
+        <v>54.1656025343942</v>
       </c>
     </row>
     <row r="37">
@@ -2266,49 +2266,49 @@
         </is>
       </c>
       <c r="B37">
-        <v>862.241889316996</v>
+        <v>960.415627128731</v>
       </c>
       <c r="C37">
-        <v>20.5238966222511</v>
+        <v>23.6401264565384</v>
       </c>
       <c r="D37">
-        <v>15.6792161710433</v>
+        <v>14.9278732964563</v>
       </c>
       <c r="E37">
-        <v>19.5299547786147</v>
+        <v>16.8873930618606</v>
       </c>
       <c r="F37">
-        <v>48.1304623070966</v>
+        <v>50.5617845833257</v>
       </c>
       <c r="G37">
-        <v>4.86334602265598</v>
+        <v>4.53051574682526</v>
       </c>
       <c r="H37">
-        <v>21.4920137988735</v>
+        <v>17.8650312677089</v>
       </c>
       <c r="I37">
-        <v>11.3637257121944</v>
+        <v>6.77913601764803</v>
       </c>
       <c r="J37">
-        <v>36.5335155366321</v>
+        <v>38.2477262152685</v>
       </c>
       <c r="K37">
-        <v>30.2900651122861</v>
+        <v>24.3872251806654</v>
       </c>
       <c r="L37">
-        <v>27.2905807801095</v>
+        <v>28.1745353351013</v>
       </c>
       <c r="M37">
-        <v>33.7199334438467</v>
+        <v>34.5889333756377</v>
       </c>
       <c r="N37">
-        <v>21.9803556064496</v>
+        <v>15.8286470937101</v>
       </c>
       <c r="O37">
-        <v>1199.90408212405</v>
+        <v>1116.18612869962</v>
       </c>
       <c r="P37">
-        <v>62.8947404943607</v>
+        <v>55.4410834312764</v>
       </c>
     </row>
     <row r="38">
@@ -2318,49 +2318,49 @@
         </is>
       </c>
       <c r="B38">
-        <v>775.752414489335</v>
+        <v>940.560263206573</v>
       </c>
       <c r="C38">
-        <v>26.6608068959587</v>
+        <v>21.7622281669399</v>
       </c>
       <c r="D38">
-        <v>11.6965369031343</v>
+        <v>11.9603400017292</v>
       </c>
       <c r="E38">
-        <v>61.9120136656863</v>
+        <v>61.8447276935806</v>
       </c>
       <c r="F38">
-        <v>2.19924846850928</v>
+        <v>2.05510722232459</v>
       </c>
       <c r="G38">
-        <v>7.87666980489302</v>
+        <v>6.47340603227969</v>
       </c>
       <c r="H38">
-        <v>7.81506918504638</v>
+        <v>3.82556205795488</v>
       </c>
       <c r="I38">
-        <v>6.83523200644018</v>
+        <v>3.96146554782686</v>
       </c>
       <c r="J38">
-        <v>32.267763928007</v>
+        <v>34.1593137186668</v>
       </c>
       <c r="K38">
-        <v>19.0786380258014</v>
+        <v>13.9241376682707</v>
       </c>
       <c r="L38">
-        <v>62.3717530688974</v>
+        <v>49.2407852580723</v>
       </c>
       <c r="M38">
-        <v>23.4510628894178</v>
+        <v>22.927814894731</v>
       </c>
       <c r="N38">
-        <v>27.2439536505525</v>
+        <v>17.1731930494405</v>
       </c>
       <c r="O38">
-        <v>1299.65091663527</v>
+        <v>1218.6099247836</v>
       </c>
       <c r="P38">
-        <v>68.9722948409795</v>
+        <v>55.9146184946458</v>
       </c>
     </row>
     <row r="39">
@@ -2370,49 +2370,49 @@
         </is>
       </c>
       <c r="B39">
-        <v>3017.68341008883</v>
+        <v>3441.41079234574</v>
       </c>
       <c r="C39">
-        <v>115.507425552668</v>
+        <v>95.81622959711569</v>
       </c>
       <c r="D39">
-        <v>68.4893789910511</v>
+        <v>57.7974486171868</v>
       </c>
       <c r="E39">
-        <v>112.61142912166</v>
+        <v>103.691378273151</v>
       </c>
       <c r="F39">
-        <v>40.0985451580171</v>
+        <v>45.5802970234375</v>
       </c>
       <c r="G39">
-        <v>109.663376223636</v>
+        <v>106.066077142951</v>
       </c>
       <c r="H39">
-        <v>60.7434806256127</v>
+        <v>59.5629441689842</v>
       </c>
       <c r="I39">
-        <v>58.2055708633203</v>
+        <v>57.2116819570731</v>
       </c>
       <c r="J39">
-        <v>206.636082779735</v>
+        <v>179.940917446408</v>
       </c>
       <c r="K39">
-        <v>118.371842411125</v>
+        <v>89.9599713318653</v>
       </c>
       <c r="L39">
-        <v>138.332038063967</v>
+        <v>120.596074350165</v>
       </c>
       <c r="M39">
-        <v>91.90802965119831</v>
+        <v>68.2116911517973</v>
       </c>
       <c r="N39">
-        <v>103.823673367217</v>
+        <v>111.472944172054</v>
       </c>
       <c r="O39">
-        <v>4466.77186111482</v>
+        <v>4178.44352745185</v>
       </c>
       <c r="P39">
-        <v>80.2398250479914</v>
+        <v>71.0749525040427</v>
       </c>
     </row>
     <row r="40">
@@ -2422,49 +2422,49 @@
         </is>
       </c>
       <c r="B40">
-        <v>246.453570694857</v>
+        <v>290.676799109307</v>
       </c>
       <c r="C40">
-        <v>3.83207895878129</v>
+        <v>5.27319902837602</v>
       </c>
       <c r="D40">
-        <v>9.991406649741499</v>
+        <v>9.317677739313441</v>
       </c>
       <c r="E40">
-        <v>4.12281248377772</v>
+        <v>2.58261593324653</v>
       </c>
       <c r="F40">
-        <v>2.30991207275283</v>
+        <v>2.69837368131965</v>
       </c>
       <c r="G40">
-        <v>3.36834200987919</v>
+        <v>4.19456209611584</v>
       </c>
       <c r="H40">
-        <v>6.96154910914895</v>
+        <v>5.19631489127464</v>
       </c>
       <c r="I40">
-        <v>2.15192681265482</v>
+        <v>1.91002058903826</v>
       </c>
       <c r="J40">
-        <v>11.9718423153184</v>
+        <v>12.1634570404107</v>
       </c>
       <c r="K40">
-        <v>5.57480130304296</v>
+        <v>5.66902336872352</v>
       </c>
       <c r="L40">
-        <v>16.8848787778411</v>
+        <v>13.6840745026048</v>
       </c>
       <c r="M40">
-        <v>9.697381165961099</v>
+        <v>6.11987841202484</v>
       </c>
       <c r="N40">
-        <v>25.9158665281709</v>
+        <v>23.1335831789624</v>
       </c>
       <c r="O40">
-        <v>391.107306660411</v>
+        <v>362.861595374907</v>
       </c>
       <c r="P40">
-        <v>2.40730232203336</v>
+        <v>2.97109892366523</v>
       </c>
     </row>
     <row r="41">
@@ -2474,49 +2474,49 @@
         </is>
       </c>
       <c r="B41">
-        <v>941.545663209249</v>
+        <v>1095.74303480327</v>
       </c>
       <c r="C41">
-        <v>16.6710212855087</v>
+        <v>13.1752353241587</v>
       </c>
       <c r="D41">
-        <v>120.366395866644</v>
+        <v>101.606841911268</v>
       </c>
       <c r="E41">
-        <v>56.0479954773348</v>
+        <v>43.5833310210257</v>
       </c>
       <c r="F41">
-        <v>3.07352732158895</v>
+        <v>3.30070711632737</v>
       </c>
       <c r="G41">
-        <v>36.7517187012578</v>
+        <v>32.3732416622295</v>
       </c>
       <c r="H41">
-        <v>35.8731018994364</v>
+        <v>35.7540556431595</v>
       </c>
       <c r="I41">
-        <v>7.6166600719733</v>
+        <v>4.40228214445366</v>
       </c>
       <c r="J41">
-        <v>45.6044967877285</v>
+        <v>34.7932229864233</v>
       </c>
       <c r="K41">
-        <v>48.5300545167765</v>
+        <v>46.1893749672906</v>
       </c>
       <c r="L41">
-        <v>27.3257509481344</v>
+        <v>22.2613475018944</v>
       </c>
       <c r="M41">
-        <v>39.6050059609986</v>
+        <v>33.9403934392502</v>
       </c>
       <c r="N41">
-        <v>26.0981685025949</v>
+        <v>18.0194325651692</v>
       </c>
       <c r="O41">
-        <v>1353.85396544145</v>
+        <v>1294.64534841308</v>
       </c>
       <c r="P41">
-        <v>22.9481604402163</v>
+        <v>14.4244718702768</v>
       </c>
     </row>
     <row r="42">
@@ -2526,49 +2526,49 @@
         </is>
       </c>
       <c r="B42">
-        <v>142.174373342604</v>
+        <v>169.132085500394</v>
       </c>
       <c r="C42">
-        <v>8.94398383448903</v>
+        <v>9.81939382279824</v>
       </c>
       <c r="D42">
-        <v>2.26857383962846</v>
+        <v>1.29846829366444</v>
       </c>
       <c r="E42">
-        <v>5.10711998428148</v>
+        <v>5.13546922740644</v>
       </c>
       <c r="F42">
-        <v>1.84084217035186</v>
+        <v>1.82678346118098</v>
       </c>
       <c r="G42">
-        <v>0.915857834595745</v>
+        <v>0.804072572456488</v>
       </c>
       <c r="H42">
-        <v>1.80750502089786</v>
+        <v>2.46748692171641</v>
       </c>
       <c r="I42">
-        <v>1.17427935272739</v>
+        <v>1.124811745453</v>
       </c>
       <c r="J42">
-        <v>3.79007332648863</v>
+        <v>3.89514715456642</v>
       </c>
       <c r="K42">
-        <v>7.66134503267897</v>
+        <v>7.46397629342492</v>
       </c>
       <c r="L42">
-        <v>7.91306047040003</v>
+        <v>5.94687498384549</v>
       </c>
       <c r="M42">
-        <v>2.98940139059281</v>
+        <v>3.17697536887735</v>
       </c>
       <c r="N42">
-        <v>8.772860081021159</v>
+        <v>5.84019768190719</v>
       </c>
       <c r="O42">
-        <v>285.658919911771</v>
+        <v>260.989941165335</v>
       </c>
       <c r="P42">
-        <v>46.2927454328257</v>
+        <v>46.4914820867376</v>
       </c>
     </row>
     <row r="43">
@@ -2578,49 +2578,49 @@
         </is>
       </c>
       <c r="B43">
-        <v>1394.12413607078</v>
+        <v>1563.04523722246</v>
       </c>
       <c r="C43">
-        <v>43.1124173515606</v>
+        <v>50.4639662881845</v>
       </c>
       <c r="D43">
-        <v>55.6181972743879</v>
+        <v>45.8230862648332</v>
       </c>
       <c r="E43">
-        <v>69.4761510271366</v>
+        <v>68.736558453195</v>
       </c>
       <c r="F43">
-        <v>10.8901866142274</v>
+        <v>11.9509376745373</v>
       </c>
       <c r="G43">
-        <v>31.9633529213219</v>
+        <v>22.9564016444186</v>
       </c>
       <c r="H43">
-        <v>40.8223781865671</v>
+        <v>46.6174230764291</v>
       </c>
       <c r="I43">
-        <v>21.8398942225212</v>
+        <v>9.838384236945631</v>
       </c>
       <c r="J43">
-        <v>75.3947304274909</v>
+        <v>69.7749992723483</v>
       </c>
       <c r="K43">
-        <v>53.8148799763959</v>
+        <v>46.5230107181627</v>
       </c>
       <c r="L43">
-        <v>53.9077675569566</v>
+        <v>51.4588269321692</v>
       </c>
       <c r="M43">
-        <v>92.3181491053013</v>
+        <v>80.8407974368612</v>
       </c>
       <c r="N43">
-        <v>70.470933201416</v>
+        <v>82.9091389291613</v>
       </c>
       <c r="O43">
-        <v>1995.80707672749</v>
+        <v>1868.88282934976</v>
       </c>
       <c r="P43">
-        <v>45.1211480323551</v>
+        <v>44.0335518316179</v>
       </c>
     </row>
     <row r="44">
@@ -2630,49 +2630,49 @@
         </is>
       </c>
       <c r="B44">
-        <v>4782.09063368578</v>
+        <v>5497.8744559585</v>
       </c>
       <c r="C44">
-        <v>159.300285216323</v>
+        <v>138.174368203564</v>
       </c>
       <c r="D44">
-        <v>81.81779485295159</v>
+        <v>52.1200025210173</v>
       </c>
       <c r="E44">
-        <v>99.4906044392387</v>
+        <v>115.219923461221</v>
       </c>
       <c r="F44">
-        <v>202.323993409505</v>
+        <v>211.298015692362</v>
       </c>
       <c r="G44">
-        <v>125.991089739101</v>
+        <v>114.055287156095</v>
       </c>
       <c r="H44">
-        <v>64.0872762977888</v>
+        <v>48.8067990086477</v>
       </c>
       <c r="I44">
-        <v>51.8257828679066</v>
+        <v>37.8976009488323</v>
       </c>
       <c r="J44">
-        <v>162.564559741912</v>
+        <v>158.932548700558</v>
       </c>
       <c r="K44">
-        <v>143.374763501216</v>
+        <v>120.271538027647</v>
       </c>
       <c r="L44">
-        <v>253.075445203686</v>
+        <v>227.366634409783</v>
       </c>
       <c r="M44">
-        <v>153.234558802882</v>
+        <v>126.617566009215</v>
       </c>
       <c r="N44">
-        <v>110.239813425414</v>
+        <v>106.043498407156</v>
       </c>
       <c r="O44">
-        <v>7564.76554620421</v>
+        <v>6995.952771741</v>
       </c>
       <c r="P44">
-        <v>224.085691239365</v>
+        <v>193.401932206129</v>
       </c>
     </row>
     <row r="45">
@@ -2682,49 +2682,49 @@
         </is>
       </c>
       <c r="B45">
-        <v>439.784863720302</v>
+        <v>493.702696445238</v>
       </c>
       <c r="C45">
-        <v>18.6620068904775</v>
+        <v>16.6522044428837</v>
       </c>
       <c r="D45">
-        <v>4.76075310141285</v>
+        <v>3.7364137817531</v>
       </c>
       <c r="E45">
-        <v>12.3782601392585</v>
+        <v>16.9561427626475</v>
       </c>
       <c r="F45">
-        <v>19.1414854281973</v>
+        <v>18.8428465407066</v>
       </c>
       <c r="G45">
-        <v>9.90205058241825</v>
+        <v>6.62662771802735</v>
       </c>
       <c r="H45">
-        <v>4.1397966446952</v>
+        <v>3.41254768309029</v>
       </c>
       <c r="I45">
-        <v>6.42384243730407</v>
+        <v>8.62737936032741</v>
       </c>
       <c r="J45">
-        <v>18.0611292229923</v>
+        <v>18.7095751482215</v>
       </c>
       <c r="K45">
-        <v>14.2185844746379</v>
+        <v>15.2939113640989</v>
       </c>
       <c r="L45">
-        <v>24.8809717657525</v>
+        <v>20.224822312847</v>
       </c>
       <c r="M45">
-        <v>28.0709174675773</v>
+        <v>30.1248325376175</v>
       </c>
       <c r="N45">
-        <v>26.795173488612</v>
+        <v>17.4504354497761</v>
       </c>
       <c r="O45">
-        <v>842.156717048613</v>
+        <v>803.483828894045</v>
       </c>
       <c r="P45">
-        <v>17.9714332570821</v>
+        <v>12.6467807004119</v>
       </c>
     </row>
     <row r="46">
@@ -2734,49 +2734,49 @@
         </is>
       </c>
       <c r="B46">
-        <v>114.806539237672</v>
+        <v>138.014144787009</v>
       </c>
       <c r="C46">
-        <v>5.25466518628602</v>
+        <v>4.17987549465483</v>
       </c>
       <c r="D46">
-        <v>1.66759606372999</v>
+        <v>1.3881744267284</v>
       </c>
       <c r="E46">
-        <v>7.32203121518098</v>
+        <v>6.74225274056354</v>
       </c>
       <c r="F46">
-        <v>1.06745581250564</v>
+        <v>1.50989647203372</v>
       </c>
       <c r="G46">
-        <v>1.02113908237002</v>
+        <v>0.776815404589873</v>
       </c>
       <c r="H46">
-        <v>1.25806418139033</v>
+        <v>1.21617859970584</v>
       </c>
       <c r="I46">
-        <v>2.29827933330863</v>
+        <v>1.67479682913084</v>
       </c>
       <c r="J46">
-        <v>5.24885105247168</v>
+        <v>4.56782559745289</v>
       </c>
       <c r="K46">
-        <v>4.48731621165011</v>
+        <v>4.97623531963489</v>
       </c>
       <c r="L46">
-        <v>10.6731662907813</v>
+        <v>9.791980831463</v>
       </c>
       <c r="M46">
-        <v>5.14258387185157</v>
+        <v>2.94979117571248</v>
       </c>
       <c r="N46">
-        <v>6.841357978697</v>
+        <v>7.40661482868365</v>
       </c>
       <c r="O46">
-        <v>248.953815352082</v>
+        <v>234.369133216757</v>
       </c>
       <c r="P46">
-        <v>12.2233750747162</v>
+        <v>11.0125207566563</v>
       </c>
     </row>
     <row r="47">
@@ -2786,49 +2786,49 @@
         </is>
       </c>
       <c r="B47">
-        <v>1524.73538823644</v>
+        <v>1772.55732260799</v>
       </c>
       <c r="C47">
-        <v>63.6218307647423</v>
+        <v>67.562707382413</v>
       </c>
       <c r="D47">
-        <v>49.1455174704506</v>
+        <v>44.7848270042756</v>
       </c>
       <c r="E47">
-        <v>71.9210169354009</v>
+        <v>63.7706118404315</v>
       </c>
       <c r="F47">
-        <v>16.9799380218521</v>
+        <v>11.0995113849858</v>
       </c>
       <c r="G47">
-        <v>31.5372174316409</v>
+        <v>21.7119257688613</v>
       </c>
       <c r="H47">
-        <v>28.9361699943764</v>
+        <v>27.4605807693532</v>
       </c>
       <c r="I47">
-        <v>16.3579480452625</v>
+        <v>13.3888512369548</v>
       </c>
       <c r="J47">
-        <v>46.6132307299132</v>
+        <v>32.1732153315328</v>
       </c>
       <c r="K47">
-        <v>39.7130545514734</v>
+        <v>26.294492784504</v>
       </c>
       <c r="L47">
-        <v>52.1843704372965</v>
+        <v>48.2965922624728</v>
       </c>
       <c r="M47">
-        <v>83.71199031921461</v>
+        <v>77.5818899472562</v>
       </c>
       <c r="N47">
-        <v>51.2857922411359</v>
+        <v>48.0861195999813</v>
       </c>
       <c r="O47">
-        <v>2796.58205598791</v>
+        <v>2599.19720365344</v>
       </c>
       <c r="P47">
-        <v>46.0261940732223</v>
+        <v>43.3225924305097</v>
       </c>
     </row>
     <row r="48">
@@ -2838,49 +2838,49 @@
         </is>
       </c>
       <c r="B48">
-        <v>1309.6308579879</v>
+        <v>1466.79654150542</v>
       </c>
       <c r="C48">
-        <v>24.350390083078</v>
+        <v>33.667170213155</v>
       </c>
       <c r="D48">
-        <v>12.1147980761831</v>
+        <v>13.6186750845519</v>
       </c>
       <c r="E48">
-        <v>66.81725802321419</v>
+        <v>56.7295433741466</v>
       </c>
       <c r="F48">
-        <v>13.3629247528586</v>
+        <v>10.674395666433</v>
       </c>
       <c r="G48">
-        <v>17.5285624274745</v>
+        <v>20.702667403395</v>
       </c>
       <c r="H48">
-        <v>13.3895719757332</v>
+        <v>14.985805675604</v>
       </c>
       <c r="I48">
-        <v>10.0043587763068</v>
+        <v>15.5856313120549</v>
       </c>
       <c r="J48">
-        <v>34.7117572617223</v>
+        <v>37.4242917135192</v>
       </c>
       <c r="K48">
-        <v>17.8594889062592</v>
+        <v>16.4462865216041</v>
       </c>
       <c r="L48">
-        <v>46.3872792205469</v>
+        <v>34.8344605563596</v>
       </c>
       <c r="M48">
-        <v>159.923858825688</v>
+        <v>158.771600068597</v>
       </c>
       <c r="N48">
-        <v>21.6806168766802</v>
+        <v>17.2547885298895</v>
       </c>
       <c r="O48">
-        <v>2285.17816156041</v>
+        <v>2124.0632517552</v>
       </c>
       <c r="P48">
-        <v>112.790780393233</v>
+        <v>111.575647788196</v>
       </c>
     </row>
     <row r="49">
@@ -2890,49 +2890,49 @@
         </is>
       </c>
       <c r="B49">
-        <v>592.087640663053</v>
+        <v>660.3704075278</v>
       </c>
       <c r="C49">
-        <v>9.242279699262999</v>
+        <v>10.1939047203271</v>
       </c>
       <c r="D49">
-        <v>5.71144252421068</v>
+        <v>5.12469007586626</v>
       </c>
       <c r="E49">
-        <v>11.6254551208439</v>
+        <v>8.48103367432301</v>
       </c>
       <c r="F49">
-        <v>33.7796890831646</v>
+        <v>31.9790345062709</v>
       </c>
       <c r="G49">
-        <v>16.3911202187802</v>
+        <v>15.4988101337927</v>
       </c>
       <c r="H49">
-        <v>5.18991093936247</v>
+        <v>9.968470308973821</v>
       </c>
       <c r="I49">
-        <v>9.735957097699989</v>
+        <v>8.378026329302671</v>
       </c>
       <c r="J49">
-        <v>22.1289304416686</v>
+        <v>18.406125008158</v>
       </c>
       <c r="K49">
-        <v>10.3758488864476</v>
+        <v>8.89069432939754</v>
       </c>
       <c r="L49">
-        <v>5.07938246208108</v>
+        <v>4.47043019615571</v>
       </c>
       <c r="M49">
-        <v>7.69252338334858</v>
+        <v>5.14528020080295</v>
       </c>
       <c r="N49">
-        <v>4.61519368093179</v>
+        <v>4.3853642620461</v>
       </c>
       <c r="O49">
-        <v>600.512886118303</v>
+        <v>557.9889146123689</v>
       </c>
       <c r="P49">
-        <v>10.2864943254592</v>
+        <v>8.987026801889691</v>
       </c>
     </row>
     <row r="50">
@@ -2942,49 +2942,49 @@
         </is>
       </c>
       <c r="B50">
-        <v>999.666798395548</v>
+        <v>1166.8487522818</v>
       </c>
       <c r="C50">
-        <v>88.7908507091316</v>
+        <v>96.68782084422089</v>
       </c>
       <c r="D50">
-        <v>9.96199349843215</v>
+        <v>13.0300152912046</v>
       </c>
       <c r="E50">
-        <v>135.290901496771</v>
+        <v>147.216880500021</v>
       </c>
       <c r="F50">
-        <v>3.49536066593503</v>
+        <v>2.06815025113376</v>
       </c>
       <c r="G50">
-        <v>21.7485412827463</v>
+        <v>12.8205409809565</v>
       </c>
       <c r="H50">
-        <v>37.8606047746954</v>
+        <v>44.8174807913493</v>
       </c>
       <c r="I50">
-        <v>21.0703890426082</v>
+        <v>17.1209807889117</v>
       </c>
       <c r="J50">
-        <v>113.088907965751</v>
+        <v>92.2434536833881</v>
       </c>
       <c r="K50">
-        <v>123.018001272053</v>
+        <v>91.9982054184246</v>
       </c>
       <c r="L50">
-        <v>86.0583966339043</v>
+        <v>81.1246123884743</v>
       </c>
       <c r="M50">
-        <v>49.1574175477836</v>
+        <v>38.6464364975839</v>
       </c>
       <c r="N50">
-        <v>69.7155264217011</v>
+        <v>53.7170557635057</v>
       </c>
       <c r="O50">
-        <v>1879.64147445941</v>
+        <v>1782.76966144858</v>
       </c>
       <c r="P50">
-        <v>137.182113957133</v>
+        <v>132.531394216704</v>
       </c>
     </row>
     <row r="51">
@@ -2994,49 +2994,49 @@
         </is>
       </c>
       <c r="B51">
-        <v>104.408110010767</v>
+        <v>124.24089872544</v>
       </c>
       <c r="C51">
-        <v>1.52619094276783</v>
+        <v>1.14435038062557</v>
       </c>
       <c r="D51">
-        <v>0.52887984379797</v>
+        <v>0.652771059409504</v>
       </c>
       <c r="E51">
-        <v>1.94468388312922</v>
+        <v>2.49280810011417</v>
       </c>
       <c r="F51">
-        <v>24.0898484435674</v>
+        <v>22.649862344845</v>
       </c>
       <c r="G51">
-        <v>2.33575871736937</v>
+        <v>2.65266101720093</v>
       </c>
       <c r="H51">
-        <v>0.329489494687851</v>
+        <v>0.140857755365367</v>
       </c>
       <c r="I51">
-        <v>0.816283024029805</v>
+        <v>1.34919619300345</v>
       </c>
       <c r="J51">
-        <v>1.8646715679801</v>
+        <v>0.87644258012421</v>
       </c>
       <c r="K51">
-        <v>0.949020601096269</v>
+        <v>1.29874588795464</v>
       </c>
       <c r="L51">
-        <v>0.719235805800686</v>
+        <v>0.478579324339376</v>
       </c>
       <c r="M51">
-        <v>0.910154415259588</v>
+        <v>0.8330097349325341</v>
       </c>
       <c r="N51">
-        <v>1.65865336203325</v>
+        <v>1.32363552257461</v>
       </c>
       <c r="O51">
-        <v>192.281130906559</v>
+        <v>179.94009842276</v>
       </c>
       <c r="P51">
-        <v>14.6767052489716</v>
+        <v>14.1955590052385</v>
       </c>
     </row>
     <row r="52">

</xml_diff>

<commit_message>
re-run baseline no weights census
</commit_message>
<xml_diff>
--- a/1-Data-Codes/2-Final_Data/L_1999.xlsx
+++ b/1-Data-Codes/2-Final_Data/L_1999.xlsx
@@ -446,49 +446,49 @@
         </is>
       </c>
       <c r="B2">
-        <v>1135.18881365623</v>
+        <v>1135.48729347885</v>
       </c>
       <c r="C2">
-        <v>42.3178011847934</v>
+        <v>44.5664218543703</v>
       </c>
       <c r="D2">
-        <v>74.7337735879002</v>
+        <v>81.93327631017161</v>
       </c>
       <c r="E2">
-        <v>63.6785457493553</v>
+        <v>69.5120376030609</v>
       </c>
       <c r="F2">
-        <v>13.4368607340841</v>
+        <v>14.045687576745</v>
       </c>
       <c r="G2">
-        <v>23.5618526923543</v>
+        <v>23.6439519269782</v>
       </c>
       <c r="H2">
-        <v>23.9452243980703</v>
+        <v>24.4617068445191</v>
       </c>
       <c r="I2">
-        <v>15.7906203078371</v>
+        <v>16.1338430068282</v>
       </c>
       <c r="J2">
-        <v>74.3224654278584</v>
+        <v>73.50005732099631</v>
       </c>
       <c r="K2">
-        <v>29.0479281666022</v>
+        <v>29.9780559205028</v>
       </c>
       <c r="L2">
-        <v>32.3772136989468</v>
+        <v>31.7303579987598</v>
       </c>
       <c r="M2">
-        <v>45.4878225041676</v>
+        <v>44.5894873297757</v>
       </c>
       <c r="N2">
-        <v>28.1876811426365</v>
+        <v>29.8762986623722</v>
       </c>
       <c r="O2">
-        <v>1509.9249166291</v>
+        <v>1488.43270487204</v>
       </c>
       <c r="P2">
-        <v>44.0392899361222</v>
+        <v>48.149629110105</v>
       </c>
     </row>
     <row r="3">
@@ -498,49 +498,49 @@
         </is>
       </c>
       <c r="B3">
-        <v>122.134448120069</v>
+        <v>122.187768793274</v>
       </c>
       <c r="C3">
-        <v>5.46097197331019</v>
+        <v>5.60916263484923</v>
       </c>
       <c r="D3">
-        <v>0.318881531563936</v>
+        <v>0.342210936818704</v>
       </c>
       <c r="E3">
-        <v>1.55336542989893</v>
+        <v>1.6521454538564</v>
       </c>
       <c r="F3">
-        <v>11.8313303429281</v>
+        <v>10.882744882506</v>
       </c>
       <c r="G3">
-        <v>0.556343971429742</v>
+        <v>0.484879359510227</v>
       </c>
       <c r="H3">
-        <v>0.187225567982631</v>
+        <v>0.137807384573123</v>
       </c>
       <c r="I3">
-        <v>0.362835433982273</v>
+        <v>0.325649689434762</v>
       </c>
       <c r="J3">
-        <v>0.619021337140772</v>
+        <v>0.6169735126045221</v>
       </c>
       <c r="K3">
-        <v>0.35169274726533</v>
+        <v>0.375601687487167</v>
       </c>
       <c r="L3">
-        <v>0.415467514806318</v>
+        <v>0.373266400650578</v>
       </c>
       <c r="M3">
-        <v>1.14907992877945</v>
+        <v>1.17020342644666</v>
       </c>
       <c r="N3">
-        <v>0.629363077926164</v>
+        <v>0.62666945841026</v>
       </c>
       <c r="O3">
-        <v>250.681682284364</v>
+        <v>249.618269742767</v>
       </c>
       <c r="P3">
-        <v>9.220222529631011</v>
+        <v>11.0685784278885</v>
       </c>
     </row>
     <row r="4">
@@ -550,49 +550,49 @@
         </is>
       </c>
       <c r="B4">
-        <v>1240.74579613221</v>
+        <v>1241.33645830977</v>
       </c>
       <c r="C4">
-        <v>15.4807434792308</v>
+        <v>15.7574779092328</v>
       </c>
       <c r="D4">
-        <v>9.54452215961803</v>
+        <v>9.58051632840885</v>
       </c>
       <c r="E4">
-        <v>23.7243004098078</v>
+        <v>23.8073986645255</v>
       </c>
       <c r="F4">
-        <v>15.1119156731307</v>
+        <v>19.262472214183</v>
       </c>
       <c r="G4">
-        <v>16.009941678993</v>
+        <v>15.8744945923269</v>
       </c>
       <c r="H4">
-        <v>4.00461382176535</v>
+        <v>3.98665170290601</v>
       </c>
       <c r="I4">
-        <v>9.144620049732801</v>
+        <v>9.27081568944285</v>
       </c>
       <c r="J4">
-        <v>20.8963741975786</v>
+        <v>20.9719885228322</v>
       </c>
       <c r="K4">
-        <v>13.7755344362703</v>
+        <v>13.4136780751201</v>
       </c>
       <c r="L4">
-        <v>87.1820667855087</v>
+        <v>83.3226857150629</v>
       </c>
       <c r="M4">
-        <v>65.2106621659395</v>
+        <v>62.7235370263331</v>
       </c>
       <c r="N4">
-        <v>22.1108796294986</v>
+        <v>22.0154096319291</v>
       </c>
       <c r="O4">
-        <v>1966.50073116682</v>
+        <v>1962.27339776396</v>
       </c>
       <c r="P4">
-        <v>29.2227652318479</v>
+        <v>35.0684848719284</v>
       </c>
     </row>
     <row r="5">
@@ -602,49 +602,49 @@
         </is>
       </c>
       <c r="B5">
-        <v>669.8988378240171</v>
+        <v>669.911010555118</v>
       </c>
       <c r="C5">
-        <v>55.3278338426033</v>
+        <v>57.6695753668606</v>
       </c>
       <c r="D5">
-        <v>12.2060704389086</v>
+        <v>13.7111778353737</v>
       </c>
       <c r="E5">
-        <v>43.2462074099102</v>
+        <v>45.9616833386279</v>
       </c>
       <c r="F5">
-        <v>6.38872439093436</v>
+        <v>6.92006781643665</v>
       </c>
       <c r="G5">
-        <v>14.6090648443407</v>
+        <v>15.5036345366593</v>
       </c>
       <c r="H5">
-        <v>13.6936952692507</v>
+        <v>14.446742206714</v>
       </c>
       <c r="I5">
-        <v>7.40122871161231</v>
+        <v>7.45204111681842</v>
       </c>
       <c r="J5">
-        <v>33.4631067057645</v>
+        <v>34.9976000678135</v>
       </c>
       <c r="K5">
-        <v>22.9433455830181</v>
+        <v>23.7279736159094</v>
       </c>
       <c r="L5">
-        <v>24.8167225994503</v>
+        <v>25.3638870307312</v>
       </c>
       <c r="M5">
-        <v>20.3486161406732</v>
+        <v>21.0745001139989</v>
       </c>
       <c r="N5">
-        <v>19.7826177469781</v>
+        <v>20.3440799225031</v>
       </c>
       <c r="O5">
-        <v>872.020631984263</v>
+        <v>848.31555700066</v>
       </c>
       <c r="P5">
-        <v>51.5637574261005</v>
+        <v>62.3109303936003</v>
       </c>
     </row>
     <row r="6">
@@ -654,49 +654,49 @@
         </is>
       </c>
       <c r="B6">
-        <v>8065.62284421136</v>
+        <v>8068.01597138699</v>
       </c>
       <c r="C6">
-        <v>215.613514576068</v>
+        <v>219.153251192781</v>
       </c>
       <c r="D6">
-        <v>220.652935752209</v>
+        <v>221.316412579899</v>
       </c>
       <c r="E6">
-        <v>149.821998287247</v>
+        <v>151.021671220342</v>
       </c>
       <c r="F6">
-        <v>51.9933137971965</v>
+        <v>52.4787379943768</v>
       </c>
       <c r="G6">
-        <v>121.938537732485</v>
+        <v>121.233168936277</v>
       </c>
       <c r="H6">
-        <v>68.6198614406982</v>
+        <v>68.55116461304171</v>
       </c>
       <c r="I6">
-        <v>60.6252347650398</v>
+        <v>60.5702496170953</v>
       </c>
       <c r="J6">
-        <v>214.08642788402</v>
+        <v>213.299138856482</v>
       </c>
       <c r="K6">
-        <v>143.223306672207</v>
+        <v>141.983349781675</v>
       </c>
       <c r="L6">
-        <v>647.130127512445</v>
+        <v>641.317785063782</v>
       </c>
       <c r="M6">
-        <v>292.732747742694</v>
+        <v>290.988419770296</v>
       </c>
       <c r="N6">
-        <v>329.920574943559</v>
+        <v>328.573323559475</v>
       </c>
       <c r="O6">
-        <v>12647.635741177</v>
+        <v>12608.3110662438</v>
       </c>
       <c r="P6">
-        <v>303.265256511425</v>
+        <v>346.068712189263</v>
       </c>
     </row>
     <row r="7">
@@ -706,49 +706,49 @@
         </is>
       </c>
       <c r="B7">
-        <v>798.098059691086</v>
+        <v>799.347927012172</v>
       </c>
       <c r="C7">
-        <v>32.1246437258313</v>
+        <v>33.7837601321617</v>
       </c>
       <c r="D7">
-        <v>4.50722082724485</v>
+        <v>4.42116549982983</v>
       </c>
       <c r="E7">
-        <v>21.3011049505876</v>
+        <v>20.6752326625443</v>
       </c>
       <c r="F7">
-        <v>19.2519386170862</v>
+        <v>21.4907876688862</v>
       </c>
       <c r="G7">
-        <v>9.558465812085849</v>
+        <v>9.169501692979059</v>
       </c>
       <c r="H7">
-        <v>9.23237651824849</v>
+        <v>8.809682261518359</v>
       </c>
       <c r="I7">
-        <v>12.310449351796</v>
+        <v>12.0706994823371</v>
       </c>
       <c r="J7">
-        <v>19.9668065372535</v>
+        <v>19.5315142372735</v>
       </c>
       <c r="K7">
-        <v>24.3798858133587</v>
+        <v>23.6701909897393</v>
       </c>
       <c r="L7">
-        <v>74.5585796072936</v>
+        <v>70.8473377864275</v>
       </c>
       <c r="M7">
-        <v>22.6955834424592</v>
+        <v>21.7385446072222</v>
       </c>
       <c r="N7">
-        <v>30.123482765796</v>
+        <v>28.9405315976424</v>
       </c>
       <c r="O7">
-        <v>1918.83034843363</v>
+        <v>1910.4511464325</v>
       </c>
       <c r="P7">
-        <v>30.986193017169</v>
+        <v>42.9771170477</v>
       </c>
     </row>
     <row r="8">
@@ -758,49 +758,49 @@
         </is>
       </c>
       <c r="B8">
-        <v>732.271086936338</v>
+        <v>732.218840543785</v>
       </c>
       <c r="C8">
-        <v>15.3157234784114</v>
+        <v>15.347169893396</v>
       </c>
       <c r="D8">
-        <v>9.26917632727551</v>
+        <v>9.125014295784951</v>
       </c>
       <c r="E8">
-        <v>23.4498623096123</v>
+        <v>23.9003644591612</v>
       </c>
       <c r="F8">
-        <v>0.634649548590429</v>
+        <v>0.656695187514766</v>
       </c>
       <c r="G8">
-        <v>27.2579537970251</v>
+        <v>26.988771909823</v>
       </c>
       <c r="H8">
-        <v>16.2179567484797</v>
+        <v>16.1365607981953</v>
       </c>
       <c r="I8">
-        <v>3.24328729958166</v>
+        <v>3.33233112396467</v>
       </c>
       <c r="J8">
-        <v>53.2781356550127</v>
+        <v>52.9432643751739</v>
       </c>
       <c r="K8">
-        <v>34.4905398936856</v>
+        <v>34.4317200251243</v>
       </c>
       <c r="L8">
-        <v>43.5594363413017</v>
+        <v>43.1183023802237</v>
       </c>
       <c r="M8">
-        <v>61.6894082520791</v>
+        <v>61.8226971582118</v>
       </c>
       <c r="N8">
-        <v>30.5135722554273</v>
+        <v>30.4357448816717</v>
       </c>
       <c r="O8">
-        <v>1348.38273043871</v>
+        <v>1348.61668729633</v>
       </c>
       <c r="P8">
-        <v>7.53204555197108</v>
+        <v>8.03140050513387</v>
       </c>
     </row>
     <row r="9">
@@ -810,49 +810,49 @@
         </is>
       </c>
       <c r="B9">
-        <v>169.581791390621</v>
+        <v>169.673860070052</v>
       </c>
       <c r="C9">
-        <v>9.525491653512169</v>
+        <v>9.91014311723748</v>
       </c>
       <c r="D9">
-        <v>1.54667802329591</v>
+        <v>1.49323723167674</v>
       </c>
       <c r="E9">
-        <v>4.75823739594938</v>
+        <v>4.98072742935074</v>
       </c>
       <c r="F9">
-        <v>2.20140063814299</v>
+        <v>2.24718923256507</v>
       </c>
       <c r="G9">
-        <v>24.1164832192323</v>
+        <v>23.1039126261056</v>
       </c>
       <c r="H9">
-        <v>4.38324285851102</v>
+        <v>4.40307269101314</v>
       </c>
       <c r="I9">
-        <v>0.475087274203607</v>
+        <v>0.490363954522155</v>
       </c>
       <c r="J9">
-        <v>4.02758079011299</v>
+        <v>3.90931176394084</v>
       </c>
       <c r="K9">
-        <v>3.62932807034281</v>
+        <v>3.49069271823525</v>
       </c>
       <c r="L9">
-        <v>2.08374673738736</v>
+        <v>2.02904884510876</v>
       </c>
       <c r="M9">
-        <v>9.034288557334481</v>
+        <v>8.170240879001749</v>
       </c>
       <c r="N9">
-        <v>4.54567386877641</v>
+        <v>4.64288414095906</v>
       </c>
       <c r="O9">
-        <v>306.068267698569</v>
+        <v>307.099412130316</v>
       </c>
       <c r="P9">
-        <v>5.14379189574991</v>
+        <v>5.4769932416575</v>
       </c>
     </row>
     <row r="10">
@@ -862,49 +862,49 @@
         </is>
       </c>
       <c r="B10">
-        <v>4155.87378432247</v>
+        <v>4156.16788916902</v>
       </c>
       <c r="C10">
-        <v>51.3877483377485</v>
+        <v>52.1304080613648</v>
       </c>
       <c r="D10">
-        <v>40.9781641503937</v>
+        <v>41.3972911230059</v>
       </c>
       <c r="E10">
-        <v>63.4758417112558</v>
+        <v>64.98169018464461</v>
       </c>
       <c r="F10">
-        <v>15.1449788033135</v>
+        <v>15.8252731370916</v>
       </c>
       <c r="G10">
-        <v>44.946116035875</v>
+        <v>45.0673535927581</v>
       </c>
       <c r="H10">
-        <v>22.6568496947612</v>
+        <v>22.9268610530952</v>
       </c>
       <c r="I10">
-        <v>33.7812473404631</v>
+        <v>34.1369317962428</v>
       </c>
       <c r="J10">
-        <v>48.1276450883185</v>
+        <v>48.5380022924371</v>
       </c>
       <c r="K10">
-        <v>50.9994162223429</v>
+        <v>51.7061432172712</v>
       </c>
       <c r="L10">
-        <v>123.989118503279</v>
+        <v>123.59463265336</v>
       </c>
       <c r="M10">
-        <v>91.1772070848089</v>
+        <v>91.9852563087468</v>
       </c>
       <c r="N10">
-        <v>108.538627869107</v>
+        <v>108.211422566353</v>
       </c>
       <c r="O10">
-        <v>6578.13393913221</v>
+        <v>6565.66050358734</v>
       </c>
       <c r="P10">
-        <v>97.62016727326051</v>
+        <v>104.501192826889</v>
       </c>
     </row>
     <row r="11">
@@ -914,49 +914,49 @@
         </is>
       </c>
       <c r="B11">
-        <v>1741.91473615403</v>
+        <v>1740.32681192068</v>
       </c>
       <c r="C11">
-        <v>69.106250247151</v>
+        <v>71.72167381058161</v>
       </c>
       <c r="D11">
-        <v>148.904973868985</v>
+        <v>161.281861663833</v>
       </c>
       <c r="E11">
-        <v>100.322251582501</v>
+        <v>103.482325077325</v>
       </c>
       <c r="F11">
-        <v>11.9711445599424</v>
+        <v>14.2935019641032</v>
       </c>
       <c r="G11">
-        <v>40.2194201411509</v>
+        <v>41.0201773893097</v>
       </c>
       <c r="H11">
-        <v>35.564230341198</v>
+        <v>36.8365010052706</v>
       </c>
       <c r="I11">
-        <v>24.4181682369547</v>
+        <v>24.7521998782634</v>
       </c>
       <c r="J11">
-        <v>47.7170886523411</v>
+        <v>49.5172201415401</v>
       </c>
       <c r="K11">
-        <v>52.9670700772414</v>
+        <v>55.1667165361065</v>
       </c>
       <c r="L11">
-        <v>74.6668901865955</v>
+        <v>73.3706537554673</v>
       </c>
       <c r="M11">
-        <v>74.52131385193169</v>
+        <v>76.68700016380809</v>
       </c>
       <c r="N11">
-        <v>62.9107486166155</v>
+        <v>62.7657141309602</v>
       </c>
       <c r="O11">
-        <v>3147.35150141657</v>
+        <v>3113.82175768112</v>
       </c>
       <c r="P11">
-        <v>46.8155438812274</v>
+        <v>54.3272166960543</v>
       </c>
     </row>
     <row r="12">
@@ -966,49 +966,49 @@
         </is>
       </c>
       <c r="B12">
-        <v>285.34460254059</v>
+        <v>285.42539335805</v>
       </c>
       <c r="C12">
-        <v>7.21712161617232</v>
+        <v>7.49034351551562</v>
       </c>
       <c r="D12">
-        <v>5.33393142569112</v>
+        <v>5.14451592654142</v>
       </c>
       <c r="E12">
-        <v>2.08798825269767</v>
+        <v>2.06884101634215</v>
       </c>
       <c r="F12">
-        <v>0.621285209626775</v>
+        <v>0.6346459717024811</v>
       </c>
       <c r="G12">
-        <v>1.10861745293824</v>
+        <v>1.14811855318093</v>
       </c>
       <c r="H12">
-        <v>0.5771280253971161</v>
+        <v>0.618499445795885</v>
       </c>
       <c r="I12">
-        <v>1.86131082013011</v>
+        <v>1.83156781976234</v>
       </c>
       <c r="J12">
-        <v>0.737091569385229</v>
+        <v>0.736151875467848</v>
       </c>
       <c r="K12">
-        <v>1.10389332281509</v>
+        <v>1.0569870305054</v>
       </c>
       <c r="L12">
-        <v>2.16686435475239</v>
+        <v>2.12654162570377</v>
       </c>
       <c r="M12">
-        <v>4.33865284747964</v>
+        <v>4.20129709986389</v>
       </c>
       <c r="N12">
-        <v>2.02212022391424</v>
+        <v>2.04065245879417</v>
       </c>
       <c r="O12">
-        <v>515.869889931801</v>
+        <v>513.10589910788</v>
       </c>
       <c r="P12">
-        <v>16.8217864902152</v>
+        <v>19.5828292785009</v>
       </c>
     </row>
     <row r="13">
@@ -1018,49 +1018,49 @@
         </is>
       </c>
       <c r="B13">
-        <v>279.521360754267</v>
+        <v>279.316947168336</v>
       </c>
       <c r="C13">
-        <v>25.4739009221648</v>
+        <v>26.4611089985023</v>
       </c>
       <c r="D13">
-        <v>2.1972811231101</v>
+        <v>2.23677356828865</v>
       </c>
       <c r="E13">
-        <v>17.5667140103248</v>
+        <v>18.3439929191514</v>
       </c>
       <c r="F13">
-        <v>3.91629219595469</v>
+        <v>5.34598067884514</v>
       </c>
       <c r="G13">
-        <v>5.87240816893709</v>
+        <v>6.19506229449579</v>
       </c>
       <c r="H13">
-        <v>2.64971236145343</v>
+        <v>2.58661213214654</v>
       </c>
       <c r="I13">
-        <v>2.27957214542785</v>
+        <v>2.24566950764871</v>
       </c>
       <c r="J13">
-        <v>5.28179538502378</v>
+        <v>5.24793327323585</v>
       </c>
       <c r="K13">
-        <v>3.43476306961557</v>
+        <v>3.27294042917227</v>
       </c>
       <c r="L13">
-        <v>27.3950092828702</v>
+        <v>22.7009167501858</v>
       </c>
       <c r="M13">
-        <v>5.91497585900167</v>
+        <v>5.96954665010173</v>
       </c>
       <c r="N13">
-        <v>8.14122341494766</v>
+        <v>7.78715761979447</v>
       </c>
       <c r="O13">
-        <v>465.761047080822</v>
+        <v>460.323475299125</v>
       </c>
       <c r="P13">
-        <v>33.1308122140711</v>
+        <v>40.5027506989631</v>
       </c>
     </row>
     <row r="14">
@@ -1070,49 +1070,49 @@
         </is>
       </c>
       <c r="B14">
-        <v>2607.80041876381</v>
+        <v>2607.66100352227</v>
       </c>
       <c r="C14">
-        <v>109.728449517516</v>
+        <v>111.442745575307</v>
       </c>
       <c r="D14">
-        <v>21.5214670851961</v>
+        <v>21.0089783305342</v>
       </c>
       <c r="E14">
-        <v>97.27234258239621</v>
+        <v>98.4948480897929</v>
       </c>
       <c r="F14">
-        <v>24.3398357894274</v>
+        <v>28.4834110363151</v>
       </c>
       <c r="G14">
-        <v>94.438851080296</v>
+        <v>94.78006208345209</v>
       </c>
       <c r="H14">
-        <v>60.1118137213668</v>
+        <v>63.2946831931367</v>
       </c>
       <c r="I14">
-        <v>40.3123367654725</v>
+        <v>43.0632645240671</v>
       </c>
       <c r="J14">
-        <v>187.318120615459</v>
+        <v>191.669662183732</v>
       </c>
       <c r="K14">
-        <v>175.981185775079</v>
+        <v>186.449804501076</v>
       </c>
       <c r="L14">
-        <v>174.263149491053</v>
+        <v>170.082482634257</v>
       </c>
       <c r="M14">
-        <v>103.003521751381</v>
+        <v>113.526163755925</v>
       </c>
       <c r="N14">
-        <v>103.018428530777</v>
+        <v>102.434491778485</v>
       </c>
       <c r="O14">
-        <v>4893.94129456476</v>
+        <v>4838.25853420331</v>
       </c>
       <c r="P14">
-        <v>71.9838396832991</v>
+        <v>94.38492030563199</v>
       </c>
     </row>
     <row r="15">
@@ -1122,49 +1122,49 @@
         </is>
       </c>
       <c r="B15">
-        <v>1274.24852138504</v>
+        <v>1273.61364549769</v>
       </c>
       <c r="C15">
-        <v>40.7574350406332</v>
+        <v>41.6315463890083</v>
       </c>
       <c r="D15">
-        <v>15.5512419075726</v>
+        <v>16.2038510987569</v>
       </c>
       <c r="E15">
-        <v>59.367444836932</v>
+        <v>62.4873591587808</v>
       </c>
       <c r="F15">
-        <v>13.322758924939</v>
+        <v>13.844326936655</v>
       </c>
       <c r="G15">
-        <v>53.8255190851531</v>
+        <v>51.3646757867811</v>
       </c>
       <c r="H15">
-        <v>53.9579645421384</v>
+        <v>57.3245583253174</v>
       </c>
       <c r="I15">
-        <v>29.9093668991293</v>
+        <v>32.1054084083315</v>
       </c>
       <c r="J15">
-        <v>172.340107180695</v>
+        <v>176.775084555979</v>
       </c>
       <c r="K15">
-        <v>90.8628017601599</v>
+        <v>92.8490908811999</v>
       </c>
       <c r="L15">
-        <v>76.1578616888779</v>
+        <v>79.28391730486641</v>
       </c>
       <c r="M15">
-        <v>180.008750701318</v>
+        <v>187.983756584865</v>
       </c>
       <c r="N15">
-        <v>73.5195488732488</v>
+        <v>79.1721171668276</v>
       </c>
       <c r="O15">
-        <v>2105.99154879748</v>
+        <v>2072.65721027932</v>
       </c>
       <c r="P15">
-        <v>41.0454304332696</v>
+        <v>43.5697536822203</v>
       </c>
     </row>
     <row r="16">
@@ -1174,49 +1174,49 @@
         </is>
       </c>
       <c r="B16">
-        <v>525.2840771028911</v>
+        <v>525.329268196106</v>
       </c>
       <c r="C16">
-        <v>62.2679375080077</v>
+        <v>63.0171667327319</v>
       </c>
       <c r="D16">
-        <v>10.8496908573793</v>
+        <v>11.488939202495</v>
       </c>
       <c r="E16">
-        <v>23.4441395179479</v>
+        <v>23.5847350799749</v>
       </c>
       <c r="F16">
-        <v>4.01702625098515</v>
+        <v>4.75891008257289</v>
       </c>
       <c r="G16">
-        <v>13.1972585052821</v>
+        <v>13.2720732756752</v>
       </c>
       <c r="H16">
-        <v>15.7645511511325</v>
+        <v>16.5512131627371</v>
       </c>
       <c r="I16">
-        <v>12.9177066389516</v>
+        <v>14.0240998242554</v>
       </c>
       <c r="J16">
-        <v>45.8848906347759</v>
+        <v>48.6018234838021</v>
       </c>
       <c r="K16">
-        <v>41.5473272136403</v>
+        <v>43.838089698979</v>
       </c>
       <c r="L16">
-        <v>41.4045464069817</v>
+        <v>40.6937167728265</v>
       </c>
       <c r="M16">
-        <v>21.3329315378442</v>
+        <v>23.4108915605615</v>
       </c>
       <c r="N16">
-        <v>21.9448710499765</v>
+        <v>22.3918788775409</v>
       </c>
       <c r="O16">
-        <v>1137.15163066966</v>
+        <v>1112.9695398154</v>
       </c>
       <c r="P16">
-        <v>75.67304190182971</v>
+        <v>88.7492811816302</v>
       </c>
     </row>
     <row r="17">
@@ -1226,49 +1226,49 @@
         </is>
       </c>
       <c r="B17">
-        <v>518.185838032459</v>
+        <v>517.412802846861</v>
       </c>
       <c r="C17">
-        <v>33.1597948459845</v>
+        <v>31.1941007634496</v>
       </c>
       <c r="D17">
-        <v>6.48428416032837</v>
+        <v>6.28021010183021</v>
       </c>
       <c r="E17">
-        <v>17.6345600749995</v>
+        <v>17.1876199146569</v>
       </c>
       <c r="F17">
-        <v>14.9241369453861</v>
+        <v>16.7923931547689</v>
       </c>
       <c r="G17">
-        <v>15.5409941393631</v>
+        <v>14.9405457214147</v>
       </c>
       <c r="H17">
-        <v>13.8574008756505</v>
+        <v>14.7334895854207</v>
       </c>
       <c r="I17">
-        <v>7.60017091442411</v>
+        <v>7.90698047484265</v>
       </c>
       <c r="J17">
-        <v>19.887156956852</v>
+        <v>21.4984060213313</v>
       </c>
       <c r="K17">
-        <v>26.4484406812223</v>
+        <v>27.5859862247131</v>
       </c>
       <c r="L17">
-        <v>17.2316001474305</v>
+        <v>16.8467274255398</v>
       </c>
       <c r="M17">
-        <v>82.6945607496279</v>
+        <v>78.36599954552629</v>
       </c>
       <c r="N17">
-        <v>15.78010282037</v>
+        <v>15.6929790419982</v>
       </c>
       <c r="O17">
-        <v>1015.80052049418</v>
+        <v>998.403854362566</v>
       </c>
       <c r="P17">
-        <v>54.9979053333502</v>
+        <v>75.38537198671381</v>
       </c>
     </row>
     <row r="18">
@@ -1278,49 +1278,49 @@
         </is>
       </c>
       <c r="B18">
-        <v>1073.55123297812</v>
+        <v>1073.37789210975</v>
       </c>
       <c r="C18">
-        <v>31.2892496787696</v>
+        <v>31.8601436031113</v>
       </c>
       <c r="D18">
-        <v>28.084265483299</v>
+        <v>29.2223734772783</v>
       </c>
       <c r="E18">
-        <v>41.3164909797841</v>
+        <v>41.4155279507991</v>
       </c>
       <c r="F18">
-        <v>32.1991057698849</v>
+        <v>33.5558134698057</v>
       </c>
       <c r="G18">
-        <v>27.8634299467051</v>
+        <v>27.7570779044703</v>
       </c>
       <c r="H18">
-        <v>25.6568684128206</v>
+        <v>25.612380815194</v>
       </c>
       <c r="I18">
-        <v>12.3638247460912</v>
+        <v>12.0258602785601</v>
       </c>
       <c r="J18">
-        <v>46.5266982949393</v>
+        <v>46.5734361699815</v>
       </c>
       <c r="K18">
-        <v>43.5919203837869</v>
+        <v>43.0943727078498</v>
       </c>
       <c r="L18">
-        <v>42.7681644954294</v>
+        <v>42.4744268472089</v>
       </c>
       <c r="M18">
-        <v>68.1798468733557</v>
+        <v>67.24302460349671</v>
       </c>
       <c r="N18">
-        <v>32.990380897135</v>
+        <v>32.789500836758</v>
       </c>
       <c r="O18">
-        <v>1348.02735244854</v>
+        <v>1346.80744490903</v>
       </c>
       <c r="P18">
-        <v>39.8802438219429</v>
+        <v>40.4797995273144</v>
       </c>
     </row>
     <row r="19">
@@ -1330,49 +1330,49 @@
         </is>
       </c>
       <c r="B19">
-        <v>1157.33073806959</v>
+        <v>1157.18700933011</v>
       </c>
       <c r="C19">
-        <v>24.989464643417</v>
+        <v>26.3277212640222</v>
       </c>
       <c r="D19">
-        <v>10.1683425878407</v>
+        <v>10.7678435849071</v>
       </c>
       <c r="E19">
-        <v>33.6460221879987</v>
+        <v>38.8244582465557</v>
       </c>
       <c r="F19">
-        <v>71.81907477490741</v>
+        <v>72.154611395777</v>
       </c>
       <c r="G19">
-        <v>45.4011911129627</v>
+        <v>45.4633679657433</v>
       </c>
       <c r="H19">
-        <v>7.44363293934931</v>
+        <v>7.78389092537919</v>
       </c>
       <c r="I19">
-        <v>9.1574901232744</v>
+        <v>9.340010140509721</v>
       </c>
       <c r="J19">
-        <v>16.9079903623923</v>
+        <v>17.3930253711594</v>
       </c>
       <c r="K19">
-        <v>15.5265661491249</v>
+        <v>15.6611115207748</v>
       </c>
       <c r="L19">
-        <v>10.457165044643</v>
+        <v>10.1075073587769</v>
       </c>
       <c r="M19">
-        <v>32.3990354332521</v>
+        <v>31.2028648999523</v>
       </c>
       <c r="N19">
-        <v>14.6951732807632</v>
+        <v>14.5821743082416</v>
       </c>
       <c r="O19">
-        <v>1605.84995198521</v>
+        <v>1593.99222655993</v>
       </c>
       <c r="P19">
-        <v>35.4680544609767</v>
+        <v>40.4720702838611</v>
       </c>
     </row>
     <row r="20">
@@ -1382,49 +1382,49 @@
         </is>
       </c>
       <c r="B20">
-        <v>290.191096273086</v>
+        <v>290.093414153043</v>
       </c>
       <c r="C20">
-        <v>8.22058540720562</v>
+        <v>8.2928635672263</v>
       </c>
       <c r="D20">
-        <v>16.5079573194346</v>
+        <v>17.6751669020983</v>
       </c>
       <c r="E20">
-        <v>30.2823180145749</v>
+        <v>34.468347803596</v>
       </c>
       <c r="F20">
-        <v>0.528264107045317</v>
+        <v>0.524612423204785</v>
       </c>
       <c r="G20">
-        <v>1.70292488845246</v>
+        <v>1.74424743166042</v>
       </c>
       <c r="H20">
-        <v>3.62152155228363</v>
+        <v>3.45065163589507</v>
       </c>
       <c r="I20">
-        <v>0.8733595331530341</v>
+        <v>0.866444872660783</v>
       </c>
       <c r="J20">
-        <v>7.02343753594825</v>
+        <v>7.01689870947362</v>
       </c>
       <c r="K20">
-        <v>6.32492810547335</v>
+        <v>6.14927569347231</v>
       </c>
       <c r="L20">
-        <v>9.853495875788781</v>
+        <v>8.73906586278334</v>
       </c>
       <c r="M20">
-        <v>18.6945198124802</v>
+        <v>16.7152892699895</v>
       </c>
       <c r="N20">
-        <v>5.83376155222658</v>
+        <v>5.90405233248486</v>
       </c>
       <c r="O20">
-        <v>494.516155261351</v>
+        <v>486.713905261301</v>
       </c>
       <c r="P20">
-        <v>20.5093596148315</v>
+        <v>26.3294489344467</v>
       </c>
     </row>
     <row r="21">
@@ -1434,49 +1434,49 @@
         </is>
       </c>
       <c r="B21">
-        <v>1022.25144180056</v>
+        <v>1021.91760778442</v>
       </c>
       <c r="C21">
-        <v>24.7754130104498</v>
+        <v>25.5911807103292</v>
       </c>
       <c r="D21">
-        <v>14.9076613607593</v>
+        <v>15.9593237691319</v>
       </c>
       <c r="E21">
-        <v>35.452399710902</v>
+        <v>36.3364561863973</v>
       </c>
       <c r="F21">
-        <v>4.75415520058742</v>
+        <v>5.07975346229691</v>
       </c>
       <c r="G21">
-        <v>12.9635070015906</v>
+        <v>12.9271882601696</v>
       </c>
       <c r="H21">
-        <v>21.0617222280265</v>
+        <v>21.7069166797058</v>
       </c>
       <c r="I21">
-        <v>6.19710089281051</v>
+        <v>6.2172226340261</v>
       </c>
       <c r="J21">
-        <v>15.9481377712949</v>
+        <v>16.4454370129543</v>
       </c>
       <c r="K21">
-        <v>23.3257475905414</v>
+        <v>23.8383944731013</v>
       </c>
       <c r="L21">
-        <v>30.7485236834812</v>
+        <v>30.7560855393513</v>
       </c>
       <c r="M21">
-        <v>44.8885621802011</v>
+        <v>44.9105962175723</v>
       </c>
       <c r="N21">
-        <v>13.1019852879852</v>
+        <v>13.1755181815938</v>
       </c>
       <c r="O21">
-        <v>2431.00485286683</v>
+        <v>2424.02901932583</v>
       </c>
       <c r="P21">
-        <v>17.0383542471953</v>
+        <v>19.5288645963408</v>
       </c>
     </row>
     <row r="22">
@@ -1486,49 +1486,49 @@
         </is>
       </c>
       <c r="B22">
-        <v>1320.17250664152</v>
+        <v>1319.92090758344</v>
       </c>
       <c r="C22">
-        <v>27.5192842695545</v>
+        <v>27.4501730007263</v>
       </c>
       <c r="D22">
-        <v>35.7643241037472</v>
+        <v>36.5208529414012</v>
       </c>
       <c r="E22">
-        <v>35.6129558245425</v>
+        <v>37.3131765447563</v>
       </c>
       <c r="F22">
-        <v>3.23037736588833</v>
+        <v>3.57577047264755</v>
       </c>
       <c r="G22">
-        <v>26.5661269755522</v>
+        <v>26.5312134597614</v>
       </c>
       <c r="H22">
-        <v>28.0945421105138</v>
+        <v>28.9406734238767</v>
       </c>
       <c r="I22">
-        <v>9.033609103782149</v>
+        <v>9.59402350953906</v>
       </c>
       <c r="J22">
-        <v>57.9879605785338</v>
+        <v>58.9723466996799</v>
       </c>
       <c r="K22">
-        <v>46.50709913251</v>
+        <v>46.6851544368629</v>
       </c>
       <c r="L22">
-        <v>137.221579260459</v>
+        <v>135.137414371265</v>
       </c>
       <c r="M22">
-        <v>20.947042700381</v>
+        <v>20.8780838218686</v>
       </c>
       <c r="N22">
-        <v>87.1523252827007</v>
+        <v>87.7357789266074</v>
       </c>
       <c r="O22">
-        <v>2705.12239914191</v>
+        <v>2698.91750047281</v>
       </c>
       <c r="P22">
-        <v>16.4983194759445</v>
+        <v>19.2573823022897</v>
       </c>
     </row>
     <row r="23">
@@ -1538,49 +1538,49 @@
         </is>
       </c>
       <c r="B23">
-        <v>2211.85858535593</v>
+        <v>2213.7472250945</v>
       </c>
       <c r="C23">
-        <v>45.3131907473137</v>
+        <v>48.4738286385693</v>
       </c>
       <c r="D23">
-        <v>19.2189273418558</v>
+        <v>19.4706122521258</v>
       </c>
       <c r="E23">
-        <v>61.7279960072984</v>
+        <v>68.7093126695125</v>
       </c>
       <c r="F23">
-        <v>6.11397522267134</v>
+        <v>7.93279994645569</v>
       </c>
       <c r="G23">
-        <v>59.6108196610638</v>
+        <v>59.4560449657059</v>
       </c>
       <c r="H23">
-        <v>65.4819391719049</v>
+        <v>68.97751533295779</v>
       </c>
       <c r="I23">
-        <v>23.460893019655</v>
+        <v>25.4961726768083</v>
       </c>
       <c r="J23">
-        <v>170.553762841297</v>
+        <v>174.959384681964</v>
       </c>
       <c r="K23">
-        <v>142.011246841773</v>
+        <v>143.69207272903</v>
       </c>
       <c r="L23">
-        <v>56.1864938367034</v>
+        <v>56.3827353047278</v>
       </c>
       <c r="M23">
-        <v>560.7568177589191</v>
+        <v>535.288748883229</v>
       </c>
       <c r="N23">
-        <v>89.3590173094302</v>
+        <v>88.48205959323551</v>
       </c>
       <c r="O23">
-        <v>3443.96273235335</v>
+        <v>3423.56507098326</v>
       </c>
       <c r="P23">
-        <v>50.9522158651002</v>
+        <v>71.9350295821738</v>
       </c>
     </row>
     <row r="24">
@@ -1590,49 +1590,49 @@
         </is>
       </c>
       <c r="B24">
-        <v>826.968409480562</v>
+        <v>825.265416313743</v>
       </c>
       <c r="C24">
-        <v>63.2215421657409</v>
+        <v>72.3932212434287</v>
       </c>
       <c r="D24">
-        <v>8.63023605829834</v>
+        <v>9.46269863360032</v>
       </c>
       <c r="E24">
-        <v>64.6080153218809</v>
+        <v>62.7108308944636</v>
       </c>
       <c r="F24">
-        <v>19.7203335516002</v>
+        <v>21.5042439801716</v>
       </c>
       <c r="G24">
-        <v>20.3329298751263</v>
+        <v>19.7569806360387</v>
       </c>
       <c r="H24">
-        <v>29.4011629266768</v>
+        <v>29.8713282979592</v>
       </c>
       <c r="I24">
-        <v>11.2015567467349</v>
+        <v>12.644189894175</v>
       </c>
       <c r="J24">
-        <v>51.867355660309</v>
+        <v>54.4799956332256</v>
       </c>
       <c r="K24">
-        <v>70.1677364650437</v>
+        <v>71.1798620939563</v>
       </c>
       <c r="L24">
-        <v>82.15103254116301</v>
+        <v>77.1282770770442</v>
       </c>
       <c r="M24">
-        <v>19.0156761217904</v>
+        <v>21.5761452933052</v>
       </c>
       <c r="N24">
-        <v>63.2781894005934</v>
+        <v>60.9836364006158</v>
       </c>
       <c r="O24">
-        <v>2044.81638256349</v>
+        <v>1988.7224188593</v>
       </c>
       <c r="P24">
-        <v>79.7475971086125</v>
+        <v>127.448910736586</v>
       </c>
     </row>
     <row r="25">
@@ -1642,49 +1642,49 @@
         </is>
       </c>
       <c r="B25">
-        <v>753.451003050306</v>
+        <v>753.477027354863</v>
       </c>
       <c r="C25">
-        <v>31.4365005544667</v>
+        <v>33.7484208174312</v>
       </c>
       <c r="D25">
-        <v>22.7240548498533</v>
+        <v>25.0790488705348</v>
       </c>
       <c r="E25">
-        <v>33.0566784968585</v>
+        <v>35.3662920839638</v>
       </c>
       <c r="F25">
-        <v>16.9936514551962</v>
+        <v>16.871239300236</v>
       </c>
       <c r="G25">
-        <v>10.347623678432</v>
+        <v>9.932461031570339</v>
       </c>
       <c r="H25">
-        <v>15.515743967408</v>
+        <v>16.3129868896381</v>
       </c>
       <c r="I25">
-        <v>6.05589676693947</v>
+        <v>6.14852552937311</v>
       </c>
       <c r="J25">
-        <v>20.8664134716444</v>
+        <v>21.6586060267646</v>
       </c>
       <c r="K25">
-        <v>16.6267819157681</v>
+        <v>18.1133303591583</v>
       </c>
       <c r="L25">
-        <v>35.471172538024</v>
+        <v>36.286256811415</v>
       </c>
       <c r="M25">
-        <v>25.1599883868036</v>
+        <v>24.5108042019192</v>
       </c>
       <c r="N25">
-        <v>41.5788191020324</v>
+        <v>46.8538696032329</v>
       </c>
       <c r="O25">
-        <v>881.326022494683</v>
+        <v>861.8540700739781</v>
       </c>
       <c r="P25">
-        <v>38.2778688136127</v>
+        <v>42.6752805879508</v>
       </c>
     </row>
     <row r="26">
@@ -1694,49 +1694,49 @@
         </is>
       </c>
       <c r="B26">
-        <v>1211.36904122188</v>
+        <v>1211.59900725343</v>
       </c>
       <c r="C26">
-        <v>54.1857762392431</v>
+        <v>57.6244913248475</v>
       </c>
       <c r="D26">
-        <v>13.1341786474932</v>
+        <v>15.3640667749152</v>
       </c>
       <c r="E26">
-        <v>52.1528165010251</v>
+        <v>54.2946472587776</v>
       </c>
       <c r="F26">
-        <v>2.24049352725855</v>
+        <v>2.70606016862925</v>
       </c>
       <c r="G26">
-        <v>38.1168391713816</v>
+        <v>36.5475972916115</v>
       </c>
       <c r="H26">
-        <v>23.658405558306</v>
+        <v>24.1005012057104</v>
       </c>
       <c r="I26">
-        <v>14.5554631277053</v>
+        <v>16.5122926542018</v>
       </c>
       <c r="J26">
-        <v>55.7445455650377</v>
+        <v>58.2393140039036</v>
       </c>
       <c r="K26">
-        <v>49.8715729720607</v>
+        <v>51.2490175526671</v>
       </c>
       <c r="L26">
-        <v>41.3629025203206</v>
+        <v>43.0073410751875</v>
       </c>
       <c r="M26">
-        <v>89.318882498778</v>
+        <v>89.3543218076461</v>
       </c>
       <c r="N26">
-        <v>35.1583347174218</v>
+        <v>37.8305163229315</v>
       </c>
       <c r="O26">
-        <v>2206.51241757385</v>
+        <v>2170.54850253683</v>
       </c>
       <c r="P26">
-        <v>56.6682576907221</v>
+        <v>75.0722503011938</v>
       </c>
     </row>
     <row r="27">
@@ -1746,49 +1746,49 @@
         </is>
       </c>
       <c r="B27">
-        <v>198.068798798614</v>
+        <v>197.781526133985</v>
       </c>
       <c r="C27">
-        <v>3.05341982531712</v>
+        <v>3.15457129467759</v>
       </c>
       <c r="D27">
-        <v>0.9955292415534</v>
+        <v>0.98338197200545</v>
       </c>
       <c r="E27">
-        <v>10.0375407479542</v>
+        <v>10.2516368788223</v>
       </c>
       <c r="F27">
-        <v>6.6586867052002</v>
+        <v>7.36691335827176</v>
       </c>
       <c r="G27">
-        <v>0.857149051581188</v>
+        <v>0.805255255191805</v>
       </c>
       <c r="H27">
-        <v>0.460709959498793</v>
+        <v>0.466151591229967</v>
       </c>
       <c r="I27">
-        <v>0.7348231716836811</v>
+        <v>0.7545981535591591</v>
       </c>
       <c r="J27">
-        <v>4.572434639616</v>
+        <v>4.42445147120486</v>
       </c>
       <c r="K27">
-        <v>1.6795367509643</v>
+        <v>1.65510006356165</v>
       </c>
       <c r="L27">
-        <v>2.89898958982554</v>
+        <v>2.49670817932606</v>
       </c>
       <c r="M27">
-        <v>1.41107979620659</v>
+        <v>1.39637818207779</v>
       </c>
       <c r="N27">
-        <v>5.08083501583339</v>
+        <v>5.03569717794889</v>
       </c>
       <c r="O27">
-        <v>366.908825594306</v>
+        <v>355.341735840045</v>
       </c>
       <c r="P27">
-        <v>34.3119138363313</v>
+        <v>45.8161671725802</v>
       </c>
     </row>
     <row r="28">
@@ -1798,49 +1798,49 @@
         </is>
       </c>
       <c r="B28">
-        <v>297.186296023329</v>
+        <v>295.811536529527</v>
       </c>
       <c r="C28">
-        <v>37.6163424162801</v>
+        <v>36.0777271841448</v>
       </c>
       <c r="D28">
-        <v>2.00125862506064</v>
+        <v>1.91940253849662</v>
       </c>
       <c r="E28">
-        <v>8.07735346157506</v>
+        <v>7.36832457678458</v>
       </c>
       <c r="F28">
-        <v>2.08424993651022</v>
+        <v>2.4710641708044</v>
       </c>
       <c r="G28">
-        <v>6.16984152208343</v>
+        <v>5.82852915700548</v>
       </c>
       <c r="H28">
-        <v>7.29213953463013</v>
+        <v>7.18533945080842</v>
       </c>
       <c r="I28">
-        <v>4.76217064389216</v>
+        <v>4.58652228864949</v>
       </c>
       <c r="J28">
-        <v>16.5601618902001</v>
+        <v>17.5471293464473</v>
       </c>
       <c r="K28">
-        <v>16.3599933176807</v>
+        <v>18.2202040159315</v>
       </c>
       <c r="L28">
-        <v>12.5793660946819</v>
+        <v>11.46357773795</v>
       </c>
       <c r="M28">
-        <v>9.77839028390285</v>
+        <v>10.6223757119752</v>
       </c>
       <c r="N28">
-        <v>11.8013051544899</v>
+        <v>11.2779214917986</v>
       </c>
       <c r="O28">
-        <v>706.014278764447</v>
+        <v>675.795171719188</v>
       </c>
       <c r="P28">
-        <v>56.4644150966501</v>
+        <v>88.57273684590351</v>
       </c>
     </row>
     <row r="29">
@@ -1850,49 +1850,49 @@
         </is>
       </c>
       <c r="B29">
-        <v>445.33081265613</v>
+        <v>445.521763084919</v>
       </c>
       <c r="C29">
-        <v>7.14862654569855</v>
+        <v>7.13485556077118</v>
       </c>
       <c r="D29">
-        <v>3.14278263143969</v>
+        <v>3.08537328796952</v>
       </c>
       <c r="E29">
-        <v>6.32623478197431</v>
+        <v>6.25233658620925</v>
       </c>
       <c r="F29">
-        <v>12.6470478851313</v>
+        <v>16.1843986410172</v>
       </c>
       <c r="G29">
-        <v>2.37292659297252</v>
+        <v>2.35487379939831</v>
       </c>
       <c r="H29">
-        <v>2.92419957438374</v>
+        <v>2.82044652319323</v>
       </c>
       <c r="I29">
-        <v>4.84428993797819</v>
+        <v>4.9867608104406</v>
       </c>
       <c r="J29">
-        <v>8.23447894337723</v>
+        <v>8.220953830634819</v>
       </c>
       <c r="K29">
-        <v>3.82770233306319</v>
+        <v>3.74546814538973</v>
       </c>
       <c r="L29">
-        <v>6.66450906289299</v>
+        <v>6.66196455347275</v>
       </c>
       <c r="M29">
-        <v>3.09801735231986</v>
+        <v>3.09631261033343</v>
       </c>
       <c r="N29">
-        <v>13.3344282905513</v>
+        <v>13.2078563870818</v>
       </c>
       <c r="O29">
-        <v>868.027020948231</v>
+        <v>863.720724622278</v>
       </c>
       <c r="P29">
-        <v>3.69074579587906</v>
+        <v>4.61973488891429</v>
       </c>
     </row>
     <row r="30">
@@ -1902,49 +1902,49 @@
         </is>
       </c>
       <c r="B30">
-        <v>228.917861171919</v>
+        <v>228.860112025043</v>
       </c>
       <c r="C30">
-        <v>5.13533121304133</v>
+        <v>5.01714372651166</v>
       </c>
       <c r="D30">
-        <v>5.78257095882123</v>
+        <v>5.93015861792272</v>
       </c>
       <c r="E30">
-        <v>12.227021845569</v>
+        <v>13.8724367449755</v>
       </c>
       <c r="F30">
-        <v>0.795750401366961</v>
+        <v>0.810354574080822</v>
       </c>
       <c r="G30">
-        <v>5.10507702342012</v>
+        <v>4.81946061682052</v>
       </c>
       <c r="H30">
-        <v>4.86813100906616</v>
+        <v>4.8092285083036</v>
       </c>
       <c r="I30">
-        <v>2.37546792746762</v>
+        <v>2.37517930919883</v>
       </c>
       <c r="J30">
-        <v>18.394866889611</v>
+        <v>19.1222395669186</v>
       </c>
       <c r="K30">
-        <v>14.6474583619366</v>
+        <v>15.2440670009337</v>
       </c>
       <c r="L30">
-        <v>45.1277718086934</v>
+        <v>40.2824880956667</v>
       </c>
       <c r="M30">
-        <v>10.0271168791002</v>
+        <v>9.720983269745419</v>
       </c>
       <c r="N30">
-        <v>18.0192276202355</v>
+        <v>17.9639516194025</v>
       </c>
       <c r="O30">
-        <v>502.170396637849</v>
+        <v>502.923417183263</v>
       </c>
       <c r="P30">
-        <v>6.78181116725589</v>
+        <v>8.624640056566079</v>
       </c>
     </row>
     <row r="31">
@@ -1954,49 +1954,49 @@
         </is>
       </c>
       <c r="B31">
-        <v>1889.91289291983</v>
+        <v>1889.98310944363</v>
       </c>
       <c r="C31">
-        <v>47.4407365205255</v>
+        <v>47.5198041724566</v>
       </c>
       <c r="D31">
-        <v>47.6445938420026</v>
+        <v>47.2686920428081</v>
       </c>
       <c r="E31">
-        <v>37.1627535361506</v>
+        <v>36.9566747319437</v>
       </c>
       <c r="F31">
-        <v>13.2075071040745</v>
+        <v>13.5435243639425</v>
       </c>
       <c r="G31">
-        <v>144.680126536621</v>
+        <v>144.516339594529</v>
       </c>
       <c r="H31">
-        <v>28.7593588736586</v>
+        <v>29.7108955567559</v>
       </c>
       <c r="I31">
-        <v>22.6506626814694</v>
+        <v>23.6993029162458</v>
       </c>
       <c r="J31">
-        <v>48.2771864481988</v>
+        <v>48.7671679866381</v>
       </c>
       <c r="K31">
-        <v>44.3587906591388</v>
+        <v>44.4821139957357</v>
       </c>
       <c r="L31">
-        <v>62.9639970576173</v>
+        <v>62.5754077410979</v>
       </c>
       <c r="M31">
-        <v>33.3240782264315</v>
+        <v>33.2903054565144</v>
       </c>
       <c r="N31">
-        <v>75.13393628341031</v>
+        <v>74.9726353052904</v>
       </c>
       <c r="O31">
-        <v>3527.13618462325</v>
+        <v>3524.15288459541</v>
       </c>
       <c r="P31">
-        <v>11.3261286920993</v>
+        <v>12.5400761014738</v>
       </c>
     </row>
     <row r="32">
@@ -2006,49 +2006,49 @@
         </is>
       </c>
       <c r="B32">
-        <v>473.728210834676</v>
+        <v>473.834772063755</v>
       </c>
       <c r="C32">
-        <v>4.03538823577729</v>
+        <v>4.01702775374432</v>
       </c>
       <c r="D32">
-        <v>5.13419106496751</v>
+        <v>5.12204121886709</v>
       </c>
       <c r="E32">
-        <v>5.08644962456041</v>
+        <v>5.06386682615973</v>
       </c>
       <c r="F32">
-        <v>22.8316361671845</v>
+        <v>23.9643313111575</v>
       </c>
       <c r="G32">
-        <v>2.08518628481926</v>
+        <v>2.02087841016015</v>
       </c>
       <c r="H32">
-        <v>1.17380811693295</v>
+        <v>1.03566516931919</v>
       </c>
       <c r="I32">
-        <v>3.68872469107949</v>
+        <v>3.9218456563082</v>
       </c>
       <c r="J32">
-        <v>2.24490439821536</v>
+        <v>2.2194215979696</v>
       </c>
       <c r="K32">
-        <v>4.79173071122071</v>
+        <v>4.6576548326151</v>
       </c>
       <c r="L32">
-        <v>18.0969261585994</v>
+        <v>16.7210038648063</v>
       </c>
       <c r="M32">
-        <v>5.00106982438256</v>
+        <v>4.69056307072334</v>
       </c>
       <c r="N32">
-        <v>12.770265458501</v>
+        <v>12.8838240798249</v>
       </c>
       <c r="O32">
-        <v>677.645789820646</v>
+        <v>672.886150540676</v>
       </c>
       <c r="P32">
-        <v>22.2324926540663</v>
+        <v>27.5077276495438</v>
       </c>
     </row>
     <row r="33">
@@ -2058,49 +2058,49 @@
         </is>
       </c>
       <c r="B33">
-        <v>4910.26219953421</v>
+        <v>4905.21127534394</v>
       </c>
       <c r="C33">
-        <v>83.3629347250874</v>
+        <v>86.00970890327871</v>
       </c>
       <c r="D33">
-        <v>159.5269083539</v>
+        <v>153.573466349566</v>
       </c>
       <c r="E33">
-        <v>86.9268650219052</v>
+        <v>96.016378124669</v>
       </c>
       <c r="F33">
-        <v>12.3523376401576</v>
+        <v>14.0697374241101</v>
       </c>
       <c r="G33">
-        <v>88.58548615942691</v>
+        <v>90.98820189909991</v>
       </c>
       <c r="H33">
-        <v>45.9198042188132</v>
+        <v>49.7796478115795</v>
       </c>
       <c r="I33">
-        <v>39.2390775216367</v>
+        <v>44.3535610010758</v>
       </c>
       <c r="J33">
-        <v>118.021424011456</v>
+        <v>130.699758607032</v>
       </c>
       <c r="K33">
-        <v>118.142175637293</v>
+        <v>128.381901953012</v>
       </c>
       <c r="L33">
-        <v>149.492032667454</v>
+        <v>155.277877539617</v>
       </c>
       <c r="M33">
-        <v>85.6043758373565</v>
+        <v>90.8539971637025</v>
       </c>
       <c r="N33">
-        <v>148.938098568321</v>
+        <v>155.366331552381</v>
       </c>
       <c r="O33">
-        <v>7529.86911910634</v>
+        <v>7448.50062031088</v>
       </c>
       <c r="P33">
-        <v>54.5457616617931</v>
+        <v>81.70613668120249</v>
       </c>
     </row>
     <row r="34">
@@ -2110,49 +2110,49 @@
         </is>
       </c>
       <c r="B34">
-        <v>1743.23869632779</v>
+        <v>1743.23732468222</v>
       </c>
       <c r="C34">
-        <v>73.63820169104051</v>
+        <v>75.0493786668296</v>
       </c>
       <c r="D34">
-        <v>218.22095122479</v>
+        <v>226.934728017481</v>
       </c>
       <c r="E34">
-        <v>92.2373158471942</v>
+        <v>94.210700651305</v>
       </c>
       <c r="F34">
-        <v>6.7343552519582</v>
+        <v>7.0859824903759</v>
       </c>
       <c r="G34">
-        <v>71.57869308107701</v>
+        <v>70.92318389284419</v>
       </c>
       <c r="H34">
-        <v>47.605434876738</v>
+        <v>47.0815213921329</v>
       </c>
       <c r="I34">
-        <v>28.9863533986977</v>
+        <v>29.075408758777</v>
       </c>
       <c r="J34">
-        <v>65.2617192110261</v>
+        <v>65.61556007195711</v>
       </c>
       <c r="K34">
-        <v>65.6024289609946</v>
+        <v>64.5810853654193</v>
       </c>
       <c r="L34">
-        <v>113.59825380947</v>
+        <v>113.010285547249</v>
       </c>
       <c r="M34">
-        <v>57.4201158965304</v>
+        <v>56.9887964376095</v>
       </c>
       <c r="N34">
-        <v>135.579348354435</v>
+        <v>138.567003575855</v>
       </c>
       <c r="O34">
-        <v>2859.94593626492</v>
+        <v>2844.30583854767</v>
       </c>
       <c r="P34">
-        <v>76.2972769015412</v>
+        <v>79.2782830004776</v>
       </c>
     </row>
     <row r="35">
@@ -2162,49 +2162,49 @@
         </is>
       </c>
       <c r="B35">
-        <v>124.482654159572</v>
+        <v>124.429567641775</v>
       </c>
       <c r="C35">
-        <v>6.31492649095531</v>
+        <v>6.22084980780112</v>
       </c>
       <c r="D35">
-        <v>1.0905505991715</v>
+        <v>1.02551969991013</v>
       </c>
       <c r="E35">
-        <v>2.14895300180184</v>
+        <v>1.88862216293055</v>
       </c>
       <c r="F35">
-        <v>4.82644236115781</v>
+        <v>5.41110034238808</v>
       </c>
       <c r="G35">
-        <v>0.41477591579805</v>
+        <v>0.38898215305793</v>
       </c>
       <c r="H35">
-        <v>0.4903994124122</v>
+        <v>0.466161537601055</v>
       </c>
       <c r="I35">
-        <v>0.7749413985279791</v>
+        <v>0.752918814203203</v>
       </c>
       <c r="J35">
-        <v>2.23263516292676</v>
+        <v>2.18325630782508</v>
       </c>
       <c r="K35">
-        <v>6.44351831715818</v>
+        <v>6.61540174547108</v>
       </c>
       <c r="L35">
-        <v>2.73199183000942</v>
+        <v>2.52201963773618</v>
       </c>
       <c r="M35">
-        <v>2.02374515767686</v>
+        <v>2.19045293751281</v>
       </c>
       <c r="N35">
-        <v>2.78261891471948</v>
+        <v>2.61518027730733</v>
       </c>
       <c r="O35">
-        <v>262.588339384703</v>
+        <v>250.32998135967</v>
       </c>
       <c r="P35">
-        <v>31.4720609906055</v>
+        <v>43.7785386720057</v>
       </c>
     </row>
     <row r="36">
@@ -2214,49 +2214,49 @@
         </is>
       </c>
       <c r="B36">
-        <v>2534.87612366498</v>
+        <v>2533.64267914652</v>
       </c>
       <c r="C36">
-        <v>74.5565554855702</v>
+        <v>77.07802538453601</v>
       </c>
       <c r="D36">
-        <v>25.4903147450348</v>
+        <v>26.2352244048559</v>
       </c>
       <c r="E36">
-        <v>97.9112366382801</v>
+        <v>99.9590922081949</v>
       </c>
       <c r="F36">
-        <v>29.3746466140433</v>
+        <v>32.0029398622052</v>
       </c>
       <c r="G36">
-        <v>93.442914530144</v>
+        <v>91.901261925784</v>
       </c>
       <c r="H36">
-        <v>115.584936737433</v>
+        <v>122.674013567748</v>
       </c>
       <c r="I36">
-        <v>51.4525178283299</v>
+        <v>54.076361188286</v>
       </c>
       <c r="J36">
-        <v>270.358393695575</v>
+        <v>277.930200065621</v>
       </c>
       <c r="K36">
-        <v>156.693198042291</v>
+        <v>160.60699593305</v>
       </c>
       <c r="L36">
-        <v>110.632480620026</v>
+        <v>111.66037332014</v>
       </c>
       <c r="M36">
-        <v>254.461705270415</v>
+        <v>262.55135778575</v>
       </c>
       <c r="N36">
-        <v>93.2689469550069</v>
+        <v>96.1262034422238</v>
       </c>
       <c r="O36">
-        <v>4107.84181632007</v>
+        <v>4064.16320918155</v>
       </c>
       <c r="P36">
-        <v>62.233418822489</v>
+        <v>67.57126855321241</v>
       </c>
     </row>
     <row r="37">
@@ -2266,49 +2266,49 @@
         </is>
       </c>
       <c r="B37">
-        <v>843.889914721594</v>
+        <v>843.709682661491</v>
       </c>
       <c r="C37">
-        <v>21.0108112061508</v>
+        <v>22.6409504398064</v>
       </c>
       <c r="D37">
-        <v>11.4655766747176</v>
+        <v>13.4781874627523</v>
       </c>
       <c r="E37">
-        <v>20.6827284507991</v>
+        <v>22.4133165509355</v>
       </c>
       <c r="F37">
-        <v>46.7955126093578</v>
+        <v>50.7806455510647</v>
       </c>
       <c r="G37">
-        <v>4.4846805903446</v>
+        <v>4.49803424587164</v>
       </c>
       <c r="H37">
-        <v>16.6634570748756</v>
+        <v>17.4512384346201</v>
       </c>
       <c r="I37">
-        <v>11.611919744276</v>
+        <v>12.3327014179516</v>
       </c>
       <c r="J37">
-        <v>32.9700560208477</v>
+        <v>34.2406464956178</v>
       </c>
       <c r="K37">
-        <v>34.2577706459505</v>
+        <v>34.0555997492766</v>
       </c>
       <c r="L37">
-        <v>27.6294247947973</v>
+        <v>26.9180653008603</v>
       </c>
       <c r="M37">
-        <v>30.1530276306805</v>
+        <v>29.5650214499214</v>
       </c>
       <c r="N37">
-        <v>20.9352448674344</v>
+        <v>20.8095502745057</v>
       </c>
       <c r="O37">
-        <v>1235.42739141034</v>
+        <v>1210.40153645868</v>
       </c>
       <c r="P37">
-        <v>51.1492920158169</v>
+        <v>65.831631964624</v>
       </c>
     </row>
     <row r="38">
@@ -2318,49 +2318,49 @@
         </is>
       </c>
       <c r="B38">
-        <v>755.442832787387</v>
+        <v>755.271119625177</v>
       </c>
       <c r="C38">
-        <v>26.9563898691235</v>
+        <v>28.8617239462659</v>
       </c>
       <c r="D38">
-        <v>10.5541264483059</v>
+        <v>10.2558838790753</v>
       </c>
       <c r="E38">
-        <v>56.4729704666715</v>
+        <v>60.6294103055649</v>
       </c>
       <c r="F38">
-        <v>1.8212202189506</v>
+        <v>1.90563326379461</v>
       </c>
       <c r="G38">
-        <v>9.08120243508843</v>
+        <v>9.02847928288756</v>
       </c>
       <c r="H38">
-        <v>9.092233825407771</v>
+        <v>8.748336038686761</v>
       </c>
       <c r="I38">
-        <v>8.58579202615902</v>
+        <v>8.365776779694221</v>
       </c>
       <c r="J38">
-        <v>29.8334475887961</v>
+        <v>29.6968283290288</v>
       </c>
       <c r="K38">
-        <v>22.019523226337</v>
+        <v>21.0143469279747</v>
       </c>
       <c r="L38">
-        <v>64.64603611324181</v>
+        <v>60.3069833089966</v>
       </c>
       <c r="M38">
-        <v>25.9658704843271</v>
+        <v>25.3217602109315</v>
       </c>
       <c r="N38">
-        <v>27.0344459806272</v>
+        <v>26.4900458041164</v>
       </c>
       <c r="O38">
-        <v>1318.98941852266</v>
+        <v>1309.15415445002</v>
       </c>
       <c r="P38">
-        <v>61.9680196488585</v>
+        <v>73.4130474897174</v>
       </c>
     </row>
     <row r="39">
@@ -2370,49 +2370,49 @@
         </is>
       </c>
       <c r="B39">
-        <v>2965.97546810724</v>
+        <v>2964.12250532011</v>
       </c>
       <c r="C39">
-        <v>108.238772550815</v>
+        <v>109.894857307009</v>
       </c>
       <c r="D39">
-        <v>61.5400669314464</v>
+        <v>66.4939340138794</v>
       </c>
       <c r="E39">
-        <v>111.987413311639</v>
+        <v>126.309228263253</v>
       </c>
       <c r="F39">
-        <v>26.7059330498329</v>
+        <v>31.6483806280465</v>
       </c>
       <c r="G39">
-        <v>110.904450576837</v>
+        <v>105.233015866184</v>
       </c>
       <c r="H39">
-        <v>54.5410397293744</v>
+        <v>58.4031903184028</v>
       </c>
       <c r="I39">
-        <v>57.0922535276983</v>
+        <v>64.1568392470255</v>
       </c>
       <c r="J39">
-        <v>202.228167546389</v>
+        <v>217.37791197357</v>
       </c>
       <c r="K39">
-        <v>114.60954170096</v>
+        <v>122.493286921513</v>
       </c>
       <c r="L39">
-        <v>144.822083825932</v>
+        <v>145.53263825825</v>
       </c>
       <c r="M39">
-        <v>76.31889392033369</v>
+        <v>80.14024523365509</v>
       </c>
       <c r="N39">
-        <v>100.573325252903</v>
+        <v>104.499683707312</v>
       </c>
       <c r="O39">
-        <v>4584.36178679153</v>
+        <v>4500.82680304619</v>
       </c>
       <c r="P39">
-        <v>68.5982479763196</v>
+        <v>91.3649246948425</v>
       </c>
     </row>
     <row r="40">
@@ -2422,49 +2422,49 @@
         </is>
       </c>
       <c r="B40">
-        <v>242.122506540541</v>
+        <v>242.111267661067</v>
       </c>
       <c r="C40">
-        <v>4.54985601378076</v>
+        <v>4.51807599682357</v>
       </c>
       <c r="D40">
-        <v>10.5584302899445</v>
+        <v>10.557535376253</v>
       </c>
       <c r="E40">
-        <v>4.14650179653692</v>
+        <v>4.15811888507987</v>
       </c>
       <c r="F40">
-        <v>0.868851350062159</v>
+        <v>0.853220654899253</v>
       </c>
       <c r="G40">
-        <v>3.17294038524599</v>
+        <v>3.31704847562119</v>
       </c>
       <c r="H40">
-        <v>8.16807766803826</v>
+        <v>8.28915444792356</v>
       </c>
       <c r="I40">
-        <v>1.81977924419548</v>
+        <v>1.83436565953236</v>
       </c>
       <c r="J40">
-        <v>12.3365214809725</v>
+        <v>12.2556521908219</v>
       </c>
       <c r="K40">
-        <v>7.12171459917086</v>
+        <v>7.06377969889926</v>
       </c>
       <c r="L40">
-        <v>15.0228619588098</v>
+        <v>15.0668376369324</v>
       </c>
       <c r="M40">
-        <v>9.45280117721035</v>
+        <v>9.410758262557639</v>
       </c>
       <c r="N40">
-        <v>27.2979782488272</v>
+        <v>27.0279132184732</v>
       </c>
       <c r="O40">
-        <v>391.988628898185</v>
+        <v>392.100262792304</v>
       </c>
       <c r="P40">
-        <v>2.16051647725363</v>
+        <v>2.22397517158537</v>
       </c>
     </row>
     <row r="41">
@@ -2474,49 +2474,49 @@
         </is>
       </c>
       <c r="B41">
-        <v>910.281705966952</v>
+        <v>909.775989457335</v>
       </c>
       <c r="C41">
-        <v>19.6122059954044</v>
+        <v>20.8673042328778</v>
       </c>
       <c r="D41">
-        <v>105.944766375325</v>
+        <v>113.414450160661</v>
       </c>
       <c r="E41">
-        <v>47.2333446015643</v>
+        <v>49.2000545746391</v>
       </c>
       <c r="F41">
-        <v>3.891646043372</v>
+        <v>3.97008750869141</v>
       </c>
       <c r="G41">
-        <v>38.2434311037615</v>
+        <v>38.2727623201785</v>
       </c>
       <c r="H41">
-        <v>36.4954706419519</v>
+        <v>36.9406480075226</v>
       </c>
       <c r="I41">
-        <v>8.0943084451613</v>
+        <v>8.13271670514955</v>
       </c>
       <c r="J41">
-        <v>48.2038386559906</v>
+        <v>49.0758624845891</v>
       </c>
       <c r="K41">
-        <v>49.3110771002355</v>
+        <v>50.7512814090104</v>
       </c>
       <c r="L41">
-        <v>32.4816855272431</v>
+        <v>31.7941612555451</v>
       </c>
       <c r="M41">
-        <v>39.7423602918265</v>
+        <v>38.9547088931238</v>
       </c>
       <c r="N41">
-        <v>21.5328201126345</v>
+        <v>21.586150911319</v>
       </c>
       <c r="O41">
-        <v>1405.64625975783</v>
+        <v>1392.23822256069</v>
       </c>
       <c r="P41">
-        <v>18.8017230436822</v>
+        <v>20.5422431815977</v>
       </c>
     </row>
     <row r="42">
@@ -2526,49 +2526,49 @@
         </is>
       </c>
       <c r="B42">
-        <v>133.519573673448</v>
+        <v>133.79708652343</v>
       </c>
       <c r="C42">
-        <v>10.6726564449988</v>
+        <v>10.4301325007805</v>
       </c>
       <c r="D42">
-        <v>1.47627442397302</v>
+        <v>1.47078380442001</v>
       </c>
       <c r="E42">
-        <v>6.42171231173378</v>
+        <v>5.95211814628219</v>
       </c>
       <c r="F42">
-        <v>1.85532685531145</v>
+        <v>1.72987865116983</v>
       </c>
       <c r="G42">
-        <v>1.23005300050617</v>
+        <v>1.12512243703385</v>
       </c>
       <c r="H42">
-        <v>1.82839031388895</v>
+        <v>1.59286528404367</v>
       </c>
       <c r="I42">
-        <v>1.13607032195354</v>
+        <v>1.07682164056634</v>
       </c>
       <c r="J42">
-        <v>3.74322480623212</v>
+        <v>3.51145351984565</v>
       </c>
       <c r="K42">
-        <v>7.27892849885128</v>
+        <v>7.39988212761826</v>
       </c>
       <c r="L42">
-        <v>9.45412959924886</v>
+        <v>8.08892430484299</v>
       </c>
       <c r="M42">
-        <v>2.92975542202465</v>
+        <v>3.01195675418452</v>
       </c>
       <c r="N42">
-        <v>9.00213181379412</v>
+        <v>8.436326649428601</v>
       </c>
       <c r="O42">
-        <v>304.273278188445</v>
+        <v>294.127065084046</v>
       </c>
       <c r="P42">
-        <v>31.7350920364198</v>
+        <v>44.8061802831379</v>
       </c>
     </row>
     <row r="43">
@@ -2578,49 +2578,49 @@
         </is>
       </c>
       <c r="B43">
-        <v>1364.03210078119</v>
+        <v>1363.49487527055</v>
       </c>
       <c r="C43">
-        <v>43.0407040933021</v>
+        <v>42.959304092964</v>
       </c>
       <c r="D43">
-        <v>48.0907841791125</v>
+        <v>52.7832965876934</v>
       </c>
       <c r="E43">
-        <v>67.7308974194178</v>
+        <v>68.3261041417081</v>
       </c>
       <c r="F43">
-        <v>8.50305095308874</v>
+        <v>9.232406113889491</v>
       </c>
       <c r="G43">
-        <v>33.1504440820608</v>
+        <v>33.4719897276316</v>
       </c>
       <c r="H43">
-        <v>30.7599024803664</v>
+        <v>32.5160224288339</v>
       </c>
       <c r="I43">
-        <v>18.1362324355662</v>
+        <v>19.1853906619937</v>
       </c>
       <c r="J43">
-        <v>70.5723326622401</v>
+        <v>74.794860624241</v>
       </c>
       <c r="K43">
-        <v>47.6142554179271</v>
+        <v>50.1520707824092</v>
       </c>
       <c r="L43">
-        <v>63.8737149654391</v>
+        <v>66.2109663292822</v>
       </c>
       <c r="M43">
-        <v>83.9895421571897</v>
+        <v>89.18946569754971</v>
       </c>
       <c r="N43">
-        <v>75.91714526186119</v>
+        <v>78.902152115173</v>
       </c>
       <c r="O43">
-        <v>2060.84860952589</v>
+        <v>2032.13353588383</v>
       </c>
       <c r="P43">
-        <v>38.4689610276313</v>
+        <v>41.376236984544</v>
       </c>
     </row>
     <row r="44">
@@ -2630,49 +2630,49 @@
         </is>
       </c>
       <c r="B44">
-        <v>4625.41236074091</v>
+        <v>4626.71281988018</v>
       </c>
       <c r="C44">
-        <v>155.241693904852</v>
+        <v>161.271434796998</v>
       </c>
       <c r="D44">
-        <v>80.2928149608523</v>
+        <v>80.6540235951824</v>
       </c>
       <c r="E44">
-        <v>100.670683673247</v>
+        <v>103.762992793462</v>
       </c>
       <c r="F44">
-        <v>223.832672748314</v>
+        <v>229.898527296229</v>
       </c>
       <c r="G44">
-        <v>132.359902793031</v>
+        <v>132.250577910355</v>
       </c>
       <c r="H44">
-        <v>63.1183898166902</v>
+        <v>65.0970591047699</v>
       </c>
       <c r="I44">
-        <v>46.6469785174754</v>
+        <v>49.693627224402</v>
       </c>
       <c r="J44">
-        <v>148.221437120876</v>
+        <v>153.736994161916</v>
       </c>
       <c r="K44">
-        <v>138.188988516402</v>
+        <v>138.498644150235</v>
       </c>
       <c r="L44">
-        <v>273.656869880897</v>
+        <v>257.368795253005</v>
       </c>
       <c r="M44">
-        <v>143.399107420702</v>
+        <v>146.324031544094</v>
       </c>
       <c r="N44">
-        <v>100.73658408358</v>
+        <v>99.5800964822793</v>
       </c>
       <c r="O44">
-        <v>7783.886804106001</v>
+        <v>7719.12915204494</v>
       </c>
       <c r="P44">
-        <v>180.146099366082</v>
+        <v>231.832611411872</v>
       </c>
     </row>
     <row r="45">
@@ -2682,49 +2682,49 @@
         </is>
       </c>
       <c r="B45">
-        <v>431.024860541427</v>
+        <v>430.927526461313</v>
       </c>
       <c r="C45">
-        <v>18.1827931859174</v>
+        <v>18.5605896409447</v>
       </c>
       <c r="D45">
-        <v>3.67159322193382</v>
+        <v>3.57269518034541</v>
       </c>
       <c r="E45">
-        <v>12.7120801232177</v>
+        <v>12.7558886280491</v>
       </c>
       <c r="F45">
-        <v>15.4242299482497</v>
+        <v>19.5458975605057</v>
       </c>
       <c r="G45">
-        <v>9.51934782527033</v>
+        <v>9.23473361293871</v>
       </c>
       <c r="H45">
-        <v>4.82884284460958</v>
+        <v>4.74474571090822</v>
       </c>
       <c r="I45">
-        <v>5.9976408343434</v>
+        <v>5.98240610998342</v>
       </c>
       <c r="J45">
-        <v>17.2753928785169</v>
+        <v>17.3660402414428</v>
       </c>
       <c r="K45">
-        <v>11.5847965495783</v>
+        <v>11.4929330233406</v>
       </c>
       <c r="L45">
-        <v>23.0714939506821</v>
+        <v>22.234308934794</v>
       </c>
       <c r="M45">
-        <v>28.5736741137439</v>
+        <v>29.5655841186372</v>
       </c>
       <c r="N45">
-        <v>26.3368122985905</v>
+        <v>25.4728893031295</v>
       </c>
       <c r="O45">
-        <v>866.544895975063</v>
+        <v>857.146012352436</v>
       </c>
       <c r="P45">
-        <v>15.2725570203976</v>
+        <v>21.4187604327728</v>
       </c>
     </row>
     <row r="46">
@@ -2734,49 +2734,49 @@
         </is>
       </c>
       <c r="B46">
-        <v>112.703907773908</v>
+        <v>112.758388081157</v>
       </c>
       <c r="C46">
-        <v>4.91100205716425</v>
+        <v>5.28309945080182</v>
       </c>
       <c r="D46">
-        <v>2.04652301834727</v>
+        <v>2.1416838128661</v>
       </c>
       <c r="E46">
-        <v>6.8751333928917</v>
+        <v>7.60693941581408</v>
       </c>
       <c r="F46">
-        <v>0.9797199177955021</v>
+        <v>0.9556463597686941</v>
       </c>
       <c r="G46">
-        <v>1.27528091718694</v>
+        <v>1.11359581671912</v>
       </c>
       <c r="H46">
-        <v>1.52488188747745</v>
+        <v>1.42430495919068</v>
       </c>
       <c r="I46">
-        <v>2.55375645448921</v>
+        <v>2.50683459886039</v>
       </c>
       <c r="J46">
-        <v>5.2587159862584</v>
+        <v>5.25545779475684</v>
       </c>
       <c r="K46">
-        <v>4.4820398904838</v>
+        <v>4.38581442280862</v>
       </c>
       <c r="L46">
-        <v>13.9453387810592</v>
+        <v>11.3451503213337</v>
       </c>
       <c r="M46">
-        <v>4.74505504247851</v>
+        <v>4.60769530799818</v>
       </c>
       <c r="N46">
-        <v>7.41267017137721</v>
+        <v>8.04959007858926</v>
       </c>
       <c r="O46">
-        <v>254.334884531566</v>
+        <v>252.968500183701</v>
       </c>
       <c r="P46">
-        <v>9.449059332671551</v>
+        <v>12.0952685507889</v>
       </c>
     </row>
     <row r="47">
@@ -2786,49 +2786,49 @@
         </is>
       </c>
       <c r="B47">
-        <v>1501.69098533247</v>
+        <v>1501.01741312715</v>
       </c>
       <c r="C47">
-        <v>55.3380076158805</v>
+        <v>58.7142476030089</v>
       </c>
       <c r="D47">
-        <v>60.9311679481634</v>
+        <v>65.7135855839356</v>
       </c>
       <c r="E47">
-        <v>58.1120773204635</v>
+        <v>60.433576318206</v>
       </c>
       <c r="F47">
-        <v>12.7594852259309</v>
+        <v>14.2012491566674</v>
       </c>
       <c r="G47">
-        <v>38.9172064662768</v>
+        <v>39.4866280427861</v>
       </c>
       <c r="H47">
-        <v>23.256637756184</v>
+        <v>24.1967950350023</v>
       </c>
       <c r="I47">
-        <v>16.7623964633812</v>
+        <v>17.5560441613017</v>
       </c>
       <c r="J47">
-        <v>45.9736523952971</v>
+        <v>46.969594171665</v>
       </c>
       <c r="K47">
-        <v>43.7577691456057</v>
+        <v>43.6901286721973</v>
       </c>
       <c r="L47">
-        <v>60.6114495758357</v>
+        <v>60.175210185934</v>
       </c>
       <c r="M47">
-        <v>79.01058499142501</v>
+        <v>76.5452640965753</v>
       </c>
       <c r="N47">
-        <v>47.0624041824384</v>
+        <v>48.4721261451484</v>
       </c>
       <c r="O47">
-        <v>2818.87538469559</v>
+        <v>2800.77679463433</v>
       </c>
       <c r="P47">
-        <v>57.454618965874</v>
+        <v>62.565171146894</v>
       </c>
     </row>
     <row r="48">
@@ -2838,49 +2838,49 @@
         </is>
       </c>
       <c r="B48">
-        <v>1276.11743924831</v>
+        <v>1276.59330180204</v>
       </c>
       <c r="C48">
-        <v>32.8803747593796</v>
+        <v>33.6854710557315</v>
       </c>
       <c r="D48">
-        <v>9.50085359651524</v>
+        <v>9.36566825724128</v>
       </c>
       <c r="E48">
-        <v>66.9371126225133</v>
+        <v>70.19842313873861</v>
       </c>
       <c r="F48">
-        <v>12.9508492920574</v>
+        <v>14.0562879703826</v>
       </c>
       <c r="G48">
-        <v>18.2161597547414</v>
+        <v>18.1656805607057</v>
       </c>
       <c r="H48">
-        <v>9.67512165253034</v>
+        <v>9.475147004194859</v>
       </c>
       <c r="I48">
-        <v>13.8604814579986</v>
+        <v>13.9867012189852</v>
       </c>
       <c r="J48">
-        <v>36.1546953215759</v>
+        <v>35.6279143264785</v>
       </c>
       <c r="K48">
-        <v>20.6935513100965</v>
+        <v>20.4310587260488</v>
       </c>
       <c r="L48">
-        <v>43.0001440760115</v>
+        <v>40.9755365096403</v>
       </c>
       <c r="M48">
-        <v>167.978048968643</v>
+        <v>159.443653489928</v>
       </c>
       <c r="N48">
-        <v>27.6328637366917</v>
+        <v>26.9975700310294</v>
       </c>
       <c r="O48">
-        <v>2324.00504667159</v>
+        <v>2312.86082003354</v>
       </c>
       <c r="P48">
-        <v>90.3196212893301</v>
+        <v>108.059129633321</v>
       </c>
     </row>
     <row r="49">
@@ -2890,49 +2890,49 @@
         </is>
       </c>
       <c r="B49">
-        <v>567.235852727996</v>
+        <v>567.207804639821</v>
       </c>
       <c r="C49">
-        <v>7.88870648829224</v>
+        <v>8.10256714101781</v>
       </c>
       <c r="D49">
-        <v>5.23873318898563</v>
+        <v>5.39014425719142</v>
       </c>
       <c r="E49">
-        <v>14.9973920787983</v>
+        <v>15.2155247893951</v>
       </c>
       <c r="F49">
-        <v>33.1109671554213</v>
+        <v>34.4756523154218</v>
       </c>
       <c r="G49">
-        <v>18.9675875900509</v>
+        <v>18.3693983987949</v>
       </c>
       <c r="H49">
-        <v>5.30567549789398</v>
+        <v>5.24254966880989</v>
       </c>
       <c r="I49">
-        <v>9.62237788346067</v>
+        <v>9.21267290265541</v>
       </c>
       <c r="J49">
-        <v>21.4648591414997</v>
+        <v>21.1541552680865</v>
       </c>
       <c r="K49">
-        <v>8.32928304134863</v>
+        <v>7.92883477874916</v>
       </c>
       <c r="L49">
-        <v>5.24877991182855</v>
+        <v>5.21390641004226</v>
       </c>
       <c r="M49">
-        <v>8.540541410680079</v>
+        <v>8.67979751511966</v>
       </c>
       <c r="N49">
-        <v>3.99759944238266</v>
+        <v>4.16184073556886</v>
       </c>
       <c r="O49">
-        <v>622.922991337198</v>
+        <v>622.273851300224</v>
       </c>
       <c r="P49">
-        <v>9.095453597964701</v>
+        <v>9.33810037290448</v>
       </c>
     </row>
     <row r="50">
@@ -2942,49 +2942,49 @@
         </is>
       </c>
       <c r="B50">
-        <v>1010.6152229456</v>
+        <v>1009.20568555495</v>
       </c>
       <c r="C50">
-        <v>88.97638353523691</v>
+        <v>95.1642967441305</v>
       </c>
       <c r="D50">
-        <v>9.654859302823951</v>
+        <v>10.3685775467368</v>
       </c>
       <c r="E50">
-        <v>118.965083501013</v>
+        <v>124.435940791811</v>
       </c>
       <c r="F50">
-        <v>6.50642255890701</v>
+        <v>7.79743574398362</v>
       </c>
       <c r="G50">
-        <v>24.3100529386284</v>
+        <v>21.5759529152287</v>
       </c>
       <c r="H50">
-        <v>30.5652954656772</v>
+        <v>30.6799403835483</v>
       </c>
       <c r="I50">
-        <v>21.8235514747898</v>
+        <v>23.686568114812</v>
       </c>
       <c r="J50">
-        <v>107.564012607243</v>
+        <v>108.955328402193</v>
       </c>
       <c r="K50">
-        <v>131.85705636918</v>
+        <v>128.916839975351</v>
       </c>
       <c r="L50">
-        <v>89.1398518150835</v>
+        <v>83.2010845142045</v>
       </c>
       <c r="M50">
-        <v>47.471096103778</v>
+        <v>46.9185865231954</v>
       </c>
       <c r="N50">
-        <v>68.0818582273141</v>
+        <v>70.1348009864773</v>
       </c>
       <c r="O50">
-        <v>1929.06740104032</v>
+        <v>1875.0349651701</v>
       </c>
       <c r="P50">
-        <v>87.6270345467303</v>
+        <v>136.149179065612</v>
       </c>
     </row>
     <row r="51">
@@ -2994,49 +2994,49 @@
         </is>
       </c>
       <c r="B51">
-        <v>101.561258405316</v>
+        <v>101.471351742184</v>
       </c>
       <c r="C51">
-        <v>1.38896341700134</v>
+        <v>1.33766741472365</v>
       </c>
       <c r="D51">
-        <v>0.641677201833149</v>
+        <v>0.718788196185491</v>
       </c>
       <c r="E51">
-        <v>1.47235282992845</v>
+        <v>1.53649243871845</v>
       </c>
       <c r="F51">
-        <v>23.4242390350605</v>
+        <v>24.6848201163378</v>
       </c>
       <c r="G51">
-        <v>2.36619626030656</v>
+        <v>2.27212783683166</v>
       </c>
       <c r="H51">
-        <v>0.382915689093577</v>
+        <v>0.328173450897239</v>
       </c>
       <c r="I51">
-        <v>1.59142706699555</v>
+        <v>1.66324335234095</v>
       </c>
       <c r="J51">
-        <v>2.03312853144423</v>
+        <v>1.80511509406996</v>
       </c>
       <c r="K51">
-        <v>1.15232960645779</v>
+        <v>1.09280351195799</v>
       </c>
       <c r="L51">
-        <v>0.602023330668606</v>
+        <v>0.602887557343727</v>
       </c>
       <c r="M51">
-        <v>0.84766680784815</v>
+        <v>0.794742846305704</v>
       </c>
       <c r="N51">
-        <v>1.57661888224809</v>
+        <v>1.55357044079648</v>
       </c>
       <c r="O51">
-        <v>198.449773382502</v>
+        <v>194.684532393126</v>
       </c>
       <c r="P51">
-        <v>11.7247164766102</v>
+        <v>14.6689705314946</v>
       </c>
     </row>
     <row r="52">

</xml_diff>